<commit_message>
removed duplicate entry for Thomas Nicole
</commit_message>
<xml_diff>
--- a/src/main/resources/results/Ergebnisse Excel 2018.xlsx
+++ b/src/main/resources/results/Ergebnisse Excel 2018.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C0DEEDB2-3DDD-474D-A248-56F301B49F8E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="08.04.WE" sheetId="30" r:id="rId1"/>
     <sheet name="14.04.ES" sheetId="31" r:id="rId2"/>
     <sheet name="14.04.RE" sheetId="32" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2532" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2530" uniqueCount="202">
   <si>
     <t>Ort</t>
   </si>
@@ -628,7 +627,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -717,9 +716,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Standard 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="1"/>
+    <cellStyle name="Standard 4" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -754,7 +753,7 @@
         <xdr:cNvPr id="2" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20B498EC-182A-4181-917A-602AEB452E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{20B498EC-182A-4181-917A-602AEB452E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -828,7 +827,7 @@
         <xdr:cNvPr id="3" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CE2411C-5471-4F3F-8B68-04E35CED8E7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4CE2411C-5471-4F3F-8B68-04E35CED8E7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -902,7 +901,7 @@
         <xdr:cNvPr id="4" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3743E6C-8BFA-4837-A821-7D24D7E03156}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C3743E6C-8BFA-4837-A821-7D24D7E03156}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -981,7 +980,7 @@
         <xdr:cNvPr id="2" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53F4F544-178A-48E5-B1F4-189F85DA7BED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53F4F544-178A-48E5-B1F4-189F85DA7BED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1055,7 +1054,7 @@
         <xdr:cNvPr id="3" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A34C1F7A-D0A8-4FDF-8665-3CF196E869BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A34C1F7A-D0A8-4FDF-8665-3CF196E869BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1129,7 +1128,7 @@
         <xdr:cNvPr id="4" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D3BACFE-B0FF-4B8F-B0D4-112389EA32EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2D3BACFE-B0FF-4B8F-B0D4-112389EA32EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1208,7 +1207,7 @@
         <xdr:cNvPr id="2" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F19E5A8-F619-4868-8110-72BBFF13158C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F19E5A8-F619-4868-8110-72BBFF13158C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1282,7 +1281,7 @@
         <xdr:cNvPr id="3" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEE1E2BB-2400-4A0B-8D99-6B0F60646AB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEE1E2BB-2400-4A0B-8D99-6B0F60646AB0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1356,7 +1355,7 @@
         <xdr:cNvPr id="4" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{458B0779-3FCA-44E4-8C2F-7E1B815FB4B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{458B0779-3FCA-44E4-8C2F-7E1B815FB4B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1415,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1458,7 +1457,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1491,26 +1490,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1543,23 +1525,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1735,530 +1700,530 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="21" width="2.7265625" style="8" customWidth="1"/>
-    <col min="22" max="22" width="4.453125" style="8" customWidth="1"/>
-    <col min="23" max="23" width="7.453125" style="8" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="256" width="11.453125" style="1"/>
-    <col min="257" max="257" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="21" width="2.7109375" style="8" customWidth="1"/>
+    <col min="22" max="22" width="4.42578125" style="8" customWidth="1"/>
+    <col min="23" max="23" width="7.42578125" style="8" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="256" width="11.42578125" style="1"/>
+    <col min="257" max="257" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="260" max="277" width="2.7265625" style="1" customWidth="1"/>
-    <col min="278" max="278" width="4.453125" style="1" customWidth="1"/>
+    <col min="260" max="277" width="2.7109375" style="1" customWidth="1"/>
+    <col min="278" max="278" width="4.42578125" style="1" customWidth="1"/>
     <col min="279" max="279" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="280" max="280" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="281" max="512" width="11.453125" style="1"/>
-    <col min="513" max="513" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="281" max="512" width="11.42578125" style="1"/>
+    <col min="513" max="513" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="515" max="515" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="516" max="533" width="2.7265625" style="1" customWidth="1"/>
-    <col min="534" max="534" width="4.453125" style="1" customWidth="1"/>
+    <col min="516" max="533" width="2.7109375" style="1" customWidth="1"/>
+    <col min="534" max="534" width="4.42578125" style="1" customWidth="1"/>
     <col min="535" max="535" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="536" max="536" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="537" max="768" width="11.453125" style="1"/>
-    <col min="769" max="769" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="536" max="536" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="537" max="768" width="11.42578125" style="1"/>
+    <col min="769" max="769" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="771" max="771" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="772" max="789" width="2.7265625" style="1" customWidth="1"/>
-    <col min="790" max="790" width="4.453125" style="1" customWidth="1"/>
+    <col min="772" max="789" width="2.7109375" style="1" customWidth="1"/>
+    <col min="790" max="790" width="4.42578125" style="1" customWidth="1"/>
     <col min="791" max="791" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="792" max="792" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="793" max="1024" width="11.453125" style="1"/>
-    <col min="1025" max="1025" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="792" max="792" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="793" max="1024" width="11.42578125" style="1"/>
+    <col min="1025" max="1025" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1027" max="1027" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1045" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1046" max="1046" width="4.453125" style="1" customWidth="1"/>
+    <col min="1028" max="1045" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1046" max="1046" width="4.42578125" style="1" customWidth="1"/>
     <col min="1047" max="1047" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1048" max="1048" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1049" max="1280" width="11.453125" style="1"/>
-    <col min="1281" max="1281" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1048" max="1048" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1049" max="1280" width="11.42578125" style="1"/>
+    <col min="1281" max="1281" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1283" max="1283" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1301" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1302" max="1302" width="4.453125" style="1" customWidth="1"/>
+    <col min="1284" max="1301" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1302" max="1302" width="4.42578125" style="1" customWidth="1"/>
     <col min="1303" max="1303" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1304" max="1304" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1305" max="1536" width="11.453125" style="1"/>
-    <col min="1537" max="1537" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1304" max="1304" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1305" max="1536" width="11.42578125" style="1"/>
+    <col min="1537" max="1537" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1539" max="1539" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1557" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1558" max="1558" width="4.453125" style="1" customWidth="1"/>
+    <col min="1540" max="1557" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1558" max="1558" width="4.42578125" style="1" customWidth="1"/>
     <col min="1559" max="1559" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1560" max="1560" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1561" max="1792" width="11.453125" style="1"/>
-    <col min="1793" max="1793" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1560" max="1560" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1561" max="1792" width="11.42578125" style="1"/>
+    <col min="1793" max="1793" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1795" max="1795" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1813" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1814" max="1814" width="4.453125" style="1" customWidth="1"/>
+    <col min="1796" max="1813" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1814" max="1814" width="4.42578125" style="1" customWidth="1"/>
     <col min="1815" max="1815" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1816" max="1816" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1817" max="2048" width="11.453125" style="1"/>
-    <col min="2049" max="2049" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1816" max="1816" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1817" max="2048" width="11.42578125" style="1"/>
+    <col min="2049" max="2049" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2051" max="2051" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2069" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2070" max="2070" width="4.453125" style="1" customWidth="1"/>
+    <col min="2052" max="2069" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2070" max="2070" width="4.42578125" style="1" customWidth="1"/>
     <col min="2071" max="2071" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2072" max="2072" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2073" max="2304" width="11.453125" style="1"/>
-    <col min="2305" max="2305" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2072" max="2072" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2073" max="2304" width="11.42578125" style="1"/>
+    <col min="2305" max="2305" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2307" max="2307" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2325" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2326" max="2326" width="4.453125" style="1" customWidth="1"/>
+    <col min="2308" max="2325" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2326" max="2326" width="4.42578125" style="1" customWidth="1"/>
     <col min="2327" max="2327" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2328" max="2328" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2329" max="2560" width="11.453125" style="1"/>
-    <col min="2561" max="2561" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2328" max="2328" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2329" max="2560" width="11.42578125" style="1"/>
+    <col min="2561" max="2561" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2563" max="2563" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2581" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2582" max="2582" width="4.453125" style="1" customWidth="1"/>
+    <col min="2564" max="2581" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2582" max="2582" width="4.42578125" style="1" customWidth="1"/>
     <col min="2583" max="2583" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2584" max="2584" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2585" max="2816" width="11.453125" style="1"/>
-    <col min="2817" max="2817" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2584" max="2584" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2585" max="2816" width="11.42578125" style="1"/>
+    <col min="2817" max="2817" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2819" max="2819" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2837" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2838" max="2838" width="4.453125" style="1" customWidth="1"/>
+    <col min="2820" max="2837" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2838" max="2838" width="4.42578125" style="1" customWidth="1"/>
     <col min="2839" max="2839" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2840" max="2840" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2841" max="3072" width="11.453125" style="1"/>
-    <col min="3073" max="3073" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2840" max="2840" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2841" max="3072" width="11.42578125" style="1"/>
+    <col min="3073" max="3073" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3075" max="3075" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3093" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3094" max="3094" width="4.453125" style="1" customWidth="1"/>
+    <col min="3076" max="3093" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3094" max="3094" width="4.42578125" style="1" customWidth="1"/>
     <col min="3095" max="3095" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3096" max="3096" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3097" max="3328" width="11.453125" style="1"/>
-    <col min="3329" max="3329" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3096" max="3096" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3097" max="3328" width="11.42578125" style="1"/>
+    <col min="3329" max="3329" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3331" max="3331" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3349" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3350" max="3350" width="4.453125" style="1" customWidth="1"/>
+    <col min="3332" max="3349" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3350" max="3350" width="4.42578125" style="1" customWidth="1"/>
     <col min="3351" max="3351" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3352" max="3352" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3353" max="3584" width="11.453125" style="1"/>
-    <col min="3585" max="3585" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3352" max="3352" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3353" max="3584" width="11.42578125" style="1"/>
+    <col min="3585" max="3585" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3587" max="3587" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3605" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3606" max="3606" width="4.453125" style="1" customWidth="1"/>
+    <col min="3588" max="3605" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3606" max="3606" width="4.42578125" style="1" customWidth="1"/>
     <col min="3607" max="3607" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3608" max="3608" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3609" max="3840" width="11.453125" style="1"/>
-    <col min="3841" max="3841" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3608" max="3608" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3609" max="3840" width="11.42578125" style="1"/>
+    <col min="3841" max="3841" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3843" max="3843" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3861" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3862" max="3862" width="4.453125" style="1" customWidth="1"/>
+    <col min="3844" max="3861" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3862" max="3862" width="4.42578125" style="1" customWidth="1"/>
     <col min="3863" max="3863" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3864" max="3864" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3865" max="4096" width="11.453125" style="1"/>
-    <col min="4097" max="4097" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3864" max="3864" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3865" max="4096" width="11.42578125" style="1"/>
+    <col min="4097" max="4097" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4099" max="4099" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4117" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4118" max="4118" width="4.453125" style="1" customWidth="1"/>
+    <col min="4100" max="4117" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4118" max="4118" width="4.42578125" style="1" customWidth="1"/>
     <col min="4119" max="4119" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4120" max="4120" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4121" max="4352" width="11.453125" style="1"/>
-    <col min="4353" max="4353" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4120" max="4120" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4121" max="4352" width="11.42578125" style="1"/>
+    <col min="4353" max="4353" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4355" max="4355" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4373" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4374" max="4374" width="4.453125" style="1" customWidth="1"/>
+    <col min="4356" max="4373" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4374" max="4374" width="4.42578125" style="1" customWidth="1"/>
     <col min="4375" max="4375" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4376" max="4376" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4377" max="4608" width="11.453125" style="1"/>
-    <col min="4609" max="4609" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4376" max="4376" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4377" max="4608" width="11.42578125" style="1"/>
+    <col min="4609" max="4609" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4611" max="4611" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4629" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4630" max="4630" width="4.453125" style="1" customWidth="1"/>
+    <col min="4612" max="4629" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4630" max="4630" width="4.42578125" style="1" customWidth="1"/>
     <col min="4631" max="4631" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4632" max="4632" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4633" max="4864" width="11.453125" style="1"/>
-    <col min="4865" max="4865" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4632" max="4632" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4633" max="4864" width="11.42578125" style="1"/>
+    <col min="4865" max="4865" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4867" max="4867" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4885" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4886" max="4886" width="4.453125" style="1" customWidth="1"/>
+    <col min="4868" max="4885" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4886" max="4886" width="4.42578125" style="1" customWidth="1"/>
     <col min="4887" max="4887" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4888" max="4888" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4889" max="5120" width="11.453125" style="1"/>
-    <col min="5121" max="5121" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4888" max="4888" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4889" max="5120" width="11.42578125" style="1"/>
+    <col min="5121" max="5121" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5123" max="5123" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5141" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5142" max="5142" width="4.453125" style="1" customWidth="1"/>
+    <col min="5124" max="5141" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5142" max="5142" width="4.42578125" style="1" customWidth="1"/>
     <col min="5143" max="5143" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5144" max="5144" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5145" max="5376" width="11.453125" style="1"/>
-    <col min="5377" max="5377" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5144" max="5144" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5145" max="5376" width="11.42578125" style="1"/>
+    <col min="5377" max="5377" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5379" max="5379" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5397" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5398" max="5398" width="4.453125" style="1" customWidth="1"/>
+    <col min="5380" max="5397" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5398" max="5398" width="4.42578125" style="1" customWidth="1"/>
     <col min="5399" max="5399" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5400" max="5400" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5401" max="5632" width="11.453125" style="1"/>
-    <col min="5633" max="5633" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5400" max="5400" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5401" max="5632" width="11.42578125" style="1"/>
+    <col min="5633" max="5633" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5635" max="5635" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5653" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5654" max="5654" width="4.453125" style="1" customWidth="1"/>
+    <col min="5636" max="5653" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5654" max="5654" width="4.42578125" style="1" customWidth="1"/>
     <col min="5655" max="5655" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5656" max="5656" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5657" max="5888" width="11.453125" style="1"/>
-    <col min="5889" max="5889" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5656" max="5656" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5657" max="5888" width="11.42578125" style="1"/>
+    <col min="5889" max="5889" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5891" max="5891" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5909" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5910" max="5910" width="4.453125" style="1" customWidth="1"/>
+    <col min="5892" max="5909" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5910" max="5910" width="4.42578125" style="1" customWidth="1"/>
     <col min="5911" max="5911" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5912" max="5912" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5913" max="6144" width="11.453125" style="1"/>
-    <col min="6145" max="6145" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5912" max="5912" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5913" max="6144" width="11.42578125" style="1"/>
+    <col min="6145" max="6145" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6147" max="6147" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6165" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6166" max="6166" width="4.453125" style="1" customWidth="1"/>
+    <col min="6148" max="6165" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6166" max="6166" width="4.42578125" style="1" customWidth="1"/>
     <col min="6167" max="6167" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6168" max="6168" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6169" max="6400" width="11.453125" style="1"/>
-    <col min="6401" max="6401" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6168" max="6168" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6169" max="6400" width="11.42578125" style="1"/>
+    <col min="6401" max="6401" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6403" max="6403" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6421" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6422" max="6422" width="4.453125" style="1" customWidth="1"/>
+    <col min="6404" max="6421" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6422" max="6422" width="4.42578125" style="1" customWidth="1"/>
     <col min="6423" max="6423" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6424" max="6424" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6425" max="6656" width="11.453125" style="1"/>
-    <col min="6657" max="6657" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6424" max="6424" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6425" max="6656" width="11.42578125" style="1"/>
+    <col min="6657" max="6657" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6659" max="6659" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6677" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6678" max="6678" width="4.453125" style="1" customWidth="1"/>
+    <col min="6660" max="6677" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6678" max="6678" width="4.42578125" style="1" customWidth="1"/>
     <col min="6679" max="6679" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6680" max="6680" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6681" max="6912" width="11.453125" style="1"/>
-    <col min="6913" max="6913" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6680" max="6680" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6681" max="6912" width="11.42578125" style="1"/>
+    <col min="6913" max="6913" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6915" max="6915" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6933" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6934" max="6934" width="4.453125" style="1" customWidth="1"/>
+    <col min="6916" max="6933" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6934" max="6934" width="4.42578125" style="1" customWidth="1"/>
     <col min="6935" max="6935" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6936" max="6936" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6937" max="7168" width="11.453125" style="1"/>
-    <col min="7169" max="7169" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6936" max="6936" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6937" max="7168" width="11.42578125" style="1"/>
+    <col min="7169" max="7169" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7171" max="7171" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7189" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7190" max="7190" width="4.453125" style="1" customWidth="1"/>
+    <col min="7172" max="7189" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7190" max="7190" width="4.42578125" style="1" customWidth="1"/>
     <col min="7191" max="7191" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7192" max="7192" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7193" max="7424" width="11.453125" style="1"/>
-    <col min="7425" max="7425" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7192" max="7192" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7193" max="7424" width="11.42578125" style="1"/>
+    <col min="7425" max="7425" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7427" max="7427" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7445" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7446" max="7446" width="4.453125" style="1" customWidth="1"/>
+    <col min="7428" max="7445" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7446" max="7446" width="4.42578125" style="1" customWidth="1"/>
     <col min="7447" max="7447" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7448" max="7448" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7449" max="7680" width="11.453125" style="1"/>
-    <col min="7681" max="7681" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7448" max="7448" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7449" max="7680" width="11.42578125" style="1"/>
+    <col min="7681" max="7681" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7683" max="7683" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7701" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7702" max="7702" width="4.453125" style="1" customWidth="1"/>
+    <col min="7684" max="7701" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7702" max="7702" width="4.42578125" style="1" customWidth="1"/>
     <col min="7703" max="7703" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7704" max="7704" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7705" max="7936" width="11.453125" style="1"/>
-    <col min="7937" max="7937" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7704" max="7704" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7705" max="7936" width="11.42578125" style="1"/>
+    <col min="7937" max="7937" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7939" max="7939" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7957" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7958" max="7958" width="4.453125" style="1" customWidth="1"/>
+    <col min="7940" max="7957" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7958" max="7958" width="4.42578125" style="1" customWidth="1"/>
     <col min="7959" max="7959" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7960" max="7960" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7961" max="8192" width="11.453125" style="1"/>
-    <col min="8193" max="8193" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7960" max="7960" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7961" max="8192" width="11.42578125" style="1"/>
+    <col min="8193" max="8193" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8195" max="8195" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8213" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8214" max="8214" width="4.453125" style="1" customWidth="1"/>
+    <col min="8196" max="8213" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8214" max="8214" width="4.42578125" style="1" customWidth="1"/>
     <col min="8215" max="8215" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8216" max="8216" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8217" max="8448" width="11.453125" style="1"/>
-    <col min="8449" max="8449" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8216" max="8216" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8217" max="8448" width="11.42578125" style="1"/>
+    <col min="8449" max="8449" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8451" max="8451" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8469" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8470" max="8470" width="4.453125" style="1" customWidth="1"/>
+    <col min="8452" max="8469" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8470" max="8470" width="4.42578125" style="1" customWidth="1"/>
     <col min="8471" max="8471" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8472" max="8472" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8473" max="8704" width="11.453125" style="1"/>
-    <col min="8705" max="8705" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8472" max="8472" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8473" max="8704" width="11.42578125" style="1"/>
+    <col min="8705" max="8705" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8707" max="8707" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8725" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8726" max="8726" width="4.453125" style="1" customWidth="1"/>
+    <col min="8708" max="8725" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8726" max="8726" width="4.42578125" style="1" customWidth="1"/>
     <col min="8727" max="8727" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8728" max="8728" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8729" max="8960" width="11.453125" style="1"/>
-    <col min="8961" max="8961" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8728" max="8728" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8729" max="8960" width="11.42578125" style="1"/>
+    <col min="8961" max="8961" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8963" max="8963" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8981" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8982" max="8982" width="4.453125" style="1" customWidth="1"/>
+    <col min="8964" max="8981" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8982" max="8982" width="4.42578125" style="1" customWidth="1"/>
     <col min="8983" max="8983" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8984" max="8984" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8985" max="9216" width="11.453125" style="1"/>
-    <col min="9217" max="9217" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8984" max="8984" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8985" max="9216" width="11.42578125" style="1"/>
+    <col min="9217" max="9217" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9219" max="9219" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9237" width="2.7265625" style="1" customWidth="1"/>
-    <col min="9238" max="9238" width="4.453125" style="1" customWidth="1"/>
+    <col min="9220" max="9237" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9238" max="9238" width="4.42578125" style="1" customWidth="1"/>
     <col min="9239" max="9239" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9240" max="9240" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9241" max="9472" width="11.453125" style="1"/>
-    <col min="9473" max="9473" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9240" max="9240" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9241" max="9472" width="11.42578125" style="1"/>
+    <col min="9473" max="9473" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9475" max="9475" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9493" width="2.7265625" style="1" customWidth="1"/>
-    <col min="9494" max="9494" width="4.453125" style="1" customWidth="1"/>
+    <col min="9476" max="9493" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9494" max="9494" width="4.42578125" style="1" customWidth="1"/>
     <col min="9495" max="9495" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9496" max="9496" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9497" max="9728" width="11.453125" style="1"/>
-    <col min="9729" max="9729" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9496" max="9496" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9497" max="9728" width="11.42578125" style="1"/>
+    <col min="9729" max="9729" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9731" max="9731" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9749" width="2.7265625" style="1" customWidth="1"/>
-    <col min="9750" max="9750" width="4.453125" style="1" customWidth="1"/>
+    <col min="9732" max="9749" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9750" max="9750" width="4.42578125" style="1" customWidth="1"/>
     <col min="9751" max="9751" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9752" max="9752" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9753" max="9984" width="11.453125" style="1"/>
-    <col min="9985" max="9985" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9752" max="9752" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9753" max="9984" width="11.42578125" style="1"/>
+    <col min="9985" max="9985" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9987" max="9987" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9988" max="10005" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10006" max="10006" width="4.453125" style="1" customWidth="1"/>
+    <col min="9988" max="10005" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10006" max="10006" width="4.42578125" style="1" customWidth="1"/>
     <col min="10007" max="10007" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10008" max="10008" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10009" max="10240" width="11.453125" style="1"/>
-    <col min="10241" max="10241" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10008" max="10008" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10009" max="10240" width="11.42578125" style="1"/>
+    <col min="10241" max="10241" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10243" max="10243" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10261" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10262" max="10262" width="4.453125" style="1" customWidth="1"/>
+    <col min="10244" max="10261" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10262" max="10262" width="4.42578125" style="1" customWidth="1"/>
     <col min="10263" max="10263" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10264" max="10264" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10265" max="10496" width="11.453125" style="1"/>
-    <col min="10497" max="10497" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10264" max="10264" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10265" max="10496" width="11.42578125" style="1"/>
+    <col min="10497" max="10497" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10499" max="10499" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10517" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10518" max="10518" width="4.453125" style="1" customWidth="1"/>
+    <col min="10500" max="10517" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10518" max="10518" width="4.42578125" style="1" customWidth="1"/>
     <col min="10519" max="10519" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10520" max="10520" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10521" max="10752" width="11.453125" style="1"/>
-    <col min="10753" max="10753" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10520" max="10520" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10521" max="10752" width="11.42578125" style="1"/>
+    <col min="10753" max="10753" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10755" max="10755" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10773" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10774" max="10774" width="4.453125" style="1" customWidth="1"/>
+    <col min="10756" max="10773" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10774" max="10774" width="4.42578125" style="1" customWidth="1"/>
     <col min="10775" max="10775" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10776" max="10776" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10777" max="11008" width="11.453125" style="1"/>
-    <col min="11009" max="11009" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10776" max="10776" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10777" max="11008" width="11.42578125" style="1"/>
+    <col min="11009" max="11009" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11011" max="11011" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11029" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11030" max="11030" width="4.453125" style="1" customWidth="1"/>
+    <col min="11012" max="11029" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11030" max="11030" width="4.42578125" style="1" customWidth="1"/>
     <col min="11031" max="11031" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11032" max="11032" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11033" max="11264" width="11.453125" style="1"/>
-    <col min="11265" max="11265" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11032" max="11032" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11033" max="11264" width="11.42578125" style="1"/>
+    <col min="11265" max="11265" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11267" max="11267" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11285" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11286" max="11286" width="4.453125" style="1" customWidth="1"/>
+    <col min="11268" max="11285" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11286" max="11286" width="4.42578125" style="1" customWidth="1"/>
     <col min="11287" max="11287" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11288" max="11288" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11289" max="11520" width="11.453125" style="1"/>
-    <col min="11521" max="11521" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11288" max="11288" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11289" max="11520" width="11.42578125" style="1"/>
+    <col min="11521" max="11521" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11523" max="11523" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11541" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11542" max="11542" width="4.453125" style="1" customWidth="1"/>
+    <col min="11524" max="11541" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11542" max="11542" width="4.42578125" style="1" customWidth="1"/>
     <col min="11543" max="11543" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11544" max="11544" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11545" max="11776" width="11.453125" style="1"/>
-    <col min="11777" max="11777" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11544" max="11544" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11545" max="11776" width="11.42578125" style="1"/>
+    <col min="11777" max="11777" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11779" max="11779" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11797" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11798" max="11798" width="4.453125" style="1" customWidth="1"/>
+    <col min="11780" max="11797" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11798" max="11798" width="4.42578125" style="1" customWidth="1"/>
     <col min="11799" max="11799" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11800" max="11800" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11801" max="12032" width="11.453125" style="1"/>
-    <col min="12033" max="12033" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11800" max="11800" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11801" max="12032" width="11.42578125" style="1"/>
+    <col min="12033" max="12033" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12035" max="12035" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12053" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12054" max="12054" width="4.453125" style="1" customWidth="1"/>
+    <col min="12036" max="12053" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12054" max="12054" width="4.42578125" style="1" customWidth="1"/>
     <col min="12055" max="12055" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12056" max="12056" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12057" max="12288" width="11.453125" style="1"/>
-    <col min="12289" max="12289" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12056" max="12056" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12057" max="12288" width="11.42578125" style="1"/>
+    <col min="12289" max="12289" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12291" max="12291" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12309" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12310" max="12310" width="4.453125" style="1" customWidth="1"/>
+    <col min="12292" max="12309" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12310" max="12310" width="4.42578125" style="1" customWidth="1"/>
     <col min="12311" max="12311" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12312" max="12312" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12313" max="12544" width="11.453125" style="1"/>
-    <col min="12545" max="12545" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12312" max="12312" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12313" max="12544" width="11.42578125" style="1"/>
+    <col min="12545" max="12545" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12547" max="12547" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12565" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12566" max="12566" width="4.453125" style="1" customWidth="1"/>
+    <col min="12548" max="12565" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12566" max="12566" width="4.42578125" style="1" customWidth="1"/>
     <col min="12567" max="12567" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12568" max="12568" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12569" max="12800" width="11.453125" style="1"/>
-    <col min="12801" max="12801" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12568" max="12568" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12569" max="12800" width="11.42578125" style="1"/>
+    <col min="12801" max="12801" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12803" max="12803" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12821" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12822" max="12822" width="4.453125" style="1" customWidth="1"/>
+    <col min="12804" max="12821" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12822" max="12822" width="4.42578125" style="1" customWidth="1"/>
     <col min="12823" max="12823" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12824" max="12824" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12825" max="13056" width="11.453125" style="1"/>
-    <col min="13057" max="13057" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12824" max="12824" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12825" max="13056" width="11.42578125" style="1"/>
+    <col min="13057" max="13057" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13059" max="13059" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13077" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13078" max="13078" width="4.453125" style="1" customWidth="1"/>
+    <col min="13060" max="13077" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13078" max="13078" width="4.42578125" style="1" customWidth="1"/>
     <col min="13079" max="13079" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13080" max="13080" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13081" max="13312" width="11.453125" style="1"/>
-    <col min="13313" max="13313" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13080" max="13080" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13081" max="13312" width="11.42578125" style="1"/>
+    <col min="13313" max="13313" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13315" max="13315" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13333" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13334" max="13334" width="4.453125" style="1" customWidth="1"/>
+    <col min="13316" max="13333" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13334" max="13334" width="4.42578125" style="1" customWidth="1"/>
     <col min="13335" max="13335" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13336" max="13336" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13337" max="13568" width="11.453125" style="1"/>
-    <col min="13569" max="13569" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13336" max="13336" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13337" max="13568" width="11.42578125" style="1"/>
+    <col min="13569" max="13569" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13571" max="13571" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13589" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13590" max="13590" width="4.453125" style="1" customWidth="1"/>
+    <col min="13572" max="13589" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13590" max="13590" width="4.42578125" style="1" customWidth="1"/>
     <col min="13591" max="13591" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13592" max="13592" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13593" max="13824" width="11.453125" style="1"/>
-    <col min="13825" max="13825" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13592" max="13592" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13593" max="13824" width="11.42578125" style="1"/>
+    <col min="13825" max="13825" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13827" max="13827" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13845" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13846" max="13846" width="4.453125" style="1" customWidth="1"/>
+    <col min="13828" max="13845" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13846" max="13846" width="4.42578125" style="1" customWidth="1"/>
     <col min="13847" max="13847" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13848" max="13848" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13849" max="14080" width="11.453125" style="1"/>
-    <col min="14081" max="14081" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13848" max="13848" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13849" max="14080" width="11.42578125" style="1"/>
+    <col min="14081" max="14081" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14083" max="14083" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14101" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14102" max="14102" width="4.453125" style="1" customWidth="1"/>
+    <col min="14084" max="14101" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14102" max="14102" width="4.42578125" style="1" customWidth="1"/>
     <col min="14103" max="14103" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14104" max="14104" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14105" max="14336" width="11.453125" style="1"/>
-    <col min="14337" max="14337" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14104" max="14104" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14105" max="14336" width="11.42578125" style="1"/>
+    <col min="14337" max="14337" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14339" max="14339" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14357" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14358" max="14358" width="4.453125" style="1" customWidth="1"/>
+    <col min="14340" max="14357" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14358" max="14358" width="4.42578125" style="1" customWidth="1"/>
     <col min="14359" max="14359" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14360" max="14360" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14361" max="14592" width="11.453125" style="1"/>
-    <col min="14593" max="14593" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14360" max="14360" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14361" max="14592" width="11.42578125" style="1"/>
+    <col min="14593" max="14593" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14595" max="14595" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14613" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14614" max="14614" width="4.453125" style="1" customWidth="1"/>
+    <col min="14596" max="14613" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14614" max="14614" width="4.42578125" style="1" customWidth="1"/>
     <col min="14615" max="14615" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14616" max="14616" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14617" max="14848" width="11.453125" style="1"/>
-    <col min="14849" max="14849" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14616" max="14616" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14617" max="14848" width="11.42578125" style="1"/>
+    <col min="14849" max="14849" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14851" max="14851" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14869" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14870" max="14870" width="4.453125" style="1" customWidth="1"/>
+    <col min="14852" max="14869" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14870" max="14870" width="4.42578125" style="1" customWidth="1"/>
     <col min="14871" max="14871" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14872" max="14872" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14873" max="15104" width="11.453125" style="1"/>
-    <col min="15105" max="15105" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14872" max="14872" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14873" max="15104" width="11.42578125" style="1"/>
+    <col min="15105" max="15105" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15107" max="15107" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15125" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15126" max="15126" width="4.453125" style="1" customWidth="1"/>
+    <col min="15108" max="15125" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15126" max="15126" width="4.42578125" style="1" customWidth="1"/>
     <col min="15127" max="15127" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15128" max="15128" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15129" max="15360" width="11.453125" style="1"/>
-    <col min="15361" max="15361" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15128" max="15128" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15129" max="15360" width="11.42578125" style="1"/>
+    <col min="15361" max="15361" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15363" max="15363" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15381" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15382" max="15382" width="4.453125" style="1" customWidth="1"/>
+    <col min="15364" max="15381" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15382" max="15382" width="4.42578125" style="1" customWidth="1"/>
     <col min="15383" max="15383" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15384" max="15384" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15385" max="15616" width="11.453125" style="1"/>
-    <col min="15617" max="15617" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15384" max="15384" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15385" max="15616" width="11.42578125" style="1"/>
+    <col min="15617" max="15617" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15619" max="15619" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15637" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15638" max="15638" width="4.453125" style="1" customWidth="1"/>
+    <col min="15620" max="15637" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15638" max="15638" width="4.42578125" style="1" customWidth="1"/>
     <col min="15639" max="15639" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15640" max="15640" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15641" max="15872" width="11.453125" style="1"/>
-    <col min="15873" max="15873" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15640" max="15640" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15641" max="15872" width="11.42578125" style="1"/>
+    <col min="15873" max="15873" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15875" max="15875" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15893" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15894" max="15894" width="4.453125" style="1" customWidth="1"/>
+    <col min="15876" max="15893" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15894" max="15894" width="4.42578125" style="1" customWidth="1"/>
     <col min="15895" max="15895" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15896" max="15896" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15897" max="16128" width="11.453125" style="1"/>
-    <col min="16129" max="16129" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15896" max="15896" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15897" max="16128" width="11.42578125" style="1"/>
+    <col min="16129" max="16129" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16131" max="16131" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16149" width="2.7265625" style="1" customWidth="1"/>
-    <col min="16150" max="16150" width="4.453125" style="1" customWidth="1"/>
+    <col min="16132" max="16149" width="2.7109375" style="1" customWidth="1"/>
+    <col min="16150" max="16150" width="4.42578125" style="1" customWidth="1"/>
     <col min="16151" max="16151" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="16152" max="16152" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16153" max="16384" width="11.453125" style="1"/>
+    <col min="16152" max="16152" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16153" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2292,7 +2257,7 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
     </row>
-    <row r="2" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2322,7 +2287,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
     </row>
-    <row r="3" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2352,7 +2317,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
     </row>
-    <row r="4" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2382,7 +2347,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2390,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2473,7 +2438,7 @@
       </c>
       <c r="AB7" s="12"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2548,7 +2513,7 @@
       </c>
       <c r="Y8" s="8"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2698,7 +2663,7 @@
       </c>
       <c r="Y10" s="8"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -2773,7 +2738,7 @@
       </c>
       <c r="Y11" s="8"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -2848,7 +2813,7 @@
       </c>
       <c r="Y12" s="8"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -2923,7 +2888,7 @@
       </c>
       <c r="Y13" s="8"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -2998,7 +2963,7 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -3073,7 +3038,7 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -3148,7 +3113,7 @@
       </c>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -3223,7 +3188,7 @@
       </c>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -3298,7 +3263,7 @@
       </c>
       <c r="Y18" s="8"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
@@ -3373,7 +3338,7 @@
       </c>
       <c r="Y19" s="8"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
@@ -3448,7 +3413,7 @@
       </c>
       <c r="Y20" s="8"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -3598,7 +3563,7 @@
       </c>
       <c r="Y22" s="8"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
@@ -3748,7 +3713,7 @@
       </c>
       <c r="Y24" s="8"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
@@ -3823,7 +3788,7 @@
       </c>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
@@ -8986,7 +8951,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B50 IX8:IX50 ST8:ST50 ACP8:ACP50 AML8:AML50 AWH8:AWH50 BGD8:BGD50 BPZ8:BPZ50 BZV8:BZV50 CJR8:CJR50 CTN8:CTN50 DDJ8:DDJ50 DNF8:DNF50 DXB8:DXB50 EGX8:EGX50 EQT8:EQT50 FAP8:FAP50 FKL8:FKL50 FUH8:FUH50 GED8:GED50 GNZ8:GNZ50 GXV8:GXV50 HHR8:HHR50 HRN8:HRN50 IBJ8:IBJ50 ILF8:ILF50 IVB8:IVB50 JEX8:JEX50 JOT8:JOT50 JYP8:JYP50 KIL8:KIL50 KSH8:KSH50 LCD8:LCD50 LLZ8:LLZ50 LVV8:LVV50 MFR8:MFR50 MPN8:MPN50 MZJ8:MZJ50 NJF8:NJF50 NTB8:NTB50 OCX8:OCX50 OMT8:OMT50 OWP8:OWP50 PGL8:PGL50 PQH8:PQH50 QAD8:QAD50 QJZ8:QJZ50 QTV8:QTV50 RDR8:RDR50 RNN8:RNN50 RXJ8:RXJ50 SHF8:SHF50 SRB8:SRB50 TAX8:TAX50 TKT8:TKT50 TUP8:TUP50 UEL8:UEL50 UOH8:UOH50 UYD8:UYD50 VHZ8:VHZ50 VRV8:VRV50 WBR8:WBR50 WLN8:WLN50 WVJ8:WVJ50 B65544:B65586 IX65544:IX65586 ST65544:ST65586 ACP65544:ACP65586 AML65544:AML65586 AWH65544:AWH65586 BGD65544:BGD65586 BPZ65544:BPZ65586 BZV65544:BZV65586 CJR65544:CJR65586 CTN65544:CTN65586 DDJ65544:DDJ65586 DNF65544:DNF65586 DXB65544:DXB65586 EGX65544:EGX65586 EQT65544:EQT65586 FAP65544:FAP65586 FKL65544:FKL65586 FUH65544:FUH65586 GED65544:GED65586 GNZ65544:GNZ65586 GXV65544:GXV65586 HHR65544:HHR65586 HRN65544:HRN65586 IBJ65544:IBJ65586 ILF65544:ILF65586 IVB65544:IVB65586 JEX65544:JEX65586 JOT65544:JOT65586 JYP65544:JYP65586 KIL65544:KIL65586 KSH65544:KSH65586 LCD65544:LCD65586 LLZ65544:LLZ65586 LVV65544:LVV65586 MFR65544:MFR65586 MPN65544:MPN65586 MZJ65544:MZJ65586 NJF65544:NJF65586 NTB65544:NTB65586 OCX65544:OCX65586 OMT65544:OMT65586 OWP65544:OWP65586 PGL65544:PGL65586 PQH65544:PQH65586 QAD65544:QAD65586 QJZ65544:QJZ65586 QTV65544:QTV65586 RDR65544:RDR65586 RNN65544:RNN65586 RXJ65544:RXJ65586 SHF65544:SHF65586 SRB65544:SRB65586 TAX65544:TAX65586 TKT65544:TKT65586 TUP65544:TUP65586 UEL65544:UEL65586 UOH65544:UOH65586 UYD65544:UYD65586 VHZ65544:VHZ65586 VRV65544:VRV65586 WBR65544:WBR65586 WLN65544:WLN65586 WVJ65544:WVJ65586 B131080:B131122 IX131080:IX131122 ST131080:ST131122 ACP131080:ACP131122 AML131080:AML131122 AWH131080:AWH131122 BGD131080:BGD131122 BPZ131080:BPZ131122 BZV131080:BZV131122 CJR131080:CJR131122 CTN131080:CTN131122 DDJ131080:DDJ131122 DNF131080:DNF131122 DXB131080:DXB131122 EGX131080:EGX131122 EQT131080:EQT131122 FAP131080:FAP131122 FKL131080:FKL131122 FUH131080:FUH131122 GED131080:GED131122 GNZ131080:GNZ131122 GXV131080:GXV131122 HHR131080:HHR131122 HRN131080:HRN131122 IBJ131080:IBJ131122 ILF131080:ILF131122 IVB131080:IVB131122 JEX131080:JEX131122 JOT131080:JOT131122 JYP131080:JYP131122 KIL131080:KIL131122 KSH131080:KSH131122 LCD131080:LCD131122 LLZ131080:LLZ131122 LVV131080:LVV131122 MFR131080:MFR131122 MPN131080:MPN131122 MZJ131080:MZJ131122 NJF131080:NJF131122 NTB131080:NTB131122 OCX131080:OCX131122 OMT131080:OMT131122 OWP131080:OWP131122 PGL131080:PGL131122 PQH131080:PQH131122 QAD131080:QAD131122 QJZ131080:QJZ131122 QTV131080:QTV131122 RDR131080:RDR131122 RNN131080:RNN131122 RXJ131080:RXJ131122 SHF131080:SHF131122 SRB131080:SRB131122 TAX131080:TAX131122 TKT131080:TKT131122 TUP131080:TUP131122 UEL131080:UEL131122 UOH131080:UOH131122 UYD131080:UYD131122 VHZ131080:VHZ131122 VRV131080:VRV131122 WBR131080:WBR131122 WLN131080:WLN131122 WVJ131080:WVJ131122 B196616:B196658 IX196616:IX196658 ST196616:ST196658 ACP196616:ACP196658 AML196616:AML196658 AWH196616:AWH196658 BGD196616:BGD196658 BPZ196616:BPZ196658 BZV196616:BZV196658 CJR196616:CJR196658 CTN196616:CTN196658 DDJ196616:DDJ196658 DNF196616:DNF196658 DXB196616:DXB196658 EGX196616:EGX196658 EQT196616:EQT196658 FAP196616:FAP196658 FKL196616:FKL196658 FUH196616:FUH196658 GED196616:GED196658 GNZ196616:GNZ196658 GXV196616:GXV196658 HHR196616:HHR196658 HRN196616:HRN196658 IBJ196616:IBJ196658 ILF196616:ILF196658 IVB196616:IVB196658 JEX196616:JEX196658 JOT196616:JOT196658 JYP196616:JYP196658 KIL196616:KIL196658 KSH196616:KSH196658 LCD196616:LCD196658 LLZ196616:LLZ196658 LVV196616:LVV196658 MFR196616:MFR196658 MPN196616:MPN196658 MZJ196616:MZJ196658 NJF196616:NJF196658 NTB196616:NTB196658 OCX196616:OCX196658 OMT196616:OMT196658 OWP196616:OWP196658 PGL196616:PGL196658 PQH196616:PQH196658 QAD196616:QAD196658 QJZ196616:QJZ196658 QTV196616:QTV196658 RDR196616:RDR196658 RNN196616:RNN196658 RXJ196616:RXJ196658 SHF196616:SHF196658 SRB196616:SRB196658 TAX196616:TAX196658 TKT196616:TKT196658 TUP196616:TUP196658 UEL196616:UEL196658 UOH196616:UOH196658 UYD196616:UYD196658 VHZ196616:VHZ196658 VRV196616:VRV196658 WBR196616:WBR196658 WLN196616:WLN196658 WVJ196616:WVJ196658 B262152:B262194 IX262152:IX262194 ST262152:ST262194 ACP262152:ACP262194 AML262152:AML262194 AWH262152:AWH262194 BGD262152:BGD262194 BPZ262152:BPZ262194 BZV262152:BZV262194 CJR262152:CJR262194 CTN262152:CTN262194 DDJ262152:DDJ262194 DNF262152:DNF262194 DXB262152:DXB262194 EGX262152:EGX262194 EQT262152:EQT262194 FAP262152:FAP262194 FKL262152:FKL262194 FUH262152:FUH262194 GED262152:GED262194 GNZ262152:GNZ262194 GXV262152:GXV262194 HHR262152:HHR262194 HRN262152:HRN262194 IBJ262152:IBJ262194 ILF262152:ILF262194 IVB262152:IVB262194 JEX262152:JEX262194 JOT262152:JOT262194 JYP262152:JYP262194 KIL262152:KIL262194 KSH262152:KSH262194 LCD262152:LCD262194 LLZ262152:LLZ262194 LVV262152:LVV262194 MFR262152:MFR262194 MPN262152:MPN262194 MZJ262152:MZJ262194 NJF262152:NJF262194 NTB262152:NTB262194 OCX262152:OCX262194 OMT262152:OMT262194 OWP262152:OWP262194 PGL262152:PGL262194 PQH262152:PQH262194 QAD262152:QAD262194 QJZ262152:QJZ262194 QTV262152:QTV262194 RDR262152:RDR262194 RNN262152:RNN262194 RXJ262152:RXJ262194 SHF262152:SHF262194 SRB262152:SRB262194 TAX262152:TAX262194 TKT262152:TKT262194 TUP262152:TUP262194 UEL262152:UEL262194 UOH262152:UOH262194 UYD262152:UYD262194 VHZ262152:VHZ262194 VRV262152:VRV262194 WBR262152:WBR262194 WLN262152:WLN262194 WVJ262152:WVJ262194 B327688:B327730 IX327688:IX327730 ST327688:ST327730 ACP327688:ACP327730 AML327688:AML327730 AWH327688:AWH327730 BGD327688:BGD327730 BPZ327688:BPZ327730 BZV327688:BZV327730 CJR327688:CJR327730 CTN327688:CTN327730 DDJ327688:DDJ327730 DNF327688:DNF327730 DXB327688:DXB327730 EGX327688:EGX327730 EQT327688:EQT327730 FAP327688:FAP327730 FKL327688:FKL327730 FUH327688:FUH327730 GED327688:GED327730 GNZ327688:GNZ327730 GXV327688:GXV327730 HHR327688:HHR327730 HRN327688:HRN327730 IBJ327688:IBJ327730 ILF327688:ILF327730 IVB327688:IVB327730 JEX327688:JEX327730 JOT327688:JOT327730 JYP327688:JYP327730 KIL327688:KIL327730 KSH327688:KSH327730 LCD327688:LCD327730 LLZ327688:LLZ327730 LVV327688:LVV327730 MFR327688:MFR327730 MPN327688:MPN327730 MZJ327688:MZJ327730 NJF327688:NJF327730 NTB327688:NTB327730 OCX327688:OCX327730 OMT327688:OMT327730 OWP327688:OWP327730 PGL327688:PGL327730 PQH327688:PQH327730 QAD327688:QAD327730 QJZ327688:QJZ327730 QTV327688:QTV327730 RDR327688:RDR327730 RNN327688:RNN327730 RXJ327688:RXJ327730 SHF327688:SHF327730 SRB327688:SRB327730 TAX327688:TAX327730 TKT327688:TKT327730 TUP327688:TUP327730 UEL327688:UEL327730 UOH327688:UOH327730 UYD327688:UYD327730 VHZ327688:VHZ327730 VRV327688:VRV327730 WBR327688:WBR327730 WLN327688:WLN327730 WVJ327688:WVJ327730 B393224:B393266 IX393224:IX393266 ST393224:ST393266 ACP393224:ACP393266 AML393224:AML393266 AWH393224:AWH393266 BGD393224:BGD393266 BPZ393224:BPZ393266 BZV393224:BZV393266 CJR393224:CJR393266 CTN393224:CTN393266 DDJ393224:DDJ393266 DNF393224:DNF393266 DXB393224:DXB393266 EGX393224:EGX393266 EQT393224:EQT393266 FAP393224:FAP393266 FKL393224:FKL393266 FUH393224:FUH393266 GED393224:GED393266 GNZ393224:GNZ393266 GXV393224:GXV393266 HHR393224:HHR393266 HRN393224:HRN393266 IBJ393224:IBJ393266 ILF393224:ILF393266 IVB393224:IVB393266 JEX393224:JEX393266 JOT393224:JOT393266 JYP393224:JYP393266 KIL393224:KIL393266 KSH393224:KSH393266 LCD393224:LCD393266 LLZ393224:LLZ393266 LVV393224:LVV393266 MFR393224:MFR393266 MPN393224:MPN393266 MZJ393224:MZJ393266 NJF393224:NJF393266 NTB393224:NTB393266 OCX393224:OCX393266 OMT393224:OMT393266 OWP393224:OWP393266 PGL393224:PGL393266 PQH393224:PQH393266 QAD393224:QAD393266 QJZ393224:QJZ393266 QTV393224:QTV393266 RDR393224:RDR393266 RNN393224:RNN393266 RXJ393224:RXJ393266 SHF393224:SHF393266 SRB393224:SRB393266 TAX393224:TAX393266 TKT393224:TKT393266 TUP393224:TUP393266 UEL393224:UEL393266 UOH393224:UOH393266 UYD393224:UYD393266 VHZ393224:VHZ393266 VRV393224:VRV393266 WBR393224:WBR393266 WLN393224:WLN393266 WVJ393224:WVJ393266 B458760:B458802 IX458760:IX458802 ST458760:ST458802 ACP458760:ACP458802 AML458760:AML458802 AWH458760:AWH458802 BGD458760:BGD458802 BPZ458760:BPZ458802 BZV458760:BZV458802 CJR458760:CJR458802 CTN458760:CTN458802 DDJ458760:DDJ458802 DNF458760:DNF458802 DXB458760:DXB458802 EGX458760:EGX458802 EQT458760:EQT458802 FAP458760:FAP458802 FKL458760:FKL458802 FUH458760:FUH458802 GED458760:GED458802 GNZ458760:GNZ458802 GXV458760:GXV458802 HHR458760:HHR458802 HRN458760:HRN458802 IBJ458760:IBJ458802 ILF458760:ILF458802 IVB458760:IVB458802 JEX458760:JEX458802 JOT458760:JOT458802 JYP458760:JYP458802 KIL458760:KIL458802 KSH458760:KSH458802 LCD458760:LCD458802 LLZ458760:LLZ458802 LVV458760:LVV458802 MFR458760:MFR458802 MPN458760:MPN458802 MZJ458760:MZJ458802 NJF458760:NJF458802 NTB458760:NTB458802 OCX458760:OCX458802 OMT458760:OMT458802 OWP458760:OWP458802 PGL458760:PGL458802 PQH458760:PQH458802 QAD458760:QAD458802 QJZ458760:QJZ458802 QTV458760:QTV458802 RDR458760:RDR458802 RNN458760:RNN458802 RXJ458760:RXJ458802 SHF458760:SHF458802 SRB458760:SRB458802 TAX458760:TAX458802 TKT458760:TKT458802 TUP458760:TUP458802 UEL458760:UEL458802 UOH458760:UOH458802 UYD458760:UYD458802 VHZ458760:VHZ458802 VRV458760:VRV458802 WBR458760:WBR458802 WLN458760:WLN458802 WVJ458760:WVJ458802 B524296:B524338 IX524296:IX524338 ST524296:ST524338 ACP524296:ACP524338 AML524296:AML524338 AWH524296:AWH524338 BGD524296:BGD524338 BPZ524296:BPZ524338 BZV524296:BZV524338 CJR524296:CJR524338 CTN524296:CTN524338 DDJ524296:DDJ524338 DNF524296:DNF524338 DXB524296:DXB524338 EGX524296:EGX524338 EQT524296:EQT524338 FAP524296:FAP524338 FKL524296:FKL524338 FUH524296:FUH524338 GED524296:GED524338 GNZ524296:GNZ524338 GXV524296:GXV524338 HHR524296:HHR524338 HRN524296:HRN524338 IBJ524296:IBJ524338 ILF524296:ILF524338 IVB524296:IVB524338 JEX524296:JEX524338 JOT524296:JOT524338 JYP524296:JYP524338 KIL524296:KIL524338 KSH524296:KSH524338 LCD524296:LCD524338 LLZ524296:LLZ524338 LVV524296:LVV524338 MFR524296:MFR524338 MPN524296:MPN524338 MZJ524296:MZJ524338 NJF524296:NJF524338 NTB524296:NTB524338 OCX524296:OCX524338 OMT524296:OMT524338 OWP524296:OWP524338 PGL524296:PGL524338 PQH524296:PQH524338 QAD524296:QAD524338 QJZ524296:QJZ524338 QTV524296:QTV524338 RDR524296:RDR524338 RNN524296:RNN524338 RXJ524296:RXJ524338 SHF524296:SHF524338 SRB524296:SRB524338 TAX524296:TAX524338 TKT524296:TKT524338 TUP524296:TUP524338 UEL524296:UEL524338 UOH524296:UOH524338 UYD524296:UYD524338 VHZ524296:VHZ524338 VRV524296:VRV524338 WBR524296:WBR524338 WLN524296:WLN524338 WVJ524296:WVJ524338 B589832:B589874 IX589832:IX589874 ST589832:ST589874 ACP589832:ACP589874 AML589832:AML589874 AWH589832:AWH589874 BGD589832:BGD589874 BPZ589832:BPZ589874 BZV589832:BZV589874 CJR589832:CJR589874 CTN589832:CTN589874 DDJ589832:DDJ589874 DNF589832:DNF589874 DXB589832:DXB589874 EGX589832:EGX589874 EQT589832:EQT589874 FAP589832:FAP589874 FKL589832:FKL589874 FUH589832:FUH589874 GED589832:GED589874 GNZ589832:GNZ589874 GXV589832:GXV589874 HHR589832:HHR589874 HRN589832:HRN589874 IBJ589832:IBJ589874 ILF589832:ILF589874 IVB589832:IVB589874 JEX589832:JEX589874 JOT589832:JOT589874 JYP589832:JYP589874 KIL589832:KIL589874 KSH589832:KSH589874 LCD589832:LCD589874 LLZ589832:LLZ589874 LVV589832:LVV589874 MFR589832:MFR589874 MPN589832:MPN589874 MZJ589832:MZJ589874 NJF589832:NJF589874 NTB589832:NTB589874 OCX589832:OCX589874 OMT589832:OMT589874 OWP589832:OWP589874 PGL589832:PGL589874 PQH589832:PQH589874 QAD589832:QAD589874 QJZ589832:QJZ589874 QTV589832:QTV589874 RDR589832:RDR589874 RNN589832:RNN589874 RXJ589832:RXJ589874 SHF589832:SHF589874 SRB589832:SRB589874 TAX589832:TAX589874 TKT589832:TKT589874 TUP589832:TUP589874 UEL589832:UEL589874 UOH589832:UOH589874 UYD589832:UYD589874 VHZ589832:VHZ589874 VRV589832:VRV589874 WBR589832:WBR589874 WLN589832:WLN589874 WVJ589832:WVJ589874 B655368:B655410 IX655368:IX655410 ST655368:ST655410 ACP655368:ACP655410 AML655368:AML655410 AWH655368:AWH655410 BGD655368:BGD655410 BPZ655368:BPZ655410 BZV655368:BZV655410 CJR655368:CJR655410 CTN655368:CTN655410 DDJ655368:DDJ655410 DNF655368:DNF655410 DXB655368:DXB655410 EGX655368:EGX655410 EQT655368:EQT655410 FAP655368:FAP655410 FKL655368:FKL655410 FUH655368:FUH655410 GED655368:GED655410 GNZ655368:GNZ655410 GXV655368:GXV655410 HHR655368:HHR655410 HRN655368:HRN655410 IBJ655368:IBJ655410 ILF655368:ILF655410 IVB655368:IVB655410 JEX655368:JEX655410 JOT655368:JOT655410 JYP655368:JYP655410 KIL655368:KIL655410 KSH655368:KSH655410 LCD655368:LCD655410 LLZ655368:LLZ655410 LVV655368:LVV655410 MFR655368:MFR655410 MPN655368:MPN655410 MZJ655368:MZJ655410 NJF655368:NJF655410 NTB655368:NTB655410 OCX655368:OCX655410 OMT655368:OMT655410 OWP655368:OWP655410 PGL655368:PGL655410 PQH655368:PQH655410 QAD655368:QAD655410 QJZ655368:QJZ655410 QTV655368:QTV655410 RDR655368:RDR655410 RNN655368:RNN655410 RXJ655368:RXJ655410 SHF655368:SHF655410 SRB655368:SRB655410 TAX655368:TAX655410 TKT655368:TKT655410 TUP655368:TUP655410 UEL655368:UEL655410 UOH655368:UOH655410 UYD655368:UYD655410 VHZ655368:VHZ655410 VRV655368:VRV655410 WBR655368:WBR655410 WLN655368:WLN655410 WVJ655368:WVJ655410 B720904:B720946 IX720904:IX720946 ST720904:ST720946 ACP720904:ACP720946 AML720904:AML720946 AWH720904:AWH720946 BGD720904:BGD720946 BPZ720904:BPZ720946 BZV720904:BZV720946 CJR720904:CJR720946 CTN720904:CTN720946 DDJ720904:DDJ720946 DNF720904:DNF720946 DXB720904:DXB720946 EGX720904:EGX720946 EQT720904:EQT720946 FAP720904:FAP720946 FKL720904:FKL720946 FUH720904:FUH720946 GED720904:GED720946 GNZ720904:GNZ720946 GXV720904:GXV720946 HHR720904:HHR720946 HRN720904:HRN720946 IBJ720904:IBJ720946 ILF720904:ILF720946 IVB720904:IVB720946 JEX720904:JEX720946 JOT720904:JOT720946 JYP720904:JYP720946 KIL720904:KIL720946 KSH720904:KSH720946 LCD720904:LCD720946 LLZ720904:LLZ720946 LVV720904:LVV720946 MFR720904:MFR720946 MPN720904:MPN720946 MZJ720904:MZJ720946 NJF720904:NJF720946 NTB720904:NTB720946 OCX720904:OCX720946 OMT720904:OMT720946 OWP720904:OWP720946 PGL720904:PGL720946 PQH720904:PQH720946 QAD720904:QAD720946 QJZ720904:QJZ720946 QTV720904:QTV720946 RDR720904:RDR720946 RNN720904:RNN720946 RXJ720904:RXJ720946 SHF720904:SHF720946 SRB720904:SRB720946 TAX720904:TAX720946 TKT720904:TKT720946 TUP720904:TUP720946 UEL720904:UEL720946 UOH720904:UOH720946 UYD720904:UYD720946 VHZ720904:VHZ720946 VRV720904:VRV720946 WBR720904:WBR720946 WLN720904:WLN720946 WVJ720904:WVJ720946 B786440:B786482 IX786440:IX786482 ST786440:ST786482 ACP786440:ACP786482 AML786440:AML786482 AWH786440:AWH786482 BGD786440:BGD786482 BPZ786440:BPZ786482 BZV786440:BZV786482 CJR786440:CJR786482 CTN786440:CTN786482 DDJ786440:DDJ786482 DNF786440:DNF786482 DXB786440:DXB786482 EGX786440:EGX786482 EQT786440:EQT786482 FAP786440:FAP786482 FKL786440:FKL786482 FUH786440:FUH786482 GED786440:GED786482 GNZ786440:GNZ786482 GXV786440:GXV786482 HHR786440:HHR786482 HRN786440:HRN786482 IBJ786440:IBJ786482 ILF786440:ILF786482 IVB786440:IVB786482 JEX786440:JEX786482 JOT786440:JOT786482 JYP786440:JYP786482 KIL786440:KIL786482 KSH786440:KSH786482 LCD786440:LCD786482 LLZ786440:LLZ786482 LVV786440:LVV786482 MFR786440:MFR786482 MPN786440:MPN786482 MZJ786440:MZJ786482 NJF786440:NJF786482 NTB786440:NTB786482 OCX786440:OCX786482 OMT786440:OMT786482 OWP786440:OWP786482 PGL786440:PGL786482 PQH786440:PQH786482 QAD786440:QAD786482 QJZ786440:QJZ786482 QTV786440:QTV786482 RDR786440:RDR786482 RNN786440:RNN786482 RXJ786440:RXJ786482 SHF786440:SHF786482 SRB786440:SRB786482 TAX786440:TAX786482 TKT786440:TKT786482 TUP786440:TUP786482 UEL786440:UEL786482 UOH786440:UOH786482 UYD786440:UYD786482 VHZ786440:VHZ786482 VRV786440:VRV786482 WBR786440:WBR786482 WLN786440:WLN786482 WVJ786440:WVJ786482 B851976:B852018 IX851976:IX852018 ST851976:ST852018 ACP851976:ACP852018 AML851976:AML852018 AWH851976:AWH852018 BGD851976:BGD852018 BPZ851976:BPZ852018 BZV851976:BZV852018 CJR851976:CJR852018 CTN851976:CTN852018 DDJ851976:DDJ852018 DNF851976:DNF852018 DXB851976:DXB852018 EGX851976:EGX852018 EQT851976:EQT852018 FAP851976:FAP852018 FKL851976:FKL852018 FUH851976:FUH852018 GED851976:GED852018 GNZ851976:GNZ852018 GXV851976:GXV852018 HHR851976:HHR852018 HRN851976:HRN852018 IBJ851976:IBJ852018 ILF851976:ILF852018 IVB851976:IVB852018 JEX851976:JEX852018 JOT851976:JOT852018 JYP851976:JYP852018 KIL851976:KIL852018 KSH851976:KSH852018 LCD851976:LCD852018 LLZ851976:LLZ852018 LVV851976:LVV852018 MFR851976:MFR852018 MPN851976:MPN852018 MZJ851976:MZJ852018 NJF851976:NJF852018 NTB851976:NTB852018 OCX851976:OCX852018 OMT851976:OMT852018 OWP851976:OWP852018 PGL851976:PGL852018 PQH851976:PQH852018 QAD851976:QAD852018 QJZ851976:QJZ852018 QTV851976:QTV852018 RDR851976:RDR852018 RNN851976:RNN852018 RXJ851976:RXJ852018 SHF851976:SHF852018 SRB851976:SRB852018 TAX851976:TAX852018 TKT851976:TKT852018 TUP851976:TUP852018 UEL851976:UEL852018 UOH851976:UOH852018 UYD851976:UYD852018 VHZ851976:VHZ852018 VRV851976:VRV852018 WBR851976:WBR852018 WLN851976:WLN852018 WVJ851976:WVJ852018 B917512:B917554 IX917512:IX917554 ST917512:ST917554 ACP917512:ACP917554 AML917512:AML917554 AWH917512:AWH917554 BGD917512:BGD917554 BPZ917512:BPZ917554 BZV917512:BZV917554 CJR917512:CJR917554 CTN917512:CTN917554 DDJ917512:DDJ917554 DNF917512:DNF917554 DXB917512:DXB917554 EGX917512:EGX917554 EQT917512:EQT917554 FAP917512:FAP917554 FKL917512:FKL917554 FUH917512:FUH917554 GED917512:GED917554 GNZ917512:GNZ917554 GXV917512:GXV917554 HHR917512:HHR917554 HRN917512:HRN917554 IBJ917512:IBJ917554 ILF917512:ILF917554 IVB917512:IVB917554 JEX917512:JEX917554 JOT917512:JOT917554 JYP917512:JYP917554 KIL917512:KIL917554 KSH917512:KSH917554 LCD917512:LCD917554 LLZ917512:LLZ917554 LVV917512:LVV917554 MFR917512:MFR917554 MPN917512:MPN917554 MZJ917512:MZJ917554 NJF917512:NJF917554 NTB917512:NTB917554 OCX917512:OCX917554 OMT917512:OMT917554 OWP917512:OWP917554 PGL917512:PGL917554 PQH917512:PQH917554 QAD917512:QAD917554 QJZ917512:QJZ917554 QTV917512:QTV917554 RDR917512:RDR917554 RNN917512:RNN917554 RXJ917512:RXJ917554 SHF917512:SHF917554 SRB917512:SRB917554 TAX917512:TAX917554 TKT917512:TKT917554 TUP917512:TUP917554 UEL917512:UEL917554 UOH917512:UOH917554 UYD917512:UYD917554 VHZ917512:VHZ917554 VRV917512:VRV917554 WBR917512:WBR917554 WLN917512:WLN917554 WVJ917512:WVJ917554 B983048:B983090 IX983048:IX983090 ST983048:ST983090 ACP983048:ACP983090 AML983048:AML983090 AWH983048:AWH983090 BGD983048:BGD983090 BPZ983048:BPZ983090 BZV983048:BZV983090 CJR983048:CJR983090 CTN983048:CTN983090 DDJ983048:DDJ983090 DNF983048:DNF983090 DXB983048:DXB983090 EGX983048:EGX983090 EQT983048:EQT983090 FAP983048:FAP983090 FKL983048:FKL983090 FUH983048:FUH983090 GED983048:GED983090 GNZ983048:GNZ983090 GXV983048:GXV983090 HHR983048:HHR983090 HRN983048:HRN983090 IBJ983048:IBJ983090 ILF983048:ILF983090 IVB983048:IVB983090 JEX983048:JEX983090 JOT983048:JOT983090 JYP983048:JYP983090 KIL983048:KIL983090 KSH983048:KSH983090 LCD983048:LCD983090 LLZ983048:LLZ983090 LVV983048:LVV983090 MFR983048:MFR983090 MPN983048:MPN983090 MZJ983048:MZJ983090 NJF983048:NJF983090 NTB983048:NTB983090 OCX983048:OCX983090 OMT983048:OMT983090 OWP983048:OWP983090 PGL983048:PGL983090 PQH983048:PQH983090 QAD983048:QAD983090 QJZ983048:QJZ983090 QTV983048:QTV983090 RDR983048:RDR983090 RNN983048:RNN983090 RXJ983048:RXJ983090 SHF983048:SHF983090 SRB983048:SRB983090 TAX983048:TAX983090 TKT983048:TKT983090 TUP983048:TUP983090 UEL983048:UEL983090 UOH983048:UOH983090 UYD983048:UYD983090 VHZ983048:VHZ983090 VRV983048:VRV983090 WBR983048:WBR983090 WLN983048:WLN983090 WVJ983048:WVJ983090" xr:uid="{A2926E5D-23AC-49E6-871D-24C174CBC328}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B50 IX8:IX50 ST8:ST50 ACP8:ACP50 AML8:AML50 AWH8:AWH50 BGD8:BGD50 BPZ8:BPZ50 BZV8:BZV50 CJR8:CJR50 CTN8:CTN50 DDJ8:DDJ50 DNF8:DNF50 DXB8:DXB50 EGX8:EGX50 EQT8:EQT50 FAP8:FAP50 FKL8:FKL50 FUH8:FUH50 GED8:GED50 GNZ8:GNZ50 GXV8:GXV50 HHR8:HHR50 HRN8:HRN50 IBJ8:IBJ50 ILF8:ILF50 IVB8:IVB50 JEX8:JEX50 JOT8:JOT50 JYP8:JYP50 KIL8:KIL50 KSH8:KSH50 LCD8:LCD50 LLZ8:LLZ50 LVV8:LVV50 MFR8:MFR50 MPN8:MPN50 MZJ8:MZJ50 NJF8:NJF50 NTB8:NTB50 OCX8:OCX50 OMT8:OMT50 OWP8:OWP50 PGL8:PGL50 PQH8:PQH50 QAD8:QAD50 QJZ8:QJZ50 QTV8:QTV50 RDR8:RDR50 RNN8:RNN50 RXJ8:RXJ50 SHF8:SHF50 SRB8:SRB50 TAX8:TAX50 TKT8:TKT50 TUP8:TUP50 UEL8:UEL50 UOH8:UOH50 UYD8:UYD50 VHZ8:VHZ50 VRV8:VRV50 WBR8:WBR50 WLN8:WLN50 WVJ8:WVJ50 B65544:B65586 IX65544:IX65586 ST65544:ST65586 ACP65544:ACP65586 AML65544:AML65586 AWH65544:AWH65586 BGD65544:BGD65586 BPZ65544:BPZ65586 BZV65544:BZV65586 CJR65544:CJR65586 CTN65544:CTN65586 DDJ65544:DDJ65586 DNF65544:DNF65586 DXB65544:DXB65586 EGX65544:EGX65586 EQT65544:EQT65586 FAP65544:FAP65586 FKL65544:FKL65586 FUH65544:FUH65586 GED65544:GED65586 GNZ65544:GNZ65586 GXV65544:GXV65586 HHR65544:HHR65586 HRN65544:HRN65586 IBJ65544:IBJ65586 ILF65544:ILF65586 IVB65544:IVB65586 JEX65544:JEX65586 JOT65544:JOT65586 JYP65544:JYP65586 KIL65544:KIL65586 KSH65544:KSH65586 LCD65544:LCD65586 LLZ65544:LLZ65586 LVV65544:LVV65586 MFR65544:MFR65586 MPN65544:MPN65586 MZJ65544:MZJ65586 NJF65544:NJF65586 NTB65544:NTB65586 OCX65544:OCX65586 OMT65544:OMT65586 OWP65544:OWP65586 PGL65544:PGL65586 PQH65544:PQH65586 QAD65544:QAD65586 QJZ65544:QJZ65586 QTV65544:QTV65586 RDR65544:RDR65586 RNN65544:RNN65586 RXJ65544:RXJ65586 SHF65544:SHF65586 SRB65544:SRB65586 TAX65544:TAX65586 TKT65544:TKT65586 TUP65544:TUP65586 UEL65544:UEL65586 UOH65544:UOH65586 UYD65544:UYD65586 VHZ65544:VHZ65586 VRV65544:VRV65586 WBR65544:WBR65586 WLN65544:WLN65586 WVJ65544:WVJ65586 B131080:B131122 IX131080:IX131122 ST131080:ST131122 ACP131080:ACP131122 AML131080:AML131122 AWH131080:AWH131122 BGD131080:BGD131122 BPZ131080:BPZ131122 BZV131080:BZV131122 CJR131080:CJR131122 CTN131080:CTN131122 DDJ131080:DDJ131122 DNF131080:DNF131122 DXB131080:DXB131122 EGX131080:EGX131122 EQT131080:EQT131122 FAP131080:FAP131122 FKL131080:FKL131122 FUH131080:FUH131122 GED131080:GED131122 GNZ131080:GNZ131122 GXV131080:GXV131122 HHR131080:HHR131122 HRN131080:HRN131122 IBJ131080:IBJ131122 ILF131080:ILF131122 IVB131080:IVB131122 JEX131080:JEX131122 JOT131080:JOT131122 JYP131080:JYP131122 KIL131080:KIL131122 KSH131080:KSH131122 LCD131080:LCD131122 LLZ131080:LLZ131122 LVV131080:LVV131122 MFR131080:MFR131122 MPN131080:MPN131122 MZJ131080:MZJ131122 NJF131080:NJF131122 NTB131080:NTB131122 OCX131080:OCX131122 OMT131080:OMT131122 OWP131080:OWP131122 PGL131080:PGL131122 PQH131080:PQH131122 QAD131080:QAD131122 QJZ131080:QJZ131122 QTV131080:QTV131122 RDR131080:RDR131122 RNN131080:RNN131122 RXJ131080:RXJ131122 SHF131080:SHF131122 SRB131080:SRB131122 TAX131080:TAX131122 TKT131080:TKT131122 TUP131080:TUP131122 UEL131080:UEL131122 UOH131080:UOH131122 UYD131080:UYD131122 VHZ131080:VHZ131122 VRV131080:VRV131122 WBR131080:WBR131122 WLN131080:WLN131122 WVJ131080:WVJ131122 B196616:B196658 IX196616:IX196658 ST196616:ST196658 ACP196616:ACP196658 AML196616:AML196658 AWH196616:AWH196658 BGD196616:BGD196658 BPZ196616:BPZ196658 BZV196616:BZV196658 CJR196616:CJR196658 CTN196616:CTN196658 DDJ196616:DDJ196658 DNF196616:DNF196658 DXB196616:DXB196658 EGX196616:EGX196658 EQT196616:EQT196658 FAP196616:FAP196658 FKL196616:FKL196658 FUH196616:FUH196658 GED196616:GED196658 GNZ196616:GNZ196658 GXV196616:GXV196658 HHR196616:HHR196658 HRN196616:HRN196658 IBJ196616:IBJ196658 ILF196616:ILF196658 IVB196616:IVB196658 JEX196616:JEX196658 JOT196616:JOT196658 JYP196616:JYP196658 KIL196616:KIL196658 KSH196616:KSH196658 LCD196616:LCD196658 LLZ196616:LLZ196658 LVV196616:LVV196658 MFR196616:MFR196658 MPN196616:MPN196658 MZJ196616:MZJ196658 NJF196616:NJF196658 NTB196616:NTB196658 OCX196616:OCX196658 OMT196616:OMT196658 OWP196616:OWP196658 PGL196616:PGL196658 PQH196616:PQH196658 QAD196616:QAD196658 QJZ196616:QJZ196658 QTV196616:QTV196658 RDR196616:RDR196658 RNN196616:RNN196658 RXJ196616:RXJ196658 SHF196616:SHF196658 SRB196616:SRB196658 TAX196616:TAX196658 TKT196616:TKT196658 TUP196616:TUP196658 UEL196616:UEL196658 UOH196616:UOH196658 UYD196616:UYD196658 VHZ196616:VHZ196658 VRV196616:VRV196658 WBR196616:WBR196658 WLN196616:WLN196658 WVJ196616:WVJ196658 B262152:B262194 IX262152:IX262194 ST262152:ST262194 ACP262152:ACP262194 AML262152:AML262194 AWH262152:AWH262194 BGD262152:BGD262194 BPZ262152:BPZ262194 BZV262152:BZV262194 CJR262152:CJR262194 CTN262152:CTN262194 DDJ262152:DDJ262194 DNF262152:DNF262194 DXB262152:DXB262194 EGX262152:EGX262194 EQT262152:EQT262194 FAP262152:FAP262194 FKL262152:FKL262194 FUH262152:FUH262194 GED262152:GED262194 GNZ262152:GNZ262194 GXV262152:GXV262194 HHR262152:HHR262194 HRN262152:HRN262194 IBJ262152:IBJ262194 ILF262152:ILF262194 IVB262152:IVB262194 JEX262152:JEX262194 JOT262152:JOT262194 JYP262152:JYP262194 KIL262152:KIL262194 KSH262152:KSH262194 LCD262152:LCD262194 LLZ262152:LLZ262194 LVV262152:LVV262194 MFR262152:MFR262194 MPN262152:MPN262194 MZJ262152:MZJ262194 NJF262152:NJF262194 NTB262152:NTB262194 OCX262152:OCX262194 OMT262152:OMT262194 OWP262152:OWP262194 PGL262152:PGL262194 PQH262152:PQH262194 QAD262152:QAD262194 QJZ262152:QJZ262194 QTV262152:QTV262194 RDR262152:RDR262194 RNN262152:RNN262194 RXJ262152:RXJ262194 SHF262152:SHF262194 SRB262152:SRB262194 TAX262152:TAX262194 TKT262152:TKT262194 TUP262152:TUP262194 UEL262152:UEL262194 UOH262152:UOH262194 UYD262152:UYD262194 VHZ262152:VHZ262194 VRV262152:VRV262194 WBR262152:WBR262194 WLN262152:WLN262194 WVJ262152:WVJ262194 B327688:B327730 IX327688:IX327730 ST327688:ST327730 ACP327688:ACP327730 AML327688:AML327730 AWH327688:AWH327730 BGD327688:BGD327730 BPZ327688:BPZ327730 BZV327688:BZV327730 CJR327688:CJR327730 CTN327688:CTN327730 DDJ327688:DDJ327730 DNF327688:DNF327730 DXB327688:DXB327730 EGX327688:EGX327730 EQT327688:EQT327730 FAP327688:FAP327730 FKL327688:FKL327730 FUH327688:FUH327730 GED327688:GED327730 GNZ327688:GNZ327730 GXV327688:GXV327730 HHR327688:HHR327730 HRN327688:HRN327730 IBJ327688:IBJ327730 ILF327688:ILF327730 IVB327688:IVB327730 JEX327688:JEX327730 JOT327688:JOT327730 JYP327688:JYP327730 KIL327688:KIL327730 KSH327688:KSH327730 LCD327688:LCD327730 LLZ327688:LLZ327730 LVV327688:LVV327730 MFR327688:MFR327730 MPN327688:MPN327730 MZJ327688:MZJ327730 NJF327688:NJF327730 NTB327688:NTB327730 OCX327688:OCX327730 OMT327688:OMT327730 OWP327688:OWP327730 PGL327688:PGL327730 PQH327688:PQH327730 QAD327688:QAD327730 QJZ327688:QJZ327730 QTV327688:QTV327730 RDR327688:RDR327730 RNN327688:RNN327730 RXJ327688:RXJ327730 SHF327688:SHF327730 SRB327688:SRB327730 TAX327688:TAX327730 TKT327688:TKT327730 TUP327688:TUP327730 UEL327688:UEL327730 UOH327688:UOH327730 UYD327688:UYD327730 VHZ327688:VHZ327730 VRV327688:VRV327730 WBR327688:WBR327730 WLN327688:WLN327730 WVJ327688:WVJ327730 B393224:B393266 IX393224:IX393266 ST393224:ST393266 ACP393224:ACP393266 AML393224:AML393266 AWH393224:AWH393266 BGD393224:BGD393266 BPZ393224:BPZ393266 BZV393224:BZV393266 CJR393224:CJR393266 CTN393224:CTN393266 DDJ393224:DDJ393266 DNF393224:DNF393266 DXB393224:DXB393266 EGX393224:EGX393266 EQT393224:EQT393266 FAP393224:FAP393266 FKL393224:FKL393266 FUH393224:FUH393266 GED393224:GED393266 GNZ393224:GNZ393266 GXV393224:GXV393266 HHR393224:HHR393266 HRN393224:HRN393266 IBJ393224:IBJ393266 ILF393224:ILF393266 IVB393224:IVB393266 JEX393224:JEX393266 JOT393224:JOT393266 JYP393224:JYP393266 KIL393224:KIL393266 KSH393224:KSH393266 LCD393224:LCD393266 LLZ393224:LLZ393266 LVV393224:LVV393266 MFR393224:MFR393266 MPN393224:MPN393266 MZJ393224:MZJ393266 NJF393224:NJF393266 NTB393224:NTB393266 OCX393224:OCX393266 OMT393224:OMT393266 OWP393224:OWP393266 PGL393224:PGL393266 PQH393224:PQH393266 QAD393224:QAD393266 QJZ393224:QJZ393266 QTV393224:QTV393266 RDR393224:RDR393266 RNN393224:RNN393266 RXJ393224:RXJ393266 SHF393224:SHF393266 SRB393224:SRB393266 TAX393224:TAX393266 TKT393224:TKT393266 TUP393224:TUP393266 UEL393224:UEL393266 UOH393224:UOH393266 UYD393224:UYD393266 VHZ393224:VHZ393266 VRV393224:VRV393266 WBR393224:WBR393266 WLN393224:WLN393266 WVJ393224:WVJ393266 B458760:B458802 IX458760:IX458802 ST458760:ST458802 ACP458760:ACP458802 AML458760:AML458802 AWH458760:AWH458802 BGD458760:BGD458802 BPZ458760:BPZ458802 BZV458760:BZV458802 CJR458760:CJR458802 CTN458760:CTN458802 DDJ458760:DDJ458802 DNF458760:DNF458802 DXB458760:DXB458802 EGX458760:EGX458802 EQT458760:EQT458802 FAP458760:FAP458802 FKL458760:FKL458802 FUH458760:FUH458802 GED458760:GED458802 GNZ458760:GNZ458802 GXV458760:GXV458802 HHR458760:HHR458802 HRN458760:HRN458802 IBJ458760:IBJ458802 ILF458760:ILF458802 IVB458760:IVB458802 JEX458760:JEX458802 JOT458760:JOT458802 JYP458760:JYP458802 KIL458760:KIL458802 KSH458760:KSH458802 LCD458760:LCD458802 LLZ458760:LLZ458802 LVV458760:LVV458802 MFR458760:MFR458802 MPN458760:MPN458802 MZJ458760:MZJ458802 NJF458760:NJF458802 NTB458760:NTB458802 OCX458760:OCX458802 OMT458760:OMT458802 OWP458760:OWP458802 PGL458760:PGL458802 PQH458760:PQH458802 QAD458760:QAD458802 QJZ458760:QJZ458802 QTV458760:QTV458802 RDR458760:RDR458802 RNN458760:RNN458802 RXJ458760:RXJ458802 SHF458760:SHF458802 SRB458760:SRB458802 TAX458760:TAX458802 TKT458760:TKT458802 TUP458760:TUP458802 UEL458760:UEL458802 UOH458760:UOH458802 UYD458760:UYD458802 VHZ458760:VHZ458802 VRV458760:VRV458802 WBR458760:WBR458802 WLN458760:WLN458802 WVJ458760:WVJ458802 B524296:B524338 IX524296:IX524338 ST524296:ST524338 ACP524296:ACP524338 AML524296:AML524338 AWH524296:AWH524338 BGD524296:BGD524338 BPZ524296:BPZ524338 BZV524296:BZV524338 CJR524296:CJR524338 CTN524296:CTN524338 DDJ524296:DDJ524338 DNF524296:DNF524338 DXB524296:DXB524338 EGX524296:EGX524338 EQT524296:EQT524338 FAP524296:FAP524338 FKL524296:FKL524338 FUH524296:FUH524338 GED524296:GED524338 GNZ524296:GNZ524338 GXV524296:GXV524338 HHR524296:HHR524338 HRN524296:HRN524338 IBJ524296:IBJ524338 ILF524296:ILF524338 IVB524296:IVB524338 JEX524296:JEX524338 JOT524296:JOT524338 JYP524296:JYP524338 KIL524296:KIL524338 KSH524296:KSH524338 LCD524296:LCD524338 LLZ524296:LLZ524338 LVV524296:LVV524338 MFR524296:MFR524338 MPN524296:MPN524338 MZJ524296:MZJ524338 NJF524296:NJF524338 NTB524296:NTB524338 OCX524296:OCX524338 OMT524296:OMT524338 OWP524296:OWP524338 PGL524296:PGL524338 PQH524296:PQH524338 QAD524296:QAD524338 QJZ524296:QJZ524338 QTV524296:QTV524338 RDR524296:RDR524338 RNN524296:RNN524338 RXJ524296:RXJ524338 SHF524296:SHF524338 SRB524296:SRB524338 TAX524296:TAX524338 TKT524296:TKT524338 TUP524296:TUP524338 UEL524296:UEL524338 UOH524296:UOH524338 UYD524296:UYD524338 VHZ524296:VHZ524338 VRV524296:VRV524338 WBR524296:WBR524338 WLN524296:WLN524338 WVJ524296:WVJ524338 B589832:B589874 IX589832:IX589874 ST589832:ST589874 ACP589832:ACP589874 AML589832:AML589874 AWH589832:AWH589874 BGD589832:BGD589874 BPZ589832:BPZ589874 BZV589832:BZV589874 CJR589832:CJR589874 CTN589832:CTN589874 DDJ589832:DDJ589874 DNF589832:DNF589874 DXB589832:DXB589874 EGX589832:EGX589874 EQT589832:EQT589874 FAP589832:FAP589874 FKL589832:FKL589874 FUH589832:FUH589874 GED589832:GED589874 GNZ589832:GNZ589874 GXV589832:GXV589874 HHR589832:HHR589874 HRN589832:HRN589874 IBJ589832:IBJ589874 ILF589832:ILF589874 IVB589832:IVB589874 JEX589832:JEX589874 JOT589832:JOT589874 JYP589832:JYP589874 KIL589832:KIL589874 KSH589832:KSH589874 LCD589832:LCD589874 LLZ589832:LLZ589874 LVV589832:LVV589874 MFR589832:MFR589874 MPN589832:MPN589874 MZJ589832:MZJ589874 NJF589832:NJF589874 NTB589832:NTB589874 OCX589832:OCX589874 OMT589832:OMT589874 OWP589832:OWP589874 PGL589832:PGL589874 PQH589832:PQH589874 QAD589832:QAD589874 QJZ589832:QJZ589874 QTV589832:QTV589874 RDR589832:RDR589874 RNN589832:RNN589874 RXJ589832:RXJ589874 SHF589832:SHF589874 SRB589832:SRB589874 TAX589832:TAX589874 TKT589832:TKT589874 TUP589832:TUP589874 UEL589832:UEL589874 UOH589832:UOH589874 UYD589832:UYD589874 VHZ589832:VHZ589874 VRV589832:VRV589874 WBR589832:WBR589874 WLN589832:WLN589874 WVJ589832:WVJ589874 B655368:B655410 IX655368:IX655410 ST655368:ST655410 ACP655368:ACP655410 AML655368:AML655410 AWH655368:AWH655410 BGD655368:BGD655410 BPZ655368:BPZ655410 BZV655368:BZV655410 CJR655368:CJR655410 CTN655368:CTN655410 DDJ655368:DDJ655410 DNF655368:DNF655410 DXB655368:DXB655410 EGX655368:EGX655410 EQT655368:EQT655410 FAP655368:FAP655410 FKL655368:FKL655410 FUH655368:FUH655410 GED655368:GED655410 GNZ655368:GNZ655410 GXV655368:GXV655410 HHR655368:HHR655410 HRN655368:HRN655410 IBJ655368:IBJ655410 ILF655368:ILF655410 IVB655368:IVB655410 JEX655368:JEX655410 JOT655368:JOT655410 JYP655368:JYP655410 KIL655368:KIL655410 KSH655368:KSH655410 LCD655368:LCD655410 LLZ655368:LLZ655410 LVV655368:LVV655410 MFR655368:MFR655410 MPN655368:MPN655410 MZJ655368:MZJ655410 NJF655368:NJF655410 NTB655368:NTB655410 OCX655368:OCX655410 OMT655368:OMT655410 OWP655368:OWP655410 PGL655368:PGL655410 PQH655368:PQH655410 QAD655368:QAD655410 QJZ655368:QJZ655410 QTV655368:QTV655410 RDR655368:RDR655410 RNN655368:RNN655410 RXJ655368:RXJ655410 SHF655368:SHF655410 SRB655368:SRB655410 TAX655368:TAX655410 TKT655368:TKT655410 TUP655368:TUP655410 UEL655368:UEL655410 UOH655368:UOH655410 UYD655368:UYD655410 VHZ655368:VHZ655410 VRV655368:VRV655410 WBR655368:WBR655410 WLN655368:WLN655410 WVJ655368:WVJ655410 B720904:B720946 IX720904:IX720946 ST720904:ST720946 ACP720904:ACP720946 AML720904:AML720946 AWH720904:AWH720946 BGD720904:BGD720946 BPZ720904:BPZ720946 BZV720904:BZV720946 CJR720904:CJR720946 CTN720904:CTN720946 DDJ720904:DDJ720946 DNF720904:DNF720946 DXB720904:DXB720946 EGX720904:EGX720946 EQT720904:EQT720946 FAP720904:FAP720946 FKL720904:FKL720946 FUH720904:FUH720946 GED720904:GED720946 GNZ720904:GNZ720946 GXV720904:GXV720946 HHR720904:HHR720946 HRN720904:HRN720946 IBJ720904:IBJ720946 ILF720904:ILF720946 IVB720904:IVB720946 JEX720904:JEX720946 JOT720904:JOT720946 JYP720904:JYP720946 KIL720904:KIL720946 KSH720904:KSH720946 LCD720904:LCD720946 LLZ720904:LLZ720946 LVV720904:LVV720946 MFR720904:MFR720946 MPN720904:MPN720946 MZJ720904:MZJ720946 NJF720904:NJF720946 NTB720904:NTB720946 OCX720904:OCX720946 OMT720904:OMT720946 OWP720904:OWP720946 PGL720904:PGL720946 PQH720904:PQH720946 QAD720904:QAD720946 QJZ720904:QJZ720946 QTV720904:QTV720946 RDR720904:RDR720946 RNN720904:RNN720946 RXJ720904:RXJ720946 SHF720904:SHF720946 SRB720904:SRB720946 TAX720904:TAX720946 TKT720904:TKT720946 TUP720904:TUP720946 UEL720904:UEL720946 UOH720904:UOH720946 UYD720904:UYD720946 VHZ720904:VHZ720946 VRV720904:VRV720946 WBR720904:WBR720946 WLN720904:WLN720946 WVJ720904:WVJ720946 B786440:B786482 IX786440:IX786482 ST786440:ST786482 ACP786440:ACP786482 AML786440:AML786482 AWH786440:AWH786482 BGD786440:BGD786482 BPZ786440:BPZ786482 BZV786440:BZV786482 CJR786440:CJR786482 CTN786440:CTN786482 DDJ786440:DDJ786482 DNF786440:DNF786482 DXB786440:DXB786482 EGX786440:EGX786482 EQT786440:EQT786482 FAP786440:FAP786482 FKL786440:FKL786482 FUH786440:FUH786482 GED786440:GED786482 GNZ786440:GNZ786482 GXV786440:GXV786482 HHR786440:HHR786482 HRN786440:HRN786482 IBJ786440:IBJ786482 ILF786440:ILF786482 IVB786440:IVB786482 JEX786440:JEX786482 JOT786440:JOT786482 JYP786440:JYP786482 KIL786440:KIL786482 KSH786440:KSH786482 LCD786440:LCD786482 LLZ786440:LLZ786482 LVV786440:LVV786482 MFR786440:MFR786482 MPN786440:MPN786482 MZJ786440:MZJ786482 NJF786440:NJF786482 NTB786440:NTB786482 OCX786440:OCX786482 OMT786440:OMT786482 OWP786440:OWP786482 PGL786440:PGL786482 PQH786440:PQH786482 QAD786440:QAD786482 QJZ786440:QJZ786482 QTV786440:QTV786482 RDR786440:RDR786482 RNN786440:RNN786482 RXJ786440:RXJ786482 SHF786440:SHF786482 SRB786440:SRB786482 TAX786440:TAX786482 TKT786440:TKT786482 TUP786440:TUP786482 UEL786440:UEL786482 UOH786440:UOH786482 UYD786440:UYD786482 VHZ786440:VHZ786482 VRV786440:VRV786482 WBR786440:WBR786482 WLN786440:WLN786482 WVJ786440:WVJ786482 B851976:B852018 IX851976:IX852018 ST851976:ST852018 ACP851976:ACP852018 AML851976:AML852018 AWH851976:AWH852018 BGD851976:BGD852018 BPZ851976:BPZ852018 BZV851976:BZV852018 CJR851976:CJR852018 CTN851976:CTN852018 DDJ851976:DDJ852018 DNF851976:DNF852018 DXB851976:DXB852018 EGX851976:EGX852018 EQT851976:EQT852018 FAP851976:FAP852018 FKL851976:FKL852018 FUH851976:FUH852018 GED851976:GED852018 GNZ851976:GNZ852018 GXV851976:GXV852018 HHR851976:HHR852018 HRN851976:HRN852018 IBJ851976:IBJ852018 ILF851976:ILF852018 IVB851976:IVB852018 JEX851976:JEX852018 JOT851976:JOT852018 JYP851976:JYP852018 KIL851976:KIL852018 KSH851976:KSH852018 LCD851976:LCD852018 LLZ851976:LLZ852018 LVV851976:LVV852018 MFR851976:MFR852018 MPN851976:MPN852018 MZJ851976:MZJ852018 NJF851976:NJF852018 NTB851976:NTB852018 OCX851976:OCX852018 OMT851976:OMT852018 OWP851976:OWP852018 PGL851976:PGL852018 PQH851976:PQH852018 QAD851976:QAD852018 QJZ851976:QJZ852018 QTV851976:QTV852018 RDR851976:RDR852018 RNN851976:RNN852018 RXJ851976:RXJ852018 SHF851976:SHF852018 SRB851976:SRB852018 TAX851976:TAX852018 TKT851976:TKT852018 TUP851976:TUP852018 UEL851976:UEL852018 UOH851976:UOH852018 UYD851976:UYD852018 VHZ851976:VHZ852018 VRV851976:VRV852018 WBR851976:WBR852018 WLN851976:WLN852018 WVJ851976:WVJ852018 B917512:B917554 IX917512:IX917554 ST917512:ST917554 ACP917512:ACP917554 AML917512:AML917554 AWH917512:AWH917554 BGD917512:BGD917554 BPZ917512:BPZ917554 BZV917512:BZV917554 CJR917512:CJR917554 CTN917512:CTN917554 DDJ917512:DDJ917554 DNF917512:DNF917554 DXB917512:DXB917554 EGX917512:EGX917554 EQT917512:EQT917554 FAP917512:FAP917554 FKL917512:FKL917554 FUH917512:FUH917554 GED917512:GED917554 GNZ917512:GNZ917554 GXV917512:GXV917554 HHR917512:HHR917554 HRN917512:HRN917554 IBJ917512:IBJ917554 ILF917512:ILF917554 IVB917512:IVB917554 JEX917512:JEX917554 JOT917512:JOT917554 JYP917512:JYP917554 KIL917512:KIL917554 KSH917512:KSH917554 LCD917512:LCD917554 LLZ917512:LLZ917554 LVV917512:LVV917554 MFR917512:MFR917554 MPN917512:MPN917554 MZJ917512:MZJ917554 NJF917512:NJF917554 NTB917512:NTB917554 OCX917512:OCX917554 OMT917512:OMT917554 OWP917512:OWP917554 PGL917512:PGL917554 PQH917512:PQH917554 QAD917512:QAD917554 QJZ917512:QJZ917554 QTV917512:QTV917554 RDR917512:RDR917554 RNN917512:RNN917554 RXJ917512:RXJ917554 SHF917512:SHF917554 SRB917512:SRB917554 TAX917512:TAX917554 TKT917512:TKT917554 TUP917512:TUP917554 UEL917512:UEL917554 UOH917512:UOH917554 UYD917512:UYD917554 VHZ917512:VHZ917554 VRV917512:VRV917554 WBR917512:WBR917554 WLN917512:WLN917554 WVJ917512:WVJ917554 B983048:B983090 IX983048:IX983090 ST983048:ST983090 ACP983048:ACP983090 AML983048:AML983090 AWH983048:AWH983090 BGD983048:BGD983090 BPZ983048:BPZ983090 BZV983048:BZV983090 CJR983048:CJR983090 CTN983048:CTN983090 DDJ983048:DDJ983090 DNF983048:DNF983090 DXB983048:DXB983090 EGX983048:EGX983090 EQT983048:EQT983090 FAP983048:FAP983090 FKL983048:FKL983090 FUH983048:FUH983090 GED983048:GED983090 GNZ983048:GNZ983090 GXV983048:GXV983090 HHR983048:HHR983090 HRN983048:HRN983090 IBJ983048:IBJ983090 ILF983048:ILF983090 IVB983048:IVB983090 JEX983048:JEX983090 JOT983048:JOT983090 JYP983048:JYP983090 KIL983048:KIL983090 KSH983048:KSH983090 LCD983048:LCD983090 LLZ983048:LLZ983090 LVV983048:LVV983090 MFR983048:MFR983090 MPN983048:MPN983090 MZJ983048:MZJ983090 NJF983048:NJF983090 NTB983048:NTB983090 OCX983048:OCX983090 OMT983048:OMT983090 OWP983048:OWP983090 PGL983048:PGL983090 PQH983048:PQH983090 QAD983048:QAD983090 QJZ983048:QJZ983090 QTV983048:QTV983090 RDR983048:RDR983090 RNN983048:RNN983090 RXJ983048:RXJ983090 SHF983048:SHF983090 SRB983048:SRB983090 TAX983048:TAX983090 TKT983048:TKT983090 TUP983048:TUP983090 UEL983048:UEL983090 UOH983048:UOH983090 UYD983048:UYD983090 VHZ983048:VHZ983090 VRV983048:VRV983090 WBR983048:WBR983090 WLN983048:WLN983090 WVJ983048:WVJ983090">
       <formula1>8</formula1>
       <formula2>8</formula2>
     </dataValidation>
@@ -8997,530 +8962,530 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370F73DA-448C-4452-A197-9E365B49E20F}">
-  <dimension ref="A1:AB300"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB299"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="21" width="2.7265625" style="8" customWidth="1"/>
-    <col min="22" max="22" width="4.453125" style="8" customWidth="1"/>
-    <col min="23" max="23" width="7.453125" style="8" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="256" width="11.453125" style="1"/>
-    <col min="257" max="257" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="21" width="2.7109375" style="8" customWidth="1"/>
+    <col min="22" max="22" width="4.42578125" style="8" customWidth="1"/>
+    <col min="23" max="23" width="7.42578125" style="8" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="256" width="11.42578125" style="1"/>
+    <col min="257" max="257" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="260" max="277" width="2.7265625" style="1" customWidth="1"/>
-    <col min="278" max="278" width="4.453125" style="1" customWidth="1"/>
+    <col min="260" max="277" width="2.7109375" style="1" customWidth="1"/>
+    <col min="278" max="278" width="4.42578125" style="1" customWidth="1"/>
     <col min="279" max="279" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="280" max="280" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="281" max="512" width="11.453125" style="1"/>
-    <col min="513" max="513" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="281" max="512" width="11.42578125" style="1"/>
+    <col min="513" max="513" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="515" max="515" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="516" max="533" width="2.7265625" style="1" customWidth="1"/>
-    <col min="534" max="534" width="4.453125" style="1" customWidth="1"/>
+    <col min="516" max="533" width="2.7109375" style="1" customWidth="1"/>
+    <col min="534" max="534" width="4.42578125" style="1" customWidth="1"/>
     <col min="535" max="535" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="536" max="536" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="537" max="768" width="11.453125" style="1"/>
-    <col min="769" max="769" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="536" max="536" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="537" max="768" width="11.42578125" style="1"/>
+    <col min="769" max="769" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="771" max="771" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="772" max="789" width="2.7265625" style="1" customWidth="1"/>
-    <col min="790" max="790" width="4.453125" style="1" customWidth="1"/>
+    <col min="772" max="789" width="2.7109375" style="1" customWidth="1"/>
+    <col min="790" max="790" width="4.42578125" style="1" customWidth="1"/>
     <col min="791" max="791" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="792" max="792" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="793" max="1024" width="11.453125" style="1"/>
-    <col min="1025" max="1025" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="792" max="792" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="793" max="1024" width="11.42578125" style="1"/>
+    <col min="1025" max="1025" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1027" max="1027" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1045" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1046" max="1046" width="4.453125" style="1" customWidth="1"/>
+    <col min="1028" max="1045" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1046" max="1046" width="4.42578125" style="1" customWidth="1"/>
     <col min="1047" max="1047" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1048" max="1048" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1049" max="1280" width="11.453125" style="1"/>
-    <col min="1281" max="1281" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1048" max="1048" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1049" max="1280" width="11.42578125" style="1"/>
+    <col min="1281" max="1281" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1283" max="1283" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1301" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1302" max="1302" width="4.453125" style="1" customWidth="1"/>
+    <col min="1284" max="1301" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1302" max="1302" width="4.42578125" style="1" customWidth="1"/>
     <col min="1303" max="1303" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1304" max="1304" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1305" max="1536" width="11.453125" style="1"/>
-    <col min="1537" max="1537" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1304" max="1304" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1305" max="1536" width="11.42578125" style="1"/>
+    <col min="1537" max="1537" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1539" max="1539" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1557" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1558" max="1558" width="4.453125" style="1" customWidth="1"/>
+    <col min="1540" max="1557" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1558" max="1558" width="4.42578125" style="1" customWidth="1"/>
     <col min="1559" max="1559" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1560" max="1560" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1561" max="1792" width="11.453125" style="1"/>
-    <col min="1793" max="1793" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1560" max="1560" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1561" max="1792" width="11.42578125" style="1"/>
+    <col min="1793" max="1793" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1795" max="1795" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1813" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1814" max="1814" width="4.453125" style="1" customWidth="1"/>
+    <col min="1796" max="1813" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1814" max="1814" width="4.42578125" style="1" customWidth="1"/>
     <col min="1815" max="1815" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1816" max="1816" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1817" max="2048" width="11.453125" style="1"/>
-    <col min="2049" max="2049" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1816" max="1816" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1817" max="2048" width="11.42578125" style="1"/>
+    <col min="2049" max="2049" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2051" max="2051" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2069" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2070" max="2070" width="4.453125" style="1" customWidth="1"/>
+    <col min="2052" max="2069" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2070" max="2070" width="4.42578125" style="1" customWidth="1"/>
     <col min="2071" max="2071" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2072" max="2072" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2073" max="2304" width="11.453125" style="1"/>
-    <col min="2305" max="2305" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2072" max="2072" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2073" max="2304" width="11.42578125" style="1"/>
+    <col min="2305" max="2305" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2307" max="2307" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2325" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2326" max="2326" width="4.453125" style="1" customWidth="1"/>
+    <col min="2308" max="2325" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2326" max="2326" width="4.42578125" style="1" customWidth="1"/>
     <col min="2327" max="2327" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2328" max="2328" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2329" max="2560" width="11.453125" style="1"/>
-    <col min="2561" max="2561" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2328" max="2328" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2329" max="2560" width="11.42578125" style="1"/>
+    <col min="2561" max="2561" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2563" max="2563" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2581" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2582" max="2582" width="4.453125" style="1" customWidth="1"/>
+    <col min="2564" max="2581" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2582" max="2582" width="4.42578125" style="1" customWidth="1"/>
     <col min="2583" max="2583" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2584" max="2584" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2585" max="2816" width="11.453125" style="1"/>
-    <col min="2817" max="2817" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2584" max="2584" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2585" max="2816" width="11.42578125" style="1"/>
+    <col min="2817" max="2817" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2819" max="2819" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2837" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2838" max="2838" width="4.453125" style="1" customWidth="1"/>
+    <col min="2820" max="2837" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2838" max="2838" width="4.42578125" style="1" customWidth="1"/>
     <col min="2839" max="2839" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2840" max="2840" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2841" max="3072" width="11.453125" style="1"/>
-    <col min="3073" max="3073" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2840" max="2840" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2841" max="3072" width="11.42578125" style="1"/>
+    <col min="3073" max="3073" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3075" max="3075" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3093" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3094" max="3094" width="4.453125" style="1" customWidth="1"/>
+    <col min="3076" max="3093" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3094" max="3094" width="4.42578125" style="1" customWidth="1"/>
     <col min="3095" max="3095" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3096" max="3096" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3097" max="3328" width="11.453125" style="1"/>
-    <col min="3329" max="3329" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3096" max="3096" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3097" max="3328" width="11.42578125" style="1"/>
+    <col min="3329" max="3329" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3331" max="3331" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3349" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3350" max="3350" width="4.453125" style="1" customWidth="1"/>
+    <col min="3332" max="3349" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3350" max="3350" width="4.42578125" style="1" customWidth="1"/>
     <col min="3351" max="3351" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3352" max="3352" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3353" max="3584" width="11.453125" style="1"/>
-    <col min="3585" max="3585" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3352" max="3352" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3353" max="3584" width="11.42578125" style="1"/>
+    <col min="3585" max="3585" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3587" max="3587" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3605" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3606" max="3606" width="4.453125" style="1" customWidth="1"/>
+    <col min="3588" max="3605" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3606" max="3606" width="4.42578125" style="1" customWidth="1"/>
     <col min="3607" max="3607" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3608" max="3608" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3609" max="3840" width="11.453125" style="1"/>
-    <col min="3841" max="3841" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3608" max="3608" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3609" max="3840" width="11.42578125" style="1"/>
+    <col min="3841" max="3841" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3843" max="3843" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3861" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3862" max="3862" width="4.453125" style="1" customWidth="1"/>
+    <col min="3844" max="3861" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3862" max="3862" width="4.42578125" style="1" customWidth="1"/>
     <col min="3863" max="3863" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3864" max="3864" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3865" max="4096" width="11.453125" style="1"/>
-    <col min="4097" max="4097" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3864" max="3864" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3865" max="4096" width="11.42578125" style="1"/>
+    <col min="4097" max="4097" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4099" max="4099" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4117" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4118" max="4118" width="4.453125" style="1" customWidth="1"/>
+    <col min="4100" max="4117" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4118" max="4118" width="4.42578125" style="1" customWidth="1"/>
     <col min="4119" max="4119" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4120" max="4120" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4121" max="4352" width="11.453125" style="1"/>
-    <col min="4353" max="4353" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4120" max="4120" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4121" max="4352" width="11.42578125" style="1"/>
+    <col min="4353" max="4353" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4355" max="4355" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4373" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4374" max="4374" width="4.453125" style="1" customWidth="1"/>
+    <col min="4356" max="4373" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4374" max="4374" width="4.42578125" style="1" customWidth="1"/>
     <col min="4375" max="4375" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4376" max="4376" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4377" max="4608" width="11.453125" style="1"/>
-    <col min="4609" max="4609" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4376" max="4376" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4377" max="4608" width="11.42578125" style="1"/>
+    <col min="4609" max="4609" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4611" max="4611" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4629" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4630" max="4630" width="4.453125" style="1" customWidth="1"/>
+    <col min="4612" max="4629" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4630" max="4630" width="4.42578125" style="1" customWidth="1"/>
     <col min="4631" max="4631" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4632" max="4632" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4633" max="4864" width="11.453125" style="1"/>
-    <col min="4865" max="4865" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4632" max="4632" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4633" max="4864" width="11.42578125" style="1"/>
+    <col min="4865" max="4865" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4867" max="4867" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4885" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4886" max="4886" width="4.453125" style="1" customWidth="1"/>
+    <col min="4868" max="4885" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4886" max="4886" width="4.42578125" style="1" customWidth="1"/>
     <col min="4887" max="4887" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4888" max="4888" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4889" max="5120" width="11.453125" style="1"/>
-    <col min="5121" max="5121" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4888" max="4888" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4889" max="5120" width="11.42578125" style="1"/>
+    <col min="5121" max="5121" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5123" max="5123" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5141" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5142" max="5142" width="4.453125" style="1" customWidth="1"/>
+    <col min="5124" max="5141" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5142" max="5142" width="4.42578125" style="1" customWidth="1"/>
     <col min="5143" max="5143" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5144" max="5144" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5145" max="5376" width="11.453125" style="1"/>
-    <col min="5377" max="5377" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5144" max="5144" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5145" max="5376" width="11.42578125" style="1"/>
+    <col min="5377" max="5377" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5379" max="5379" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5397" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5398" max="5398" width="4.453125" style="1" customWidth="1"/>
+    <col min="5380" max="5397" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5398" max="5398" width="4.42578125" style="1" customWidth="1"/>
     <col min="5399" max="5399" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5400" max="5400" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5401" max="5632" width="11.453125" style="1"/>
-    <col min="5633" max="5633" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5400" max="5400" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5401" max="5632" width="11.42578125" style="1"/>
+    <col min="5633" max="5633" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5635" max="5635" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5653" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5654" max="5654" width="4.453125" style="1" customWidth="1"/>
+    <col min="5636" max="5653" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5654" max="5654" width="4.42578125" style="1" customWidth="1"/>
     <col min="5655" max="5655" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5656" max="5656" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5657" max="5888" width="11.453125" style="1"/>
-    <col min="5889" max="5889" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5656" max="5656" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5657" max="5888" width="11.42578125" style="1"/>
+    <col min="5889" max="5889" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5891" max="5891" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5909" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5910" max="5910" width="4.453125" style="1" customWidth="1"/>
+    <col min="5892" max="5909" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5910" max="5910" width="4.42578125" style="1" customWidth="1"/>
     <col min="5911" max="5911" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5912" max="5912" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5913" max="6144" width="11.453125" style="1"/>
-    <col min="6145" max="6145" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5912" max="5912" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5913" max="6144" width="11.42578125" style="1"/>
+    <col min="6145" max="6145" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6147" max="6147" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6165" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6166" max="6166" width="4.453125" style="1" customWidth="1"/>
+    <col min="6148" max="6165" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6166" max="6166" width="4.42578125" style="1" customWidth="1"/>
     <col min="6167" max="6167" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6168" max="6168" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6169" max="6400" width="11.453125" style="1"/>
-    <col min="6401" max="6401" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6168" max="6168" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6169" max="6400" width="11.42578125" style="1"/>
+    <col min="6401" max="6401" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6403" max="6403" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6421" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6422" max="6422" width="4.453125" style="1" customWidth="1"/>
+    <col min="6404" max="6421" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6422" max="6422" width="4.42578125" style="1" customWidth="1"/>
     <col min="6423" max="6423" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6424" max="6424" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6425" max="6656" width="11.453125" style="1"/>
-    <col min="6657" max="6657" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6424" max="6424" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6425" max="6656" width="11.42578125" style="1"/>
+    <col min="6657" max="6657" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6659" max="6659" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6677" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6678" max="6678" width="4.453125" style="1" customWidth="1"/>
+    <col min="6660" max="6677" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6678" max="6678" width="4.42578125" style="1" customWidth="1"/>
     <col min="6679" max="6679" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6680" max="6680" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6681" max="6912" width="11.453125" style="1"/>
-    <col min="6913" max="6913" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6680" max="6680" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6681" max="6912" width="11.42578125" style="1"/>
+    <col min="6913" max="6913" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6915" max="6915" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6933" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6934" max="6934" width="4.453125" style="1" customWidth="1"/>
+    <col min="6916" max="6933" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6934" max="6934" width="4.42578125" style="1" customWidth="1"/>
     <col min="6935" max="6935" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6936" max="6936" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6937" max="7168" width="11.453125" style="1"/>
-    <col min="7169" max="7169" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6936" max="6936" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6937" max="7168" width="11.42578125" style="1"/>
+    <col min="7169" max="7169" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7171" max="7171" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7189" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7190" max="7190" width="4.453125" style="1" customWidth="1"/>
+    <col min="7172" max="7189" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7190" max="7190" width="4.42578125" style="1" customWidth="1"/>
     <col min="7191" max="7191" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7192" max="7192" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7193" max="7424" width="11.453125" style="1"/>
-    <col min="7425" max="7425" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7192" max="7192" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7193" max="7424" width="11.42578125" style="1"/>
+    <col min="7425" max="7425" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7427" max="7427" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7445" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7446" max="7446" width="4.453125" style="1" customWidth="1"/>
+    <col min="7428" max="7445" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7446" max="7446" width="4.42578125" style="1" customWidth="1"/>
     <col min="7447" max="7447" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7448" max="7448" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7449" max="7680" width="11.453125" style="1"/>
-    <col min="7681" max="7681" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7448" max="7448" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7449" max="7680" width="11.42578125" style="1"/>
+    <col min="7681" max="7681" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7683" max="7683" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7701" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7702" max="7702" width="4.453125" style="1" customWidth="1"/>
+    <col min="7684" max="7701" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7702" max="7702" width="4.42578125" style="1" customWidth="1"/>
     <col min="7703" max="7703" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7704" max="7704" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7705" max="7936" width="11.453125" style="1"/>
-    <col min="7937" max="7937" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7704" max="7704" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7705" max="7936" width="11.42578125" style="1"/>
+    <col min="7937" max="7937" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7939" max="7939" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7957" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7958" max="7958" width="4.453125" style="1" customWidth="1"/>
+    <col min="7940" max="7957" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7958" max="7958" width="4.42578125" style="1" customWidth="1"/>
     <col min="7959" max="7959" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7960" max="7960" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7961" max="8192" width="11.453125" style="1"/>
-    <col min="8193" max="8193" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7960" max="7960" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7961" max="8192" width="11.42578125" style="1"/>
+    <col min="8193" max="8193" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8195" max="8195" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8213" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8214" max="8214" width="4.453125" style="1" customWidth="1"/>
+    <col min="8196" max="8213" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8214" max="8214" width="4.42578125" style="1" customWidth="1"/>
     <col min="8215" max="8215" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8216" max="8216" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8217" max="8448" width="11.453125" style="1"/>
-    <col min="8449" max="8449" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8216" max="8216" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8217" max="8448" width="11.42578125" style="1"/>
+    <col min="8449" max="8449" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8451" max="8451" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8469" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8470" max="8470" width="4.453125" style="1" customWidth="1"/>
+    <col min="8452" max="8469" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8470" max="8470" width="4.42578125" style="1" customWidth="1"/>
     <col min="8471" max="8471" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8472" max="8472" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8473" max="8704" width="11.453125" style="1"/>
-    <col min="8705" max="8705" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8472" max="8472" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8473" max="8704" width="11.42578125" style="1"/>
+    <col min="8705" max="8705" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8707" max="8707" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8725" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8726" max="8726" width="4.453125" style="1" customWidth="1"/>
+    <col min="8708" max="8725" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8726" max="8726" width="4.42578125" style="1" customWidth="1"/>
     <col min="8727" max="8727" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8728" max="8728" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8729" max="8960" width="11.453125" style="1"/>
-    <col min="8961" max="8961" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8728" max="8728" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8729" max="8960" width="11.42578125" style="1"/>
+    <col min="8961" max="8961" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8963" max="8963" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8981" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8982" max="8982" width="4.453125" style="1" customWidth="1"/>
+    <col min="8964" max="8981" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8982" max="8982" width="4.42578125" style="1" customWidth="1"/>
     <col min="8983" max="8983" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8984" max="8984" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8985" max="9216" width="11.453125" style="1"/>
-    <col min="9217" max="9217" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8984" max="8984" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8985" max="9216" width="11.42578125" style="1"/>
+    <col min="9217" max="9217" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9219" max="9219" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9237" width="2.7265625" style="1" customWidth="1"/>
-    <col min="9238" max="9238" width="4.453125" style="1" customWidth="1"/>
+    <col min="9220" max="9237" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9238" max="9238" width="4.42578125" style="1" customWidth="1"/>
     <col min="9239" max="9239" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9240" max="9240" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9241" max="9472" width="11.453125" style="1"/>
-    <col min="9473" max="9473" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9240" max="9240" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9241" max="9472" width="11.42578125" style="1"/>
+    <col min="9473" max="9473" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9475" max="9475" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9493" width="2.7265625" style="1" customWidth="1"/>
-    <col min="9494" max="9494" width="4.453125" style="1" customWidth="1"/>
+    <col min="9476" max="9493" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9494" max="9494" width="4.42578125" style="1" customWidth="1"/>
     <col min="9495" max="9495" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9496" max="9496" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9497" max="9728" width="11.453125" style="1"/>
-    <col min="9729" max="9729" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9496" max="9496" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9497" max="9728" width="11.42578125" style="1"/>
+    <col min="9729" max="9729" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9731" max="9731" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9749" width="2.7265625" style="1" customWidth="1"/>
-    <col min="9750" max="9750" width="4.453125" style="1" customWidth="1"/>
+    <col min="9732" max="9749" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9750" max="9750" width="4.42578125" style="1" customWidth="1"/>
     <col min="9751" max="9751" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9752" max="9752" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9753" max="9984" width="11.453125" style="1"/>
-    <col min="9985" max="9985" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9752" max="9752" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9753" max="9984" width="11.42578125" style="1"/>
+    <col min="9985" max="9985" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9987" max="9987" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9988" max="10005" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10006" max="10006" width="4.453125" style="1" customWidth="1"/>
+    <col min="9988" max="10005" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10006" max="10006" width="4.42578125" style="1" customWidth="1"/>
     <col min="10007" max="10007" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10008" max="10008" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10009" max="10240" width="11.453125" style="1"/>
-    <col min="10241" max="10241" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10008" max="10008" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10009" max="10240" width="11.42578125" style="1"/>
+    <col min="10241" max="10241" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10243" max="10243" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10261" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10262" max="10262" width="4.453125" style="1" customWidth="1"/>
+    <col min="10244" max="10261" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10262" max="10262" width="4.42578125" style="1" customWidth="1"/>
     <col min="10263" max="10263" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10264" max="10264" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10265" max="10496" width="11.453125" style="1"/>
-    <col min="10497" max="10497" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10264" max="10264" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10265" max="10496" width="11.42578125" style="1"/>
+    <col min="10497" max="10497" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10499" max="10499" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10517" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10518" max="10518" width="4.453125" style="1" customWidth="1"/>
+    <col min="10500" max="10517" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10518" max="10518" width="4.42578125" style="1" customWidth="1"/>
     <col min="10519" max="10519" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10520" max="10520" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10521" max="10752" width="11.453125" style="1"/>
-    <col min="10753" max="10753" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10520" max="10520" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10521" max="10752" width="11.42578125" style="1"/>
+    <col min="10753" max="10753" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10755" max="10755" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10773" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10774" max="10774" width="4.453125" style="1" customWidth="1"/>
+    <col min="10756" max="10773" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10774" max="10774" width="4.42578125" style="1" customWidth="1"/>
     <col min="10775" max="10775" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10776" max="10776" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10777" max="11008" width="11.453125" style="1"/>
-    <col min="11009" max="11009" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10776" max="10776" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10777" max="11008" width="11.42578125" style="1"/>
+    <col min="11009" max="11009" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11011" max="11011" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11029" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11030" max="11030" width="4.453125" style="1" customWidth="1"/>
+    <col min="11012" max="11029" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11030" max="11030" width="4.42578125" style="1" customWidth="1"/>
     <col min="11031" max="11031" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11032" max="11032" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11033" max="11264" width="11.453125" style="1"/>
-    <col min="11265" max="11265" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11032" max="11032" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11033" max="11264" width="11.42578125" style="1"/>
+    <col min="11265" max="11265" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11267" max="11267" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11285" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11286" max="11286" width="4.453125" style="1" customWidth="1"/>
+    <col min="11268" max="11285" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11286" max="11286" width="4.42578125" style="1" customWidth="1"/>
     <col min="11287" max="11287" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11288" max="11288" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11289" max="11520" width="11.453125" style="1"/>
-    <col min="11521" max="11521" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11288" max="11288" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11289" max="11520" width="11.42578125" style="1"/>
+    <col min="11521" max="11521" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11523" max="11523" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11541" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11542" max="11542" width="4.453125" style="1" customWidth="1"/>
+    <col min="11524" max="11541" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11542" max="11542" width="4.42578125" style="1" customWidth="1"/>
     <col min="11543" max="11543" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11544" max="11544" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11545" max="11776" width="11.453125" style="1"/>
-    <col min="11777" max="11777" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11544" max="11544" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11545" max="11776" width="11.42578125" style="1"/>
+    <col min="11777" max="11777" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11779" max="11779" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11797" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11798" max="11798" width="4.453125" style="1" customWidth="1"/>
+    <col min="11780" max="11797" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11798" max="11798" width="4.42578125" style="1" customWidth="1"/>
     <col min="11799" max="11799" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11800" max="11800" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11801" max="12032" width="11.453125" style="1"/>
-    <col min="12033" max="12033" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11800" max="11800" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11801" max="12032" width="11.42578125" style="1"/>
+    <col min="12033" max="12033" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12035" max="12035" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12053" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12054" max="12054" width="4.453125" style="1" customWidth="1"/>
+    <col min="12036" max="12053" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12054" max="12054" width="4.42578125" style="1" customWidth="1"/>
     <col min="12055" max="12055" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12056" max="12056" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12057" max="12288" width="11.453125" style="1"/>
-    <col min="12289" max="12289" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12056" max="12056" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12057" max="12288" width="11.42578125" style="1"/>
+    <col min="12289" max="12289" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12291" max="12291" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12309" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12310" max="12310" width="4.453125" style="1" customWidth="1"/>
+    <col min="12292" max="12309" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12310" max="12310" width="4.42578125" style="1" customWidth="1"/>
     <col min="12311" max="12311" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12312" max="12312" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12313" max="12544" width="11.453125" style="1"/>
-    <col min="12545" max="12545" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12312" max="12312" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12313" max="12544" width="11.42578125" style="1"/>
+    <col min="12545" max="12545" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12547" max="12547" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12565" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12566" max="12566" width="4.453125" style="1" customWidth="1"/>
+    <col min="12548" max="12565" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12566" max="12566" width="4.42578125" style="1" customWidth="1"/>
     <col min="12567" max="12567" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12568" max="12568" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12569" max="12800" width="11.453125" style="1"/>
-    <col min="12801" max="12801" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12568" max="12568" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12569" max="12800" width="11.42578125" style="1"/>
+    <col min="12801" max="12801" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12803" max="12803" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12821" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12822" max="12822" width="4.453125" style="1" customWidth="1"/>
+    <col min="12804" max="12821" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12822" max="12822" width="4.42578125" style="1" customWidth="1"/>
     <col min="12823" max="12823" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12824" max="12824" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12825" max="13056" width="11.453125" style="1"/>
-    <col min="13057" max="13057" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12824" max="12824" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12825" max="13056" width="11.42578125" style="1"/>
+    <col min="13057" max="13057" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13059" max="13059" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13077" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13078" max="13078" width="4.453125" style="1" customWidth="1"/>
+    <col min="13060" max="13077" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13078" max="13078" width="4.42578125" style="1" customWidth="1"/>
     <col min="13079" max="13079" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13080" max="13080" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13081" max="13312" width="11.453125" style="1"/>
-    <col min="13313" max="13313" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13080" max="13080" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13081" max="13312" width="11.42578125" style="1"/>
+    <col min="13313" max="13313" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13315" max="13315" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13333" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13334" max="13334" width="4.453125" style="1" customWidth="1"/>
+    <col min="13316" max="13333" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13334" max="13334" width="4.42578125" style="1" customWidth="1"/>
     <col min="13335" max="13335" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13336" max="13336" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13337" max="13568" width="11.453125" style="1"/>
-    <col min="13569" max="13569" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13336" max="13336" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13337" max="13568" width="11.42578125" style="1"/>
+    <col min="13569" max="13569" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13571" max="13571" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13589" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13590" max="13590" width="4.453125" style="1" customWidth="1"/>
+    <col min="13572" max="13589" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13590" max="13590" width="4.42578125" style="1" customWidth="1"/>
     <col min="13591" max="13591" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13592" max="13592" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13593" max="13824" width="11.453125" style="1"/>
-    <col min="13825" max="13825" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13592" max="13592" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13593" max="13824" width="11.42578125" style="1"/>
+    <col min="13825" max="13825" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13827" max="13827" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13845" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13846" max="13846" width="4.453125" style="1" customWidth="1"/>
+    <col min="13828" max="13845" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13846" max="13846" width="4.42578125" style="1" customWidth="1"/>
     <col min="13847" max="13847" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13848" max="13848" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13849" max="14080" width="11.453125" style="1"/>
-    <col min="14081" max="14081" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13848" max="13848" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13849" max="14080" width="11.42578125" style="1"/>
+    <col min="14081" max="14081" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14083" max="14083" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14101" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14102" max="14102" width="4.453125" style="1" customWidth="1"/>
+    <col min="14084" max="14101" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14102" max="14102" width="4.42578125" style="1" customWidth="1"/>
     <col min="14103" max="14103" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14104" max="14104" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14105" max="14336" width="11.453125" style="1"/>
-    <col min="14337" max="14337" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14104" max="14104" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14105" max="14336" width="11.42578125" style="1"/>
+    <col min="14337" max="14337" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14339" max="14339" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14357" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14358" max="14358" width="4.453125" style="1" customWidth="1"/>
+    <col min="14340" max="14357" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14358" max="14358" width="4.42578125" style="1" customWidth="1"/>
     <col min="14359" max="14359" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14360" max="14360" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14361" max="14592" width="11.453125" style="1"/>
-    <col min="14593" max="14593" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14360" max="14360" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14361" max="14592" width="11.42578125" style="1"/>
+    <col min="14593" max="14593" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14595" max="14595" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14613" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14614" max="14614" width="4.453125" style="1" customWidth="1"/>
+    <col min="14596" max="14613" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14614" max="14614" width="4.42578125" style="1" customWidth="1"/>
     <col min="14615" max="14615" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14616" max="14616" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14617" max="14848" width="11.453125" style="1"/>
-    <col min="14849" max="14849" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14616" max="14616" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14617" max="14848" width="11.42578125" style="1"/>
+    <col min="14849" max="14849" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14851" max="14851" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14869" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14870" max="14870" width="4.453125" style="1" customWidth="1"/>
+    <col min="14852" max="14869" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14870" max="14870" width="4.42578125" style="1" customWidth="1"/>
     <col min="14871" max="14871" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14872" max="14872" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14873" max="15104" width="11.453125" style="1"/>
-    <col min="15105" max="15105" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14872" max="14872" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14873" max="15104" width="11.42578125" style="1"/>
+    <col min="15105" max="15105" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15107" max="15107" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15125" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15126" max="15126" width="4.453125" style="1" customWidth="1"/>
+    <col min="15108" max="15125" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15126" max="15126" width="4.42578125" style="1" customWidth="1"/>
     <col min="15127" max="15127" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15128" max="15128" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15129" max="15360" width="11.453125" style="1"/>
-    <col min="15361" max="15361" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15128" max="15128" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15129" max="15360" width="11.42578125" style="1"/>
+    <col min="15361" max="15361" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15363" max="15363" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15381" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15382" max="15382" width="4.453125" style="1" customWidth="1"/>
+    <col min="15364" max="15381" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15382" max="15382" width="4.42578125" style="1" customWidth="1"/>
     <col min="15383" max="15383" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15384" max="15384" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15385" max="15616" width="11.453125" style="1"/>
-    <col min="15617" max="15617" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15384" max="15384" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15385" max="15616" width="11.42578125" style="1"/>
+    <col min="15617" max="15617" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15619" max="15619" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15637" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15638" max="15638" width="4.453125" style="1" customWidth="1"/>
+    <col min="15620" max="15637" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15638" max="15638" width="4.42578125" style="1" customWidth="1"/>
     <col min="15639" max="15639" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15640" max="15640" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15641" max="15872" width="11.453125" style="1"/>
-    <col min="15873" max="15873" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15640" max="15640" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15641" max="15872" width="11.42578125" style="1"/>
+    <col min="15873" max="15873" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15875" max="15875" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15893" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15894" max="15894" width="4.453125" style="1" customWidth="1"/>
+    <col min="15876" max="15893" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15894" max="15894" width="4.42578125" style="1" customWidth="1"/>
     <col min="15895" max="15895" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15896" max="15896" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15897" max="16128" width="11.453125" style="1"/>
-    <col min="16129" max="16129" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15896" max="15896" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15897" max="16128" width="11.42578125" style="1"/>
+    <col min="16129" max="16129" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16131" max="16131" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16149" width="2.7265625" style="1" customWidth="1"/>
-    <col min="16150" max="16150" width="4.453125" style="1" customWidth="1"/>
+    <col min="16132" max="16149" width="2.7109375" style="1" customWidth="1"/>
+    <col min="16150" max="16150" width="4.42578125" style="1" customWidth="1"/>
     <col min="16151" max="16151" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="16152" max="16152" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16153" max="16384" width="11.453125" style="1"/>
+    <col min="16152" max="16152" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16153" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9554,7 +9519,7 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
     </row>
-    <row r="2" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -9584,7 +9549,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
     </row>
-    <row r="3" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -9614,7 +9579,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
     </row>
-    <row r="4" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -9644,7 +9609,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -9652,7 +9617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -9735,7 +9700,7 @@
       </c>
       <c r="AB7" s="12"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -9885,7 +9850,7 @@
       </c>
       <c r="Y9" s="8"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -9960,7 +9925,7 @@
       </c>
       <c r="Y10" s="8"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -10035,7 +10000,7 @@
       </c>
       <c r="Y11" s="8"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -10110,7 +10075,7 @@
       </c>
       <c r="Y12" s="8"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -10185,7 +10150,7 @@
       </c>
       <c r="Y13" s="8"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>113</v>
       </c>
@@ -10260,7 +10225,7 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -10335,7 +10300,7 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -10410,7 +10375,7 @@
       </c>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -10485,7 +10450,7 @@
       </c>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>115</v>
       </c>
@@ -10635,7 +10600,7 @@
       </c>
       <c r="Y19" s="8"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>117</v>
       </c>
@@ -10785,7 +10750,7 @@
       </c>
       <c r="Y21" s="8"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -10860,7 +10825,7 @@
       </c>
       <c r="Y22" s="8"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -10935,7 +10900,7 @@
       </c>
       <c r="Y23" s="8"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -11010,7 +10975,7 @@
       </c>
       <c r="Y24" s="8"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>123</v>
       </c>
@@ -11085,7 +11050,7 @@
       </c>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
@@ -11687,61 +11652,61 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C34" s="8">
-        <v>2.4</v>
+        <v>5.5</v>
       </c>
       <c r="D34" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E34" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G34" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H34" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I34" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J34" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K34" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L34" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M34" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N34" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O34" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P34" s="8">
         <v>6</v>
       </c>
       <c r="Q34" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R34" s="8">
         <v>5</v>
       </c>
       <c r="S34" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T34" s="8">
         <v>4</v>
@@ -11753,7 +11718,7 @@
         <v>85</v>
       </c>
       <c r="W34" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="X34" s="8">
         <v>80</v>
@@ -11762,61 +11727,61 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C35" s="8">
-        <v>5.5</v>
+        <v>19.2</v>
       </c>
       <c r="D35" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E35" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F35" s="8">
         <v>5</v>
       </c>
       <c r="G35" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H35" s="8">
+        <v>6</v>
+      </c>
+      <c r="I35" s="8">
+        <v>4</v>
+      </c>
+      <c r="J35" s="8">
+        <v>5</v>
+      </c>
+      <c r="K35" s="8">
+        <v>3</v>
+      </c>
+      <c r="L35" s="8">
+        <v>6</v>
+      </c>
+      <c r="M35" s="8">
+        <v>6</v>
+      </c>
+      <c r="N35" s="8">
+        <v>4</v>
+      </c>
+      <c r="O35" s="8">
+        <v>5</v>
+      </c>
+      <c r="P35" s="8">
         <v>7</v>
       </c>
-      <c r="I35" s="8">
-        <v>5</v>
-      </c>
-      <c r="J35" s="8">
-        <v>4</v>
-      </c>
-      <c r="K35" s="8">
-        <v>3</v>
-      </c>
-      <c r="L35" s="8">
-        <v>6</v>
-      </c>
-      <c r="M35" s="8">
-        <v>4</v>
-      </c>
-      <c r="N35" s="8">
-        <v>4</v>
-      </c>
-      <c r="O35" s="8">
-        <v>6</v>
-      </c>
-      <c r="P35" s="8">
-        <v>6</v>
-      </c>
       <c r="Q35" s="8">
         <v>4</v>
       </c>
       <c r="R35" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S35" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T35" s="8">
         <v>4</v>
@@ -11825,37 +11790,37 @@
         <v>5</v>
       </c>
       <c r="V35" s="8">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="W35" s="1">
-        <v>8</v>
+        <v>-5</v>
       </c>
       <c r="X35" s="8">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Y35" s="8"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>134</v>
+        <v>81</v>
       </c>
       <c r="C36" s="8">
-        <v>19.2</v>
+        <v>6.4</v>
       </c>
       <c r="D36" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E36" s="8">
         <v>5</v>
       </c>
       <c r="F36" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G36" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H36" s="8">
         <v>6</v>
@@ -11867,13 +11832,13 @@
         <v>5</v>
       </c>
       <c r="K36" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L36" s="8">
         <v>6</v>
       </c>
       <c r="M36" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N36" s="8">
         <v>4</v>
@@ -11885,52 +11850,52 @@
         <v>7</v>
       </c>
       <c r="Q36" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R36" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S36" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T36" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U36" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V36" s="8">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="W36" s="1">
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="X36" s="8">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="Y36" s="8"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C37" s="8">
-        <v>6.4</v>
+        <v>6.9</v>
       </c>
       <c r="D37" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F37" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G37" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H37" s="8">
         <v>6</v>
@@ -11942,7 +11907,7 @@
         <v>5</v>
       </c>
       <c r="K37" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L37" s="8">
         <v>6</v>
@@ -11954,7 +11919,7 @@
         <v>4</v>
       </c>
       <c r="O37" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P37" s="8">
         <v>7</v>
@@ -11963,46 +11928,45 @@
         <v>5</v>
       </c>
       <c r="R37" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S37" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T37" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U37" s="8">
         <v>6</v>
       </c>
       <c r="V37" s="8">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="W37" s="1">
         <v>10</v>
       </c>
       <c r="X37" s="8">
-        <v>83</v>
-      </c>
-      <c r="Y37" s="8"/>
+        <v>84</v>
+      </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
       <c r="C38" s="8">
-        <v>6.9</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D38" s="8">
         <v>4</v>
       </c>
       <c r="E38" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F38" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G38" s="8">
         <v>5</v>
@@ -12011,16 +11975,16 @@
         <v>6</v>
       </c>
       <c r="I38" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J38" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K38" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L38" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M38" s="8">
         <v>5</v>
@@ -12029,10 +11993,10 @@
         <v>4</v>
       </c>
       <c r="O38" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P38" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q38" s="8">
         <v>5</v>
@@ -12044,30 +12008,30 @@
         <v>4</v>
       </c>
       <c r="T38" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U38" s="8">
         <v>6</v>
       </c>
       <c r="V38" s="8">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="W38" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="X38" s="8">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>136</v>
+        <v>91</v>
       </c>
       <c r="C39" s="8">
-        <v>9.3000000000000007</v>
+        <v>26.8</v>
       </c>
       <c r="D39" s="8">
         <v>4</v>
@@ -12076,58 +12040,58 @@
         <v>5</v>
       </c>
       <c r="F39" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G39" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H39" s="8">
         <v>6</v>
       </c>
       <c r="I39" s="8">
+        <v>4</v>
+      </c>
+      <c r="J39" s="8">
+        <v>4</v>
+      </c>
+      <c r="K39" s="8">
+        <v>5</v>
+      </c>
+      <c r="L39" s="8">
+        <v>6</v>
+      </c>
+      <c r="M39" s="8">
+        <v>5</v>
+      </c>
+      <c r="N39" s="8">
+        <v>3</v>
+      </c>
+      <c r="O39" s="8">
+        <v>5</v>
+      </c>
+      <c r="P39" s="8">
         <v>7</v>
       </c>
-      <c r="J39" s="8">
-        <v>6</v>
-      </c>
-      <c r="K39" s="8">
-        <v>4</v>
-      </c>
-      <c r="L39" s="8">
-        <v>5</v>
-      </c>
-      <c r="M39" s="8">
-        <v>5</v>
-      </c>
-      <c r="N39" s="8">
-        <v>4</v>
-      </c>
-      <c r="O39" s="8">
-        <v>5</v>
-      </c>
-      <c r="P39" s="8">
-        <v>6</v>
-      </c>
       <c r="Q39" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R39" s="8">
+        <v>8</v>
+      </c>
+      <c r="S39" s="8">
+        <v>6</v>
+      </c>
+      <c r="T39" s="8">
         <v>7</v>
       </c>
-      <c r="S39" s="8">
-        <v>4</v>
-      </c>
-      <c r="T39" s="8">
-        <v>3</v>
-      </c>
       <c r="U39" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V39" s="8">
         <v>93</v>
       </c>
       <c r="W39" s="1">
-        <v>12</v>
+        <v>-6</v>
       </c>
       <c r="X39" s="8">
         <v>88</v>
@@ -12135,13 +12099,13 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C40" s="8">
-        <v>26.8</v>
+        <v>7.4</v>
       </c>
       <c r="D40" s="8">
         <v>4</v>
@@ -12153,69 +12117,69 @@
         <v>5</v>
       </c>
       <c r="G40" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H40" s="8">
         <v>6</v>
       </c>
       <c r="I40" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J40" s="8">
         <v>4</v>
       </c>
       <c r="K40" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L40" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M40" s="8">
         <v>5</v>
       </c>
       <c r="N40" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O40" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P40" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q40" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R40" s="8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S40" s="8">
         <v>6</v>
       </c>
       <c r="T40" s="8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="U40" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V40" s="8">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="W40" s="1">
-        <v>-6</v>
+        <v>15</v>
       </c>
       <c r="X40" s="8">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="C41" s="8">
-        <v>7.4</v>
+        <v>16.7</v>
       </c>
       <c r="D41" s="8">
         <v>4</v>
@@ -12227,132 +12191,75 @@
         <v>5</v>
       </c>
       <c r="G41" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H41" s="8">
         <v>6</v>
       </c>
       <c r="I41" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J41" s="8">
         <v>4</v>
       </c>
       <c r="K41" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L41" s="8">
+        <v>6</v>
+      </c>
+      <c r="M41" s="8">
+        <v>6</v>
+      </c>
+      <c r="N41" s="8">
+        <v>6</v>
+      </c>
+      <c r="O41" s="8">
+        <v>6</v>
+      </c>
+      <c r="P41" s="8">
+        <v>9</v>
+      </c>
+      <c r="Q41" s="8">
+        <v>6</v>
+      </c>
+      <c r="R41" s="8">
         <v>7</v>
       </c>
-      <c r="M41" s="8">
-        <v>5</v>
-      </c>
-      <c r="N41" s="8">
-        <v>4</v>
-      </c>
-      <c r="O41" s="8">
-        <v>6</v>
-      </c>
-      <c r="P41" s="8">
-        <v>8</v>
-      </c>
-      <c r="Q41" s="8">
-        <v>6</v>
-      </c>
-      <c r="R41" s="8">
-        <v>6</v>
-      </c>
       <c r="S41" s="8">
         <v>6</v>
       </c>
       <c r="T41" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="U41" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V41" s="8">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="W41" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="X41" s="8">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C42" s="8">
-        <v>16.7</v>
-      </c>
-      <c r="D42" s="8">
-        <v>4</v>
-      </c>
-      <c r="E42" s="8">
-        <v>5</v>
-      </c>
-      <c r="F42" s="8">
-        <v>5</v>
-      </c>
-      <c r="G42" s="8">
-        <v>6</v>
-      </c>
-      <c r="H42" s="8">
-        <v>6</v>
-      </c>
-      <c r="I42" s="8">
-        <v>3</v>
-      </c>
-      <c r="J42" s="8">
-        <v>4</v>
-      </c>
-      <c r="K42" s="8">
-        <v>5</v>
-      </c>
-      <c r="L42" s="8">
-        <v>6</v>
-      </c>
-      <c r="M42" s="8">
-        <v>6</v>
-      </c>
-      <c r="N42" s="8">
-        <v>6</v>
-      </c>
-      <c r="O42" s="8">
-        <v>6</v>
-      </c>
-      <c r="P42" s="8">
-        <v>9</v>
-      </c>
-      <c r="Q42" s="8">
-        <v>6</v>
-      </c>
-      <c r="R42" s="8">
-        <v>7</v>
-      </c>
-      <c r="S42" s="8">
-        <v>6</v>
-      </c>
-      <c r="T42" s="8">
-        <v>5</v>
-      </c>
-      <c r="U42" s="8">
-        <v>7</v>
-      </c>
-      <c r="V42" s="8">
-        <v>102</v>
-      </c>
-      <c r="W42" s="1">
-        <v>13</v>
-      </c>
-      <c r="X42" s="8">
-        <v>97</v>
+        <v>106</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="V42" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="W42" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X42" s="8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
@@ -15028,9 +14935,6 @@
       <c r="A200" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C200" s="8" t="s">
-        <v>107</v>
-      </c>
       <c r="V200" s="8" t="s">
         <v>107</v>
       </c>
@@ -15202,7 +15106,7 @@
       <c r="V212" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="W212" s="1" t="e">
+      <c r="W212" s="8" t="e">
         <v>#VALUE!</v>
       </c>
       <c r="X212" s="8" t="s">
@@ -15241,15 +15145,6 @@
       <c r="A215" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="V215" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="W215" s="8" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="X215" s="8" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="216" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
@@ -15671,14 +15566,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B50 IX8:IX50 ST8:ST50 ACP8:ACP50 AML8:AML50 AWH8:AWH50 BGD8:BGD50 BPZ8:BPZ50 BZV8:BZV50 CJR8:CJR50 CTN8:CTN50 DDJ8:DDJ50 DNF8:DNF50 DXB8:DXB50 EGX8:EGX50 EQT8:EQT50 FAP8:FAP50 FKL8:FKL50 FUH8:FUH50 GED8:GED50 GNZ8:GNZ50 GXV8:GXV50 HHR8:HHR50 HRN8:HRN50 IBJ8:IBJ50 ILF8:ILF50 IVB8:IVB50 JEX8:JEX50 JOT8:JOT50 JYP8:JYP50 KIL8:KIL50 KSH8:KSH50 LCD8:LCD50 LLZ8:LLZ50 LVV8:LVV50 MFR8:MFR50 MPN8:MPN50 MZJ8:MZJ50 NJF8:NJF50 NTB8:NTB50 OCX8:OCX50 OMT8:OMT50 OWP8:OWP50 PGL8:PGL50 PQH8:PQH50 QAD8:QAD50 QJZ8:QJZ50 QTV8:QTV50 RDR8:RDR50 RNN8:RNN50 RXJ8:RXJ50 SHF8:SHF50 SRB8:SRB50 TAX8:TAX50 TKT8:TKT50 TUP8:TUP50 UEL8:UEL50 UOH8:UOH50 UYD8:UYD50 VHZ8:VHZ50 VRV8:VRV50 WBR8:WBR50 WLN8:WLN50 WVJ8:WVJ50 B65544:B65586 IX65544:IX65586 ST65544:ST65586 ACP65544:ACP65586 AML65544:AML65586 AWH65544:AWH65586 BGD65544:BGD65586 BPZ65544:BPZ65586 BZV65544:BZV65586 CJR65544:CJR65586 CTN65544:CTN65586 DDJ65544:DDJ65586 DNF65544:DNF65586 DXB65544:DXB65586 EGX65544:EGX65586 EQT65544:EQT65586 FAP65544:FAP65586 FKL65544:FKL65586 FUH65544:FUH65586 GED65544:GED65586 GNZ65544:GNZ65586 GXV65544:GXV65586 HHR65544:HHR65586 HRN65544:HRN65586 IBJ65544:IBJ65586 ILF65544:ILF65586 IVB65544:IVB65586 JEX65544:JEX65586 JOT65544:JOT65586 JYP65544:JYP65586 KIL65544:KIL65586 KSH65544:KSH65586 LCD65544:LCD65586 LLZ65544:LLZ65586 LVV65544:LVV65586 MFR65544:MFR65586 MPN65544:MPN65586 MZJ65544:MZJ65586 NJF65544:NJF65586 NTB65544:NTB65586 OCX65544:OCX65586 OMT65544:OMT65586 OWP65544:OWP65586 PGL65544:PGL65586 PQH65544:PQH65586 QAD65544:QAD65586 QJZ65544:QJZ65586 QTV65544:QTV65586 RDR65544:RDR65586 RNN65544:RNN65586 RXJ65544:RXJ65586 SHF65544:SHF65586 SRB65544:SRB65586 TAX65544:TAX65586 TKT65544:TKT65586 TUP65544:TUP65586 UEL65544:UEL65586 UOH65544:UOH65586 UYD65544:UYD65586 VHZ65544:VHZ65586 VRV65544:VRV65586 WBR65544:WBR65586 WLN65544:WLN65586 WVJ65544:WVJ65586 B131080:B131122 IX131080:IX131122 ST131080:ST131122 ACP131080:ACP131122 AML131080:AML131122 AWH131080:AWH131122 BGD131080:BGD131122 BPZ131080:BPZ131122 BZV131080:BZV131122 CJR131080:CJR131122 CTN131080:CTN131122 DDJ131080:DDJ131122 DNF131080:DNF131122 DXB131080:DXB131122 EGX131080:EGX131122 EQT131080:EQT131122 FAP131080:FAP131122 FKL131080:FKL131122 FUH131080:FUH131122 GED131080:GED131122 GNZ131080:GNZ131122 GXV131080:GXV131122 HHR131080:HHR131122 HRN131080:HRN131122 IBJ131080:IBJ131122 ILF131080:ILF131122 IVB131080:IVB131122 JEX131080:JEX131122 JOT131080:JOT131122 JYP131080:JYP131122 KIL131080:KIL131122 KSH131080:KSH131122 LCD131080:LCD131122 LLZ131080:LLZ131122 LVV131080:LVV131122 MFR131080:MFR131122 MPN131080:MPN131122 MZJ131080:MZJ131122 NJF131080:NJF131122 NTB131080:NTB131122 OCX131080:OCX131122 OMT131080:OMT131122 OWP131080:OWP131122 PGL131080:PGL131122 PQH131080:PQH131122 QAD131080:QAD131122 QJZ131080:QJZ131122 QTV131080:QTV131122 RDR131080:RDR131122 RNN131080:RNN131122 RXJ131080:RXJ131122 SHF131080:SHF131122 SRB131080:SRB131122 TAX131080:TAX131122 TKT131080:TKT131122 TUP131080:TUP131122 UEL131080:UEL131122 UOH131080:UOH131122 UYD131080:UYD131122 VHZ131080:VHZ131122 VRV131080:VRV131122 WBR131080:WBR131122 WLN131080:WLN131122 WVJ131080:WVJ131122 B196616:B196658 IX196616:IX196658 ST196616:ST196658 ACP196616:ACP196658 AML196616:AML196658 AWH196616:AWH196658 BGD196616:BGD196658 BPZ196616:BPZ196658 BZV196616:BZV196658 CJR196616:CJR196658 CTN196616:CTN196658 DDJ196616:DDJ196658 DNF196616:DNF196658 DXB196616:DXB196658 EGX196616:EGX196658 EQT196616:EQT196658 FAP196616:FAP196658 FKL196616:FKL196658 FUH196616:FUH196658 GED196616:GED196658 GNZ196616:GNZ196658 GXV196616:GXV196658 HHR196616:HHR196658 HRN196616:HRN196658 IBJ196616:IBJ196658 ILF196616:ILF196658 IVB196616:IVB196658 JEX196616:JEX196658 JOT196616:JOT196658 JYP196616:JYP196658 KIL196616:KIL196658 KSH196616:KSH196658 LCD196616:LCD196658 LLZ196616:LLZ196658 LVV196616:LVV196658 MFR196616:MFR196658 MPN196616:MPN196658 MZJ196616:MZJ196658 NJF196616:NJF196658 NTB196616:NTB196658 OCX196616:OCX196658 OMT196616:OMT196658 OWP196616:OWP196658 PGL196616:PGL196658 PQH196616:PQH196658 QAD196616:QAD196658 QJZ196616:QJZ196658 QTV196616:QTV196658 RDR196616:RDR196658 RNN196616:RNN196658 RXJ196616:RXJ196658 SHF196616:SHF196658 SRB196616:SRB196658 TAX196616:TAX196658 TKT196616:TKT196658 TUP196616:TUP196658 UEL196616:UEL196658 UOH196616:UOH196658 UYD196616:UYD196658 VHZ196616:VHZ196658 VRV196616:VRV196658 WBR196616:WBR196658 WLN196616:WLN196658 WVJ196616:WVJ196658 B262152:B262194 IX262152:IX262194 ST262152:ST262194 ACP262152:ACP262194 AML262152:AML262194 AWH262152:AWH262194 BGD262152:BGD262194 BPZ262152:BPZ262194 BZV262152:BZV262194 CJR262152:CJR262194 CTN262152:CTN262194 DDJ262152:DDJ262194 DNF262152:DNF262194 DXB262152:DXB262194 EGX262152:EGX262194 EQT262152:EQT262194 FAP262152:FAP262194 FKL262152:FKL262194 FUH262152:FUH262194 GED262152:GED262194 GNZ262152:GNZ262194 GXV262152:GXV262194 HHR262152:HHR262194 HRN262152:HRN262194 IBJ262152:IBJ262194 ILF262152:ILF262194 IVB262152:IVB262194 JEX262152:JEX262194 JOT262152:JOT262194 JYP262152:JYP262194 KIL262152:KIL262194 KSH262152:KSH262194 LCD262152:LCD262194 LLZ262152:LLZ262194 LVV262152:LVV262194 MFR262152:MFR262194 MPN262152:MPN262194 MZJ262152:MZJ262194 NJF262152:NJF262194 NTB262152:NTB262194 OCX262152:OCX262194 OMT262152:OMT262194 OWP262152:OWP262194 PGL262152:PGL262194 PQH262152:PQH262194 QAD262152:QAD262194 QJZ262152:QJZ262194 QTV262152:QTV262194 RDR262152:RDR262194 RNN262152:RNN262194 RXJ262152:RXJ262194 SHF262152:SHF262194 SRB262152:SRB262194 TAX262152:TAX262194 TKT262152:TKT262194 TUP262152:TUP262194 UEL262152:UEL262194 UOH262152:UOH262194 UYD262152:UYD262194 VHZ262152:VHZ262194 VRV262152:VRV262194 WBR262152:WBR262194 WLN262152:WLN262194 WVJ262152:WVJ262194 B327688:B327730 IX327688:IX327730 ST327688:ST327730 ACP327688:ACP327730 AML327688:AML327730 AWH327688:AWH327730 BGD327688:BGD327730 BPZ327688:BPZ327730 BZV327688:BZV327730 CJR327688:CJR327730 CTN327688:CTN327730 DDJ327688:DDJ327730 DNF327688:DNF327730 DXB327688:DXB327730 EGX327688:EGX327730 EQT327688:EQT327730 FAP327688:FAP327730 FKL327688:FKL327730 FUH327688:FUH327730 GED327688:GED327730 GNZ327688:GNZ327730 GXV327688:GXV327730 HHR327688:HHR327730 HRN327688:HRN327730 IBJ327688:IBJ327730 ILF327688:ILF327730 IVB327688:IVB327730 JEX327688:JEX327730 JOT327688:JOT327730 JYP327688:JYP327730 KIL327688:KIL327730 KSH327688:KSH327730 LCD327688:LCD327730 LLZ327688:LLZ327730 LVV327688:LVV327730 MFR327688:MFR327730 MPN327688:MPN327730 MZJ327688:MZJ327730 NJF327688:NJF327730 NTB327688:NTB327730 OCX327688:OCX327730 OMT327688:OMT327730 OWP327688:OWP327730 PGL327688:PGL327730 PQH327688:PQH327730 QAD327688:QAD327730 QJZ327688:QJZ327730 QTV327688:QTV327730 RDR327688:RDR327730 RNN327688:RNN327730 RXJ327688:RXJ327730 SHF327688:SHF327730 SRB327688:SRB327730 TAX327688:TAX327730 TKT327688:TKT327730 TUP327688:TUP327730 UEL327688:UEL327730 UOH327688:UOH327730 UYD327688:UYD327730 VHZ327688:VHZ327730 VRV327688:VRV327730 WBR327688:WBR327730 WLN327688:WLN327730 WVJ327688:WVJ327730 B393224:B393266 IX393224:IX393266 ST393224:ST393266 ACP393224:ACP393266 AML393224:AML393266 AWH393224:AWH393266 BGD393224:BGD393266 BPZ393224:BPZ393266 BZV393224:BZV393266 CJR393224:CJR393266 CTN393224:CTN393266 DDJ393224:DDJ393266 DNF393224:DNF393266 DXB393224:DXB393266 EGX393224:EGX393266 EQT393224:EQT393266 FAP393224:FAP393266 FKL393224:FKL393266 FUH393224:FUH393266 GED393224:GED393266 GNZ393224:GNZ393266 GXV393224:GXV393266 HHR393224:HHR393266 HRN393224:HRN393266 IBJ393224:IBJ393266 ILF393224:ILF393266 IVB393224:IVB393266 JEX393224:JEX393266 JOT393224:JOT393266 JYP393224:JYP393266 KIL393224:KIL393266 KSH393224:KSH393266 LCD393224:LCD393266 LLZ393224:LLZ393266 LVV393224:LVV393266 MFR393224:MFR393266 MPN393224:MPN393266 MZJ393224:MZJ393266 NJF393224:NJF393266 NTB393224:NTB393266 OCX393224:OCX393266 OMT393224:OMT393266 OWP393224:OWP393266 PGL393224:PGL393266 PQH393224:PQH393266 QAD393224:QAD393266 QJZ393224:QJZ393266 QTV393224:QTV393266 RDR393224:RDR393266 RNN393224:RNN393266 RXJ393224:RXJ393266 SHF393224:SHF393266 SRB393224:SRB393266 TAX393224:TAX393266 TKT393224:TKT393266 TUP393224:TUP393266 UEL393224:UEL393266 UOH393224:UOH393266 UYD393224:UYD393266 VHZ393224:VHZ393266 VRV393224:VRV393266 WBR393224:WBR393266 WLN393224:WLN393266 WVJ393224:WVJ393266 B458760:B458802 IX458760:IX458802 ST458760:ST458802 ACP458760:ACP458802 AML458760:AML458802 AWH458760:AWH458802 BGD458760:BGD458802 BPZ458760:BPZ458802 BZV458760:BZV458802 CJR458760:CJR458802 CTN458760:CTN458802 DDJ458760:DDJ458802 DNF458760:DNF458802 DXB458760:DXB458802 EGX458760:EGX458802 EQT458760:EQT458802 FAP458760:FAP458802 FKL458760:FKL458802 FUH458760:FUH458802 GED458760:GED458802 GNZ458760:GNZ458802 GXV458760:GXV458802 HHR458760:HHR458802 HRN458760:HRN458802 IBJ458760:IBJ458802 ILF458760:ILF458802 IVB458760:IVB458802 JEX458760:JEX458802 JOT458760:JOT458802 JYP458760:JYP458802 KIL458760:KIL458802 KSH458760:KSH458802 LCD458760:LCD458802 LLZ458760:LLZ458802 LVV458760:LVV458802 MFR458760:MFR458802 MPN458760:MPN458802 MZJ458760:MZJ458802 NJF458760:NJF458802 NTB458760:NTB458802 OCX458760:OCX458802 OMT458760:OMT458802 OWP458760:OWP458802 PGL458760:PGL458802 PQH458760:PQH458802 QAD458760:QAD458802 QJZ458760:QJZ458802 QTV458760:QTV458802 RDR458760:RDR458802 RNN458760:RNN458802 RXJ458760:RXJ458802 SHF458760:SHF458802 SRB458760:SRB458802 TAX458760:TAX458802 TKT458760:TKT458802 TUP458760:TUP458802 UEL458760:UEL458802 UOH458760:UOH458802 UYD458760:UYD458802 VHZ458760:VHZ458802 VRV458760:VRV458802 WBR458760:WBR458802 WLN458760:WLN458802 WVJ458760:WVJ458802 B524296:B524338 IX524296:IX524338 ST524296:ST524338 ACP524296:ACP524338 AML524296:AML524338 AWH524296:AWH524338 BGD524296:BGD524338 BPZ524296:BPZ524338 BZV524296:BZV524338 CJR524296:CJR524338 CTN524296:CTN524338 DDJ524296:DDJ524338 DNF524296:DNF524338 DXB524296:DXB524338 EGX524296:EGX524338 EQT524296:EQT524338 FAP524296:FAP524338 FKL524296:FKL524338 FUH524296:FUH524338 GED524296:GED524338 GNZ524296:GNZ524338 GXV524296:GXV524338 HHR524296:HHR524338 HRN524296:HRN524338 IBJ524296:IBJ524338 ILF524296:ILF524338 IVB524296:IVB524338 JEX524296:JEX524338 JOT524296:JOT524338 JYP524296:JYP524338 KIL524296:KIL524338 KSH524296:KSH524338 LCD524296:LCD524338 LLZ524296:LLZ524338 LVV524296:LVV524338 MFR524296:MFR524338 MPN524296:MPN524338 MZJ524296:MZJ524338 NJF524296:NJF524338 NTB524296:NTB524338 OCX524296:OCX524338 OMT524296:OMT524338 OWP524296:OWP524338 PGL524296:PGL524338 PQH524296:PQH524338 QAD524296:QAD524338 QJZ524296:QJZ524338 QTV524296:QTV524338 RDR524296:RDR524338 RNN524296:RNN524338 RXJ524296:RXJ524338 SHF524296:SHF524338 SRB524296:SRB524338 TAX524296:TAX524338 TKT524296:TKT524338 TUP524296:TUP524338 UEL524296:UEL524338 UOH524296:UOH524338 UYD524296:UYD524338 VHZ524296:VHZ524338 VRV524296:VRV524338 WBR524296:WBR524338 WLN524296:WLN524338 WVJ524296:WVJ524338 B589832:B589874 IX589832:IX589874 ST589832:ST589874 ACP589832:ACP589874 AML589832:AML589874 AWH589832:AWH589874 BGD589832:BGD589874 BPZ589832:BPZ589874 BZV589832:BZV589874 CJR589832:CJR589874 CTN589832:CTN589874 DDJ589832:DDJ589874 DNF589832:DNF589874 DXB589832:DXB589874 EGX589832:EGX589874 EQT589832:EQT589874 FAP589832:FAP589874 FKL589832:FKL589874 FUH589832:FUH589874 GED589832:GED589874 GNZ589832:GNZ589874 GXV589832:GXV589874 HHR589832:HHR589874 HRN589832:HRN589874 IBJ589832:IBJ589874 ILF589832:ILF589874 IVB589832:IVB589874 JEX589832:JEX589874 JOT589832:JOT589874 JYP589832:JYP589874 KIL589832:KIL589874 KSH589832:KSH589874 LCD589832:LCD589874 LLZ589832:LLZ589874 LVV589832:LVV589874 MFR589832:MFR589874 MPN589832:MPN589874 MZJ589832:MZJ589874 NJF589832:NJF589874 NTB589832:NTB589874 OCX589832:OCX589874 OMT589832:OMT589874 OWP589832:OWP589874 PGL589832:PGL589874 PQH589832:PQH589874 QAD589832:QAD589874 QJZ589832:QJZ589874 QTV589832:QTV589874 RDR589832:RDR589874 RNN589832:RNN589874 RXJ589832:RXJ589874 SHF589832:SHF589874 SRB589832:SRB589874 TAX589832:TAX589874 TKT589832:TKT589874 TUP589832:TUP589874 UEL589832:UEL589874 UOH589832:UOH589874 UYD589832:UYD589874 VHZ589832:VHZ589874 VRV589832:VRV589874 WBR589832:WBR589874 WLN589832:WLN589874 WVJ589832:WVJ589874 B655368:B655410 IX655368:IX655410 ST655368:ST655410 ACP655368:ACP655410 AML655368:AML655410 AWH655368:AWH655410 BGD655368:BGD655410 BPZ655368:BPZ655410 BZV655368:BZV655410 CJR655368:CJR655410 CTN655368:CTN655410 DDJ655368:DDJ655410 DNF655368:DNF655410 DXB655368:DXB655410 EGX655368:EGX655410 EQT655368:EQT655410 FAP655368:FAP655410 FKL655368:FKL655410 FUH655368:FUH655410 GED655368:GED655410 GNZ655368:GNZ655410 GXV655368:GXV655410 HHR655368:HHR655410 HRN655368:HRN655410 IBJ655368:IBJ655410 ILF655368:ILF655410 IVB655368:IVB655410 JEX655368:JEX655410 JOT655368:JOT655410 JYP655368:JYP655410 KIL655368:KIL655410 KSH655368:KSH655410 LCD655368:LCD655410 LLZ655368:LLZ655410 LVV655368:LVV655410 MFR655368:MFR655410 MPN655368:MPN655410 MZJ655368:MZJ655410 NJF655368:NJF655410 NTB655368:NTB655410 OCX655368:OCX655410 OMT655368:OMT655410 OWP655368:OWP655410 PGL655368:PGL655410 PQH655368:PQH655410 QAD655368:QAD655410 QJZ655368:QJZ655410 QTV655368:QTV655410 RDR655368:RDR655410 RNN655368:RNN655410 RXJ655368:RXJ655410 SHF655368:SHF655410 SRB655368:SRB655410 TAX655368:TAX655410 TKT655368:TKT655410 TUP655368:TUP655410 UEL655368:UEL655410 UOH655368:UOH655410 UYD655368:UYD655410 VHZ655368:VHZ655410 VRV655368:VRV655410 WBR655368:WBR655410 WLN655368:WLN655410 WVJ655368:WVJ655410 B720904:B720946 IX720904:IX720946 ST720904:ST720946 ACP720904:ACP720946 AML720904:AML720946 AWH720904:AWH720946 BGD720904:BGD720946 BPZ720904:BPZ720946 BZV720904:BZV720946 CJR720904:CJR720946 CTN720904:CTN720946 DDJ720904:DDJ720946 DNF720904:DNF720946 DXB720904:DXB720946 EGX720904:EGX720946 EQT720904:EQT720946 FAP720904:FAP720946 FKL720904:FKL720946 FUH720904:FUH720946 GED720904:GED720946 GNZ720904:GNZ720946 GXV720904:GXV720946 HHR720904:HHR720946 HRN720904:HRN720946 IBJ720904:IBJ720946 ILF720904:ILF720946 IVB720904:IVB720946 JEX720904:JEX720946 JOT720904:JOT720946 JYP720904:JYP720946 KIL720904:KIL720946 KSH720904:KSH720946 LCD720904:LCD720946 LLZ720904:LLZ720946 LVV720904:LVV720946 MFR720904:MFR720946 MPN720904:MPN720946 MZJ720904:MZJ720946 NJF720904:NJF720946 NTB720904:NTB720946 OCX720904:OCX720946 OMT720904:OMT720946 OWP720904:OWP720946 PGL720904:PGL720946 PQH720904:PQH720946 QAD720904:QAD720946 QJZ720904:QJZ720946 QTV720904:QTV720946 RDR720904:RDR720946 RNN720904:RNN720946 RXJ720904:RXJ720946 SHF720904:SHF720946 SRB720904:SRB720946 TAX720904:TAX720946 TKT720904:TKT720946 TUP720904:TUP720946 UEL720904:UEL720946 UOH720904:UOH720946 UYD720904:UYD720946 VHZ720904:VHZ720946 VRV720904:VRV720946 WBR720904:WBR720946 WLN720904:WLN720946 WVJ720904:WVJ720946 B786440:B786482 IX786440:IX786482 ST786440:ST786482 ACP786440:ACP786482 AML786440:AML786482 AWH786440:AWH786482 BGD786440:BGD786482 BPZ786440:BPZ786482 BZV786440:BZV786482 CJR786440:CJR786482 CTN786440:CTN786482 DDJ786440:DDJ786482 DNF786440:DNF786482 DXB786440:DXB786482 EGX786440:EGX786482 EQT786440:EQT786482 FAP786440:FAP786482 FKL786440:FKL786482 FUH786440:FUH786482 GED786440:GED786482 GNZ786440:GNZ786482 GXV786440:GXV786482 HHR786440:HHR786482 HRN786440:HRN786482 IBJ786440:IBJ786482 ILF786440:ILF786482 IVB786440:IVB786482 JEX786440:JEX786482 JOT786440:JOT786482 JYP786440:JYP786482 KIL786440:KIL786482 KSH786440:KSH786482 LCD786440:LCD786482 LLZ786440:LLZ786482 LVV786440:LVV786482 MFR786440:MFR786482 MPN786440:MPN786482 MZJ786440:MZJ786482 NJF786440:NJF786482 NTB786440:NTB786482 OCX786440:OCX786482 OMT786440:OMT786482 OWP786440:OWP786482 PGL786440:PGL786482 PQH786440:PQH786482 QAD786440:QAD786482 QJZ786440:QJZ786482 QTV786440:QTV786482 RDR786440:RDR786482 RNN786440:RNN786482 RXJ786440:RXJ786482 SHF786440:SHF786482 SRB786440:SRB786482 TAX786440:TAX786482 TKT786440:TKT786482 TUP786440:TUP786482 UEL786440:UEL786482 UOH786440:UOH786482 UYD786440:UYD786482 VHZ786440:VHZ786482 VRV786440:VRV786482 WBR786440:WBR786482 WLN786440:WLN786482 WVJ786440:WVJ786482 B851976:B852018 IX851976:IX852018 ST851976:ST852018 ACP851976:ACP852018 AML851976:AML852018 AWH851976:AWH852018 BGD851976:BGD852018 BPZ851976:BPZ852018 BZV851976:BZV852018 CJR851976:CJR852018 CTN851976:CTN852018 DDJ851976:DDJ852018 DNF851976:DNF852018 DXB851976:DXB852018 EGX851976:EGX852018 EQT851976:EQT852018 FAP851976:FAP852018 FKL851976:FKL852018 FUH851976:FUH852018 GED851976:GED852018 GNZ851976:GNZ852018 GXV851976:GXV852018 HHR851976:HHR852018 HRN851976:HRN852018 IBJ851976:IBJ852018 ILF851976:ILF852018 IVB851976:IVB852018 JEX851976:JEX852018 JOT851976:JOT852018 JYP851976:JYP852018 KIL851976:KIL852018 KSH851976:KSH852018 LCD851976:LCD852018 LLZ851976:LLZ852018 LVV851976:LVV852018 MFR851976:MFR852018 MPN851976:MPN852018 MZJ851976:MZJ852018 NJF851976:NJF852018 NTB851976:NTB852018 OCX851976:OCX852018 OMT851976:OMT852018 OWP851976:OWP852018 PGL851976:PGL852018 PQH851976:PQH852018 QAD851976:QAD852018 QJZ851976:QJZ852018 QTV851976:QTV852018 RDR851976:RDR852018 RNN851976:RNN852018 RXJ851976:RXJ852018 SHF851976:SHF852018 SRB851976:SRB852018 TAX851976:TAX852018 TKT851976:TKT852018 TUP851976:TUP852018 UEL851976:UEL852018 UOH851976:UOH852018 UYD851976:UYD852018 VHZ851976:VHZ852018 VRV851976:VRV852018 WBR851976:WBR852018 WLN851976:WLN852018 WVJ851976:WVJ852018 B917512:B917554 IX917512:IX917554 ST917512:ST917554 ACP917512:ACP917554 AML917512:AML917554 AWH917512:AWH917554 BGD917512:BGD917554 BPZ917512:BPZ917554 BZV917512:BZV917554 CJR917512:CJR917554 CTN917512:CTN917554 DDJ917512:DDJ917554 DNF917512:DNF917554 DXB917512:DXB917554 EGX917512:EGX917554 EQT917512:EQT917554 FAP917512:FAP917554 FKL917512:FKL917554 FUH917512:FUH917554 GED917512:GED917554 GNZ917512:GNZ917554 GXV917512:GXV917554 HHR917512:HHR917554 HRN917512:HRN917554 IBJ917512:IBJ917554 ILF917512:ILF917554 IVB917512:IVB917554 JEX917512:JEX917554 JOT917512:JOT917554 JYP917512:JYP917554 KIL917512:KIL917554 KSH917512:KSH917554 LCD917512:LCD917554 LLZ917512:LLZ917554 LVV917512:LVV917554 MFR917512:MFR917554 MPN917512:MPN917554 MZJ917512:MZJ917554 NJF917512:NJF917554 NTB917512:NTB917554 OCX917512:OCX917554 OMT917512:OMT917554 OWP917512:OWP917554 PGL917512:PGL917554 PQH917512:PQH917554 QAD917512:QAD917554 QJZ917512:QJZ917554 QTV917512:QTV917554 RDR917512:RDR917554 RNN917512:RNN917554 RXJ917512:RXJ917554 SHF917512:SHF917554 SRB917512:SRB917554 TAX917512:TAX917554 TKT917512:TKT917554 TUP917512:TUP917554 UEL917512:UEL917554 UOH917512:UOH917554 UYD917512:UYD917554 VHZ917512:VHZ917554 VRV917512:VRV917554 WBR917512:WBR917554 WLN917512:WLN917554 WVJ917512:WVJ917554 B983048:B983090 IX983048:IX983090 ST983048:ST983090 ACP983048:ACP983090 AML983048:AML983090 AWH983048:AWH983090 BGD983048:BGD983090 BPZ983048:BPZ983090 BZV983048:BZV983090 CJR983048:CJR983090 CTN983048:CTN983090 DDJ983048:DDJ983090 DNF983048:DNF983090 DXB983048:DXB983090 EGX983048:EGX983090 EQT983048:EQT983090 FAP983048:FAP983090 FKL983048:FKL983090 FUH983048:FUH983090 GED983048:GED983090 GNZ983048:GNZ983090 GXV983048:GXV983090 HHR983048:HHR983090 HRN983048:HRN983090 IBJ983048:IBJ983090 ILF983048:ILF983090 IVB983048:IVB983090 JEX983048:JEX983090 JOT983048:JOT983090 JYP983048:JYP983090 KIL983048:KIL983090 KSH983048:KSH983090 LCD983048:LCD983090 LLZ983048:LLZ983090 LVV983048:LVV983090 MFR983048:MFR983090 MPN983048:MPN983090 MZJ983048:MZJ983090 NJF983048:NJF983090 NTB983048:NTB983090 OCX983048:OCX983090 OMT983048:OMT983090 OWP983048:OWP983090 PGL983048:PGL983090 PQH983048:PQH983090 QAD983048:QAD983090 QJZ983048:QJZ983090 QTV983048:QTV983090 RDR983048:RDR983090 RNN983048:RNN983090 RXJ983048:RXJ983090 SHF983048:SHF983090 SRB983048:SRB983090 TAX983048:TAX983090 TKT983048:TKT983090 TUP983048:TUP983090 UEL983048:UEL983090 UOH983048:UOH983090 UYD983048:UYD983090 VHZ983048:VHZ983090 VRV983048:VRV983090 WBR983048:WBR983090 WLN983048:WLN983090 WVJ983048:WVJ983090" xr:uid="{8CEDB7BC-78C4-41C7-9E12-0C9372650A52}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B65543:B65585 IX65543:IX65585 ST65543:ST65585 ACP65543:ACP65585 AML65543:AML65585 AWH65543:AWH65585 BGD65543:BGD65585 BPZ65543:BPZ65585 BZV65543:BZV65585 CJR65543:CJR65585 CTN65543:CTN65585 DDJ65543:DDJ65585 DNF65543:DNF65585 DXB65543:DXB65585 EGX65543:EGX65585 EQT65543:EQT65585 FAP65543:FAP65585 FKL65543:FKL65585 FUH65543:FUH65585 GED65543:GED65585 GNZ65543:GNZ65585 GXV65543:GXV65585 HHR65543:HHR65585 HRN65543:HRN65585 IBJ65543:IBJ65585 ILF65543:ILF65585 IVB65543:IVB65585 JEX65543:JEX65585 JOT65543:JOT65585 JYP65543:JYP65585 KIL65543:KIL65585 KSH65543:KSH65585 LCD65543:LCD65585 LLZ65543:LLZ65585 LVV65543:LVV65585 MFR65543:MFR65585 MPN65543:MPN65585 MZJ65543:MZJ65585 NJF65543:NJF65585 NTB65543:NTB65585 OCX65543:OCX65585 OMT65543:OMT65585 OWP65543:OWP65585 PGL65543:PGL65585 PQH65543:PQH65585 QAD65543:QAD65585 QJZ65543:QJZ65585 QTV65543:QTV65585 RDR65543:RDR65585 RNN65543:RNN65585 RXJ65543:RXJ65585 SHF65543:SHF65585 SRB65543:SRB65585 TAX65543:TAX65585 TKT65543:TKT65585 TUP65543:TUP65585 UEL65543:UEL65585 UOH65543:UOH65585 UYD65543:UYD65585 VHZ65543:VHZ65585 VRV65543:VRV65585 WBR65543:WBR65585 WLN65543:WLN65585 WVJ65543:WVJ65585 B131079:B131121 IX131079:IX131121 ST131079:ST131121 ACP131079:ACP131121 AML131079:AML131121 AWH131079:AWH131121 BGD131079:BGD131121 BPZ131079:BPZ131121 BZV131079:BZV131121 CJR131079:CJR131121 CTN131079:CTN131121 DDJ131079:DDJ131121 DNF131079:DNF131121 DXB131079:DXB131121 EGX131079:EGX131121 EQT131079:EQT131121 FAP131079:FAP131121 FKL131079:FKL131121 FUH131079:FUH131121 GED131079:GED131121 GNZ131079:GNZ131121 GXV131079:GXV131121 HHR131079:HHR131121 HRN131079:HRN131121 IBJ131079:IBJ131121 ILF131079:ILF131121 IVB131079:IVB131121 JEX131079:JEX131121 JOT131079:JOT131121 JYP131079:JYP131121 KIL131079:KIL131121 KSH131079:KSH131121 LCD131079:LCD131121 LLZ131079:LLZ131121 LVV131079:LVV131121 MFR131079:MFR131121 MPN131079:MPN131121 MZJ131079:MZJ131121 NJF131079:NJF131121 NTB131079:NTB131121 OCX131079:OCX131121 OMT131079:OMT131121 OWP131079:OWP131121 PGL131079:PGL131121 PQH131079:PQH131121 QAD131079:QAD131121 QJZ131079:QJZ131121 QTV131079:QTV131121 RDR131079:RDR131121 RNN131079:RNN131121 RXJ131079:RXJ131121 SHF131079:SHF131121 SRB131079:SRB131121 TAX131079:TAX131121 TKT131079:TKT131121 TUP131079:TUP131121 UEL131079:UEL131121 UOH131079:UOH131121 UYD131079:UYD131121 VHZ131079:VHZ131121 VRV131079:VRV131121 WBR131079:WBR131121 WLN131079:WLN131121 WVJ131079:WVJ131121 B196615:B196657 IX196615:IX196657 ST196615:ST196657 ACP196615:ACP196657 AML196615:AML196657 AWH196615:AWH196657 BGD196615:BGD196657 BPZ196615:BPZ196657 BZV196615:BZV196657 CJR196615:CJR196657 CTN196615:CTN196657 DDJ196615:DDJ196657 DNF196615:DNF196657 DXB196615:DXB196657 EGX196615:EGX196657 EQT196615:EQT196657 FAP196615:FAP196657 FKL196615:FKL196657 FUH196615:FUH196657 GED196615:GED196657 GNZ196615:GNZ196657 GXV196615:GXV196657 HHR196615:HHR196657 HRN196615:HRN196657 IBJ196615:IBJ196657 ILF196615:ILF196657 IVB196615:IVB196657 JEX196615:JEX196657 JOT196615:JOT196657 JYP196615:JYP196657 KIL196615:KIL196657 KSH196615:KSH196657 LCD196615:LCD196657 LLZ196615:LLZ196657 LVV196615:LVV196657 MFR196615:MFR196657 MPN196615:MPN196657 MZJ196615:MZJ196657 NJF196615:NJF196657 NTB196615:NTB196657 OCX196615:OCX196657 OMT196615:OMT196657 OWP196615:OWP196657 PGL196615:PGL196657 PQH196615:PQH196657 QAD196615:QAD196657 QJZ196615:QJZ196657 QTV196615:QTV196657 RDR196615:RDR196657 RNN196615:RNN196657 RXJ196615:RXJ196657 SHF196615:SHF196657 SRB196615:SRB196657 TAX196615:TAX196657 TKT196615:TKT196657 TUP196615:TUP196657 UEL196615:UEL196657 UOH196615:UOH196657 UYD196615:UYD196657 VHZ196615:VHZ196657 VRV196615:VRV196657 WBR196615:WBR196657 WLN196615:WLN196657 WVJ196615:WVJ196657 B262151:B262193 IX262151:IX262193 ST262151:ST262193 ACP262151:ACP262193 AML262151:AML262193 AWH262151:AWH262193 BGD262151:BGD262193 BPZ262151:BPZ262193 BZV262151:BZV262193 CJR262151:CJR262193 CTN262151:CTN262193 DDJ262151:DDJ262193 DNF262151:DNF262193 DXB262151:DXB262193 EGX262151:EGX262193 EQT262151:EQT262193 FAP262151:FAP262193 FKL262151:FKL262193 FUH262151:FUH262193 GED262151:GED262193 GNZ262151:GNZ262193 GXV262151:GXV262193 HHR262151:HHR262193 HRN262151:HRN262193 IBJ262151:IBJ262193 ILF262151:ILF262193 IVB262151:IVB262193 JEX262151:JEX262193 JOT262151:JOT262193 JYP262151:JYP262193 KIL262151:KIL262193 KSH262151:KSH262193 LCD262151:LCD262193 LLZ262151:LLZ262193 LVV262151:LVV262193 MFR262151:MFR262193 MPN262151:MPN262193 MZJ262151:MZJ262193 NJF262151:NJF262193 NTB262151:NTB262193 OCX262151:OCX262193 OMT262151:OMT262193 OWP262151:OWP262193 PGL262151:PGL262193 PQH262151:PQH262193 QAD262151:QAD262193 QJZ262151:QJZ262193 QTV262151:QTV262193 RDR262151:RDR262193 RNN262151:RNN262193 RXJ262151:RXJ262193 SHF262151:SHF262193 SRB262151:SRB262193 TAX262151:TAX262193 TKT262151:TKT262193 TUP262151:TUP262193 UEL262151:UEL262193 UOH262151:UOH262193 UYD262151:UYD262193 VHZ262151:VHZ262193 VRV262151:VRV262193 WBR262151:WBR262193 WLN262151:WLN262193 WVJ262151:WVJ262193 B327687:B327729 IX327687:IX327729 ST327687:ST327729 ACP327687:ACP327729 AML327687:AML327729 AWH327687:AWH327729 BGD327687:BGD327729 BPZ327687:BPZ327729 BZV327687:BZV327729 CJR327687:CJR327729 CTN327687:CTN327729 DDJ327687:DDJ327729 DNF327687:DNF327729 DXB327687:DXB327729 EGX327687:EGX327729 EQT327687:EQT327729 FAP327687:FAP327729 FKL327687:FKL327729 FUH327687:FUH327729 GED327687:GED327729 GNZ327687:GNZ327729 GXV327687:GXV327729 HHR327687:HHR327729 HRN327687:HRN327729 IBJ327687:IBJ327729 ILF327687:ILF327729 IVB327687:IVB327729 JEX327687:JEX327729 JOT327687:JOT327729 JYP327687:JYP327729 KIL327687:KIL327729 KSH327687:KSH327729 LCD327687:LCD327729 LLZ327687:LLZ327729 LVV327687:LVV327729 MFR327687:MFR327729 MPN327687:MPN327729 MZJ327687:MZJ327729 NJF327687:NJF327729 NTB327687:NTB327729 OCX327687:OCX327729 OMT327687:OMT327729 OWP327687:OWP327729 PGL327687:PGL327729 PQH327687:PQH327729 QAD327687:QAD327729 QJZ327687:QJZ327729 QTV327687:QTV327729 RDR327687:RDR327729 RNN327687:RNN327729 RXJ327687:RXJ327729 SHF327687:SHF327729 SRB327687:SRB327729 TAX327687:TAX327729 TKT327687:TKT327729 TUP327687:TUP327729 UEL327687:UEL327729 UOH327687:UOH327729 UYD327687:UYD327729 VHZ327687:VHZ327729 VRV327687:VRV327729 WBR327687:WBR327729 WLN327687:WLN327729 WVJ327687:WVJ327729 B393223:B393265 IX393223:IX393265 ST393223:ST393265 ACP393223:ACP393265 AML393223:AML393265 AWH393223:AWH393265 BGD393223:BGD393265 BPZ393223:BPZ393265 BZV393223:BZV393265 CJR393223:CJR393265 CTN393223:CTN393265 DDJ393223:DDJ393265 DNF393223:DNF393265 DXB393223:DXB393265 EGX393223:EGX393265 EQT393223:EQT393265 FAP393223:FAP393265 FKL393223:FKL393265 FUH393223:FUH393265 GED393223:GED393265 GNZ393223:GNZ393265 GXV393223:GXV393265 HHR393223:HHR393265 HRN393223:HRN393265 IBJ393223:IBJ393265 ILF393223:ILF393265 IVB393223:IVB393265 JEX393223:JEX393265 JOT393223:JOT393265 JYP393223:JYP393265 KIL393223:KIL393265 KSH393223:KSH393265 LCD393223:LCD393265 LLZ393223:LLZ393265 LVV393223:LVV393265 MFR393223:MFR393265 MPN393223:MPN393265 MZJ393223:MZJ393265 NJF393223:NJF393265 NTB393223:NTB393265 OCX393223:OCX393265 OMT393223:OMT393265 OWP393223:OWP393265 PGL393223:PGL393265 PQH393223:PQH393265 QAD393223:QAD393265 QJZ393223:QJZ393265 QTV393223:QTV393265 RDR393223:RDR393265 RNN393223:RNN393265 RXJ393223:RXJ393265 SHF393223:SHF393265 SRB393223:SRB393265 TAX393223:TAX393265 TKT393223:TKT393265 TUP393223:TUP393265 UEL393223:UEL393265 UOH393223:UOH393265 UYD393223:UYD393265 VHZ393223:VHZ393265 VRV393223:VRV393265 WBR393223:WBR393265 WLN393223:WLN393265 WVJ393223:WVJ393265 B458759:B458801 IX458759:IX458801 ST458759:ST458801 ACP458759:ACP458801 AML458759:AML458801 AWH458759:AWH458801 BGD458759:BGD458801 BPZ458759:BPZ458801 BZV458759:BZV458801 CJR458759:CJR458801 CTN458759:CTN458801 DDJ458759:DDJ458801 DNF458759:DNF458801 DXB458759:DXB458801 EGX458759:EGX458801 EQT458759:EQT458801 FAP458759:FAP458801 FKL458759:FKL458801 FUH458759:FUH458801 GED458759:GED458801 GNZ458759:GNZ458801 GXV458759:GXV458801 HHR458759:HHR458801 HRN458759:HRN458801 IBJ458759:IBJ458801 ILF458759:ILF458801 IVB458759:IVB458801 JEX458759:JEX458801 JOT458759:JOT458801 JYP458759:JYP458801 KIL458759:KIL458801 KSH458759:KSH458801 LCD458759:LCD458801 LLZ458759:LLZ458801 LVV458759:LVV458801 MFR458759:MFR458801 MPN458759:MPN458801 MZJ458759:MZJ458801 NJF458759:NJF458801 NTB458759:NTB458801 OCX458759:OCX458801 OMT458759:OMT458801 OWP458759:OWP458801 PGL458759:PGL458801 PQH458759:PQH458801 QAD458759:QAD458801 QJZ458759:QJZ458801 QTV458759:QTV458801 RDR458759:RDR458801 RNN458759:RNN458801 RXJ458759:RXJ458801 SHF458759:SHF458801 SRB458759:SRB458801 TAX458759:TAX458801 TKT458759:TKT458801 TUP458759:TUP458801 UEL458759:UEL458801 UOH458759:UOH458801 UYD458759:UYD458801 VHZ458759:VHZ458801 VRV458759:VRV458801 WBR458759:WBR458801 WLN458759:WLN458801 WVJ458759:WVJ458801 B524295:B524337 IX524295:IX524337 ST524295:ST524337 ACP524295:ACP524337 AML524295:AML524337 AWH524295:AWH524337 BGD524295:BGD524337 BPZ524295:BPZ524337 BZV524295:BZV524337 CJR524295:CJR524337 CTN524295:CTN524337 DDJ524295:DDJ524337 DNF524295:DNF524337 DXB524295:DXB524337 EGX524295:EGX524337 EQT524295:EQT524337 FAP524295:FAP524337 FKL524295:FKL524337 FUH524295:FUH524337 GED524295:GED524337 GNZ524295:GNZ524337 GXV524295:GXV524337 HHR524295:HHR524337 HRN524295:HRN524337 IBJ524295:IBJ524337 ILF524295:ILF524337 IVB524295:IVB524337 JEX524295:JEX524337 JOT524295:JOT524337 JYP524295:JYP524337 KIL524295:KIL524337 KSH524295:KSH524337 LCD524295:LCD524337 LLZ524295:LLZ524337 LVV524295:LVV524337 MFR524295:MFR524337 MPN524295:MPN524337 MZJ524295:MZJ524337 NJF524295:NJF524337 NTB524295:NTB524337 OCX524295:OCX524337 OMT524295:OMT524337 OWP524295:OWP524337 PGL524295:PGL524337 PQH524295:PQH524337 QAD524295:QAD524337 QJZ524295:QJZ524337 QTV524295:QTV524337 RDR524295:RDR524337 RNN524295:RNN524337 RXJ524295:RXJ524337 SHF524295:SHF524337 SRB524295:SRB524337 TAX524295:TAX524337 TKT524295:TKT524337 TUP524295:TUP524337 UEL524295:UEL524337 UOH524295:UOH524337 UYD524295:UYD524337 VHZ524295:VHZ524337 VRV524295:VRV524337 WBR524295:WBR524337 WLN524295:WLN524337 WVJ524295:WVJ524337 B589831:B589873 IX589831:IX589873 ST589831:ST589873 ACP589831:ACP589873 AML589831:AML589873 AWH589831:AWH589873 BGD589831:BGD589873 BPZ589831:BPZ589873 BZV589831:BZV589873 CJR589831:CJR589873 CTN589831:CTN589873 DDJ589831:DDJ589873 DNF589831:DNF589873 DXB589831:DXB589873 EGX589831:EGX589873 EQT589831:EQT589873 FAP589831:FAP589873 FKL589831:FKL589873 FUH589831:FUH589873 GED589831:GED589873 GNZ589831:GNZ589873 GXV589831:GXV589873 HHR589831:HHR589873 HRN589831:HRN589873 IBJ589831:IBJ589873 ILF589831:ILF589873 IVB589831:IVB589873 JEX589831:JEX589873 JOT589831:JOT589873 JYP589831:JYP589873 KIL589831:KIL589873 KSH589831:KSH589873 LCD589831:LCD589873 LLZ589831:LLZ589873 LVV589831:LVV589873 MFR589831:MFR589873 MPN589831:MPN589873 MZJ589831:MZJ589873 NJF589831:NJF589873 NTB589831:NTB589873 OCX589831:OCX589873 OMT589831:OMT589873 OWP589831:OWP589873 PGL589831:PGL589873 PQH589831:PQH589873 QAD589831:QAD589873 QJZ589831:QJZ589873 QTV589831:QTV589873 RDR589831:RDR589873 RNN589831:RNN589873 RXJ589831:RXJ589873 SHF589831:SHF589873 SRB589831:SRB589873 TAX589831:TAX589873 TKT589831:TKT589873 TUP589831:TUP589873 UEL589831:UEL589873 UOH589831:UOH589873 UYD589831:UYD589873 VHZ589831:VHZ589873 VRV589831:VRV589873 WBR589831:WBR589873 WLN589831:WLN589873 WVJ589831:WVJ589873 B655367:B655409 IX655367:IX655409 ST655367:ST655409 ACP655367:ACP655409 AML655367:AML655409 AWH655367:AWH655409 BGD655367:BGD655409 BPZ655367:BPZ655409 BZV655367:BZV655409 CJR655367:CJR655409 CTN655367:CTN655409 DDJ655367:DDJ655409 DNF655367:DNF655409 DXB655367:DXB655409 EGX655367:EGX655409 EQT655367:EQT655409 FAP655367:FAP655409 FKL655367:FKL655409 FUH655367:FUH655409 GED655367:GED655409 GNZ655367:GNZ655409 GXV655367:GXV655409 HHR655367:HHR655409 HRN655367:HRN655409 IBJ655367:IBJ655409 ILF655367:ILF655409 IVB655367:IVB655409 JEX655367:JEX655409 JOT655367:JOT655409 JYP655367:JYP655409 KIL655367:KIL655409 KSH655367:KSH655409 LCD655367:LCD655409 LLZ655367:LLZ655409 LVV655367:LVV655409 MFR655367:MFR655409 MPN655367:MPN655409 MZJ655367:MZJ655409 NJF655367:NJF655409 NTB655367:NTB655409 OCX655367:OCX655409 OMT655367:OMT655409 OWP655367:OWP655409 PGL655367:PGL655409 PQH655367:PQH655409 QAD655367:QAD655409 QJZ655367:QJZ655409 QTV655367:QTV655409 RDR655367:RDR655409 RNN655367:RNN655409 RXJ655367:RXJ655409 SHF655367:SHF655409 SRB655367:SRB655409 TAX655367:TAX655409 TKT655367:TKT655409 TUP655367:TUP655409 UEL655367:UEL655409 UOH655367:UOH655409 UYD655367:UYD655409 VHZ655367:VHZ655409 VRV655367:VRV655409 WBR655367:WBR655409 WLN655367:WLN655409 WVJ655367:WVJ655409 B720903:B720945 IX720903:IX720945 ST720903:ST720945 ACP720903:ACP720945 AML720903:AML720945 AWH720903:AWH720945 BGD720903:BGD720945 BPZ720903:BPZ720945 BZV720903:BZV720945 CJR720903:CJR720945 CTN720903:CTN720945 DDJ720903:DDJ720945 DNF720903:DNF720945 DXB720903:DXB720945 EGX720903:EGX720945 EQT720903:EQT720945 FAP720903:FAP720945 FKL720903:FKL720945 FUH720903:FUH720945 GED720903:GED720945 GNZ720903:GNZ720945 GXV720903:GXV720945 HHR720903:HHR720945 HRN720903:HRN720945 IBJ720903:IBJ720945 ILF720903:ILF720945 IVB720903:IVB720945 JEX720903:JEX720945 JOT720903:JOT720945 JYP720903:JYP720945 KIL720903:KIL720945 KSH720903:KSH720945 LCD720903:LCD720945 LLZ720903:LLZ720945 LVV720903:LVV720945 MFR720903:MFR720945 MPN720903:MPN720945 MZJ720903:MZJ720945 NJF720903:NJF720945 NTB720903:NTB720945 OCX720903:OCX720945 OMT720903:OMT720945 OWP720903:OWP720945 PGL720903:PGL720945 PQH720903:PQH720945 QAD720903:QAD720945 QJZ720903:QJZ720945 QTV720903:QTV720945 RDR720903:RDR720945 RNN720903:RNN720945 RXJ720903:RXJ720945 SHF720903:SHF720945 SRB720903:SRB720945 TAX720903:TAX720945 TKT720903:TKT720945 TUP720903:TUP720945 UEL720903:UEL720945 UOH720903:UOH720945 UYD720903:UYD720945 VHZ720903:VHZ720945 VRV720903:VRV720945 WBR720903:WBR720945 WLN720903:WLN720945 WVJ720903:WVJ720945 B786439:B786481 IX786439:IX786481 ST786439:ST786481 ACP786439:ACP786481 AML786439:AML786481 AWH786439:AWH786481 BGD786439:BGD786481 BPZ786439:BPZ786481 BZV786439:BZV786481 CJR786439:CJR786481 CTN786439:CTN786481 DDJ786439:DDJ786481 DNF786439:DNF786481 DXB786439:DXB786481 EGX786439:EGX786481 EQT786439:EQT786481 FAP786439:FAP786481 FKL786439:FKL786481 FUH786439:FUH786481 GED786439:GED786481 GNZ786439:GNZ786481 GXV786439:GXV786481 HHR786439:HHR786481 HRN786439:HRN786481 IBJ786439:IBJ786481 ILF786439:ILF786481 IVB786439:IVB786481 JEX786439:JEX786481 JOT786439:JOT786481 JYP786439:JYP786481 KIL786439:KIL786481 KSH786439:KSH786481 LCD786439:LCD786481 LLZ786439:LLZ786481 LVV786439:LVV786481 MFR786439:MFR786481 MPN786439:MPN786481 MZJ786439:MZJ786481 NJF786439:NJF786481 NTB786439:NTB786481 OCX786439:OCX786481 OMT786439:OMT786481 OWP786439:OWP786481 PGL786439:PGL786481 PQH786439:PQH786481 QAD786439:QAD786481 QJZ786439:QJZ786481 QTV786439:QTV786481 RDR786439:RDR786481 RNN786439:RNN786481 RXJ786439:RXJ786481 SHF786439:SHF786481 SRB786439:SRB786481 TAX786439:TAX786481 TKT786439:TKT786481 TUP786439:TUP786481 UEL786439:UEL786481 UOH786439:UOH786481 UYD786439:UYD786481 VHZ786439:VHZ786481 VRV786439:VRV786481 WBR786439:WBR786481 WLN786439:WLN786481 WVJ786439:WVJ786481 B851975:B852017 IX851975:IX852017 ST851975:ST852017 ACP851975:ACP852017 AML851975:AML852017 AWH851975:AWH852017 BGD851975:BGD852017 BPZ851975:BPZ852017 BZV851975:BZV852017 CJR851975:CJR852017 CTN851975:CTN852017 DDJ851975:DDJ852017 DNF851975:DNF852017 DXB851975:DXB852017 EGX851975:EGX852017 EQT851975:EQT852017 FAP851975:FAP852017 FKL851975:FKL852017 FUH851975:FUH852017 GED851975:GED852017 GNZ851975:GNZ852017 GXV851975:GXV852017 HHR851975:HHR852017 HRN851975:HRN852017 IBJ851975:IBJ852017 ILF851975:ILF852017 IVB851975:IVB852017 JEX851975:JEX852017 JOT851975:JOT852017 JYP851975:JYP852017 KIL851975:KIL852017 KSH851975:KSH852017 LCD851975:LCD852017 LLZ851975:LLZ852017 LVV851975:LVV852017 MFR851975:MFR852017 MPN851975:MPN852017 MZJ851975:MZJ852017 NJF851975:NJF852017 NTB851975:NTB852017 OCX851975:OCX852017 OMT851975:OMT852017 OWP851975:OWP852017 PGL851975:PGL852017 PQH851975:PQH852017 QAD851975:QAD852017 QJZ851975:QJZ852017 QTV851975:QTV852017 RDR851975:RDR852017 RNN851975:RNN852017 RXJ851975:RXJ852017 SHF851975:SHF852017 SRB851975:SRB852017 TAX851975:TAX852017 TKT851975:TKT852017 TUP851975:TUP852017 UEL851975:UEL852017 UOH851975:UOH852017 UYD851975:UYD852017 VHZ851975:VHZ852017 VRV851975:VRV852017 WBR851975:WBR852017 WLN851975:WLN852017 WVJ851975:WVJ852017 B917511:B917553 IX917511:IX917553 ST917511:ST917553 ACP917511:ACP917553 AML917511:AML917553 AWH917511:AWH917553 BGD917511:BGD917553 BPZ917511:BPZ917553 BZV917511:BZV917553 CJR917511:CJR917553 CTN917511:CTN917553 DDJ917511:DDJ917553 DNF917511:DNF917553 DXB917511:DXB917553 EGX917511:EGX917553 EQT917511:EQT917553 FAP917511:FAP917553 FKL917511:FKL917553 FUH917511:FUH917553 GED917511:GED917553 GNZ917511:GNZ917553 GXV917511:GXV917553 HHR917511:HHR917553 HRN917511:HRN917553 IBJ917511:IBJ917553 ILF917511:ILF917553 IVB917511:IVB917553 JEX917511:JEX917553 JOT917511:JOT917553 JYP917511:JYP917553 KIL917511:KIL917553 KSH917511:KSH917553 LCD917511:LCD917553 LLZ917511:LLZ917553 LVV917511:LVV917553 MFR917511:MFR917553 MPN917511:MPN917553 MZJ917511:MZJ917553 NJF917511:NJF917553 NTB917511:NTB917553 OCX917511:OCX917553 OMT917511:OMT917553 OWP917511:OWP917553 PGL917511:PGL917553 PQH917511:PQH917553 QAD917511:QAD917553 QJZ917511:QJZ917553 QTV917511:QTV917553 RDR917511:RDR917553 RNN917511:RNN917553 RXJ917511:RXJ917553 SHF917511:SHF917553 SRB917511:SRB917553 TAX917511:TAX917553 TKT917511:TKT917553 TUP917511:TUP917553 UEL917511:UEL917553 UOH917511:UOH917553 UYD917511:UYD917553 VHZ917511:VHZ917553 VRV917511:VRV917553 WBR917511:WBR917553 WLN917511:WLN917553 WVJ917511:WVJ917553 B983047:B983089 IX983047:IX983089 ST983047:ST983089 ACP983047:ACP983089 AML983047:AML983089 AWH983047:AWH983089 BGD983047:BGD983089 BPZ983047:BPZ983089 BZV983047:BZV983089 CJR983047:CJR983089 CTN983047:CTN983089 DDJ983047:DDJ983089 DNF983047:DNF983089 DXB983047:DXB983089 EGX983047:EGX983089 EQT983047:EQT983089 FAP983047:FAP983089 FKL983047:FKL983089 FUH983047:FUH983089 GED983047:GED983089 GNZ983047:GNZ983089 GXV983047:GXV983089 HHR983047:HHR983089 HRN983047:HRN983089 IBJ983047:IBJ983089 ILF983047:ILF983089 IVB983047:IVB983089 JEX983047:JEX983089 JOT983047:JOT983089 JYP983047:JYP983089 KIL983047:KIL983089 KSH983047:KSH983089 LCD983047:LCD983089 LLZ983047:LLZ983089 LVV983047:LVV983089 MFR983047:MFR983089 MPN983047:MPN983089 MZJ983047:MZJ983089 NJF983047:NJF983089 NTB983047:NTB983089 OCX983047:OCX983089 OMT983047:OMT983089 OWP983047:OWP983089 PGL983047:PGL983089 PQH983047:PQH983089 QAD983047:QAD983089 QJZ983047:QJZ983089 QTV983047:QTV983089 RDR983047:RDR983089 RNN983047:RNN983089 RXJ983047:RXJ983089 SHF983047:SHF983089 SRB983047:SRB983089 TAX983047:TAX983089 TKT983047:TKT983089 TUP983047:TUP983089 UEL983047:UEL983089 UOH983047:UOH983089 UYD983047:UYD983089 VHZ983047:VHZ983089 VRV983047:VRV983089 WBR983047:WBR983089 WLN983047:WLN983089 WVJ983047:WVJ983089 WVJ8:WVJ49 WLN8:WLN49 WBR8:WBR49 VRV8:VRV49 VHZ8:VHZ49 UYD8:UYD49 UOH8:UOH49 UEL8:UEL49 TUP8:TUP49 TKT8:TKT49 TAX8:TAX49 SRB8:SRB49 SHF8:SHF49 RXJ8:RXJ49 RNN8:RNN49 RDR8:RDR49 QTV8:QTV49 QJZ8:QJZ49 QAD8:QAD49 PQH8:PQH49 PGL8:PGL49 OWP8:OWP49 OMT8:OMT49 OCX8:OCX49 NTB8:NTB49 NJF8:NJF49 MZJ8:MZJ49 MPN8:MPN49 MFR8:MFR49 LVV8:LVV49 LLZ8:LLZ49 LCD8:LCD49 KSH8:KSH49 KIL8:KIL49 JYP8:JYP49 JOT8:JOT49 JEX8:JEX49 IVB8:IVB49 ILF8:ILF49 IBJ8:IBJ49 HRN8:HRN49 HHR8:HHR49 GXV8:GXV49 GNZ8:GNZ49 GED8:GED49 FUH8:FUH49 FKL8:FKL49 FAP8:FAP49 EQT8:EQT49 EGX8:EGX49 DXB8:DXB49 DNF8:DNF49 DDJ8:DDJ49 CTN8:CTN49 CJR8:CJR49 BZV8:BZV49 BPZ8:BPZ49 BGD8:BGD49 AWH8:AWH49 AML8:AML49 ACP8:ACP49 ST8:ST49 IX8:IX49 B8:B49">
       <formula1>8</formula1>
       <formula2>8</formula2>
     </dataValidation>
@@ -15689,530 +15579,530 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A948D5B-AEC9-4E1F-B546-98666C12B045}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="21" width="2.7265625" style="8" customWidth="1"/>
-    <col min="22" max="22" width="4.453125" style="8" customWidth="1"/>
-    <col min="23" max="23" width="7.453125" style="8" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="256" width="11.453125" style="1"/>
-    <col min="257" max="257" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="21" width="2.7109375" style="8" customWidth="1"/>
+    <col min="22" max="22" width="4.42578125" style="8" customWidth="1"/>
+    <col min="23" max="23" width="7.42578125" style="8" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="256" width="11.42578125" style="1"/>
+    <col min="257" max="257" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="260" max="277" width="2.7265625" style="1" customWidth="1"/>
-    <col min="278" max="278" width="4.453125" style="1" customWidth="1"/>
+    <col min="260" max="277" width="2.7109375" style="1" customWidth="1"/>
+    <col min="278" max="278" width="4.42578125" style="1" customWidth="1"/>
     <col min="279" max="279" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="280" max="280" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="281" max="512" width="11.453125" style="1"/>
-    <col min="513" max="513" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="281" max="512" width="11.42578125" style="1"/>
+    <col min="513" max="513" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="515" max="515" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="516" max="533" width="2.7265625" style="1" customWidth="1"/>
-    <col min="534" max="534" width="4.453125" style="1" customWidth="1"/>
+    <col min="516" max="533" width="2.7109375" style="1" customWidth="1"/>
+    <col min="534" max="534" width="4.42578125" style="1" customWidth="1"/>
     <col min="535" max="535" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="536" max="536" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="537" max="768" width="11.453125" style="1"/>
-    <col min="769" max="769" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="536" max="536" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="537" max="768" width="11.42578125" style="1"/>
+    <col min="769" max="769" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="771" max="771" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="772" max="789" width="2.7265625" style="1" customWidth="1"/>
-    <col min="790" max="790" width="4.453125" style="1" customWidth="1"/>
+    <col min="772" max="789" width="2.7109375" style="1" customWidth="1"/>
+    <col min="790" max="790" width="4.42578125" style="1" customWidth="1"/>
     <col min="791" max="791" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="792" max="792" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="793" max="1024" width="11.453125" style="1"/>
-    <col min="1025" max="1025" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="792" max="792" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="793" max="1024" width="11.42578125" style="1"/>
+    <col min="1025" max="1025" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1027" max="1027" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1045" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1046" max="1046" width="4.453125" style="1" customWidth="1"/>
+    <col min="1028" max="1045" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1046" max="1046" width="4.42578125" style="1" customWidth="1"/>
     <col min="1047" max="1047" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1048" max="1048" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1049" max="1280" width="11.453125" style="1"/>
-    <col min="1281" max="1281" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1048" max="1048" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1049" max="1280" width="11.42578125" style="1"/>
+    <col min="1281" max="1281" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1283" max="1283" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1301" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1302" max="1302" width="4.453125" style="1" customWidth="1"/>
+    <col min="1284" max="1301" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1302" max="1302" width="4.42578125" style="1" customWidth="1"/>
     <col min="1303" max="1303" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1304" max="1304" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1305" max="1536" width="11.453125" style="1"/>
-    <col min="1537" max="1537" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1304" max="1304" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1305" max="1536" width="11.42578125" style="1"/>
+    <col min="1537" max="1537" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1539" max="1539" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1557" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1558" max="1558" width="4.453125" style="1" customWidth="1"/>
+    <col min="1540" max="1557" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1558" max="1558" width="4.42578125" style="1" customWidth="1"/>
     <col min="1559" max="1559" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1560" max="1560" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1561" max="1792" width="11.453125" style="1"/>
-    <col min="1793" max="1793" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1560" max="1560" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1561" max="1792" width="11.42578125" style="1"/>
+    <col min="1793" max="1793" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="1795" max="1795" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1813" width="2.7265625" style="1" customWidth="1"/>
-    <col min="1814" max="1814" width="4.453125" style="1" customWidth="1"/>
+    <col min="1796" max="1813" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1814" max="1814" width="4.42578125" style="1" customWidth="1"/>
     <col min="1815" max="1815" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1816" max="1816" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1817" max="2048" width="11.453125" style="1"/>
-    <col min="2049" max="2049" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1816" max="1816" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1817" max="2048" width="11.42578125" style="1"/>
+    <col min="2049" max="2049" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2051" max="2051" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2069" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2070" max="2070" width="4.453125" style="1" customWidth="1"/>
+    <col min="2052" max="2069" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2070" max="2070" width="4.42578125" style="1" customWidth="1"/>
     <col min="2071" max="2071" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2072" max="2072" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2073" max="2304" width="11.453125" style="1"/>
-    <col min="2305" max="2305" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2072" max="2072" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2073" max="2304" width="11.42578125" style="1"/>
+    <col min="2305" max="2305" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2307" max="2307" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2325" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2326" max="2326" width="4.453125" style="1" customWidth="1"/>
+    <col min="2308" max="2325" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2326" max="2326" width="4.42578125" style="1" customWidth="1"/>
     <col min="2327" max="2327" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2328" max="2328" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2329" max="2560" width="11.453125" style="1"/>
-    <col min="2561" max="2561" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2328" max="2328" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2329" max="2560" width="11.42578125" style="1"/>
+    <col min="2561" max="2561" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2563" max="2563" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2581" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2582" max="2582" width="4.453125" style="1" customWidth="1"/>
+    <col min="2564" max="2581" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2582" max="2582" width="4.42578125" style="1" customWidth="1"/>
     <col min="2583" max="2583" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2584" max="2584" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2585" max="2816" width="11.453125" style="1"/>
-    <col min="2817" max="2817" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2584" max="2584" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2585" max="2816" width="11.42578125" style="1"/>
+    <col min="2817" max="2817" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2819" max="2819" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2837" width="2.7265625" style="1" customWidth="1"/>
-    <col min="2838" max="2838" width="4.453125" style="1" customWidth="1"/>
+    <col min="2820" max="2837" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2838" max="2838" width="4.42578125" style="1" customWidth="1"/>
     <col min="2839" max="2839" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2840" max="2840" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2841" max="3072" width="11.453125" style="1"/>
-    <col min="3073" max="3073" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2840" max="2840" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2841" max="3072" width="11.42578125" style="1"/>
+    <col min="3073" max="3073" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3075" max="3075" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3093" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3094" max="3094" width="4.453125" style="1" customWidth="1"/>
+    <col min="3076" max="3093" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3094" max="3094" width="4.42578125" style="1" customWidth="1"/>
     <col min="3095" max="3095" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3096" max="3096" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3097" max="3328" width="11.453125" style="1"/>
-    <col min="3329" max="3329" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3096" max="3096" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3097" max="3328" width="11.42578125" style="1"/>
+    <col min="3329" max="3329" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3331" max="3331" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3349" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3350" max="3350" width="4.453125" style="1" customWidth="1"/>
+    <col min="3332" max="3349" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3350" max="3350" width="4.42578125" style="1" customWidth="1"/>
     <col min="3351" max="3351" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3352" max="3352" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3353" max="3584" width="11.453125" style="1"/>
-    <col min="3585" max="3585" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3352" max="3352" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3353" max="3584" width="11.42578125" style="1"/>
+    <col min="3585" max="3585" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3587" max="3587" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3605" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3606" max="3606" width="4.453125" style="1" customWidth="1"/>
+    <col min="3588" max="3605" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3606" max="3606" width="4.42578125" style="1" customWidth="1"/>
     <col min="3607" max="3607" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3608" max="3608" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3609" max="3840" width="11.453125" style="1"/>
-    <col min="3841" max="3841" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3608" max="3608" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3609" max="3840" width="11.42578125" style="1"/>
+    <col min="3841" max="3841" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3843" max="3843" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3861" width="2.7265625" style="1" customWidth="1"/>
-    <col min="3862" max="3862" width="4.453125" style="1" customWidth="1"/>
+    <col min="3844" max="3861" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3862" max="3862" width="4.42578125" style="1" customWidth="1"/>
     <col min="3863" max="3863" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3864" max="3864" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3865" max="4096" width="11.453125" style="1"/>
-    <col min="4097" max="4097" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3864" max="3864" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3865" max="4096" width="11.42578125" style="1"/>
+    <col min="4097" max="4097" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4099" max="4099" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4117" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4118" max="4118" width="4.453125" style="1" customWidth="1"/>
+    <col min="4100" max="4117" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4118" max="4118" width="4.42578125" style="1" customWidth="1"/>
     <col min="4119" max="4119" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4120" max="4120" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4121" max="4352" width="11.453125" style="1"/>
-    <col min="4353" max="4353" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4120" max="4120" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4121" max="4352" width="11.42578125" style="1"/>
+    <col min="4353" max="4353" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4355" max="4355" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4373" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4374" max="4374" width="4.453125" style="1" customWidth="1"/>
+    <col min="4356" max="4373" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4374" max="4374" width="4.42578125" style="1" customWidth="1"/>
     <col min="4375" max="4375" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4376" max="4376" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4377" max="4608" width="11.453125" style="1"/>
-    <col min="4609" max="4609" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4376" max="4376" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4377" max="4608" width="11.42578125" style="1"/>
+    <col min="4609" max="4609" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4611" max="4611" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4629" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4630" max="4630" width="4.453125" style="1" customWidth="1"/>
+    <col min="4612" max="4629" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4630" max="4630" width="4.42578125" style="1" customWidth="1"/>
     <col min="4631" max="4631" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4632" max="4632" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4633" max="4864" width="11.453125" style="1"/>
-    <col min="4865" max="4865" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4632" max="4632" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4633" max="4864" width="11.42578125" style="1"/>
+    <col min="4865" max="4865" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4867" max="4867" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4885" width="2.7265625" style="1" customWidth="1"/>
-    <col min="4886" max="4886" width="4.453125" style="1" customWidth="1"/>
+    <col min="4868" max="4885" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4886" max="4886" width="4.42578125" style="1" customWidth="1"/>
     <col min="4887" max="4887" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4888" max="4888" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4889" max="5120" width="11.453125" style="1"/>
-    <col min="5121" max="5121" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4888" max="4888" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4889" max="5120" width="11.42578125" style="1"/>
+    <col min="5121" max="5121" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5123" max="5123" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5141" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5142" max="5142" width="4.453125" style="1" customWidth="1"/>
+    <col min="5124" max="5141" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5142" max="5142" width="4.42578125" style="1" customWidth="1"/>
     <col min="5143" max="5143" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5144" max="5144" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5145" max="5376" width="11.453125" style="1"/>
-    <col min="5377" max="5377" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5144" max="5144" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5145" max="5376" width="11.42578125" style="1"/>
+    <col min="5377" max="5377" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5379" max="5379" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5397" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5398" max="5398" width="4.453125" style="1" customWidth="1"/>
+    <col min="5380" max="5397" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5398" max="5398" width="4.42578125" style="1" customWidth="1"/>
     <col min="5399" max="5399" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5400" max="5400" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5401" max="5632" width="11.453125" style="1"/>
-    <col min="5633" max="5633" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5400" max="5400" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5401" max="5632" width="11.42578125" style="1"/>
+    <col min="5633" max="5633" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5635" max="5635" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5653" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5654" max="5654" width="4.453125" style="1" customWidth="1"/>
+    <col min="5636" max="5653" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5654" max="5654" width="4.42578125" style="1" customWidth="1"/>
     <col min="5655" max="5655" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5656" max="5656" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5657" max="5888" width="11.453125" style="1"/>
-    <col min="5889" max="5889" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5656" max="5656" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5657" max="5888" width="11.42578125" style="1"/>
+    <col min="5889" max="5889" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5891" max="5891" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5909" width="2.7265625" style="1" customWidth="1"/>
-    <col min="5910" max="5910" width="4.453125" style="1" customWidth="1"/>
+    <col min="5892" max="5909" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5910" max="5910" width="4.42578125" style="1" customWidth="1"/>
     <col min="5911" max="5911" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5912" max="5912" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5913" max="6144" width="11.453125" style="1"/>
-    <col min="6145" max="6145" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5912" max="5912" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5913" max="6144" width="11.42578125" style="1"/>
+    <col min="6145" max="6145" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6147" max="6147" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6165" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6166" max="6166" width="4.453125" style="1" customWidth="1"/>
+    <col min="6148" max="6165" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6166" max="6166" width="4.42578125" style="1" customWidth="1"/>
     <col min="6167" max="6167" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6168" max="6168" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6169" max="6400" width="11.453125" style="1"/>
-    <col min="6401" max="6401" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6168" max="6168" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6169" max="6400" width="11.42578125" style="1"/>
+    <col min="6401" max="6401" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6403" max="6403" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6421" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6422" max="6422" width="4.453125" style="1" customWidth="1"/>
+    <col min="6404" max="6421" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6422" max="6422" width="4.42578125" style="1" customWidth="1"/>
     <col min="6423" max="6423" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6424" max="6424" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6425" max="6656" width="11.453125" style="1"/>
-    <col min="6657" max="6657" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6424" max="6424" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6425" max="6656" width="11.42578125" style="1"/>
+    <col min="6657" max="6657" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6659" max="6659" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6677" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6678" max="6678" width="4.453125" style="1" customWidth="1"/>
+    <col min="6660" max="6677" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6678" max="6678" width="4.42578125" style="1" customWidth="1"/>
     <col min="6679" max="6679" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6680" max="6680" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6681" max="6912" width="11.453125" style="1"/>
-    <col min="6913" max="6913" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6680" max="6680" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6681" max="6912" width="11.42578125" style="1"/>
+    <col min="6913" max="6913" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6915" max="6915" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6933" width="2.7265625" style="1" customWidth="1"/>
-    <col min="6934" max="6934" width="4.453125" style="1" customWidth="1"/>
+    <col min="6916" max="6933" width="2.7109375" style="1" customWidth="1"/>
+    <col min="6934" max="6934" width="4.42578125" style="1" customWidth="1"/>
     <col min="6935" max="6935" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6936" max="6936" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6937" max="7168" width="11.453125" style="1"/>
-    <col min="7169" max="7169" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6936" max="6936" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6937" max="7168" width="11.42578125" style="1"/>
+    <col min="7169" max="7169" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7171" max="7171" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7189" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7190" max="7190" width="4.453125" style="1" customWidth="1"/>
+    <col min="7172" max="7189" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7190" max="7190" width="4.42578125" style="1" customWidth="1"/>
     <col min="7191" max="7191" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7192" max="7192" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7193" max="7424" width="11.453125" style="1"/>
-    <col min="7425" max="7425" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7192" max="7192" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7193" max="7424" width="11.42578125" style="1"/>
+    <col min="7425" max="7425" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7427" max="7427" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7445" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7446" max="7446" width="4.453125" style="1" customWidth="1"/>
+    <col min="7428" max="7445" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7446" max="7446" width="4.42578125" style="1" customWidth="1"/>
     <col min="7447" max="7447" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7448" max="7448" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7449" max="7680" width="11.453125" style="1"/>
-    <col min="7681" max="7681" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7448" max="7448" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7449" max="7680" width="11.42578125" style="1"/>
+    <col min="7681" max="7681" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7683" max="7683" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7701" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7702" max="7702" width="4.453125" style="1" customWidth="1"/>
+    <col min="7684" max="7701" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7702" max="7702" width="4.42578125" style="1" customWidth="1"/>
     <col min="7703" max="7703" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7704" max="7704" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7705" max="7936" width="11.453125" style="1"/>
-    <col min="7937" max="7937" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7704" max="7704" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7705" max="7936" width="11.42578125" style="1"/>
+    <col min="7937" max="7937" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7939" max="7939" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7957" width="2.7265625" style="1" customWidth="1"/>
-    <col min="7958" max="7958" width="4.453125" style="1" customWidth="1"/>
+    <col min="7940" max="7957" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7958" max="7958" width="4.42578125" style="1" customWidth="1"/>
     <col min="7959" max="7959" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7960" max="7960" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7961" max="8192" width="11.453125" style="1"/>
-    <col min="8193" max="8193" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7960" max="7960" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7961" max="8192" width="11.42578125" style="1"/>
+    <col min="8193" max="8193" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8195" max="8195" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8213" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8214" max="8214" width="4.453125" style="1" customWidth="1"/>
+    <col min="8196" max="8213" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8214" max="8214" width="4.42578125" style="1" customWidth="1"/>
     <col min="8215" max="8215" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8216" max="8216" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8217" max="8448" width="11.453125" style="1"/>
-    <col min="8449" max="8449" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8216" max="8216" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8217" max="8448" width="11.42578125" style="1"/>
+    <col min="8449" max="8449" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8451" max="8451" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8469" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8470" max="8470" width="4.453125" style="1" customWidth="1"/>
+    <col min="8452" max="8469" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8470" max="8470" width="4.42578125" style="1" customWidth="1"/>
     <col min="8471" max="8471" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8472" max="8472" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8473" max="8704" width="11.453125" style="1"/>
-    <col min="8705" max="8705" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8472" max="8472" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8473" max="8704" width="11.42578125" style="1"/>
+    <col min="8705" max="8705" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8707" max="8707" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8725" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8726" max="8726" width="4.453125" style="1" customWidth="1"/>
+    <col min="8708" max="8725" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8726" max="8726" width="4.42578125" style="1" customWidth="1"/>
     <col min="8727" max="8727" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8728" max="8728" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8729" max="8960" width="11.453125" style="1"/>
-    <col min="8961" max="8961" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8728" max="8728" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8729" max="8960" width="11.42578125" style="1"/>
+    <col min="8961" max="8961" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8963" max="8963" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8981" width="2.7265625" style="1" customWidth="1"/>
-    <col min="8982" max="8982" width="4.453125" style="1" customWidth="1"/>
+    <col min="8964" max="8981" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8982" max="8982" width="4.42578125" style="1" customWidth="1"/>
     <col min="8983" max="8983" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8984" max="8984" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8985" max="9216" width="11.453125" style="1"/>
-    <col min="9217" max="9217" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8984" max="8984" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8985" max="9216" width="11.42578125" style="1"/>
+    <col min="9217" max="9217" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9219" max="9219" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9237" width="2.7265625" style="1" customWidth="1"/>
-    <col min="9238" max="9238" width="4.453125" style="1" customWidth="1"/>
+    <col min="9220" max="9237" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9238" max="9238" width="4.42578125" style="1" customWidth="1"/>
     <col min="9239" max="9239" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9240" max="9240" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9241" max="9472" width="11.453125" style="1"/>
-    <col min="9473" max="9473" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9240" max="9240" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9241" max="9472" width="11.42578125" style="1"/>
+    <col min="9473" max="9473" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9475" max="9475" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9493" width="2.7265625" style="1" customWidth="1"/>
-    <col min="9494" max="9494" width="4.453125" style="1" customWidth="1"/>
+    <col min="9476" max="9493" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9494" max="9494" width="4.42578125" style="1" customWidth="1"/>
     <col min="9495" max="9495" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9496" max="9496" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9497" max="9728" width="11.453125" style="1"/>
-    <col min="9729" max="9729" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9496" max="9496" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9497" max="9728" width="11.42578125" style="1"/>
+    <col min="9729" max="9729" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9731" max="9731" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9749" width="2.7265625" style="1" customWidth="1"/>
-    <col min="9750" max="9750" width="4.453125" style="1" customWidth="1"/>
+    <col min="9732" max="9749" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9750" max="9750" width="4.42578125" style="1" customWidth="1"/>
     <col min="9751" max="9751" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9752" max="9752" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9753" max="9984" width="11.453125" style="1"/>
-    <col min="9985" max="9985" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9752" max="9752" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9753" max="9984" width="11.42578125" style="1"/>
+    <col min="9985" max="9985" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9987" max="9987" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9988" max="10005" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10006" max="10006" width="4.453125" style="1" customWidth="1"/>
+    <col min="9988" max="10005" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10006" max="10006" width="4.42578125" style="1" customWidth="1"/>
     <col min="10007" max="10007" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10008" max="10008" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10009" max="10240" width="11.453125" style="1"/>
-    <col min="10241" max="10241" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10008" max="10008" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10009" max="10240" width="11.42578125" style="1"/>
+    <col min="10241" max="10241" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10243" max="10243" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10261" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10262" max="10262" width="4.453125" style="1" customWidth="1"/>
+    <col min="10244" max="10261" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10262" max="10262" width="4.42578125" style="1" customWidth="1"/>
     <col min="10263" max="10263" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10264" max="10264" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10265" max="10496" width="11.453125" style="1"/>
-    <col min="10497" max="10497" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10264" max="10264" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10265" max="10496" width="11.42578125" style="1"/>
+    <col min="10497" max="10497" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10499" max="10499" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10517" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10518" max="10518" width="4.453125" style="1" customWidth="1"/>
+    <col min="10500" max="10517" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10518" max="10518" width="4.42578125" style="1" customWidth="1"/>
     <col min="10519" max="10519" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10520" max="10520" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10521" max="10752" width="11.453125" style="1"/>
-    <col min="10753" max="10753" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10520" max="10520" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10521" max="10752" width="11.42578125" style="1"/>
+    <col min="10753" max="10753" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10755" max="10755" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10773" width="2.7265625" style="1" customWidth="1"/>
-    <col min="10774" max="10774" width="4.453125" style="1" customWidth="1"/>
+    <col min="10756" max="10773" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10774" max="10774" width="4.42578125" style="1" customWidth="1"/>
     <col min="10775" max="10775" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10776" max="10776" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10777" max="11008" width="11.453125" style="1"/>
-    <col min="11009" max="11009" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10776" max="10776" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10777" max="11008" width="11.42578125" style="1"/>
+    <col min="11009" max="11009" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11011" max="11011" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11029" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11030" max="11030" width="4.453125" style="1" customWidth="1"/>
+    <col min="11012" max="11029" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11030" max="11030" width="4.42578125" style="1" customWidth="1"/>
     <col min="11031" max="11031" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11032" max="11032" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11033" max="11264" width="11.453125" style="1"/>
-    <col min="11265" max="11265" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11032" max="11032" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11033" max="11264" width="11.42578125" style="1"/>
+    <col min="11265" max="11265" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11267" max="11267" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11285" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11286" max="11286" width="4.453125" style="1" customWidth="1"/>
+    <col min="11268" max="11285" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11286" max="11286" width="4.42578125" style="1" customWidth="1"/>
     <col min="11287" max="11287" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11288" max="11288" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11289" max="11520" width="11.453125" style="1"/>
-    <col min="11521" max="11521" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11288" max="11288" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11289" max="11520" width="11.42578125" style="1"/>
+    <col min="11521" max="11521" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11523" max="11523" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11541" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11542" max="11542" width="4.453125" style="1" customWidth="1"/>
+    <col min="11524" max="11541" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11542" max="11542" width="4.42578125" style="1" customWidth="1"/>
     <col min="11543" max="11543" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11544" max="11544" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11545" max="11776" width="11.453125" style="1"/>
-    <col min="11777" max="11777" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11544" max="11544" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11545" max="11776" width="11.42578125" style="1"/>
+    <col min="11777" max="11777" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11779" max="11779" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11797" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11798" max="11798" width="4.453125" style="1" customWidth="1"/>
+    <col min="11780" max="11797" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11798" max="11798" width="4.42578125" style="1" customWidth="1"/>
     <col min="11799" max="11799" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11800" max="11800" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11801" max="12032" width="11.453125" style="1"/>
-    <col min="12033" max="12033" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11800" max="11800" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11801" max="12032" width="11.42578125" style="1"/>
+    <col min="12033" max="12033" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12035" max="12035" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12053" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12054" max="12054" width="4.453125" style="1" customWidth="1"/>
+    <col min="12036" max="12053" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12054" max="12054" width="4.42578125" style="1" customWidth="1"/>
     <col min="12055" max="12055" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12056" max="12056" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12057" max="12288" width="11.453125" style="1"/>
-    <col min="12289" max="12289" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12056" max="12056" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12057" max="12288" width="11.42578125" style="1"/>
+    <col min="12289" max="12289" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12291" max="12291" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12309" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12310" max="12310" width="4.453125" style="1" customWidth="1"/>
+    <col min="12292" max="12309" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12310" max="12310" width="4.42578125" style="1" customWidth="1"/>
     <col min="12311" max="12311" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12312" max="12312" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12313" max="12544" width="11.453125" style="1"/>
-    <col min="12545" max="12545" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12312" max="12312" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12313" max="12544" width="11.42578125" style="1"/>
+    <col min="12545" max="12545" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12547" max="12547" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12565" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12566" max="12566" width="4.453125" style="1" customWidth="1"/>
+    <col min="12548" max="12565" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12566" max="12566" width="4.42578125" style="1" customWidth="1"/>
     <col min="12567" max="12567" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12568" max="12568" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12569" max="12800" width="11.453125" style="1"/>
-    <col min="12801" max="12801" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12568" max="12568" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12569" max="12800" width="11.42578125" style="1"/>
+    <col min="12801" max="12801" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12803" max="12803" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12821" width="2.7265625" style="1" customWidth="1"/>
-    <col min="12822" max="12822" width="4.453125" style="1" customWidth="1"/>
+    <col min="12804" max="12821" width="2.7109375" style="1" customWidth="1"/>
+    <col min="12822" max="12822" width="4.42578125" style="1" customWidth="1"/>
     <col min="12823" max="12823" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12824" max="12824" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12825" max="13056" width="11.453125" style="1"/>
-    <col min="13057" max="13057" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12824" max="12824" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12825" max="13056" width="11.42578125" style="1"/>
+    <col min="13057" max="13057" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13059" max="13059" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13077" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13078" max="13078" width="4.453125" style="1" customWidth="1"/>
+    <col min="13060" max="13077" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13078" max="13078" width="4.42578125" style="1" customWidth="1"/>
     <col min="13079" max="13079" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13080" max="13080" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13081" max="13312" width="11.453125" style="1"/>
-    <col min="13313" max="13313" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13080" max="13080" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13081" max="13312" width="11.42578125" style="1"/>
+    <col min="13313" max="13313" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13315" max="13315" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13333" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13334" max="13334" width="4.453125" style="1" customWidth="1"/>
+    <col min="13316" max="13333" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13334" max="13334" width="4.42578125" style="1" customWidth="1"/>
     <col min="13335" max="13335" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13336" max="13336" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13337" max="13568" width="11.453125" style="1"/>
-    <col min="13569" max="13569" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13336" max="13336" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13337" max="13568" width="11.42578125" style="1"/>
+    <col min="13569" max="13569" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13571" max="13571" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13589" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13590" max="13590" width="4.453125" style="1" customWidth="1"/>
+    <col min="13572" max="13589" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13590" max="13590" width="4.42578125" style="1" customWidth="1"/>
     <col min="13591" max="13591" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13592" max="13592" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13593" max="13824" width="11.453125" style="1"/>
-    <col min="13825" max="13825" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13592" max="13592" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13593" max="13824" width="11.42578125" style="1"/>
+    <col min="13825" max="13825" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13827" max="13827" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13845" width="2.7265625" style="1" customWidth="1"/>
-    <col min="13846" max="13846" width="4.453125" style="1" customWidth="1"/>
+    <col min="13828" max="13845" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13846" max="13846" width="4.42578125" style="1" customWidth="1"/>
     <col min="13847" max="13847" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13848" max="13848" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13849" max="14080" width="11.453125" style="1"/>
-    <col min="14081" max="14081" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13848" max="13848" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13849" max="14080" width="11.42578125" style="1"/>
+    <col min="14081" max="14081" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14083" max="14083" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14101" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14102" max="14102" width="4.453125" style="1" customWidth="1"/>
+    <col min="14084" max="14101" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14102" max="14102" width="4.42578125" style="1" customWidth="1"/>
     <col min="14103" max="14103" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14104" max="14104" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14105" max="14336" width="11.453125" style="1"/>
-    <col min="14337" max="14337" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14104" max="14104" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14105" max="14336" width="11.42578125" style="1"/>
+    <col min="14337" max="14337" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14339" max="14339" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14357" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14358" max="14358" width="4.453125" style="1" customWidth="1"/>
+    <col min="14340" max="14357" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14358" max="14358" width="4.42578125" style="1" customWidth="1"/>
     <col min="14359" max="14359" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14360" max="14360" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14361" max="14592" width="11.453125" style="1"/>
-    <col min="14593" max="14593" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14360" max="14360" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14361" max="14592" width="11.42578125" style="1"/>
+    <col min="14593" max="14593" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14595" max="14595" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14613" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14614" max="14614" width="4.453125" style="1" customWidth="1"/>
+    <col min="14596" max="14613" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14614" max="14614" width="4.42578125" style="1" customWidth="1"/>
     <col min="14615" max="14615" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14616" max="14616" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14617" max="14848" width="11.453125" style="1"/>
-    <col min="14849" max="14849" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14616" max="14616" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14617" max="14848" width="11.42578125" style="1"/>
+    <col min="14849" max="14849" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14851" max="14851" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14869" width="2.7265625" style="1" customWidth="1"/>
-    <col min="14870" max="14870" width="4.453125" style="1" customWidth="1"/>
+    <col min="14852" max="14869" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14870" max="14870" width="4.42578125" style="1" customWidth="1"/>
     <col min="14871" max="14871" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14872" max="14872" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14873" max="15104" width="11.453125" style="1"/>
-    <col min="15105" max="15105" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14872" max="14872" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14873" max="15104" width="11.42578125" style="1"/>
+    <col min="15105" max="15105" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15107" max="15107" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15125" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15126" max="15126" width="4.453125" style="1" customWidth="1"/>
+    <col min="15108" max="15125" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15126" max="15126" width="4.42578125" style="1" customWidth="1"/>
     <col min="15127" max="15127" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15128" max="15128" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15129" max="15360" width="11.453125" style="1"/>
-    <col min="15361" max="15361" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15128" max="15128" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15129" max="15360" width="11.42578125" style="1"/>
+    <col min="15361" max="15361" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15363" max="15363" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15381" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15382" max="15382" width="4.453125" style="1" customWidth="1"/>
+    <col min="15364" max="15381" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15382" max="15382" width="4.42578125" style="1" customWidth="1"/>
     <col min="15383" max="15383" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15384" max="15384" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15385" max="15616" width="11.453125" style="1"/>
-    <col min="15617" max="15617" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15384" max="15384" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15385" max="15616" width="11.42578125" style="1"/>
+    <col min="15617" max="15617" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15619" max="15619" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15637" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15638" max="15638" width="4.453125" style="1" customWidth="1"/>
+    <col min="15620" max="15637" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15638" max="15638" width="4.42578125" style="1" customWidth="1"/>
     <col min="15639" max="15639" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15640" max="15640" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15641" max="15872" width="11.453125" style="1"/>
-    <col min="15873" max="15873" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15640" max="15640" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15641" max="15872" width="11.42578125" style="1"/>
+    <col min="15873" max="15873" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15875" max="15875" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15893" width="2.7265625" style="1" customWidth="1"/>
-    <col min="15894" max="15894" width="4.453125" style="1" customWidth="1"/>
+    <col min="15876" max="15893" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15894" max="15894" width="4.42578125" style="1" customWidth="1"/>
     <col min="15895" max="15895" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15896" max="15896" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15897" max="16128" width="11.453125" style="1"/>
-    <col min="16129" max="16129" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15896" max="15896" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15897" max="16128" width="11.42578125" style="1"/>
+    <col min="16129" max="16129" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16131" max="16131" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16149" width="2.7265625" style="1" customWidth="1"/>
-    <col min="16150" max="16150" width="4.453125" style="1" customWidth="1"/>
+    <col min="16132" max="16149" width="2.7109375" style="1" customWidth="1"/>
+    <col min="16150" max="16150" width="4.42578125" style="1" customWidth="1"/>
     <col min="16151" max="16151" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="16152" max="16152" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16153" max="16384" width="11.453125" style="1"/>
+    <col min="16152" max="16152" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16153" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16246,7 +16136,7 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
     </row>
-    <row r="2" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -16276,7 +16166,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
     </row>
-    <row r="3" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -16306,7 +16196,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
     </row>
-    <row r="4" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -16336,7 +16226,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -16344,7 +16234,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -16427,7 +16317,7 @@
       </c>
       <c r="AB7" s="12"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>140</v>
       </c>
@@ -16577,7 +16467,7 @@
       </c>
       <c r="Y9" s="8"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>144</v>
       </c>
@@ -16652,7 +16542,7 @@
       </c>
       <c r="Y10" s="8"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>
@@ -16727,7 +16617,7 @@
       </c>
       <c r="Y11" s="8"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>148</v>
       </c>
@@ -16802,7 +16692,7 @@
       </c>
       <c r="Y12" s="8"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>150</v>
       </c>
@@ -16877,7 +16767,7 @@
       </c>
       <c r="Y13" s="8"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>152</v>
       </c>
@@ -16952,7 +16842,7 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>154</v>
       </c>
@@ -17027,7 +16917,7 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>156</v>
       </c>
@@ -17102,7 +16992,7 @@
       </c>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>158</v>
       </c>
@@ -17177,7 +17067,7 @@
       </c>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>160</v>
       </c>
@@ -17252,7 +17142,7 @@
       </c>
       <c r="Y18" s="8"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>162</v>
       </c>
@@ -17327,7 +17217,7 @@
       </c>
       <c r="Y19" s="8"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>164</v>
       </c>
@@ -17402,7 +17292,7 @@
       </c>
       <c r="Y20" s="8"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>166</v>
       </c>
@@ -17552,7 +17442,7 @@
       </c>
       <c r="Y22" s="8"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>170</v>
       </c>
@@ -17627,7 +17517,7 @@
       </c>
       <c r="Y23" s="8"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -17702,7 +17592,7 @@
       </c>
       <c r="Y24" s="8"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>174</v>
       </c>
@@ -17777,7 +17667,7 @@
       </c>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>176</v>
       </c>
@@ -22142,7 +22032,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B50 IX8:IX50 ST8:ST50 ACP8:ACP50 AML8:AML50 AWH8:AWH50 BGD8:BGD50 BPZ8:BPZ50 BZV8:BZV50 CJR8:CJR50 CTN8:CTN50 DDJ8:DDJ50 DNF8:DNF50 DXB8:DXB50 EGX8:EGX50 EQT8:EQT50 FAP8:FAP50 FKL8:FKL50 FUH8:FUH50 GED8:GED50 GNZ8:GNZ50 GXV8:GXV50 HHR8:HHR50 HRN8:HRN50 IBJ8:IBJ50 ILF8:ILF50 IVB8:IVB50 JEX8:JEX50 JOT8:JOT50 JYP8:JYP50 KIL8:KIL50 KSH8:KSH50 LCD8:LCD50 LLZ8:LLZ50 LVV8:LVV50 MFR8:MFR50 MPN8:MPN50 MZJ8:MZJ50 NJF8:NJF50 NTB8:NTB50 OCX8:OCX50 OMT8:OMT50 OWP8:OWP50 PGL8:PGL50 PQH8:PQH50 QAD8:QAD50 QJZ8:QJZ50 QTV8:QTV50 RDR8:RDR50 RNN8:RNN50 RXJ8:RXJ50 SHF8:SHF50 SRB8:SRB50 TAX8:TAX50 TKT8:TKT50 TUP8:TUP50 UEL8:UEL50 UOH8:UOH50 UYD8:UYD50 VHZ8:VHZ50 VRV8:VRV50 WBR8:WBR50 WLN8:WLN50 WVJ8:WVJ50 B65544:B65586 IX65544:IX65586 ST65544:ST65586 ACP65544:ACP65586 AML65544:AML65586 AWH65544:AWH65586 BGD65544:BGD65586 BPZ65544:BPZ65586 BZV65544:BZV65586 CJR65544:CJR65586 CTN65544:CTN65586 DDJ65544:DDJ65586 DNF65544:DNF65586 DXB65544:DXB65586 EGX65544:EGX65586 EQT65544:EQT65586 FAP65544:FAP65586 FKL65544:FKL65586 FUH65544:FUH65586 GED65544:GED65586 GNZ65544:GNZ65586 GXV65544:GXV65586 HHR65544:HHR65586 HRN65544:HRN65586 IBJ65544:IBJ65586 ILF65544:ILF65586 IVB65544:IVB65586 JEX65544:JEX65586 JOT65544:JOT65586 JYP65544:JYP65586 KIL65544:KIL65586 KSH65544:KSH65586 LCD65544:LCD65586 LLZ65544:LLZ65586 LVV65544:LVV65586 MFR65544:MFR65586 MPN65544:MPN65586 MZJ65544:MZJ65586 NJF65544:NJF65586 NTB65544:NTB65586 OCX65544:OCX65586 OMT65544:OMT65586 OWP65544:OWP65586 PGL65544:PGL65586 PQH65544:PQH65586 QAD65544:QAD65586 QJZ65544:QJZ65586 QTV65544:QTV65586 RDR65544:RDR65586 RNN65544:RNN65586 RXJ65544:RXJ65586 SHF65544:SHF65586 SRB65544:SRB65586 TAX65544:TAX65586 TKT65544:TKT65586 TUP65544:TUP65586 UEL65544:UEL65586 UOH65544:UOH65586 UYD65544:UYD65586 VHZ65544:VHZ65586 VRV65544:VRV65586 WBR65544:WBR65586 WLN65544:WLN65586 WVJ65544:WVJ65586 B131080:B131122 IX131080:IX131122 ST131080:ST131122 ACP131080:ACP131122 AML131080:AML131122 AWH131080:AWH131122 BGD131080:BGD131122 BPZ131080:BPZ131122 BZV131080:BZV131122 CJR131080:CJR131122 CTN131080:CTN131122 DDJ131080:DDJ131122 DNF131080:DNF131122 DXB131080:DXB131122 EGX131080:EGX131122 EQT131080:EQT131122 FAP131080:FAP131122 FKL131080:FKL131122 FUH131080:FUH131122 GED131080:GED131122 GNZ131080:GNZ131122 GXV131080:GXV131122 HHR131080:HHR131122 HRN131080:HRN131122 IBJ131080:IBJ131122 ILF131080:ILF131122 IVB131080:IVB131122 JEX131080:JEX131122 JOT131080:JOT131122 JYP131080:JYP131122 KIL131080:KIL131122 KSH131080:KSH131122 LCD131080:LCD131122 LLZ131080:LLZ131122 LVV131080:LVV131122 MFR131080:MFR131122 MPN131080:MPN131122 MZJ131080:MZJ131122 NJF131080:NJF131122 NTB131080:NTB131122 OCX131080:OCX131122 OMT131080:OMT131122 OWP131080:OWP131122 PGL131080:PGL131122 PQH131080:PQH131122 QAD131080:QAD131122 QJZ131080:QJZ131122 QTV131080:QTV131122 RDR131080:RDR131122 RNN131080:RNN131122 RXJ131080:RXJ131122 SHF131080:SHF131122 SRB131080:SRB131122 TAX131080:TAX131122 TKT131080:TKT131122 TUP131080:TUP131122 UEL131080:UEL131122 UOH131080:UOH131122 UYD131080:UYD131122 VHZ131080:VHZ131122 VRV131080:VRV131122 WBR131080:WBR131122 WLN131080:WLN131122 WVJ131080:WVJ131122 B196616:B196658 IX196616:IX196658 ST196616:ST196658 ACP196616:ACP196658 AML196616:AML196658 AWH196616:AWH196658 BGD196616:BGD196658 BPZ196616:BPZ196658 BZV196616:BZV196658 CJR196616:CJR196658 CTN196616:CTN196658 DDJ196616:DDJ196658 DNF196616:DNF196658 DXB196616:DXB196658 EGX196616:EGX196658 EQT196616:EQT196658 FAP196616:FAP196658 FKL196616:FKL196658 FUH196616:FUH196658 GED196616:GED196658 GNZ196616:GNZ196658 GXV196616:GXV196658 HHR196616:HHR196658 HRN196616:HRN196658 IBJ196616:IBJ196658 ILF196616:ILF196658 IVB196616:IVB196658 JEX196616:JEX196658 JOT196616:JOT196658 JYP196616:JYP196658 KIL196616:KIL196658 KSH196616:KSH196658 LCD196616:LCD196658 LLZ196616:LLZ196658 LVV196616:LVV196658 MFR196616:MFR196658 MPN196616:MPN196658 MZJ196616:MZJ196658 NJF196616:NJF196658 NTB196616:NTB196658 OCX196616:OCX196658 OMT196616:OMT196658 OWP196616:OWP196658 PGL196616:PGL196658 PQH196616:PQH196658 QAD196616:QAD196658 QJZ196616:QJZ196658 QTV196616:QTV196658 RDR196616:RDR196658 RNN196616:RNN196658 RXJ196616:RXJ196658 SHF196616:SHF196658 SRB196616:SRB196658 TAX196616:TAX196658 TKT196616:TKT196658 TUP196616:TUP196658 UEL196616:UEL196658 UOH196616:UOH196658 UYD196616:UYD196658 VHZ196616:VHZ196658 VRV196616:VRV196658 WBR196616:WBR196658 WLN196616:WLN196658 WVJ196616:WVJ196658 B262152:B262194 IX262152:IX262194 ST262152:ST262194 ACP262152:ACP262194 AML262152:AML262194 AWH262152:AWH262194 BGD262152:BGD262194 BPZ262152:BPZ262194 BZV262152:BZV262194 CJR262152:CJR262194 CTN262152:CTN262194 DDJ262152:DDJ262194 DNF262152:DNF262194 DXB262152:DXB262194 EGX262152:EGX262194 EQT262152:EQT262194 FAP262152:FAP262194 FKL262152:FKL262194 FUH262152:FUH262194 GED262152:GED262194 GNZ262152:GNZ262194 GXV262152:GXV262194 HHR262152:HHR262194 HRN262152:HRN262194 IBJ262152:IBJ262194 ILF262152:ILF262194 IVB262152:IVB262194 JEX262152:JEX262194 JOT262152:JOT262194 JYP262152:JYP262194 KIL262152:KIL262194 KSH262152:KSH262194 LCD262152:LCD262194 LLZ262152:LLZ262194 LVV262152:LVV262194 MFR262152:MFR262194 MPN262152:MPN262194 MZJ262152:MZJ262194 NJF262152:NJF262194 NTB262152:NTB262194 OCX262152:OCX262194 OMT262152:OMT262194 OWP262152:OWP262194 PGL262152:PGL262194 PQH262152:PQH262194 QAD262152:QAD262194 QJZ262152:QJZ262194 QTV262152:QTV262194 RDR262152:RDR262194 RNN262152:RNN262194 RXJ262152:RXJ262194 SHF262152:SHF262194 SRB262152:SRB262194 TAX262152:TAX262194 TKT262152:TKT262194 TUP262152:TUP262194 UEL262152:UEL262194 UOH262152:UOH262194 UYD262152:UYD262194 VHZ262152:VHZ262194 VRV262152:VRV262194 WBR262152:WBR262194 WLN262152:WLN262194 WVJ262152:WVJ262194 B327688:B327730 IX327688:IX327730 ST327688:ST327730 ACP327688:ACP327730 AML327688:AML327730 AWH327688:AWH327730 BGD327688:BGD327730 BPZ327688:BPZ327730 BZV327688:BZV327730 CJR327688:CJR327730 CTN327688:CTN327730 DDJ327688:DDJ327730 DNF327688:DNF327730 DXB327688:DXB327730 EGX327688:EGX327730 EQT327688:EQT327730 FAP327688:FAP327730 FKL327688:FKL327730 FUH327688:FUH327730 GED327688:GED327730 GNZ327688:GNZ327730 GXV327688:GXV327730 HHR327688:HHR327730 HRN327688:HRN327730 IBJ327688:IBJ327730 ILF327688:ILF327730 IVB327688:IVB327730 JEX327688:JEX327730 JOT327688:JOT327730 JYP327688:JYP327730 KIL327688:KIL327730 KSH327688:KSH327730 LCD327688:LCD327730 LLZ327688:LLZ327730 LVV327688:LVV327730 MFR327688:MFR327730 MPN327688:MPN327730 MZJ327688:MZJ327730 NJF327688:NJF327730 NTB327688:NTB327730 OCX327688:OCX327730 OMT327688:OMT327730 OWP327688:OWP327730 PGL327688:PGL327730 PQH327688:PQH327730 QAD327688:QAD327730 QJZ327688:QJZ327730 QTV327688:QTV327730 RDR327688:RDR327730 RNN327688:RNN327730 RXJ327688:RXJ327730 SHF327688:SHF327730 SRB327688:SRB327730 TAX327688:TAX327730 TKT327688:TKT327730 TUP327688:TUP327730 UEL327688:UEL327730 UOH327688:UOH327730 UYD327688:UYD327730 VHZ327688:VHZ327730 VRV327688:VRV327730 WBR327688:WBR327730 WLN327688:WLN327730 WVJ327688:WVJ327730 B393224:B393266 IX393224:IX393266 ST393224:ST393266 ACP393224:ACP393266 AML393224:AML393266 AWH393224:AWH393266 BGD393224:BGD393266 BPZ393224:BPZ393266 BZV393224:BZV393266 CJR393224:CJR393266 CTN393224:CTN393266 DDJ393224:DDJ393266 DNF393224:DNF393266 DXB393224:DXB393266 EGX393224:EGX393266 EQT393224:EQT393266 FAP393224:FAP393266 FKL393224:FKL393266 FUH393224:FUH393266 GED393224:GED393266 GNZ393224:GNZ393266 GXV393224:GXV393266 HHR393224:HHR393266 HRN393224:HRN393266 IBJ393224:IBJ393266 ILF393224:ILF393266 IVB393224:IVB393266 JEX393224:JEX393266 JOT393224:JOT393266 JYP393224:JYP393266 KIL393224:KIL393266 KSH393224:KSH393266 LCD393224:LCD393266 LLZ393224:LLZ393266 LVV393224:LVV393266 MFR393224:MFR393266 MPN393224:MPN393266 MZJ393224:MZJ393266 NJF393224:NJF393266 NTB393224:NTB393266 OCX393224:OCX393266 OMT393224:OMT393266 OWP393224:OWP393266 PGL393224:PGL393266 PQH393224:PQH393266 QAD393224:QAD393266 QJZ393224:QJZ393266 QTV393224:QTV393266 RDR393224:RDR393266 RNN393224:RNN393266 RXJ393224:RXJ393266 SHF393224:SHF393266 SRB393224:SRB393266 TAX393224:TAX393266 TKT393224:TKT393266 TUP393224:TUP393266 UEL393224:UEL393266 UOH393224:UOH393266 UYD393224:UYD393266 VHZ393224:VHZ393266 VRV393224:VRV393266 WBR393224:WBR393266 WLN393224:WLN393266 WVJ393224:WVJ393266 B458760:B458802 IX458760:IX458802 ST458760:ST458802 ACP458760:ACP458802 AML458760:AML458802 AWH458760:AWH458802 BGD458760:BGD458802 BPZ458760:BPZ458802 BZV458760:BZV458802 CJR458760:CJR458802 CTN458760:CTN458802 DDJ458760:DDJ458802 DNF458760:DNF458802 DXB458760:DXB458802 EGX458760:EGX458802 EQT458760:EQT458802 FAP458760:FAP458802 FKL458760:FKL458802 FUH458760:FUH458802 GED458760:GED458802 GNZ458760:GNZ458802 GXV458760:GXV458802 HHR458760:HHR458802 HRN458760:HRN458802 IBJ458760:IBJ458802 ILF458760:ILF458802 IVB458760:IVB458802 JEX458760:JEX458802 JOT458760:JOT458802 JYP458760:JYP458802 KIL458760:KIL458802 KSH458760:KSH458802 LCD458760:LCD458802 LLZ458760:LLZ458802 LVV458760:LVV458802 MFR458760:MFR458802 MPN458760:MPN458802 MZJ458760:MZJ458802 NJF458760:NJF458802 NTB458760:NTB458802 OCX458760:OCX458802 OMT458760:OMT458802 OWP458760:OWP458802 PGL458760:PGL458802 PQH458760:PQH458802 QAD458760:QAD458802 QJZ458760:QJZ458802 QTV458760:QTV458802 RDR458760:RDR458802 RNN458760:RNN458802 RXJ458760:RXJ458802 SHF458760:SHF458802 SRB458760:SRB458802 TAX458760:TAX458802 TKT458760:TKT458802 TUP458760:TUP458802 UEL458760:UEL458802 UOH458760:UOH458802 UYD458760:UYD458802 VHZ458760:VHZ458802 VRV458760:VRV458802 WBR458760:WBR458802 WLN458760:WLN458802 WVJ458760:WVJ458802 B524296:B524338 IX524296:IX524338 ST524296:ST524338 ACP524296:ACP524338 AML524296:AML524338 AWH524296:AWH524338 BGD524296:BGD524338 BPZ524296:BPZ524338 BZV524296:BZV524338 CJR524296:CJR524338 CTN524296:CTN524338 DDJ524296:DDJ524338 DNF524296:DNF524338 DXB524296:DXB524338 EGX524296:EGX524338 EQT524296:EQT524338 FAP524296:FAP524338 FKL524296:FKL524338 FUH524296:FUH524338 GED524296:GED524338 GNZ524296:GNZ524338 GXV524296:GXV524338 HHR524296:HHR524338 HRN524296:HRN524338 IBJ524296:IBJ524338 ILF524296:ILF524338 IVB524296:IVB524338 JEX524296:JEX524338 JOT524296:JOT524338 JYP524296:JYP524338 KIL524296:KIL524338 KSH524296:KSH524338 LCD524296:LCD524338 LLZ524296:LLZ524338 LVV524296:LVV524338 MFR524296:MFR524338 MPN524296:MPN524338 MZJ524296:MZJ524338 NJF524296:NJF524338 NTB524296:NTB524338 OCX524296:OCX524338 OMT524296:OMT524338 OWP524296:OWP524338 PGL524296:PGL524338 PQH524296:PQH524338 QAD524296:QAD524338 QJZ524296:QJZ524338 QTV524296:QTV524338 RDR524296:RDR524338 RNN524296:RNN524338 RXJ524296:RXJ524338 SHF524296:SHF524338 SRB524296:SRB524338 TAX524296:TAX524338 TKT524296:TKT524338 TUP524296:TUP524338 UEL524296:UEL524338 UOH524296:UOH524338 UYD524296:UYD524338 VHZ524296:VHZ524338 VRV524296:VRV524338 WBR524296:WBR524338 WLN524296:WLN524338 WVJ524296:WVJ524338 B589832:B589874 IX589832:IX589874 ST589832:ST589874 ACP589832:ACP589874 AML589832:AML589874 AWH589832:AWH589874 BGD589832:BGD589874 BPZ589832:BPZ589874 BZV589832:BZV589874 CJR589832:CJR589874 CTN589832:CTN589874 DDJ589832:DDJ589874 DNF589832:DNF589874 DXB589832:DXB589874 EGX589832:EGX589874 EQT589832:EQT589874 FAP589832:FAP589874 FKL589832:FKL589874 FUH589832:FUH589874 GED589832:GED589874 GNZ589832:GNZ589874 GXV589832:GXV589874 HHR589832:HHR589874 HRN589832:HRN589874 IBJ589832:IBJ589874 ILF589832:ILF589874 IVB589832:IVB589874 JEX589832:JEX589874 JOT589832:JOT589874 JYP589832:JYP589874 KIL589832:KIL589874 KSH589832:KSH589874 LCD589832:LCD589874 LLZ589832:LLZ589874 LVV589832:LVV589874 MFR589832:MFR589874 MPN589832:MPN589874 MZJ589832:MZJ589874 NJF589832:NJF589874 NTB589832:NTB589874 OCX589832:OCX589874 OMT589832:OMT589874 OWP589832:OWP589874 PGL589832:PGL589874 PQH589832:PQH589874 QAD589832:QAD589874 QJZ589832:QJZ589874 QTV589832:QTV589874 RDR589832:RDR589874 RNN589832:RNN589874 RXJ589832:RXJ589874 SHF589832:SHF589874 SRB589832:SRB589874 TAX589832:TAX589874 TKT589832:TKT589874 TUP589832:TUP589874 UEL589832:UEL589874 UOH589832:UOH589874 UYD589832:UYD589874 VHZ589832:VHZ589874 VRV589832:VRV589874 WBR589832:WBR589874 WLN589832:WLN589874 WVJ589832:WVJ589874 B655368:B655410 IX655368:IX655410 ST655368:ST655410 ACP655368:ACP655410 AML655368:AML655410 AWH655368:AWH655410 BGD655368:BGD655410 BPZ655368:BPZ655410 BZV655368:BZV655410 CJR655368:CJR655410 CTN655368:CTN655410 DDJ655368:DDJ655410 DNF655368:DNF655410 DXB655368:DXB655410 EGX655368:EGX655410 EQT655368:EQT655410 FAP655368:FAP655410 FKL655368:FKL655410 FUH655368:FUH655410 GED655368:GED655410 GNZ655368:GNZ655410 GXV655368:GXV655410 HHR655368:HHR655410 HRN655368:HRN655410 IBJ655368:IBJ655410 ILF655368:ILF655410 IVB655368:IVB655410 JEX655368:JEX655410 JOT655368:JOT655410 JYP655368:JYP655410 KIL655368:KIL655410 KSH655368:KSH655410 LCD655368:LCD655410 LLZ655368:LLZ655410 LVV655368:LVV655410 MFR655368:MFR655410 MPN655368:MPN655410 MZJ655368:MZJ655410 NJF655368:NJF655410 NTB655368:NTB655410 OCX655368:OCX655410 OMT655368:OMT655410 OWP655368:OWP655410 PGL655368:PGL655410 PQH655368:PQH655410 QAD655368:QAD655410 QJZ655368:QJZ655410 QTV655368:QTV655410 RDR655368:RDR655410 RNN655368:RNN655410 RXJ655368:RXJ655410 SHF655368:SHF655410 SRB655368:SRB655410 TAX655368:TAX655410 TKT655368:TKT655410 TUP655368:TUP655410 UEL655368:UEL655410 UOH655368:UOH655410 UYD655368:UYD655410 VHZ655368:VHZ655410 VRV655368:VRV655410 WBR655368:WBR655410 WLN655368:WLN655410 WVJ655368:WVJ655410 B720904:B720946 IX720904:IX720946 ST720904:ST720946 ACP720904:ACP720946 AML720904:AML720946 AWH720904:AWH720946 BGD720904:BGD720946 BPZ720904:BPZ720946 BZV720904:BZV720946 CJR720904:CJR720946 CTN720904:CTN720946 DDJ720904:DDJ720946 DNF720904:DNF720946 DXB720904:DXB720946 EGX720904:EGX720946 EQT720904:EQT720946 FAP720904:FAP720946 FKL720904:FKL720946 FUH720904:FUH720946 GED720904:GED720946 GNZ720904:GNZ720946 GXV720904:GXV720946 HHR720904:HHR720946 HRN720904:HRN720946 IBJ720904:IBJ720946 ILF720904:ILF720946 IVB720904:IVB720946 JEX720904:JEX720946 JOT720904:JOT720946 JYP720904:JYP720946 KIL720904:KIL720946 KSH720904:KSH720946 LCD720904:LCD720946 LLZ720904:LLZ720946 LVV720904:LVV720946 MFR720904:MFR720946 MPN720904:MPN720946 MZJ720904:MZJ720946 NJF720904:NJF720946 NTB720904:NTB720946 OCX720904:OCX720946 OMT720904:OMT720946 OWP720904:OWP720946 PGL720904:PGL720946 PQH720904:PQH720946 QAD720904:QAD720946 QJZ720904:QJZ720946 QTV720904:QTV720946 RDR720904:RDR720946 RNN720904:RNN720946 RXJ720904:RXJ720946 SHF720904:SHF720946 SRB720904:SRB720946 TAX720904:TAX720946 TKT720904:TKT720946 TUP720904:TUP720946 UEL720904:UEL720946 UOH720904:UOH720946 UYD720904:UYD720946 VHZ720904:VHZ720946 VRV720904:VRV720946 WBR720904:WBR720946 WLN720904:WLN720946 WVJ720904:WVJ720946 B786440:B786482 IX786440:IX786482 ST786440:ST786482 ACP786440:ACP786482 AML786440:AML786482 AWH786440:AWH786482 BGD786440:BGD786482 BPZ786440:BPZ786482 BZV786440:BZV786482 CJR786440:CJR786482 CTN786440:CTN786482 DDJ786440:DDJ786482 DNF786440:DNF786482 DXB786440:DXB786482 EGX786440:EGX786482 EQT786440:EQT786482 FAP786440:FAP786482 FKL786440:FKL786482 FUH786440:FUH786482 GED786440:GED786482 GNZ786440:GNZ786482 GXV786440:GXV786482 HHR786440:HHR786482 HRN786440:HRN786482 IBJ786440:IBJ786482 ILF786440:ILF786482 IVB786440:IVB786482 JEX786440:JEX786482 JOT786440:JOT786482 JYP786440:JYP786482 KIL786440:KIL786482 KSH786440:KSH786482 LCD786440:LCD786482 LLZ786440:LLZ786482 LVV786440:LVV786482 MFR786440:MFR786482 MPN786440:MPN786482 MZJ786440:MZJ786482 NJF786440:NJF786482 NTB786440:NTB786482 OCX786440:OCX786482 OMT786440:OMT786482 OWP786440:OWP786482 PGL786440:PGL786482 PQH786440:PQH786482 QAD786440:QAD786482 QJZ786440:QJZ786482 QTV786440:QTV786482 RDR786440:RDR786482 RNN786440:RNN786482 RXJ786440:RXJ786482 SHF786440:SHF786482 SRB786440:SRB786482 TAX786440:TAX786482 TKT786440:TKT786482 TUP786440:TUP786482 UEL786440:UEL786482 UOH786440:UOH786482 UYD786440:UYD786482 VHZ786440:VHZ786482 VRV786440:VRV786482 WBR786440:WBR786482 WLN786440:WLN786482 WVJ786440:WVJ786482 B851976:B852018 IX851976:IX852018 ST851976:ST852018 ACP851976:ACP852018 AML851976:AML852018 AWH851976:AWH852018 BGD851976:BGD852018 BPZ851976:BPZ852018 BZV851976:BZV852018 CJR851976:CJR852018 CTN851976:CTN852018 DDJ851976:DDJ852018 DNF851976:DNF852018 DXB851976:DXB852018 EGX851976:EGX852018 EQT851976:EQT852018 FAP851976:FAP852018 FKL851976:FKL852018 FUH851976:FUH852018 GED851976:GED852018 GNZ851976:GNZ852018 GXV851976:GXV852018 HHR851976:HHR852018 HRN851976:HRN852018 IBJ851976:IBJ852018 ILF851976:ILF852018 IVB851976:IVB852018 JEX851976:JEX852018 JOT851976:JOT852018 JYP851976:JYP852018 KIL851976:KIL852018 KSH851976:KSH852018 LCD851976:LCD852018 LLZ851976:LLZ852018 LVV851976:LVV852018 MFR851976:MFR852018 MPN851976:MPN852018 MZJ851976:MZJ852018 NJF851976:NJF852018 NTB851976:NTB852018 OCX851976:OCX852018 OMT851976:OMT852018 OWP851976:OWP852018 PGL851976:PGL852018 PQH851976:PQH852018 QAD851976:QAD852018 QJZ851976:QJZ852018 QTV851976:QTV852018 RDR851976:RDR852018 RNN851976:RNN852018 RXJ851976:RXJ852018 SHF851976:SHF852018 SRB851976:SRB852018 TAX851976:TAX852018 TKT851976:TKT852018 TUP851976:TUP852018 UEL851976:UEL852018 UOH851976:UOH852018 UYD851976:UYD852018 VHZ851976:VHZ852018 VRV851976:VRV852018 WBR851976:WBR852018 WLN851976:WLN852018 WVJ851976:WVJ852018 B917512:B917554 IX917512:IX917554 ST917512:ST917554 ACP917512:ACP917554 AML917512:AML917554 AWH917512:AWH917554 BGD917512:BGD917554 BPZ917512:BPZ917554 BZV917512:BZV917554 CJR917512:CJR917554 CTN917512:CTN917554 DDJ917512:DDJ917554 DNF917512:DNF917554 DXB917512:DXB917554 EGX917512:EGX917554 EQT917512:EQT917554 FAP917512:FAP917554 FKL917512:FKL917554 FUH917512:FUH917554 GED917512:GED917554 GNZ917512:GNZ917554 GXV917512:GXV917554 HHR917512:HHR917554 HRN917512:HRN917554 IBJ917512:IBJ917554 ILF917512:ILF917554 IVB917512:IVB917554 JEX917512:JEX917554 JOT917512:JOT917554 JYP917512:JYP917554 KIL917512:KIL917554 KSH917512:KSH917554 LCD917512:LCD917554 LLZ917512:LLZ917554 LVV917512:LVV917554 MFR917512:MFR917554 MPN917512:MPN917554 MZJ917512:MZJ917554 NJF917512:NJF917554 NTB917512:NTB917554 OCX917512:OCX917554 OMT917512:OMT917554 OWP917512:OWP917554 PGL917512:PGL917554 PQH917512:PQH917554 QAD917512:QAD917554 QJZ917512:QJZ917554 QTV917512:QTV917554 RDR917512:RDR917554 RNN917512:RNN917554 RXJ917512:RXJ917554 SHF917512:SHF917554 SRB917512:SRB917554 TAX917512:TAX917554 TKT917512:TKT917554 TUP917512:TUP917554 UEL917512:UEL917554 UOH917512:UOH917554 UYD917512:UYD917554 VHZ917512:VHZ917554 VRV917512:VRV917554 WBR917512:WBR917554 WLN917512:WLN917554 WVJ917512:WVJ917554 B983048:B983090 IX983048:IX983090 ST983048:ST983090 ACP983048:ACP983090 AML983048:AML983090 AWH983048:AWH983090 BGD983048:BGD983090 BPZ983048:BPZ983090 BZV983048:BZV983090 CJR983048:CJR983090 CTN983048:CTN983090 DDJ983048:DDJ983090 DNF983048:DNF983090 DXB983048:DXB983090 EGX983048:EGX983090 EQT983048:EQT983090 FAP983048:FAP983090 FKL983048:FKL983090 FUH983048:FUH983090 GED983048:GED983090 GNZ983048:GNZ983090 GXV983048:GXV983090 HHR983048:HHR983090 HRN983048:HRN983090 IBJ983048:IBJ983090 ILF983048:ILF983090 IVB983048:IVB983090 JEX983048:JEX983090 JOT983048:JOT983090 JYP983048:JYP983090 KIL983048:KIL983090 KSH983048:KSH983090 LCD983048:LCD983090 LLZ983048:LLZ983090 LVV983048:LVV983090 MFR983048:MFR983090 MPN983048:MPN983090 MZJ983048:MZJ983090 NJF983048:NJF983090 NTB983048:NTB983090 OCX983048:OCX983090 OMT983048:OMT983090 OWP983048:OWP983090 PGL983048:PGL983090 PQH983048:PQH983090 QAD983048:QAD983090 QJZ983048:QJZ983090 QTV983048:QTV983090 RDR983048:RDR983090 RNN983048:RNN983090 RXJ983048:RXJ983090 SHF983048:SHF983090 SRB983048:SRB983090 TAX983048:TAX983090 TKT983048:TKT983090 TUP983048:TUP983090 UEL983048:UEL983090 UOH983048:UOH983090 UYD983048:UYD983090 VHZ983048:VHZ983090 VRV983048:VRV983090 WBR983048:WBR983090 WLN983048:WLN983090 WVJ983048:WVJ983090" xr:uid="{3BCDAFA9-70FD-42ED-B088-113DD368B30F}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B50 IX8:IX50 ST8:ST50 ACP8:ACP50 AML8:AML50 AWH8:AWH50 BGD8:BGD50 BPZ8:BPZ50 BZV8:BZV50 CJR8:CJR50 CTN8:CTN50 DDJ8:DDJ50 DNF8:DNF50 DXB8:DXB50 EGX8:EGX50 EQT8:EQT50 FAP8:FAP50 FKL8:FKL50 FUH8:FUH50 GED8:GED50 GNZ8:GNZ50 GXV8:GXV50 HHR8:HHR50 HRN8:HRN50 IBJ8:IBJ50 ILF8:ILF50 IVB8:IVB50 JEX8:JEX50 JOT8:JOT50 JYP8:JYP50 KIL8:KIL50 KSH8:KSH50 LCD8:LCD50 LLZ8:LLZ50 LVV8:LVV50 MFR8:MFR50 MPN8:MPN50 MZJ8:MZJ50 NJF8:NJF50 NTB8:NTB50 OCX8:OCX50 OMT8:OMT50 OWP8:OWP50 PGL8:PGL50 PQH8:PQH50 QAD8:QAD50 QJZ8:QJZ50 QTV8:QTV50 RDR8:RDR50 RNN8:RNN50 RXJ8:RXJ50 SHF8:SHF50 SRB8:SRB50 TAX8:TAX50 TKT8:TKT50 TUP8:TUP50 UEL8:UEL50 UOH8:UOH50 UYD8:UYD50 VHZ8:VHZ50 VRV8:VRV50 WBR8:WBR50 WLN8:WLN50 WVJ8:WVJ50 B65544:B65586 IX65544:IX65586 ST65544:ST65586 ACP65544:ACP65586 AML65544:AML65586 AWH65544:AWH65586 BGD65544:BGD65586 BPZ65544:BPZ65586 BZV65544:BZV65586 CJR65544:CJR65586 CTN65544:CTN65586 DDJ65544:DDJ65586 DNF65544:DNF65586 DXB65544:DXB65586 EGX65544:EGX65586 EQT65544:EQT65586 FAP65544:FAP65586 FKL65544:FKL65586 FUH65544:FUH65586 GED65544:GED65586 GNZ65544:GNZ65586 GXV65544:GXV65586 HHR65544:HHR65586 HRN65544:HRN65586 IBJ65544:IBJ65586 ILF65544:ILF65586 IVB65544:IVB65586 JEX65544:JEX65586 JOT65544:JOT65586 JYP65544:JYP65586 KIL65544:KIL65586 KSH65544:KSH65586 LCD65544:LCD65586 LLZ65544:LLZ65586 LVV65544:LVV65586 MFR65544:MFR65586 MPN65544:MPN65586 MZJ65544:MZJ65586 NJF65544:NJF65586 NTB65544:NTB65586 OCX65544:OCX65586 OMT65544:OMT65586 OWP65544:OWP65586 PGL65544:PGL65586 PQH65544:PQH65586 QAD65544:QAD65586 QJZ65544:QJZ65586 QTV65544:QTV65586 RDR65544:RDR65586 RNN65544:RNN65586 RXJ65544:RXJ65586 SHF65544:SHF65586 SRB65544:SRB65586 TAX65544:TAX65586 TKT65544:TKT65586 TUP65544:TUP65586 UEL65544:UEL65586 UOH65544:UOH65586 UYD65544:UYD65586 VHZ65544:VHZ65586 VRV65544:VRV65586 WBR65544:WBR65586 WLN65544:WLN65586 WVJ65544:WVJ65586 B131080:B131122 IX131080:IX131122 ST131080:ST131122 ACP131080:ACP131122 AML131080:AML131122 AWH131080:AWH131122 BGD131080:BGD131122 BPZ131080:BPZ131122 BZV131080:BZV131122 CJR131080:CJR131122 CTN131080:CTN131122 DDJ131080:DDJ131122 DNF131080:DNF131122 DXB131080:DXB131122 EGX131080:EGX131122 EQT131080:EQT131122 FAP131080:FAP131122 FKL131080:FKL131122 FUH131080:FUH131122 GED131080:GED131122 GNZ131080:GNZ131122 GXV131080:GXV131122 HHR131080:HHR131122 HRN131080:HRN131122 IBJ131080:IBJ131122 ILF131080:ILF131122 IVB131080:IVB131122 JEX131080:JEX131122 JOT131080:JOT131122 JYP131080:JYP131122 KIL131080:KIL131122 KSH131080:KSH131122 LCD131080:LCD131122 LLZ131080:LLZ131122 LVV131080:LVV131122 MFR131080:MFR131122 MPN131080:MPN131122 MZJ131080:MZJ131122 NJF131080:NJF131122 NTB131080:NTB131122 OCX131080:OCX131122 OMT131080:OMT131122 OWP131080:OWP131122 PGL131080:PGL131122 PQH131080:PQH131122 QAD131080:QAD131122 QJZ131080:QJZ131122 QTV131080:QTV131122 RDR131080:RDR131122 RNN131080:RNN131122 RXJ131080:RXJ131122 SHF131080:SHF131122 SRB131080:SRB131122 TAX131080:TAX131122 TKT131080:TKT131122 TUP131080:TUP131122 UEL131080:UEL131122 UOH131080:UOH131122 UYD131080:UYD131122 VHZ131080:VHZ131122 VRV131080:VRV131122 WBR131080:WBR131122 WLN131080:WLN131122 WVJ131080:WVJ131122 B196616:B196658 IX196616:IX196658 ST196616:ST196658 ACP196616:ACP196658 AML196616:AML196658 AWH196616:AWH196658 BGD196616:BGD196658 BPZ196616:BPZ196658 BZV196616:BZV196658 CJR196616:CJR196658 CTN196616:CTN196658 DDJ196616:DDJ196658 DNF196616:DNF196658 DXB196616:DXB196658 EGX196616:EGX196658 EQT196616:EQT196658 FAP196616:FAP196658 FKL196616:FKL196658 FUH196616:FUH196658 GED196616:GED196658 GNZ196616:GNZ196658 GXV196616:GXV196658 HHR196616:HHR196658 HRN196616:HRN196658 IBJ196616:IBJ196658 ILF196616:ILF196658 IVB196616:IVB196658 JEX196616:JEX196658 JOT196616:JOT196658 JYP196616:JYP196658 KIL196616:KIL196658 KSH196616:KSH196658 LCD196616:LCD196658 LLZ196616:LLZ196658 LVV196616:LVV196658 MFR196616:MFR196658 MPN196616:MPN196658 MZJ196616:MZJ196658 NJF196616:NJF196658 NTB196616:NTB196658 OCX196616:OCX196658 OMT196616:OMT196658 OWP196616:OWP196658 PGL196616:PGL196658 PQH196616:PQH196658 QAD196616:QAD196658 QJZ196616:QJZ196658 QTV196616:QTV196658 RDR196616:RDR196658 RNN196616:RNN196658 RXJ196616:RXJ196658 SHF196616:SHF196658 SRB196616:SRB196658 TAX196616:TAX196658 TKT196616:TKT196658 TUP196616:TUP196658 UEL196616:UEL196658 UOH196616:UOH196658 UYD196616:UYD196658 VHZ196616:VHZ196658 VRV196616:VRV196658 WBR196616:WBR196658 WLN196616:WLN196658 WVJ196616:WVJ196658 B262152:B262194 IX262152:IX262194 ST262152:ST262194 ACP262152:ACP262194 AML262152:AML262194 AWH262152:AWH262194 BGD262152:BGD262194 BPZ262152:BPZ262194 BZV262152:BZV262194 CJR262152:CJR262194 CTN262152:CTN262194 DDJ262152:DDJ262194 DNF262152:DNF262194 DXB262152:DXB262194 EGX262152:EGX262194 EQT262152:EQT262194 FAP262152:FAP262194 FKL262152:FKL262194 FUH262152:FUH262194 GED262152:GED262194 GNZ262152:GNZ262194 GXV262152:GXV262194 HHR262152:HHR262194 HRN262152:HRN262194 IBJ262152:IBJ262194 ILF262152:ILF262194 IVB262152:IVB262194 JEX262152:JEX262194 JOT262152:JOT262194 JYP262152:JYP262194 KIL262152:KIL262194 KSH262152:KSH262194 LCD262152:LCD262194 LLZ262152:LLZ262194 LVV262152:LVV262194 MFR262152:MFR262194 MPN262152:MPN262194 MZJ262152:MZJ262194 NJF262152:NJF262194 NTB262152:NTB262194 OCX262152:OCX262194 OMT262152:OMT262194 OWP262152:OWP262194 PGL262152:PGL262194 PQH262152:PQH262194 QAD262152:QAD262194 QJZ262152:QJZ262194 QTV262152:QTV262194 RDR262152:RDR262194 RNN262152:RNN262194 RXJ262152:RXJ262194 SHF262152:SHF262194 SRB262152:SRB262194 TAX262152:TAX262194 TKT262152:TKT262194 TUP262152:TUP262194 UEL262152:UEL262194 UOH262152:UOH262194 UYD262152:UYD262194 VHZ262152:VHZ262194 VRV262152:VRV262194 WBR262152:WBR262194 WLN262152:WLN262194 WVJ262152:WVJ262194 B327688:B327730 IX327688:IX327730 ST327688:ST327730 ACP327688:ACP327730 AML327688:AML327730 AWH327688:AWH327730 BGD327688:BGD327730 BPZ327688:BPZ327730 BZV327688:BZV327730 CJR327688:CJR327730 CTN327688:CTN327730 DDJ327688:DDJ327730 DNF327688:DNF327730 DXB327688:DXB327730 EGX327688:EGX327730 EQT327688:EQT327730 FAP327688:FAP327730 FKL327688:FKL327730 FUH327688:FUH327730 GED327688:GED327730 GNZ327688:GNZ327730 GXV327688:GXV327730 HHR327688:HHR327730 HRN327688:HRN327730 IBJ327688:IBJ327730 ILF327688:ILF327730 IVB327688:IVB327730 JEX327688:JEX327730 JOT327688:JOT327730 JYP327688:JYP327730 KIL327688:KIL327730 KSH327688:KSH327730 LCD327688:LCD327730 LLZ327688:LLZ327730 LVV327688:LVV327730 MFR327688:MFR327730 MPN327688:MPN327730 MZJ327688:MZJ327730 NJF327688:NJF327730 NTB327688:NTB327730 OCX327688:OCX327730 OMT327688:OMT327730 OWP327688:OWP327730 PGL327688:PGL327730 PQH327688:PQH327730 QAD327688:QAD327730 QJZ327688:QJZ327730 QTV327688:QTV327730 RDR327688:RDR327730 RNN327688:RNN327730 RXJ327688:RXJ327730 SHF327688:SHF327730 SRB327688:SRB327730 TAX327688:TAX327730 TKT327688:TKT327730 TUP327688:TUP327730 UEL327688:UEL327730 UOH327688:UOH327730 UYD327688:UYD327730 VHZ327688:VHZ327730 VRV327688:VRV327730 WBR327688:WBR327730 WLN327688:WLN327730 WVJ327688:WVJ327730 B393224:B393266 IX393224:IX393266 ST393224:ST393266 ACP393224:ACP393266 AML393224:AML393266 AWH393224:AWH393266 BGD393224:BGD393266 BPZ393224:BPZ393266 BZV393224:BZV393266 CJR393224:CJR393266 CTN393224:CTN393266 DDJ393224:DDJ393266 DNF393224:DNF393266 DXB393224:DXB393266 EGX393224:EGX393266 EQT393224:EQT393266 FAP393224:FAP393266 FKL393224:FKL393266 FUH393224:FUH393266 GED393224:GED393266 GNZ393224:GNZ393266 GXV393224:GXV393266 HHR393224:HHR393266 HRN393224:HRN393266 IBJ393224:IBJ393266 ILF393224:ILF393266 IVB393224:IVB393266 JEX393224:JEX393266 JOT393224:JOT393266 JYP393224:JYP393266 KIL393224:KIL393266 KSH393224:KSH393266 LCD393224:LCD393266 LLZ393224:LLZ393266 LVV393224:LVV393266 MFR393224:MFR393266 MPN393224:MPN393266 MZJ393224:MZJ393266 NJF393224:NJF393266 NTB393224:NTB393266 OCX393224:OCX393266 OMT393224:OMT393266 OWP393224:OWP393266 PGL393224:PGL393266 PQH393224:PQH393266 QAD393224:QAD393266 QJZ393224:QJZ393266 QTV393224:QTV393266 RDR393224:RDR393266 RNN393224:RNN393266 RXJ393224:RXJ393266 SHF393224:SHF393266 SRB393224:SRB393266 TAX393224:TAX393266 TKT393224:TKT393266 TUP393224:TUP393266 UEL393224:UEL393266 UOH393224:UOH393266 UYD393224:UYD393266 VHZ393224:VHZ393266 VRV393224:VRV393266 WBR393224:WBR393266 WLN393224:WLN393266 WVJ393224:WVJ393266 B458760:B458802 IX458760:IX458802 ST458760:ST458802 ACP458760:ACP458802 AML458760:AML458802 AWH458760:AWH458802 BGD458760:BGD458802 BPZ458760:BPZ458802 BZV458760:BZV458802 CJR458760:CJR458802 CTN458760:CTN458802 DDJ458760:DDJ458802 DNF458760:DNF458802 DXB458760:DXB458802 EGX458760:EGX458802 EQT458760:EQT458802 FAP458760:FAP458802 FKL458760:FKL458802 FUH458760:FUH458802 GED458760:GED458802 GNZ458760:GNZ458802 GXV458760:GXV458802 HHR458760:HHR458802 HRN458760:HRN458802 IBJ458760:IBJ458802 ILF458760:ILF458802 IVB458760:IVB458802 JEX458760:JEX458802 JOT458760:JOT458802 JYP458760:JYP458802 KIL458760:KIL458802 KSH458760:KSH458802 LCD458760:LCD458802 LLZ458760:LLZ458802 LVV458760:LVV458802 MFR458760:MFR458802 MPN458760:MPN458802 MZJ458760:MZJ458802 NJF458760:NJF458802 NTB458760:NTB458802 OCX458760:OCX458802 OMT458760:OMT458802 OWP458760:OWP458802 PGL458760:PGL458802 PQH458760:PQH458802 QAD458760:QAD458802 QJZ458760:QJZ458802 QTV458760:QTV458802 RDR458760:RDR458802 RNN458760:RNN458802 RXJ458760:RXJ458802 SHF458760:SHF458802 SRB458760:SRB458802 TAX458760:TAX458802 TKT458760:TKT458802 TUP458760:TUP458802 UEL458760:UEL458802 UOH458760:UOH458802 UYD458760:UYD458802 VHZ458760:VHZ458802 VRV458760:VRV458802 WBR458760:WBR458802 WLN458760:WLN458802 WVJ458760:WVJ458802 B524296:B524338 IX524296:IX524338 ST524296:ST524338 ACP524296:ACP524338 AML524296:AML524338 AWH524296:AWH524338 BGD524296:BGD524338 BPZ524296:BPZ524338 BZV524296:BZV524338 CJR524296:CJR524338 CTN524296:CTN524338 DDJ524296:DDJ524338 DNF524296:DNF524338 DXB524296:DXB524338 EGX524296:EGX524338 EQT524296:EQT524338 FAP524296:FAP524338 FKL524296:FKL524338 FUH524296:FUH524338 GED524296:GED524338 GNZ524296:GNZ524338 GXV524296:GXV524338 HHR524296:HHR524338 HRN524296:HRN524338 IBJ524296:IBJ524338 ILF524296:ILF524338 IVB524296:IVB524338 JEX524296:JEX524338 JOT524296:JOT524338 JYP524296:JYP524338 KIL524296:KIL524338 KSH524296:KSH524338 LCD524296:LCD524338 LLZ524296:LLZ524338 LVV524296:LVV524338 MFR524296:MFR524338 MPN524296:MPN524338 MZJ524296:MZJ524338 NJF524296:NJF524338 NTB524296:NTB524338 OCX524296:OCX524338 OMT524296:OMT524338 OWP524296:OWP524338 PGL524296:PGL524338 PQH524296:PQH524338 QAD524296:QAD524338 QJZ524296:QJZ524338 QTV524296:QTV524338 RDR524296:RDR524338 RNN524296:RNN524338 RXJ524296:RXJ524338 SHF524296:SHF524338 SRB524296:SRB524338 TAX524296:TAX524338 TKT524296:TKT524338 TUP524296:TUP524338 UEL524296:UEL524338 UOH524296:UOH524338 UYD524296:UYD524338 VHZ524296:VHZ524338 VRV524296:VRV524338 WBR524296:WBR524338 WLN524296:WLN524338 WVJ524296:WVJ524338 B589832:B589874 IX589832:IX589874 ST589832:ST589874 ACP589832:ACP589874 AML589832:AML589874 AWH589832:AWH589874 BGD589832:BGD589874 BPZ589832:BPZ589874 BZV589832:BZV589874 CJR589832:CJR589874 CTN589832:CTN589874 DDJ589832:DDJ589874 DNF589832:DNF589874 DXB589832:DXB589874 EGX589832:EGX589874 EQT589832:EQT589874 FAP589832:FAP589874 FKL589832:FKL589874 FUH589832:FUH589874 GED589832:GED589874 GNZ589832:GNZ589874 GXV589832:GXV589874 HHR589832:HHR589874 HRN589832:HRN589874 IBJ589832:IBJ589874 ILF589832:ILF589874 IVB589832:IVB589874 JEX589832:JEX589874 JOT589832:JOT589874 JYP589832:JYP589874 KIL589832:KIL589874 KSH589832:KSH589874 LCD589832:LCD589874 LLZ589832:LLZ589874 LVV589832:LVV589874 MFR589832:MFR589874 MPN589832:MPN589874 MZJ589832:MZJ589874 NJF589832:NJF589874 NTB589832:NTB589874 OCX589832:OCX589874 OMT589832:OMT589874 OWP589832:OWP589874 PGL589832:PGL589874 PQH589832:PQH589874 QAD589832:QAD589874 QJZ589832:QJZ589874 QTV589832:QTV589874 RDR589832:RDR589874 RNN589832:RNN589874 RXJ589832:RXJ589874 SHF589832:SHF589874 SRB589832:SRB589874 TAX589832:TAX589874 TKT589832:TKT589874 TUP589832:TUP589874 UEL589832:UEL589874 UOH589832:UOH589874 UYD589832:UYD589874 VHZ589832:VHZ589874 VRV589832:VRV589874 WBR589832:WBR589874 WLN589832:WLN589874 WVJ589832:WVJ589874 B655368:B655410 IX655368:IX655410 ST655368:ST655410 ACP655368:ACP655410 AML655368:AML655410 AWH655368:AWH655410 BGD655368:BGD655410 BPZ655368:BPZ655410 BZV655368:BZV655410 CJR655368:CJR655410 CTN655368:CTN655410 DDJ655368:DDJ655410 DNF655368:DNF655410 DXB655368:DXB655410 EGX655368:EGX655410 EQT655368:EQT655410 FAP655368:FAP655410 FKL655368:FKL655410 FUH655368:FUH655410 GED655368:GED655410 GNZ655368:GNZ655410 GXV655368:GXV655410 HHR655368:HHR655410 HRN655368:HRN655410 IBJ655368:IBJ655410 ILF655368:ILF655410 IVB655368:IVB655410 JEX655368:JEX655410 JOT655368:JOT655410 JYP655368:JYP655410 KIL655368:KIL655410 KSH655368:KSH655410 LCD655368:LCD655410 LLZ655368:LLZ655410 LVV655368:LVV655410 MFR655368:MFR655410 MPN655368:MPN655410 MZJ655368:MZJ655410 NJF655368:NJF655410 NTB655368:NTB655410 OCX655368:OCX655410 OMT655368:OMT655410 OWP655368:OWP655410 PGL655368:PGL655410 PQH655368:PQH655410 QAD655368:QAD655410 QJZ655368:QJZ655410 QTV655368:QTV655410 RDR655368:RDR655410 RNN655368:RNN655410 RXJ655368:RXJ655410 SHF655368:SHF655410 SRB655368:SRB655410 TAX655368:TAX655410 TKT655368:TKT655410 TUP655368:TUP655410 UEL655368:UEL655410 UOH655368:UOH655410 UYD655368:UYD655410 VHZ655368:VHZ655410 VRV655368:VRV655410 WBR655368:WBR655410 WLN655368:WLN655410 WVJ655368:WVJ655410 B720904:B720946 IX720904:IX720946 ST720904:ST720946 ACP720904:ACP720946 AML720904:AML720946 AWH720904:AWH720946 BGD720904:BGD720946 BPZ720904:BPZ720946 BZV720904:BZV720946 CJR720904:CJR720946 CTN720904:CTN720946 DDJ720904:DDJ720946 DNF720904:DNF720946 DXB720904:DXB720946 EGX720904:EGX720946 EQT720904:EQT720946 FAP720904:FAP720946 FKL720904:FKL720946 FUH720904:FUH720946 GED720904:GED720946 GNZ720904:GNZ720946 GXV720904:GXV720946 HHR720904:HHR720946 HRN720904:HRN720946 IBJ720904:IBJ720946 ILF720904:ILF720946 IVB720904:IVB720946 JEX720904:JEX720946 JOT720904:JOT720946 JYP720904:JYP720946 KIL720904:KIL720946 KSH720904:KSH720946 LCD720904:LCD720946 LLZ720904:LLZ720946 LVV720904:LVV720946 MFR720904:MFR720946 MPN720904:MPN720946 MZJ720904:MZJ720946 NJF720904:NJF720946 NTB720904:NTB720946 OCX720904:OCX720946 OMT720904:OMT720946 OWP720904:OWP720946 PGL720904:PGL720946 PQH720904:PQH720946 QAD720904:QAD720946 QJZ720904:QJZ720946 QTV720904:QTV720946 RDR720904:RDR720946 RNN720904:RNN720946 RXJ720904:RXJ720946 SHF720904:SHF720946 SRB720904:SRB720946 TAX720904:TAX720946 TKT720904:TKT720946 TUP720904:TUP720946 UEL720904:UEL720946 UOH720904:UOH720946 UYD720904:UYD720946 VHZ720904:VHZ720946 VRV720904:VRV720946 WBR720904:WBR720946 WLN720904:WLN720946 WVJ720904:WVJ720946 B786440:B786482 IX786440:IX786482 ST786440:ST786482 ACP786440:ACP786482 AML786440:AML786482 AWH786440:AWH786482 BGD786440:BGD786482 BPZ786440:BPZ786482 BZV786440:BZV786482 CJR786440:CJR786482 CTN786440:CTN786482 DDJ786440:DDJ786482 DNF786440:DNF786482 DXB786440:DXB786482 EGX786440:EGX786482 EQT786440:EQT786482 FAP786440:FAP786482 FKL786440:FKL786482 FUH786440:FUH786482 GED786440:GED786482 GNZ786440:GNZ786482 GXV786440:GXV786482 HHR786440:HHR786482 HRN786440:HRN786482 IBJ786440:IBJ786482 ILF786440:ILF786482 IVB786440:IVB786482 JEX786440:JEX786482 JOT786440:JOT786482 JYP786440:JYP786482 KIL786440:KIL786482 KSH786440:KSH786482 LCD786440:LCD786482 LLZ786440:LLZ786482 LVV786440:LVV786482 MFR786440:MFR786482 MPN786440:MPN786482 MZJ786440:MZJ786482 NJF786440:NJF786482 NTB786440:NTB786482 OCX786440:OCX786482 OMT786440:OMT786482 OWP786440:OWP786482 PGL786440:PGL786482 PQH786440:PQH786482 QAD786440:QAD786482 QJZ786440:QJZ786482 QTV786440:QTV786482 RDR786440:RDR786482 RNN786440:RNN786482 RXJ786440:RXJ786482 SHF786440:SHF786482 SRB786440:SRB786482 TAX786440:TAX786482 TKT786440:TKT786482 TUP786440:TUP786482 UEL786440:UEL786482 UOH786440:UOH786482 UYD786440:UYD786482 VHZ786440:VHZ786482 VRV786440:VRV786482 WBR786440:WBR786482 WLN786440:WLN786482 WVJ786440:WVJ786482 B851976:B852018 IX851976:IX852018 ST851976:ST852018 ACP851976:ACP852018 AML851976:AML852018 AWH851976:AWH852018 BGD851976:BGD852018 BPZ851976:BPZ852018 BZV851976:BZV852018 CJR851976:CJR852018 CTN851976:CTN852018 DDJ851976:DDJ852018 DNF851976:DNF852018 DXB851976:DXB852018 EGX851976:EGX852018 EQT851976:EQT852018 FAP851976:FAP852018 FKL851976:FKL852018 FUH851976:FUH852018 GED851976:GED852018 GNZ851976:GNZ852018 GXV851976:GXV852018 HHR851976:HHR852018 HRN851976:HRN852018 IBJ851976:IBJ852018 ILF851976:ILF852018 IVB851976:IVB852018 JEX851976:JEX852018 JOT851976:JOT852018 JYP851976:JYP852018 KIL851976:KIL852018 KSH851976:KSH852018 LCD851976:LCD852018 LLZ851976:LLZ852018 LVV851976:LVV852018 MFR851976:MFR852018 MPN851976:MPN852018 MZJ851976:MZJ852018 NJF851976:NJF852018 NTB851976:NTB852018 OCX851976:OCX852018 OMT851976:OMT852018 OWP851976:OWP852018 PGL851976:PGL852018 PQH851976:PQH852018 QAD851976:QAD852018 QJZ851976:QJZ852018 QTV851976:QTV852018 RDR851976:RDR852018 RNN851976:RNN852018 RXJ851976:RXJ852018 SHF851976:SHF852018 SRB851976:SRB852018 TAX851976:TAX852018 TKT851976:TKT852018 TUP851976:TUP852018 UEL851976:UEL852018 UOH851976:UOH852018 UYD851976:UYD852018 VHZ851976:VHZ852018 VRV851976:VRV852018 WBR851976:WBR852018 WLN851976:WLN852018 WVJ851976:WVJ852018 B917512:B917554 IX917512:IX917554 ST917512:ST917554 ACP917512:ACP917554 AML917512:AML917554 AWH917512:AWH917554 BGD917512:BGD917554 BPZ917512:BPZ917554 BZV917512:BZV917554 CJR917512:CJR917554 CTN917512:CTN917554 DDJ917512:DDJ917554 DNF917512:DNF917554 DXB917512:DXB917554 EGX917512:EGX917554 EQT917512:EQT917554 FAP917512:FAP917554 FKL917512:FKL917554 FUH917512:FUH917554 GED917512:GED917554 GNZ917512:GNZ917554 GXV917512:GXV917554 HHR917512:HHR917554 HRN917512:HRN917554 IBJ917512:IBJ917554 ILF917512:ILF917554 IVB917512:IVB917554 JEX917512:JEX917554 JOT917512:JOT917554 JYP917512:JYP917554 KIL917512:KIL917554 KSH917512:KSH917554 LCD917512:LCD917554 LLZ917512:LLZ917554 LVV917512:LVV917554 MFR917512:MFR917554 MPN917512:MPN917554 MZJ917512:MZJ917554 NJF917512:NJF917554 NTB917512:NTB917554 OCX917512:OCX917554 OMT917512:OMT917554 OWP917512:OWP917554 PGL917512:PGL917554 PQH917512:PQH917554 QAD917512:QAD917554 QJZ917512:QJZ917554 QTV917512:QTV917554 RDR917512:RDR917554 RNN917512:RNN917554 RXJ917512:RXJ917554 SHF917512:SHF917554 SRB917512:SRB917554 TAX917512:TAX917554 TKT917512:TKT917554 TUP917512:TUP917554 UEL917512:UEL917554 UOH917512:UOH917554 UYD917512:UYD917554 VHZ917512:VHZ917554 VRV917512:VRV917554 WBR917512:WBR917554 WLN917512:WLN917554 WVJ917512:WVJ917554 B983048:B983090 IX983048:IX983090 ST983048:ST983090 ACP983048:ACP983090 AML983048:AML983090 AWH983048:AWH983090 BGD983048:BGD983090 BPZ983048:BPZ983090 BZV983048:BZV983090 CJR983048:CJR983090 CTN983048:CTN983090 DDJ983048:DDJ983090 DNF983048:DNF983090 DXB983048:DXB983090 EGX983048:EGX983090 EQT983048:EQT983090 FAP983048:FAP983090 FKL983048:FKL983090 FUH983048:FUH983090 GED983048:GED983090 GNZ983048:GNZ983090 GXV983048:GXV983090 HHR983048:HHR983090 HRN983048:HRN983090 IBJ983048:IBJ983090 ILF983048:ILF983090 IVB983048:IVB983090 JEX983048:JEX983090 JOT983048:JOT983090 JYP983048:JYP983090 KIL983048:KIL983090 KSH983048:KSH983090 LCD983048:LCD983090 LLZ983048:LLZ983090 LVV983048:LVV983090 MFR983048:MFR983090 MPN983048:MPN983090 MZJ983048:MZJ983090 NJF983048:NJF983090 NTB983048:NTB983090 OCX983048:OCX983090 OMT983048:OMT983090 OWP983048:OWP983090 PGL983048:PGL983090 PQH983048:PQH983090 QAD983048:QAD983090 QJZ983048:QJZ983090 QTV983048:QTV983090 RDR983048:RDR983090 RNN983048:RNN983090 RXJ983048:RXJ983090 SHF983048:SHF983090 SRB983048:SRB983090 TAX983048:TAX983090 TKT983048:TKT983090 TUP983048:TUP983090 UEL983048:UEL983090 UOH983048:UOH983090 UYD983048:UYD983090 VHZ983048:VHZ983090 VRV983048:VRV983090 WBR983048:WBR983090 WLN983048:WLN983090 WVJ983048:WVJ983090">
       <formula1>8</formula1>
       <formula2>8</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
added update results and correcture value
</commit_message>
<xml_diff>
--- a/src/main/resources/results/Ergebnisse Excel 2018.xlsx
+++ b/src/main/resources/results/Ergebnisse Excel 2018.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{436F5343-CD17-42A2-8F51-83BDEB0474D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="08.04.WE" sheetId="30" r:id="rId1"/>
     <sheet name="14.04.ES" sheetId="31" r:id="rId2"/>
     <sheet name="14.04.RE" sheetId="32" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2530" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2532" uniqueCount="206">
   <si>
     <t>Ort</t>
   </si>
@@ -623,11 +624,23 @@
   <si>
     <t>010-0048</t>
   </si>
+  <si>
+    <t>005-0008</t>
+  </si>
+  <si>
+    <t>Wolf Martina</t>
+  </si>
+  <si>
+    <t>011-0043</t>
+  </si>
+  <si>
+    <t>Jacobsen Sigrid</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -716,9 +729,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Standard 4" xfId="2"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -753,7 +766,7 @@
         <xdr:cNvPr id="2" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{20B498EC-182A-4181-917A-602AEB452E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20B498EC-182A-4181-917A-602AEB452E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -827,7 +840,7 @@
         <xdr:cNvPr id="3" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4CE2411C-5471-4F3F-8B68-04E35CED8E7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CE2411C-5471-4F3F-8B68-04E35CED8E7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -901,7 +914,7 @@
         <xdr:cNvPr id="4" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C3743E6C-8BFA-4837-A821-7D24D7E03156}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3743E6C-8BFA-4837-A821-7D24D7E03156}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -980,7 +993,7 @@
         <xdr:cNvPr id="2" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53F4F544-178A-48E5-B1F4-189F85DA7BED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53F4F544-178A-48E5-B1F4-189F85DA7BED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1054,7 +1067,7 @@
         <xdr:cNvPr id="3" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A34C1F7A-D0A8-4FDF-8665-3CF196E869BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A34C1F7A-D0A8-4FDF-8665-3CF196E869BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1128,7 +1141,7 @@
         <xdr:cNvPr id="4" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2D3BACFE-B0FF-4B8F-B0D4-112389EA32EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D3BACFE-B0FF-4B8F-B0D4-112389EA32EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1207,7 +1220,7 @@
         <xdr:cNvPr id="2" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F19E5A8-F619-4868-8110-72BBFF13158C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F19E5A8-F619-4868-8110-72BBFF13158C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1281,7 +1294,7 @@
         <xdr:cNvPr id="3" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEE1E2BB-2400-4A0B-8D99-6B0F60646AB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEE1E2BB-2400-4A0B-8D99-6B0F60646AB0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1355,7 +1368,7 @@
         <xdr:cNvPr id="4" name="Grafik 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{458B0779-3FCA-44E4-8C2F-7E1B815FB4B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{458B0779-3FCA-44E4-8C2F-7E1B815FB4B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1415,7 +1428,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1457,7 +1470,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1490,9 +1503,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1525,6 +1555,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1700,530 +1747,530 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="21" width="2.7109375" style="8" customWidth="1"/>
-    <col min="22" max="22" width="4.42578125" style="8" customWidth="1"/>
-    <col min="23" max="23" width="7.42578125" style="8" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="256" width="11.42578125" style="1"/>
-    <col min="257" max="257" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="21" width="2.7265625" style="8" customWidth="1"/>
+    <col min="22" max="22" width="4.453125" style="8" customWidth="1"/>
+    <col min="23" max="23" width="7.453125" style="8" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="256" width="11.453125" style="1"/>
+    <col min="257" max="257" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="260" max="277" width="2.7109375" style="1" customWidth="1"/>
-    <col min="278" max="278" width="4.42578125" style="1" customWidth="1"/>
+    <col min="260" max="277" width="2.7265625" style="1" customWidth="1"/>
+    <col min="278" max="278" width="4.453125" style="1" customWidth="1"/>
     <col min="279" max="279" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="280" max="280" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="281" max="512" width="11.42578125" style="1"/>
-    <col min="513" max="513" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="281" max="512" width="11.453125" style="1"/>
+    <col min="513" max="513" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="515" max="515" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="516" max="533" width="2.7109375" style="1" customWidth="1"/>
-    <col min="534" max="534" width="4.42578125" style="1" customWidth="1"/>
+    <col min="516" max="533" width="2.7265625" style="1" customWidth="1"/>
+    <col min="534" max="534" width="4.453125" style="1" customWidth="1"/>
     <col min="535" max="535" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="536" max="536" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="537" max="768" width="11.42578125" style="1"/>
-    <col min="769" max="769" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="536" max="536" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="537" max="768" width="11.453125" style="1"/>
+    <col min="769" max="769" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="771" max="771" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="772" max="789" width="2.7109375" style="1" customWidth="1"/>
-    <col min="790" max="790" width="4.42578125" style="1" customWidth="1"/>
+    <col min="772" max="789" width="2.7265625" style="1" customWidth="1"/>
+    <col min="790" max="790" width="4.453125" style="1" customWidth="1"/>
     <col min="791" max="791" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="792" max="792" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="793" max="1024" width="11.42578125" style="1"/>
-    <col min="1025" max="1025" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="792" max="792" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="793" max="1024" width="11.453125" style="1"/>
+    <col min="1025" max="1025" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1027" max="1027" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1045" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1046" max="1046" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1028" max="1045" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1046" max="1046" width="4.453125" style="1" customWidth="1"/>
     <col min="1047" max="1047" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1048" max="1048" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1049" max="1280" width="11.42578125" style="1"/>
-    <col min="1281" max="1281" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1048" max="1048" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1049" max="1280" width="11.453125" style="1"/>
+    <col min="1281" max="1281" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1283" max="1283" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1301" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1302" max="1302" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1284" max="1301" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1302" max="1302" width="4.453125" style="1" customWidth="1"/>
     <col min="1303" max="1303" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1304" max="1304" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1305" max="1536" width="11.42578125" style="1"/>
-    <col min="1537" max="1537" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1304" max="1304" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1305" max="1536" width="11.453125" style="1"/>
+    <col min="1537" max="1537" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1539" max="1539" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1557" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1558" max="1558" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1540" max="1557" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1558" max="1558" width="4.453125" style="1" customWidth="1"/>
     <col min="1559" max="1559" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1560" max="1560" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1561" max="1792" width="11.42578125" style="1"/>
-    <col min="1793" max="1793" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1560" max="1560" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1561" max="1792" width="11.453125" style="1"/>
+    <col min="1793" max="1793" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1795" max="1795" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1813" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1814" max="1814" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1796" max="1813" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1814" max="1814" width="4.453125" style="1" customWidth="1"/>
     <col min="1815" max="1815" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1816" max="1816" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1817" max="2048" width="11.42578125" style="1"/>
-    <col min="2049" max="2049" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1816" max="1816" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1817" max="2048" width="11.453125" style="1"/>
+    <col min="2049" max="2049" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2051" max="2051" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2069" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2070" max="2070" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2052" max="2069" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2070" max="2070" width="4.453125" style="1" customWidth="1"/>
     <col min="2071" max="2071" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2072" max="2072" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2073" max="2304" width="11.42578125" style="1"/>
-    <col min="2305" max="2305" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2072" max="2072" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2073" max="2304" width="11.453125" style="1"/>
+    <col min="2305" max="2305" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2307" max="2307" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2325" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2326" max="2326" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2308" max="2325" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2326" max="2326" width="4.453125" style="1" customWidth="1"/>
     <col min="2327" max="2327" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2328" max="2328" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2329" max="2560" width="11.42578125" style="1"/>
-    <col min="2561" max="2561" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2328" max="2328" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2329" max="2560" width="11.453125" style="1"/>
+    <col min="2561" max="2561" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2563" max="2563" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2581" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2582" max="2582" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2564" max="2581" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2582" max="2582" width="4.453125" style="1" customWidth="1"/>
     <col min="2583" max="2583" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2584" max="2584" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2585" max="2816" width="11.42578125" style="1"/>
-    <col min="2817" max="2817" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2584" max="2584" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2585" max="2816" width="11.453125" style="1"/>
+    <col min="2817" max="2817" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2819" max="2819" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2837" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2838" max="2838" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2820" max="2837" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2838" max="2838" width="4.453125" style="1" customWidth="1"/>
     <col min="2839" max="2839" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2840" max="2840" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2841" max="3072" width="11.42578125" style="1"/>
-    <col min="3073" max="3073" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2840" max="2840" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2841" max="3072" width="11.453125" style="1"/>
+    <col min="3073" max="3073" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3075" max="3075" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3093" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3094" max="3094" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3076" max="3093" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3094" max="3094" width="4.453125" style="1" customWidth="1"/>
     <col min="3095" max="3095" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3096" max="3096" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3097" max="3328" width="11.42578125" style="1"/>
-    <col min="3329" max="3329" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3096" max="3096" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3097" max="3328" width="11.453125" style="1"/>
+    <col min="3329" max="3329" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3331" max="3331" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3349" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3350" max="3350" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3332" max="3349" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3350" max="3350" width="4.453125" style="1" customWidth="1"/>
     <col min="3351" max="3351" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3352" max="3352" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3353" max="3584" width="11.42578125" style="1"/>
-    <col min="3585" max="3585" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3352" max="3352" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3353" max="3584" width="11.453125" style="1"/>
+    <col min="3585" max="3585" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3587" max="3587" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3605" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3606" max="3606" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3588" max="3605" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3606" max="3606" width="4.453125" style="1" customWidth="1"/>
     <col min="3607" max="3607" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3608" max="3608" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3609" max="3840" width="11.42578125" style="1"/>
-    <col min="3841" max="3841" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3608" max="3608" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3609" max="3840" width="11.453125" style="1"/>
+    <col min="3841" max="3841" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3843" max="3843" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3861" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3862" max="3862" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3844" max="3861" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3862" max="3862" width="4.453125" style="1" customWidth="1"/>
     <col min="3863" max="3863" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3864" max="3864" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3865" max="4096" width="11.42578125" style="1"/>
-    <col min="4097" max="4097" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3864" max="3864" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3865" max="4096" width="11.453125" style="1"/>
+    <col min="4097" max="4097" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4099" max="4099" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4117" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4118" max="4118" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4100" max="4117" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4118" max="4118" width="4.453125" style="1" customWidth="1"/>
     <col min="4119" max="4119" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4120" max="4120" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4121" max="4352" width="11.42578125" style="1"/>
-    <col min="4353" max="4353" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4120" max="4120" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4121" max="4352" width="11.453125" style="1"/>
+    <col min="4353" max="4353" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4355" max="4355" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4373" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4374" max="4374" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4356" max="4373" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4374" max="4374" width="4.453125" style="1" customWidth="1"/>
     <col min="4375" max="4375" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4376" max="4376" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4377" max="4608" width="11.42578125" style="1"/>
-    <col min="4609" max="4609" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4376" max="4376" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4377" max="4608" width="11.453125" style="1"/>
+    <col min="4609" max="4609" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4611" max="4611" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4629" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4630" max="4630" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4612" max="4629" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4630" max="4630" width="4.453125" style="1" customWidth="1"/>
     <col min="4631" max="4631" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4632" max="4632" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4633" max="4864" width="11.42578125" style="1"/>
-    <col min="4865" max="4865" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4632" max="4632" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4633" max="4864" width="11.453125" style="1"/>
+    <col min="4865" max="4865" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4867" max="4867" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4885" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4886" max="4886" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4868" max="4885" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4886" max="4886" width="4.453125" style="1" customWidth="1"/>
     <col min="4887" max="4887" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4888" max="4888" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4889" max="5120" width="11.42578125" style="1"/>
-    <col min="5121" max="5121" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4888" max="4888" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4889" max="5120" width="11.453125" style="1"/>
+    <col min="5121" max="5121" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5123" max="5123" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5141" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5142" max="5142" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5124" max="5141" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5142" max="5142" width="4.453125" style="1" customWidth="1"/>
     <col min="5143" max="5143" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5144" max="5144" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5145" max="5376" width="11.42578125" style="1"/>
-    <col min="5377" max="5377" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5144" max="5144" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5145" max="5376" width="11.453125" style="1"/>
+    <col min="5377" max="5377" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5379" max="5379" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5397" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5398" max="5398" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5380" max="5397" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5398" max="5398" width="4.453125" style="1" customWidth="1"/>
     <col min="5399" max="5399" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5400" max="5400" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5401" max="5632" width="11.42578125" style="1"/>
-    <col min="5633" max="5633" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5400" max="5400" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5401" max="5632" width="11.453125" style="1"/>
+    <col min="5633" max="5633" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5635" max="5635" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5653" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5654" max="5654" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5636" max="5653" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5654" max="5654" width="4.453125" style="1" customWidth="1"/>
     <col min="5655" max="5655" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5656" max="5656" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5657" max="5888" width="11.42578125" style="1"/>
-    <col min="5889" max="5889" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5656" max="5656" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5657" max="5888" width="11.453125" style="1"/>
+    <col min="5889" max="5889" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5891" max="5891" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5909" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5910" max="5910" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5892" max="5909" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5910" max="5910" width="4.453125" style="1" customWidth="1"/>
     <col min="5911" max="5911" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5912" max="5912" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5913" max="6144" width="11.42578125" style="1"/>
-    <col min="6145" max="6145" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5912" max="5912" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5913" max="6144" width="11.453125" style="1"/>
+    <col min="6145" max="6145" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6147" max="6147" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6165" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6166" max="6166" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6148" max="6165" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6166" max="6166" width="4.453125" style="1" customWidth="1"/>
     <col min="6167" max="6167" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6168" max="6168" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6169" max="6400" width="11.42578125" style="1"/>
-    <col min="6401" max="6401" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6168" max="6168" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6169" max="6400" width="11.453125" style="1"/>
+    <col min="6401" max="6401" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6403" max="6403" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6421" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6422" max="6422" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6404" max="6421" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6422" max="6422" width="4.453125" style="1" customWidth="1"/>
     <col min="6423" max="6423" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6424" max="6424" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6425" max="6656" width="11.42578125" style="1"/>
-    <col min="6657" max="6657" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6424" max="6424" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6425" max="6656" width="11.453125" style="1"/>
+    <col min="6657" max="6657" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6659" max="6659" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6677" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6678" max="6678" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6660" max="6677" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6678" max="6678" width="4.453125" style="1" customWidth="1"/>
     <col min="6679" max="6679" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6680" max="6680" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6681" max="6912" width="11.42578125" style="1"/>
-    <col min="6913" max="6913" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6680" max="6680" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6681" max="6912" width="11.453125" style="1"/>
+    <col min="6913" max="6913" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6915" max="6915" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6933" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6934" max="6934" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6916" max="6933" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6934" max="6934" width="4.453125" style="1" customWidth="1"/>
     <col min="6935" max="6935" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6936" max="6936" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6937" max="7168" width="11.42578125" style="1"/>
-    <col min="7169" max="7169" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6936" max="6936" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6937" max="7168" width="11.453125" style="1"/>
+    <col min="7169" max="7169" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7171" max="7171" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7189" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7190" max="7190" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7172" max="7189" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7190" max="7190" width="4.453125" style="1" customWidth="1"/>
     <col min="7191" max="7191" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7192" max="7192" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7193" max="7424" width="11.42578125" style="1"/>
-    <col min="7425" max="7425" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7192" max="7192" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7193" max="7424" width="11.453125" style="1"/>
+    <col min="7425" max="7425" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7427" max="7427" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7445" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7446" max="7446" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7428" max="7445" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7446" max="7446" width="4.453125" style="1" customWidth="1"/>
     <col min="7447" max="7447" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7448" max="7448" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7449" max="7680" width="11.42578125" style="1"/>
-    <col min="7681" max="7681" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7448" max="7448" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7449" max="7680" width="11.453125" style="1"/>
+    <col min="7681" max="7681" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7683" max="7683" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7701" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7702" max="7702" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7684" max="7701" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7702" max="7702" width="4.453125" style="1" customWidth="1"/>
     <col min="7703" max="7703" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7704" max="7704" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7705" max="7936" width="11.42578125" style="1"/>
-    <col min="7937" max="7937" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7704" max="7704" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7705" max="7936" width="11.453125" style="1"/>
+    <col min="7937" max="7937" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7939" max="7939" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7957" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7958" max="7958" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7940" max="7957" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7958" max="7958" width="4.453125" style="1" customWidth="1"/>
     <col min="7959" max="7959" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7960" max="7960" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7961" max="8192" width="11.42578125" style="1"/>
-    <col min="8193" max="8193" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7960" max="7960" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7961" max="8192" width="11.453125" style="1"/>
+    <col min="8193" max="8193" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8195" max="8195" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8213" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8214" max="8214" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8196" max="8213" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8214" max="8214" width="4.453125" style="1" customWidth="1"/>
     <col min="8215" max="8215" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8216" max="8216" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8217" max="8448" width="11.42578125" style="1"/>
-    <col min="8449" max="8449" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8216" max="8216" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8217" max="8448" width="11.453125" style="1"/>
+    <col min="8449" max="8449" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8451" max="8451" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8469" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8470" max="8470" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8452" max="8469" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8470" max="8470" width="4.453125" style="1" customWidth="1"/>
     <col min="8471" max="8471" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8472" max="8472" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8473" max="8704" width="11.42578125" style="1"/>
-    <col min="8705" max="8705" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8472" max="8472" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8473" max="8704" width="11.453125" style="1"/>
+    <col min="8705" max="8705" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8707" max="8707" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8725" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8726" max="8726" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8708" max="8725" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8726" max="8726" width="4.453125" style="1" customWidth="1"/>
     <col min="8727" max="8727" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8728" max="8728" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8729" max="8960" width="11.42578125" style="1"/>
-    <col min="8961" max="8961" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8728" max="8728" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8729" max="8960" width="11.453125" style="1"/>
+    <col min="8961" max="8961" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8963" max="8963" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8981" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8982" max="8982" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8964" max="8981" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8982" max="8982" width="4.453125" style="1" customWidth="1"/>
     <col min="8983" max="8983" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8984" max="8984" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8985" max="9216" width="11.42578125" style="1"/>
-    <col min="9217" max="9217" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8984" max="8984" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8985" max="9216" width="11.453125" style="1"/>
+    <col min="9217" max="9217" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9219" max="9219" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9237" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9238" max="9238" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9220" max="9237" width="2.7265625" style="1" customWidth="1"/>
+    <col min="9238" max="9238" width="4.453125" style="1" customWidth="1"/>
     <col min="9239" max="9239" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9240" max="9240" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9241" max="9472" width="11.42578125" style="1"/>
-    <col min="9473" max="9473" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9240" max="9240" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9241" max="9472" width="11.453125" style="1"/>
+    <col min="9473" max="9473" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9475" max="9475" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9493" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9494" max="9494" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9476" max="9493" width="2.7265625" style="1" customWidth="1"/>
+    <col min="9494" max="9494" width="4.453125" style="1" customWidth="1"/>
     <col min="9495" max="9495" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9496" max="9496" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9497" max="9728" width="11.42578125" style="1"/>
-    <col min="9729" max="9729" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9496" max="9496" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9497" max="9728" width="11.453125" style="1"/>
+    <col min="9729" max="9729" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9731" max="9731" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9749" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9750" max="9750" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9732" max="9749" width="2.7265625" style="1" customWidth="1"/>
+    <col min="9750" max="9750" width="4.453125" style="1" customWidth="1"/>
     <col min="9751" max="9751" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9752" max="9752" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9753" max="9984" width="11.42578125" style="1"/>
-    <col min="9985" max="9985" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9752" max="9752" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9753" max="9984" width="11.453125" style="1"/>
+    <col min="9985" max="9985" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9987" max="9987" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9988" max="10005" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10006" max="10006" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9988" max="10005" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10006" max="10006" width="4.453125" style="1" customWidth="1"/>
     <col min="10007" max="10007" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10008" max="10008" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10009" max="10240" width="11.42578125" style="1"/>
-    <col min="10241" max="10241" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10008" max="10008" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10009" max="10240" width="11.453125" style="1"/>
+    <col min="10241" max="10241" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10243" max="10243" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10261" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10262" max="10262" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10244" max="10261" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10262" max="10262" width="4.453125" style="1" customWidth="1"/>
     <col min="10263" max="10263" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10264" max="10264" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10265" max="10496" width="11.42578125" style="1"/>
-    <col min="10497" max="10497" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10264" max="10264" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10265" max="10496" width="11.453125" style="1"/>
+    <col min="10497" max="10497" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10499" max="10499" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10517" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10518" max="10518" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10500" max="10517" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10518" max="10518" width="4.453125" style="1" customWidth="1"/>
     <col min="10519" max="10519" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10520" max="10520" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10521" max="10752" width="11.42578125" style="1"/>
-    <col min="10753" max="10753" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10520" max="10520" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10521" max="10752" width="11.453125" style="1"/>
+    <col min="10753" max="10753" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10755" max="10755" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10773" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10774" max="10774" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10756" max="10773" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10774" max="10774" width="4.453125" style="1" customWidth="1"/>
     <col min="10775" max="10775" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10776" max="10776" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10777" max="11008" width="11.42578125" style="1"/>
-    <col min="11009" max="11009" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10776" max="10776" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10777" max="11008" width="11.453125" style="1"/>
+    <col min="11009" max="11009" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11011" max="11011" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11029" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11030" max="11030" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11012" max="11029" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11030" max="11030" width="4.453125" style="1" customWidth="1"/>
     <col min="11031" max="11031" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11032" max="11032" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11033" max="11264" width="11.42578125" style="1"/>
-    <col min="11265" max="11265" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11032" max="11032" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11033" max="11264" width="11.453125" style="1"/>
+    <col min="11265" max="11265" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11267" max="11267" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11285" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11286" max="11286" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11268" max="11285" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11286" max="11286" width="4.453125" style="1" customWidth="1"/>
     <col min="11287" max="11287" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11288" max="11288" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11289" max="11520" width="11.42578125" style="1"/>
-    <col min="11521" max="11521" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11288" max="11288" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11289" max="11520" width="11.453125" style="1"/>
+    <col min="11521" max="11521" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11523" max="11523" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11541" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11542" max="11542" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11524" max="11541" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11542" max="11542" width="4.453125" style="1" customWidth="1"/>
     <col min="11543" max="11543" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11544" max="11544" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11545" max="11776" width="11.42578125" style="1"/>
-    <col min="11777" max="11777" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11544" max="11544" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11545" max="11776" width="11.453125" style="1"/>
+    <col min="11777" max="11777" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11779" max="11779" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11797" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11798" max="11798" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11780" max="11797" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11798" max="11798" width="4.453125" style="1" customWidth="1"/>
     <col min="11799" max="11799" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11800" max="11800" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11801" max="12032" width="11.42578125" style="1"/>
-    <col min="12033" max="12033" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11800" max="11800" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11801" max="12032" width="11.453125" style="1"/>
+    <col min="12033" max="12033" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12035" max="12035" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12053" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12054" max="12054" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12036" max="12053" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12054" max="12054" width="4.453125" style="1" customWidth="1"/>
     <col min="12055" max="12055" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12056" max="12056" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12057" max="12288" width="11.42578125" style="1"/>
-    <col min="12289" max="12289" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12056" max="12056" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12057" max="12288" width="11.453125" style="1"/>
+    <col min="12289" max="12289" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12291" max="12291" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12309" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12310" max="12310" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12292" max="12309" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12310" max="12310" width="4.453125" style="1" customWidth="1"/>
     <col min="12311" max="12311" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12312" max="12312" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12313" max="12544" width="11.42578125" style="1"/>
-    <col min="12545" max="12545" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12312" max="12312" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12313" max="12544" width="11.453125" style="1"/>
+    <col min="12545" max="12545" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12547" max="12547" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12565" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12566" max="12566" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12548" max="12565" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12566" max="12566" width="4.453125" style="1" customWidth="1"/>
     <col min="12567" max="12567" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12568" max="12568" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12569" max="12800" width="11.42578125" style="1"/>
-    <col min="12801" max="12801" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12568" max="12568" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12569" max="12800" width="11.453125" style="1"/>
+    <col min="12801" max="12801" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12803" max="12803" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12821" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12822" max="12822" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12804" max="12821" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12822" max="12822" width="4.453125" style="1" customWidth="1"/>
     <col min="12823" max="12823" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12824" max="12824" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12825" max="13056" width="11.42578125" style="1"/>
-    <col min="13057" max="13057" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12824" max="12824" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12825" max="13056" width="11.453125" style="1"/>
+    <col min="13057" max="13057" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13059" max="13059" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13077" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13078" max="13078" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13060" max="13077" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13078" max="13078" width="4.453125" style="1" customWidth="1"/>
     <col min="13079" max="13079" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13080" max="13080" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13081" max="13312" width="11.42578125" style="1"/>
-    <col min="13313" max="13313" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13080" max="13080" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13081" max="13312" width="11.453125" style="1"/>
+    <col min="13313" max="13313" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13315" max="13315" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13333" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13334" max="13334" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13316" max="13333" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13334" max="13334" width="4.453125" style="1" customWidth="1"/>
     <col min="13335" max="13335" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13336" max="13336" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13337" max="13568" width="11.42578125" style="1"/>
-    <col min="13569" max="13569" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13336" max="13336" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13337" max="13568" width="11.453125" style="1"/>
+    <col min="13569" max="13569" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13571" max="13571" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13589" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13590" max="13590" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13572" max="13589" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13590" max="13590" width="4.453125" style="1" customWidth="1"/>
     <col min="13591" max="13591" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13592" max="13592" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13593" max="13824" width="11.42578125" style="1"/>
-    <col min="13825" max="13825" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13592" max="13592" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13593" max="13824" width="11.453125" style="1"/>
+    <col min="13825" max="13825" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13827" max="13827" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13845" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13846" max="13846" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13828" max="13845" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13846" max="13846" width="4.453125" style="1" customWidth="1"/>
     <col min="13847" max="13847" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13848" max="13848" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13849" max="14080" width="11.42578125" style="1"/>
-    <col min="14081" max="14081" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13848" max="13848" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13849" max="14080" width="11.453125" style="1"/>
+    <col min="14081" max="14081" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14083" max="14083" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14101" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14102" max="14102" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14084" max="14101" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14102" max="14102" width="4.453125" style="1" customWidth="1"/>
     <col min="14103" max="14103" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14104" max="14104" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14105" max="14336" width="11.42578125" style="1"/>
-    <col min="14337" max="14337" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14104" max="14104" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14105" max="14336" width="11.453125" style="1"/>
+    <col min="14337" max="14337" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14339" max="14339" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14357" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14358" max="14358" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14340" max="14357" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14358" max="14358" width="4.453125" style="1" customWidth="1"/>
     <col min="14359" max="14359" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14360" max="14360" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14361" max="14592" width="11.42578125" style="1"/>
-    <col min="14593" max="14593" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14360" max="14360" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14361" max="14592" width="11.453125" style="1"/>
+    <col min="14593" max="14593" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14595" max="14595" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14613" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14614" max="14614" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14596" max="14613" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14614" max="14614" width="4.453125" style="1" customWidth="1"/>
     <col min="14615" max="14615" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14616" max="14616" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14617" max="14848" width="11.42578125" style="1"/>
-    <col min="14849" max="14849" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14616" max="14616" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14617" max="14848" width="11.453125" style="1"/>
+    <col min="14849" max="14849" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14851" max="14851" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14869" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14870" max="14870" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14852" max="14869" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14870" max="14870" width="4.453125" style="1" customWidth="1"/>
     <col min="14871" max="14871" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14872" max="14872" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14873" max="15104" width="11.42578125" style="1"/>
-    <col min="15105" max="15105" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14872" max="14872" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14873" max="15104" width="11.453125" style="1"/>
+    <col min="15105" max="15105" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15107" max="15107" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15125" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15126" max="15126" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15108" max="15125" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15126" max="15126" width="4.453125" style="1" customWidth="1"/>
     <col min="15127" max="15127" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15128" max="15128" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15129" max="15360" width="11.42578125" style="1"/>
-    <col min="15361" max="15361" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15128" max="15128" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15129" max="15360" width="11.453125" style="1"/>
+    <col min="15361" max="15361" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15363" max="15363" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15381" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15382" max="15382" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15364" max="15381" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15382" max="15382" width="4.453125" style="1" customWidth="1"/>
     <col min="15383" max="15383" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15384" max="15384" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15385" max="15616" width="11.42578125" style="1"/>
-    <col min="15617" max="15617" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15384" max="15384" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15385" max="15616" width="11.453125" style="1"/>
+    <col min="15617" max="15617" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15619" max="15619" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15637" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15638" max="15638" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15620" max="15637" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15638" max="15638" width="4.453125" style="1" customWidth="1"/>
     <col min="15639" max="15639" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15640" max="15640" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15641" max="15872" width="11.42578125" style="1"/>
-    <col min="15873" max="15873" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15640" max="15640" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15641" max="15872" width="11.453125" style="1"/>
+    <col min="15873" max="15873" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15875" max="15875" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15893" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15894" max="15894" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15876" max="15893" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15894" max="15894" width="4.453125" style="1" customWidth="1"/>
     <col min="15895" max="15895" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15896" max="15896" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15897" max="16128" width="11.42578125" style="1"/>
-    <col min="16129" max="16129" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15896" max="15896" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15897" max="16128" width="11.453125" style="1"/>
+    <col min="16129" max="16129" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="16131" max="16131" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16149" width="2.7109375" style="1" customWidth="1"/>
-    <col min="16150" max="16150" width="4.42578125" style="1" customWidth="1"/>
+    <col min="16132" max="16149" width="2.7265625" style="1" customWidth="1"/>
+    <col min="16150" max="16150" width="4.453125" style="1" customWidth="1"/>
     <col min="16151" max="16151" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="16152" max="16152" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16153" max="16384" width="11.42578125" style="1"/>
+    <col min="16152" max="16152" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16153" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2257,7 +2304,7 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
     </row>
-    <row r="2" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2287,7 +2334,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
     </row>
-    <row r="3" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2317,7 +2364,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
     </row>
-    <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2347,7 +2394,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2355,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2438,7 +2485,7 @@
       </c>
       <c r="AB7" s="12"/>
     </row>
-    <row r="8" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2513,7 +2560,7 @@
       </c>
       <c r="Y8" s="8"/>
     </row>
-    <row r="9" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2663,7 +2710,7 @@
       </c>
       <c r="Y10" s="8"/>
     </row>
-    <row r="11" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -2738,7 +2785,7 @@
       </c>
       <c r="Y11" s="8"/>
     </row>
-    <row r="12" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -2813,7 +2860,7 @@
       </c>
       <c r="Y12" s="8"/>
     </row>
-    <row r="13" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -2888,7 +2935,7 @@
       </c>
       <c r="Y13" s="8"/>
     </row>
-    <row r="14" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -2963,7 +3010,7 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="15" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -3038,7 +3085,7 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="16" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -3113,7 +3160,7 @@
       </c>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -3188,7 +3235,7 @@
       </c>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -3263,7 +3310,7 @@
       </c>
       <c r="Y18" s="8"/>
     </row>
-    <row r="19" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
@@ -3338,7 +3385,7 @@
       </c>
       <c r="Y19" s="8"/>
     </row>
-    <row r="20" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
@@ -3413,7 +3460,7 @@
       </c>
       <c r="Y20" s="8"/>
     </row>
-    <row r="21" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -3563,7 +3610,7 @@
       </c>
       <c r="Y22" s="8"/>
     </row>
-    <row r="23" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
@@ -3713,7 +3760,7 @@
       </c>
       <c r="Y24" s="8"/>
     </row>
-    <row r="25" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
@@ -3788,7 +3835,7 @@
       </c>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
@@ -8951,7 +8998,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B50 IX8:IX50 ST8:ST50 ACP8:ACP50 AML8:AML50 AWH8:AWH50 BGD8:BGD50 BPZ8:BPZ50 BZV8:BZV50 CJR8:CJR50 CTN8:CTN50 DDJ8:DDJ50 DNF8:DNF50 DXB8:DXB50 EGX8:EGX50 EQT8:EQT50 FAP8:FAP50 FKL8:FKL50 FUH8:FUH50 GED8:GED50 GNZ8:GNZ50 GXV8:GXV50 HHR8:HHR50 HRN8:HRN50 IBJ8:IBJ50 ILF8:ILF50 IVB8:IVB50 JEX8:JEX50 JOT8:JOT50 JYP8:JYP50 KIL8:KIL50 KSH8:KSH50 LCD8:LCD50 LLZ8:LLZ50 LVV8:LVV50 MFR8:MFR50 MPN8:MPN50 MZJ8:MZJ50 NJF8:NJF50 NTB8:NTB50 OCX8:OCX50 OMT8:OMT50 OWP8:OWP50 PGL8:PGL50 PQH8:PQH50 QAD8:QAD50 QJZ8:QJZ50 QTV8:QTV50 RDR8:RDR50 RNN8:RNN50 RXJ8:RXJ50 SHF8:SHF50 SRB8:SRB50 TAX8:TAX50 TKT8:TKT50 TUP8:TUP50 UEL8:UEL50 UOH8:UOH50 UYD8:UYD50 VHZ8:VHZ50 VRV8:VRV50 WBR8:WBR50 WLN8:WLN50 WVJ8:WVJ50 B65544:B65586 IX65544:IX65586 ST65544:ST65586 ACP65544:ACP65586 AML65544:AML65586 AWH65544:AWH65586 BGD65544:BGD65586 BPZ65544:BPZ65586 BZV65544:BZV65586 CJR65544:CJR65586 CTN65544:CTN65586 DDJ65544:DDJ65586 DNF65544:DNF65586 DXB65544:DXB65586 EGX65544:EGX65586 EQT65544:EQT65586 FAP65544:FAP65586 FKL65544:FKL65586 FUH65544:FUH65586 GED65544:GED65586 GNZ65544:GNZ65586 GXV65544:GXV65586 HHR65544:HHR65586 HRN65544:HRN65586 IBJ65544:IBJ65586 ILF65544:ILF65586 IVB65544:IVB65586 JEX65544:JEX65586 JOT65544:JOT65586 JYP65544:JYP65586 KIL65544:KIL65586 KSH65544:KSH65586 LCD65544:LCD65586 LLZ65544:LLZ65586 LVV65544:LVV65586 MFR65544:MFR65586 MPN65544:MPN65586 MZJ65544:MZJ65586 NJF65544:NJF65586 NTB65544:NTB65586 OCX65544:OCX65586 OMT65544:OMT65586 OWP65544:OWP65586 PGL65544:PGL65586 PQH65544:PQH65586 QAD65544:QAD65586 QJZ65544:QJZ65586 QTV65544:QTV65586 RDR65544:RDR65586 RNN65544:RNN65586 RXJ65544:RXJ65586 SHF65544:SHF65586 SRB65544:SRB65586 TAX65544:TAX65586 TKT65544:TKT65586 TUP65544:TUP65586 UEL65544:UEL65586 UOH65544:UOH65586 UYD65544:UYD65586 VHZ65544:VHZ65586 VRV65544:VRV65586 WBR65544:WBR65586 WLN65544:WLN65586 WVJ65544:WVJ65586 B131080:B131122 IX131080:IX131122 ST131080:ST131122 ACP131080:ACP131122 AML131080:AML131122 AWH131080:AWH131122 BGD131080:BGD131122 BPZ131080:BPZ131122 BZV131080:BZV131122 CJR131080:CJR131122 CTN131080:CTN131122 DDJ131080:DDJ131122 DNF131080:DNF131122 DXB131080:DXB131122 EGX131080:EGX131122 EQT131080:EQT131122 FAP131080:FAP131122 FKL131080:FKL131122 FUH131080:FUH131122 GED131080:GED131122 GNZ131080:GNZ131122 GXV131080:GXV131122 HHR131080:HHR131122 HRN131080:HRN131122 IBJ131080:IBJ131122 ILF131080:ILF131122 IVB131080:IVB131122 JEX131080:JEX131122 JOT131080:JOT131122 JYP131080:JYP131122 KIL131080:KIL131122 KSH131080:KSH131122 LCD131080:LCD131122 LLZ131080:LLZ131122 LVV131080:LVV131122 MFR131080:MFR131122 MPN131080:MPN131122 MZJ131080:MZJ131122 NJF131080:NJF131122 NTB131080:NTB131122 OCX131080:OCX131122 OMT131080:OMT131122 OWP131080:OWP131122 PGL131080:PGL131122 PQH131080:PQH131122 QAD131080:QAD131122 QJZ131080:QJZ131122 QTV131080:QTV131122 RDR131080:RDR131122 RNN131080:RNN131122 RXJ131080:RXJ131122 SHF131080:SHF131122 SRB131080:SRB131122 TAX131080:TAX131122 TKT131080:TKT131122 TUP131080:TUP131122 UEL131080:UEL131122 UOH131080:UOH131122 UYD131080:UYD131122 VHZ131080:VHZ131122 VRV131080:VRV131122 WBR131080:WBR131122 WLN131080:WLN131122 WVJ131080:WVJ131122 B196616:B196658 IX196616:IX196658 ST196616:ST196658 ACP196616:ACP196658 AML196616:AML196658 AWH196616:AWH196658 BGD196616:BGD196658 BPZ196616:BPZ196658 BZV196616:BZV196658 CJR196616:CJR196658 CTN196616:CTN196658 DDJ196616:DDJ196658 DNF196616:DNF196658 DXB196616:DXB196658 EGX196616:EGX196658 EQT196616:EQT196658 FAP196616:FAP196658 FKL196616:FKL196658 FUH196616:FUH196658 GED196616:GED196658 GNZ196616:GNZ196658 GXV196616:GXV196658 HHR196616:HHR196658 HRN196616:HRN196658 IBJ196616:IBJ196658 ILF196616:ILF196658 IVB196616:IVB196658 JEX196616:JEX196658 JOT196616:JOT196658 JYP196616:JYP196658 KIL196616:KIL196658 KSH196616:KSH196658 LCD196616:LCD196658 LLZ196616:LLZ196658 LVV196616:LVV196658 MFR196616:MFR196658 MPN196616:MPN196658 MZJ196616:MZJ196658 NJF196616:NJF196658 NTB196616:NTB196658 OCX196616:OCX196658 OMT196616:OMT196658 OWP196616:OWP196658 PGL196616:PGL196658 PQH196616:PQH196658 QAD196616:QAD196658 QJZ196616:QJZ196658 QTV196616:QTV196658 RDR196616:RDR196658 RNN196616:RNN196658 RXJ196616:RXJ196658 SHF196616:SHF196658 SRB196616:SRB196658 TAX196616:TAX196658 TKT196616:TKT196658 TUP196616:TUP196658 UEL196616:UEL196658 UOH196616:UOH196658 UYD196616:UYD196658 VHZ196616:VHZ196658 VRV196616:VRV196658 WBR196616:WBR196658 WLN196616:WLN196658 WVJ196616:WVJ196658 B262152:B262194 IX262152:IX262194 ST262152:ST262194 ACP262152:ACP262194 AML262152:AML262194 AWH262152:AWH262194 BGD262152:BGD262194 BPZ262152:BPZ262194 BZV262152:BZV262194 CJR262152:CJR262194 CTN262152:CTN262194 DDJ262152:DDJ262194 DNF262152:DNF262194 DXB262152:DXB262194 EGX262152:EGX262194 EQT262152:EQT262194 FAP262152:FAP262194 FKL262152:FKL262194 FUH262152:FUH262194 GED262152:GED262194 GNZ262152:GNZ262194 GXV262152:GXV262194 HHR262152:HHR262194 HRN262152:HRN262194 IBJ262152:IBJ262194 ILF262152:ILF262194 IVB262152:IVB262194 JEX262152:JEX262194 JOT262152:JOT262194 JYP262152:JYP262194 KIL262152:KIL262194 KSH262152:KSH262194 LCD262152:LCD262194 LLZ262152:LLZ262194 LVV262152:LVV262194 MFR262152:MFR262194 MPN262152:MPN262194 MZJ262152:MZJ262194 NJF262152:NJF262194 NTB262152:NTB262194 OCX262152:OCX262194 OMT262152:OMT262194 OWP262152:OWP262194 PGL262152:PGL262194 PQH262152:PQH262194 QAD262152:QAD262194 QJZ262152:QJZ262194 QTV262152:QTV262194 RDR262152:RDR262194 RNN262152:RNN262194 RXJ262152:RXJ262194 SHF262152:SHF262194 SRB262152:SRB262194 TAX262152:TAX262194 TKT262152:TKT262194 TUP262152:TUP262194 UEL262152:UEL262194 UOH262152:UOH262194 UYD262152:UYD262194 VHZ262152:VHZ262194 VRV262152:VRV262194 WBR262152:WBR262194 WLN262152:WLN262194 WVJ262152:WVJ262194 B327688:B327730 IX327688:IX327730 ST327688:ST327730 ACP327688:ACP327730 AML327688:AML327730 AWH327688:AWH327730 BGD327688:BGD327730 BPZ327688:BPZ327730 BZV327688:BZV327730 CJR327688:CJR327730 CTN327688:CTN327730 DDJ327688:DDJ327730 DNF327688:DNF327730 DXB327688:DXB327730 EGX327688:EGX327730 EQT327688:EQT327730 FAP327688:FAP327730 FKL327688:FKL327730 FUH327688:FUH327730 GED327688:GED327730 GNZ327688:GNZ327730 GXV327688:GXV327730 HHR327688:HHR327730 HRN327688:HRN327730 IBJ327688:IBJ327730 ILF327688:ILF327730 IVB327688:IVB327730 JEX327688:JEX327730 JOT327688:JOT327730 JYP327688:JYP327730 KIL327688:KIL327730 KSH327688:KSH327730 LCD327688:LCD327730 LLZ327688:LLZ327730 LVV327688:LVV327730 MFR327688:MFR327730 MPN327688:MPN327730 MZJ327688:MZJ327730 NJF327688:NJF327730 NTB327688:NTB327730 OCX327688:OCX327730 OMT327688:OMT327730 OWP327688:OWP327730 PGL327688:PGL327730 PQH327688:PQH327730 QAD327688:QAD327730 QJZ327688:QJZ327730 QTV327688:QTV327730 RDR327688:RDR327730 RNN327688:RNN327730 RXJ327688:RXJ327730 SHF327688:SHF327730 SRB327688:SRB327730 TAX327688:TAX327730 TKT327688:TKT327730 TUP327688:TUP327730 UEL327688:UEL327730 UOH327688:UOH327730 UYD327688:UYD327730 VHZ327688:VHZ327730 VRV327688:VRV327730 WBR327688:WBR327730 WLN327688:WLN327730 WVJ327688:WVJ327730 B393224:B393266 IX393224:IX393266 ST393224:ST393266 ACP393224:ACP393266 AML393224:AML393266 AWH393224:AWH393266 BGD393224:BGD393266 BPZ393224:BPZ393266 BZV393224:BZV393266 CJR393224:CJR393266 CTN393224:CTN393266 DDJ393224:DDJ393266 DNF393224:DNF393266 DXB393224:DXB393266 EGX393224:EGX393266 EQT393224:EQT393266 FAP393224:FAP393266 FKL393224:FKL393266 FUH393224:FUH393266 GED393224:GED393266 GNZ393224:GNZ393266 GXV393224:GXV393266 HHR393224:HHR393266 HRN393224:HRN393266 IBJ393224:IBJ393266 ILF393224:ILF393266 IVB393224:IVB393266 JEX393224:JEX393266 JOT393224:JOT393266 JYP393224:JYP393266 KIL393224:KIL393266 KSH393224:KSH393266 LCD393224:LCD393266 LLZ393224:LLZ393266 LVV393224:LVV393266 MFR393224:MFR393266 MPN393224:MPN393266 MZJ393224:MZJ393266 NJF393224:NJF393266 NTB393224:NTB393266 OCX393224:OCX393266 OMT393224:OMT393266 OWP393224:OWP393266 PGL393224:PGL393266 PQH393224:PQH393266 QAD393224:QAD393266 QJZ393224:QJZ393266 QTV393224:QTV393266 RDR393224:RDR393266 RNN393224:RNN393266 RXJ393224:RXJ393266 SHF393224:SHF393266 SRB393224:SRB393266 TAX393224:TAX393266 TKT393224:TKT393266 TUP393224:TUP393266 UEL393224:UEL393266 UOH393224:UOH393266 UYD393224:UYD393266 VHZ393224:VHZ393266 VRV393224:VRV393266 WBR393224:WBR393266 WLN393224:WLN393266 WVJ393224:WVJ393266 B458760:B458802 IX458760:IX458802 ST458760:ST458802 ACP458760:ACP458802 AML458760:AML458802 AWH458760:AWH458802 BGD458760:BGD458802 BPZ458760:BPZ458802 BZV458760:BZV458802 CJR458760:CJR458802 CTN458760:CTN458802 DDJ458760:DDJ458802 DNF458760:DNF458802 DXB458760:DXB458802 EGX458760:EGX458802 EQT458760:EQT458802 FAP458760:FAP458802 FKL458760:FKL458802 FUH458760:FUH458802 GED458760:GED458802 GNZ458760:GNZ458802 GXV458760:GXV458802 HHR458760:HHR458802 HRN458760:HRN458802 IBJ458760:IBJ458802 ILF458760:ILF458802 IVB458760:IVB458802 JEX458760:JEX458802 JOT458760:JOT458802 JYP458760:JYP458802 KIL458760:KIL458802 KSH458760:KSH458802 LCD458760:LCD458802 LLZ458760:LLZ458802 LVV458760:LVV458802 MFR458760:MFR458802 MPN458760:MPN458802 MZJ458760:MZJ458802 NJF458760:NJF458802 NTB458760:NTB458802 OCX458760:OCX458802 OMT458760:OMT458802 OWP458760:OWP458802 PGL458760:PGL458802 PQH458760:PQH458802 QAD458760:QAD458802 QJZ458760:QJZ458802 QTV458760:QTV458802 RDR458760:RDR458802 RNN458760:RNN458802 RXJ458760:RXJ458802 SHF458760:SHF458802 SRB458760:SRB458802 TAX458760:TAX458802 TKT458760:TKT458802 TUP458760:TUP458802 UEL458760:UEL458802 UOH458760:UOH458802 UYD458760:UYD458802 VHZ458760:VHZ458802 VRV458760:VRV458802 WBR458760:WBR458802 WLN458760:WLN458802 WVJ458760:WVJ458802 B524296:B524338 IX524296:IX524338 ST524296:ST524338 ACP524296:ACP524338 AML524296:AML524338 AWH524296:AWH524338 BGD524296:BGD524338 BPZ524296:BPZ524338 BZV524296:BZV524338 CJR524296:CJR524338 CTN524296:CTN524338 DDJ524296:DDJ524338 DNF524296:DNF524338 DXB524296:DXB524338 EGX524296:EGX524338 EQT524296:EQT524338 FAP524296:FAP524338 FKL524296:FKL524338 FUH524296:FUH524338 GED524296:GED524338 GNZ524296:GNZ524338 GXV524296:GXV524338 HHR524296:HHR524338 HRN524296:HRN524338 IBJ524296:IBJ524338 ILF524296:ILF524338 IVB524296:IVB524338 JEX524296:JEX524338 JOT524296:JOT524338 JYP524296:JYP524338 KIL524296:KIL524338 KSH524296:KSH524338 LCD524296:LCD524338 LLZ524296:LLZ524338 LVV524296:LVV524338 MFR524296:MFR524338 MPN524296:MPN524338 MZJ524296:MZJ524338 NJF524296:NJF524338 NTB524296:NTB524338 OCX524296:OCX524338 OMT524296:OMT524338 OWP524296:OWP524338 PGL524296:PGL524338 PQH524296:PQH524338 QAD524296:QAD524338 QJZ524296:QJZ524338 QTV524296:QTV524338 RDR524296:RDR524338 RNN524296:RNN524338 RXJ524296:RXJ524338 SHF524296:SHF524338 SRB524296:SRB524338 TAX524296:TAX524338 TKT524296:TKT524338 TUP524296:TUP524338 UEL524296:UEL524338 UOH524296:UOH524338 UYD524296:UYD524338 VHZ524296:VHZ524338 VRV524296:VRV524338 WBR524296:WBR524338 WLN524296:WLN524338 WVJ524296:WVJ524338 B589832:B589874 IX589832:IX589874 ST589832:ST589874 ACP589832:ACP589874 AML589832:AML589874 AWH589832:AWH589874 BGD589832:BGD589874 BPZ589832:BPZ589874 BZV589832:BZV589874 CJR589832:CJR589874 CTN589832:CTN589874 DDJ589832:DDJ589874 DNF589832:DNF589874 DXB589832:DXB589874 EGX589832:EGX589874 EQT589832:EQT589874 FAP589832:FAP589874 FKL589832:FKL589874 FUH589832:FUH589874 GED589832:GED589874 GNZ589832:GNZ589874 GXV589832:GXV589874 HHR589832:HHR589874 HRN589832:HRN589874 IBJ589832:IBJ589874 ILF589832:ILF589874 IVB589832:IVB589874 JEX589832:JEX589874 JOT589832:JOT589874 JYP589832:JYP589874 KIL589832:KIL589874 KSH589832:KSH589874 LCD589832:LCD589874 LLZ589832:LLZ589874 LVV589832:LVV589874 MFR589832:MFR589874 MPN589832:MPN589874 MZJ589832:MZJ589874 NJF589832:NJF589874 NTB589832:NTB589874 OCX589832:OCX589874 OMT589832:OMT589874 OWP589832:OWP589874 PGL589832:PGL589874 PQH589832:PQH589874 QAD589832:QAD589874 QJZ589832:QJZ589874 QTV589832:QTV589874 RDR589832:RDR589874 RNN589832:RNN589874 RXJ589832:RXJ589874 SHF589832:SHF589874 SRB589832:SRB589874 TAX589832:TAX589874 TKT589832:TKT589874 TUP589832:TUP589874 UEL589832:UEL589874 UOH589832:UOH589874 UYD589832:UYD589874 VHZ589832:VHZ589874 VRV589832:VRV589874 WBR589832:WBR589874 WLN589832:WLN589874 WVJ589832:WVJ589874 B655368:B655410 IX655368:IX655410 ST655368:ST655410 ACP655368:ACP655410 AML655368:AML655410 AWH655368:AWH655410 BGD655368:BGD655410 BPZ655368:BPZ655410 BZV655368:BZV655410 CJR655368:CJR655410 CTN655368:CTN655410 DDJ655368:DDJ655410 DNF655368:DNF655410 DXB655368:DXB655410 EGX655368:EGX655410 EQT655368:EQT655410 FAP655368:FAP655410 FKL655368:FKL655410 FUH655368:FUH655410 GED655368:GED655410 GNZ655368:GNZ655410 GXV655368:GXV655410 HHR655368:HHR655410 HRN655368:HRN655410 IBJ655368:IBJ655410 ILF655368:ILF655410 IVB655368:IVB655410 JEX655368:JEX655410 JOT655368:JOT655410 JYP655368:JYP655410 KIL655368:KIL655410 KSH655368:KSH655410 LCD655368:LCD655410 LLZ655368:LLZ655410 LVV655368:LVV655410 MFR655368:MFR655410 MPN655368:MPN655410 MZJ655368:MZJ655410 NJF655368:NJF655410 NTB655368:NTB655410 OCX655368:OCX655410 OMT655368:OMT655410 OWP655368:OWP655410 PGL655368:PGL655410 PQH655368:PQH655410 QAD655368:QAD655410 QJZ655368:QJZ655410 QTV655368:QTV655410 RDR655368:RDR655410 RNN655368:RNN655410 RXJ655368:RXJ655410 SHF655368:SHF655410 SRB655368:SRB655410 TAX655368:TAX655410 TKT655368:TKT655410 TUP655368:TUP655410 UEL655368:UEL655410 UOH655368:UOH655410 UYD655368:UYD655410 VHZ655368:VHZ655410 VRV655368:VRV655410 WBR655368:WBR655410 WLN655368:WLN655410 WVJ655368:WVJ655410 B720904:B720946 IX720904:IX720946 ST720904:ST720946 ACP720904:ACP720946 AML720904:AML720946 AWH720904:AWH720946 BGD720904:BGD720946 BPZ720904:BPZ720946 BZV720904:BZV720946 CJR720904:CJR720946 CTN720904:CTN720946 DDJ720904:DDJ720946 DNF720904:DNF720946 DXB720904:DXB720946 EGX720904:EGX720946 EQT720904:EQT720946 FAP720904:FAP720946 FKL720904:FKL720946 FUH720904:FUH720946 GED720904:GED720946 GNZ720904:GNZ720946 GXV720904:GXV720946 HHR720904:HHR720946 HRN720904:HRN720946 IBJ720904:IBJ720946 ILF720904:ILF720946 IVB720904:IVB720946 JEX720904:JEX720946 JOT720904:JOT720946 JYP720904:JYP720946 KIL720904:KIL720946 KSH720904:KSH720946 LCD720904:LCD720946 LLZ720904:LLZ720946 LVV720904:LVV720946 MFR720904:MFR720946 MPN720904:MPN720946 MZJ720904:MZJ720946 NJF720904:NJF720946 NTB720904:NTB720946 OCX720904:OCX720946 OMT720904:OMT720946 OWP720904:OWP720946 PGL720904:PGL720946 PQH720904:PQH720946 QAD720904:QAD720946 QJZ720904:QJZ720946 QTV720904:QTV720946 RDR720904:RDR720946 RNN720904:RNN720946 RXJ720904:RXJ720946 SHF720904:SHF720946 SRB720904:SRB720946 TAX720904:TAX720946 TKT720904:TKT720946 TUP720904:TUP720946 UEL720904:UEL720946 UOH720904:UOH720946 UYD720904:UYD720946 VHZ720904:VHZ720946 VRV720904:VRV720946 WBR720904:WBR720946 WLN720904:WLN720946 WVJ720904:WVJ720946 B786440:B786482 IX786440:IX786482 ST786440:ST786482 ACP786440:ACP786482 AML786440:AML786482 AWH786440:AWH786482 BGD786440:BGD786482 BPZ786440:BPZ786482 BZV786440:BZV786482 CJR786440:CJR786482 CTN786440:CTN786482 DDJ786440:DDJ786482 DNF786440:DNF786482 DXB786440:DXB786482 EGX786440:EGX786482 EQT786440:EQT786482 FAP786440:FAP786482 FKL786440:FKL786482 FUH786440:FUH786482 GED786440:GED786482 GNZ786440:GNZ786482 GXV786440:GXV786482 HHR786440:HHR786482 HRN786440:HRN786482 IBJ786440:IBJ786482 ILF786440:ILF786482 IVB786440:IVB786482 JEX786440:JEX786482 JOT786440:JOT786482 JYP786440:JYP786482 KIL786440:KIL786482 KSH786440:KSH786482 LCD786440:LCD786482 LLZ786440:LLZ786482 LVV786440:LVV786482 MFR786440:MFR786482 MPN786440:MPN786482 MZJ786440:MZJ786482 NJF786440:NJF786482 NTB786440:NTB786482 OCX786440:OCX786482 OMT786440:OMT786482 OWP786440:OWP786482 PGL786440:PGL786482 PQH786440:PQH786482 QAD786440:QAD786482 QJZ786440:QJZ786482 QTV786440:QTV786482 RDR786440:RDR786482 RNN786440:RNN786482 RXJ786440:RXJ786482 SHF786440:SHF786482 SRB786440:SRB786482 TAX786440:TAX786482 TKT786440:TKT786482 TUP786440:TUP786482 UEL786440:UEL786482 UOH786440:UOH786482 UYD786440:UYD786482 VHZ786440:VHZ786482 VRV786440:VRV786482 WBR786440:WBR786482 WLN786440:WLN786482 WVJ786440:WVJ786482 B851976:B852018 IX851976:IX852018 ST851976:ST852018 ACP851976:ACP852018 AML851976:AML852018 AWH851976:AWH852018 BGD851976:BGD852018 BPZ851976:BPZ852018 BZV851976:BZV852018 CJR851976:CJR852018 CTN851976:CTN852018 DDJ851976:DDJ852018 DNF851976:DNF852018 DXB851976:DXB852018 EGX851976:EGX852018 EQT851976:EQT852018 FAP851976:FAP852018 FKL851976:FKL852018 FUH851976:FUH852018 GED851976:GED852018 GNZ851976:GNZ852018 GXV851976:GXV852018 HHR851976:HHR852018 HRN851976:HRN852018 IBJ851976:IBJ852018 ILF851976:ILF852018 IVB851976:IVB852018 JEX851976:JEX852018 JOT851976:JOT852018 JYP851976:JYP852018 KIL851976:KIL852018 KSH851976:KSH852018 LCD851976:LCD852018 LLZ851976:LLZ852018 LVV851976:LVV852018 MFR851976:MFR852018 MPN851976:MPN852018 MZJ851976:MZJ852018 NJF851976:NJF852018 NTB851976:NTB852018 OCX851976:OCX852018 OMT851976:OMT852018 OWP851976:OWP852018 PGL851976:PGL852018 PQH851976:PQH852018 QAD851976:QAD852018 QJZ851976:QJZ852018 QTV851976:QTV852018 RDR851976:RDR852018 RNN851976:RNN852018 RXJ851976:RXJ852018 SHF851976:SHF852018 SRB851976:SRB852018 TAX851976:TAX852018 TKT851976:TKT852018 TUP851976:TUP852018 UEL851976:UEL852018 UOH851976:UOH852018 UYD851976:UYD852018 VHZ851976:VHZ852018 VRV851976:VRV852018 WBR851976:WBR852018 WLN851976:WLN852018 WVJ851976:WVJ852018 B917512:B917554 IX917512:IX917554 ST917512:ST917554 ACP917512:ACP917554 AML917512:AML917554 AWH917512:AWH917554 BGD917512:BGD917554 BPZ917512:BPZ917554 BZV917512:BZV917554 CJR917512:CJR917554 CTN917512:CTN917554 DDJ917512:DDJ917554 DNF917512:DNF917554 DXB917512:DXB917554 EGX917512:EGX917554 EQT917512:EQT917554 FAP917512:FAP917554 FKL917512:FKL917554 FUH917512:FUH917554 GED917512:GED917554 GNZ917512:GNZ917554 GXV917512:GXV917554 HHR917512:HHR917554 HRN917512:HRN917554 IBJ917512:IBJ917554 ILF917512:ILF917554 IVB917512:IVB917554 JEX917512:JEX917554 JOT917512:JOT917554 JYP917512:JYP917554 KIL917512:KIL917554 KSH917512:KSH917554 LCD917512:LCD917554 LLZ917512:LLZ917554 LVV917512:LVV917554 MFR917512:MFR917554 MPN917512:MPN917554 MZJ917512:MZJ917554 NJF917512:NJF917554 NTB917512:NTB917554 OCX917512:OCX917554 OMT917512:OMT917554 OWP917512:OWP917554 PGL917512:PGL917554 PQH917512:PQH917554 QAD917512:QAD917554 QJZ917512:QJZ917554 QTV917512:QTV917554 RDR917512:RDR917554 RNN917512:RNN917554 RXJ917512:RXJ917554 SHF917512:SHF917554 SRB917512:SRB917554 TAX917512:TAX917554 TKT917512:TKT917554 TUP917512:TUP917554 UEL917512:UEL917554 UOH917512:UOH917554 UYD917512:UYD917554 VHZ917512:VHZ917554 VRV917512:VRV917554 WBR917512:WBR917554 WLN917512:WLN917554 WVJ917512:WVJ917554 B983048:B983090 IX983048:IX983090 ST983048:ST983090 ACP983048:ACP983090 AML983048:AML983090 AWH983048:AWH983090 BGD983048:BGD983090 BPZ983048:BPZ983090 BZV983048:BZV983090 CJR983048:CJR983090 CTN983048:CTN983090 DDJ983048:DDJ983090 DNF983048:DNF983090 DXB983048:DXB983090 EGX983048:EGX983090 EQT983048:EQT983090 FAP983048:FAP983090 FKL983048:FKL983090 FUH983048:FUH983090 GED983048:GED983090 GNZ983048:GNZ983090 GXV983048:GXV983090 HHR983048:HHR983090 HRN983048:HRN983090 IBJ983048:IBJ983090 ILF983048:ILF983090 IVB983048:IVB983090 JEX983048:JEX983090 JOT983048:JOT983090 JYP983048:JYP983090 KIL983048:KIL983090 KSH983048:KSH983090 LCD983048:LCD983090 LLZ983048:LLZ983090 LVV983048:LVV983090 MFR983048:MFR983090 MPN983048:MPN983090 MZJ983048:MZJ983090 NJF983048:NJF983090 NTB983048:NTB983090 OCX983048:OCX983090 OMT983048:OMT983090 OWP983048:OWP983090 PGL983048:PGL983090 PQH983048:PQH983090 QAD983048:QAD983090 QJZ983048:QJZ983090 QTV983048:QTV983090 RDR983048:RDR983090 RNN983048:RNN983090 RXJ983048:RXJ983090 SHF983048:SHF983090 SRB983048:SRB983090 TAX983048:TAX983090 TKT983048:TKT983090 TUP983048:TUP983090 UEL983048:UEL983090 UOH983048:UOH983090 UYD983048:UYD983090 VHZ983048:VHZ983090 VRV983048:VRV983090 WBR983048:WBR983090 WLN983048:WLN983090 WVJ983048:WVJ983090">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B50 IX8:IX50 ST8:ST50 ACP8:ACP50 AML8:AML50 AWH8:AWH50 BGD8:BGD50 BPZ8:BPZ50 BZV8:BZV50 CJR8:CJR50 CTN8:CTN50 DDJ8:DDJ50 DNF8:DNF50 DXB8:DXB50 EGX8:EGX50 EQT8:EQT50 FAP8:FAP50 FKL8:FKL50 FUH8:FUH50 GED8:GED50 GNZ8:GNZ50 GXV8:GXV50 HHR8:HHR50 HRN8:HRN50 IBJ8:IBJ50 ILF8:ILF50 IVB8:IVB50 JEX8:JEX50 JOT8:JOT50 JYP8:JYP50 KIL8:KIL50 KSH8:KSH50 LCD8:LCD50 LLZ8:LLZ50 LVV8:LVV50 MFR8:MFR50 MPN8:MPN50 MZJ8:MZJ50 NJF8:NJF50 NTB8:NTB50 OCX8:OCX50 OMT8:OMT50 OWP8:OWP50 PGL8:PGL50 PQH8:PQH50 QAD8:QAD50 QJZ8:QJZ50 QTV8:QTV50 RDR8:RDR50 RNN8:RNN50 RXJ8:RXJ50 SHF8:SHF50 SRB8:SRB50 TAX8:TAX50 TKT8:TKT50 TUP8:TUP50 UEL8:UEL50 UOH8:UOH50 UYD8:UYD50 VHZ8:VHZ50 VRV8:VRV50 WBR8:WBR50 WLN8:WLN50 WVJ8:WVJ50 B65544:B65586 IX65544:IX65586 ST65544:ST65586 ACP65544:ACP65586 AML65544:AML65586 AWH65544:AWH65586 BGD65544:BGD65586 BPZ65544:BPZ65586 BZV65544:BZV65586 CJR65544:CJR65586 CTN65544:CTN65586 DDJ65544:DDJ65586 DNF65544:DNF65586 DXB65544:DXB65586 EGX65544:EGX65586 EQT65544:EQT65586 FAP65544:FAP65586 FKL65544:FKL65586 FUH65544:FUH65586 GED65544:GED65586 GNZ65544:GNZ65586 GXV65544:GXV65586 HHR65544:HHR65586 HRN65544:HRN65586 IBJ65544:IBJ65586 ILF65544:ILF65586 IVB65544:IVB65586 JEX65544:JEX65586 JOT65544:JOT65586 JYP65544:JYP65586 KIL65544:KIL65586 KSH65544:KSH65586 LCD65544:LCD65586 LLZ65544:LLZ65586 LVV65544:LVV65586 MFR65544:MFR65586 MPN65544:MPN65586 MZJ65544:MZJ65586 NJF65544:NJF65586 NTB65544:NTB65586 OCX65544:OCX65586 OMT65544:OMT65586 OWP65544:OWP65586 PGL65544:PGL65586 PQH65544:PQH65586 QAD65544:QAD65586 QJZ65544:QJZ65586 QTV65544:QTV65586 RDR65544:RDR65586 RNN65544:RNN65586 RXJ65544:RXJ65586 SHF65544:SHF65586 SRB65544:SRB65586 TAX65544:TAX65586 TKT65544:TKT65586 TUP65544:TUP65586 UEL65544:UEL65586 UOH65544:UOH65586 UYD65544:UYD65586 VHZ65544:VHZ65586 VRV65544:VRV65586 WBR65544:WBR65586 WLN65544:WLN65586 WVJ65544:WVJ65586 B131080:B131122 IX131080:IX131122 ST131080:ST131122 ACP131080:ACP131122 AML131080:AML131122 AWH131080:AWH131122 BGD131080:BGD131122 BPZ131080:BPZ131122 BZV131080:BZV131122 CJR131080:CJR131122 CTN131080:CTN131122 DDJ131080:DDJ131122 DNF131080:DNF131122 DXB131080:DXB131122 EGX131080:EGX131122 EQT131080:EQT131122 FAP131080:FAP131122 FKL131080:FKL131122 FUH131080:FUH131122 GED131080:GED131122 GNZ131080:GNZ131122 GXV131080:GXV131122 HHR131080:HHR131122 HRN131080:HRN131122 IBJ131080:IBJ131122 ILF131080:ILF131122 IVB131080:IVB131122 JEX131080:JEX131122 JOT131080:JOT131122 JYP131080:JYP131122 KIL131080:KIL131122 KSH131080:KSH131122 LCD131080:LCD131122 LLZ131080:LLZ131122 LVV131080:LVV131122 MFR131080:MFR131122 MPN131080:MPN131122 MZJ131080:MZJ131122 NJF131080:NJF131122 NTB131080:NTB131122 OCX131080:OCX131122 OMT131080:OMT131122 OWP131080:OWP131122 PGL131080:PGL131122 PQH131080:PQH131122 QAD131080:QAD131122 QJZ131080:QJZ131122 QTV131080:QTV131122 RDR131080:RDR131122 RNN131080:RNN131122 RXJ131080:RXJ131122 SHF131080:SHF131122 SRB131080:SRB131122 TAX131080:TAX131122 TKT131080:TKT131122 TUP131080:TUP131122 UEL131080:UEL131122 UOH131080:UOH131122 UYD131080:UYD131122 VHZ131080:VHZ131122 VRV131080:VRV131122 WBR131080:WBR131122 WLN131080:WLN131122 WVJ131080:WVJ131122 B196616:B196658 IX196616:IX196658 ST196616:ST196658 ACP196616:ACP196658 AML196616:AML196658 AWH196616:AWH196658 BGD196616:BGD196658 BPZ196616:BPZ196658 BZV196616:BZV196658 CJR196616:CJR196658 CTN196616:CTN196658 DDJ196616:DDJ196658 DNF196616:DNF196658 DXB196616:DXB196658 EGX196616:EGX196658 EQT196616:EQT196658 FAP196616:FAP196658 FKL196616:FKL196658 FUH196616:FUH196658 GED196616:GED196658 GNZ196616:GNZ196658 GXV196616:GXV196658 HHR196616:HHR196658 HRN196616:HRN196658 IBJ196616:IBJ196658 ILF196616:ILF196658 IVB196616:IVB196658 JEX196616:JEX196658 JOT196616:JOT196658 JYP196616:JYP196658 KIL196616:KIL196658 KSH196616:KSH196658 LCD196616:LCD196658 LLZ196616:LLZ196658 LVV196616:LVV196658 MFR196616:MFR196658 MPN196616:MPN196658 MZJ196616:MZJ196658 NJF196616:NJF196658 NTB196616:NTB196658 OCX196616:OCX196658 OMT196616:OMT196658 OWP196616:OWP196658 PGL196616:PGL196658 PQH196616:PQH196658 QAD196616:QAD196658 QJZ196616:QJZ196658 QTV196616:QTV196658 RDR196616:RDR196658 RNN196616:RNN196658 RXJ196616:RXJ196658 SHF196616:SHF196658 SRB196616:SRB196658 TAX196616:TAX196658 TKT196616:TKT196658 TUP196616:TUP196658 UEL196616:UEL196658 UOH196616:UOH196658 UYD196616:UYD196658 VHZ196616:VHZ196658 VRV196616:VRV196658 WBR196616:WBR196658 WLN196616:WLN196658 WVJ196616:WVJ196658 B262152:B262194 IX262152:IX262194 ST262152:ST262194 ACP262152:ACP262194 AML262152:AML262194 AWH262152:AWH262194 BGD262152:BGD262194 BPZ262152:BPZ262194 BZV262152:BZV262194 CJR262152:CJR262194 CTN262152:CTN262194 DDJ262152:DDJ262194 DNF262152:DNF262194 DXB262152:DXB262194 EGX262152:EGX262194 EQT262152:EQT262194 FAP262152:FAP262194 FKL262152:FKL262194 FUH262152:FUH262194 GED262152:GED262194 GNZ262152:GNZ262194 GXV262152:GXV262194 HHR262152:HHR262194 HRN262152:HRN262194 IBJ262152:IBJ262194 ILF262152:ILF262194 IVB262152:IVB262194 JEX262152:JEX262194 JOT262152:JOT262194 JYP262152:JYP262194 KIL262152:KIL262194 KSH262152:KSH262194 LCD262152:LCD262194 LLZ262152:LLZ262194 LVV262152:LVV262194 MFR262152:MFR262194 MPN262152:MPN262194 MZJ262152:MZJ262194 NJF262152:NJF262194 NTB262152:NTB262194 OCX262152:OCX262194 OMT262152:OMT262194 OWP262152:OWP262194 PGL262152:PGL262194 PQH262152:PQH262194 QAD262152:QAD262194 QJZ262152:QJZ262194 QTV262152:QTV262194 RDR262152:RDR262194 RNN262152:RNN262194 RXJ262152:RXJ262194 SHF262152:SHF262194 SRB262152:SRB262194 TAX262152:TAX262194 TKT262152:TKT262194 TUP262152:TUP262194 UEL262152:UEL262194 UOH262152:UOH262194 UYD262152:UYD262194 VHZ262152:VHZ262194 VRV262152:VRV262194 WBR262152:WBR262194 WLN262152:WLN262194 WVJ262152:WVJ262194 B327688:B327730 IX327688:IX327730 ST327688:ST327730 ACP327688:ACP327730 AML327688:AML327730 AWH327688:AWH327730 BGD327688:BGD327730 BPZ327688:BPZ327730 BZV327688:BZV327730 CJR327688:CJR327730 CTN327688:CTN327730 DDJ327688:DDJ327730 DNF327688:DNF327730 DXB327688:DXB327730 EGX327688:EGX327730 EQT327688:EQT327730 FAP327688:FAP327730 FKL327688:FKL327730 FUH327688:FUH327730 GED327688:GED327730 GNZ327688:GNZ327730 GXV327688:GXV327730 HHR327688:HHR327730 HRN327688:HRN327730 IBJ327688:IBJ327730 ILF327688:ILF327730 IVB327688:IVB327730 JEX327688:JEX327730 JOT327688:JOT327730 JYP327688:JYP327730 KIL327688:KIL327730 KSH327688:KSH327730 LCD327688:LCD327730 LLZ327688:LLZ327730 LVV327688:LVV327730 MFR327688:MFR327730 MPN327688:MPN327730 MZJ327688:MZJ327730 NJF327688:NJF327730 NTB327688:NTB327730 OCX327688:OCX327730 OMT327688:OMT327730 OWP327688:OWP327730 PGL327688:PGL327730 PQH327688:PQH327730 QAD327688:QAD327730 QJZ327688:QJZ327730 QTV327688:QTV327730 RDR327688:RDR327730 RNN327688:RNN327730 RXJ327688:RXJ327730 SHF327688:SHF327730 SRB327688:SRB327730 TAX327688:TAX327730 TKT327688:TKT327730 TUP327688:TUP327730 UEL327688:UEL327730 UOH327688:UOH327730 UYD327688:UYD327730 VHZ327688:VHZ327730 VRV327688:VRV327730 WBR327688:WBR327730 WLN327688:WLN327730 WVJ327688:WVJ327730 B393224:B393266 IX393224:IX393266 ST393224:ST393266 ACP393224:ACP393266 AML393224:AML393266 AWH393224:AWH393266 BGD393224:BGD393266 BPZ393224:BPZ393266 BZV393224:BZV393266 CJR393224:CJR393266 CTN393224:CTN393266 DDJ393224:DDJ393266 DNF393224:DNF393266 DXB393224:DXB393266 EGX393224:EGX393266 EQT393224:EQT393266 FAP393224:FAP393266 FKL393224:FKL393266 FUH393224:FUH393266 GED393224:GED393266 GNZ393224:GNZ393266 GXV393224:GXV393266 HHR393224:HHR393266 HRN393224:HRN393266 IBJ393224:IBJ393266 ILF393224:ILF393266 IVB393224:IVB393266 JEX393224:JEX393266 JOT393224:JOT393266 JYP393224:JYP393266 KIL393224:KIL393266 KSH393224:KSH393266 LCD393224:LCD393266 LLZ393224:LLZ393266 LVV393224:LVV393266 MFR393224:MFR393266 MPN393224:MPN393266 MZJ393224:MZJ393266 NJF393224:NJF393266 NTB393224:NTB393266 OCX393224:OCX393266 OMT393224:OMT393266 OWP393224:OWP393266 PGL393224:PGL393266 PQH393224:PQH393266 QAD393224:QAD393266 QJZ393224:QJZ393266 QTV393224:QTV393266 RDR393224:RDR393266 RNN393224:RNN393266 RXJ393224:RXJ393266 SHF393224:SHF393266 SRB393224:SRB393266 TAX393224:TAX393266 TKT393224:TKT393266 TUP393224:TUP393266 UEL393224:UEL393266 UOH393224:UOH393266 UYD393224:UYD393266 VHZ393224:VHZ393266 VRV393224:VRV393266 WBR393224:WBR393266 WLN393224:WLN393266 WVJ393224:WVJ393266 B458760:B458802 IX458760:IX458802 ST458760:ST458802 ACP458760:ACP458802 AML458760:AML458802 AWH458760:AWH458802 BGD458760:BGD458802 BPZ458760:BPZ458802 BZV458760:BZV458802 CJR458760:CJR458802 CTN458760:CTN458802 DDJ458760:DDJ458802 DNF458760:DNF458802 DXB458760:DXB458802 EGX458760:EGX458802 EQT458760:EQT458802 FAP458760:FAP458802 FKL458760:FKL458802 FUH458760:FUH458802 GED458760:GED458802 GNZ458760:GNZ458802 GXV458760:GXV458802 HHR458760:HHR458802 HRN458760:HRN458802 IBJ458760:IBJ458802 ILF458760:ILF458802 IVB458760:IVB458802 JEX458760:JEX458802 JOT458760:JOT458802 JYP458760:JYP458802 KIL458760:KIL458802 KSH458760:KSH458802 LCD458760:LCD458802 LLZ458760:LLZ458802 LVV458760:LVV458802 MFR458760:MFR458802 MPN458760:MPN458802 MZJ458760:MZJ458802 NJF458760:NJF458802 NTB458760:NTB458802 OCX458760:OCX458802 OMT458760:OMT458802 OWP458760:OWP458802 PGL458760:PGL458802 PQH458760:PQH458802 QAD458760:QAD458802 QJZ458760:QJZ458802 QTV458760:QTV458802 RDR458760:RDR458802 RNN458760:RNN458802 RXJ458760:RXJ458802 SHF458760:SHF458802 SRB458760:SRB458802 TAX458760:TAX458802 TKT458760:TKT458802 TUP458760:TUP458802 UEL458760:UEL458802 UOH458760:UOH458802 UYD458760:UYD458802 VHZ458760:VHZ458802 VRV458760:VRV458802 WBR458760:WBR458802 WLN458760:WLN458802 WVJ458760:WVJ458802 B524296:B524338 IX524296:IX524338 ST524296:ST524338 ACP524296:ACP524338 AML524296:AML524338 AWH524296:AWH524338 BGD524296:BGD524338 BPZ524296:BPZ524338 BZV524296:BZV524338 CJR524296:CJR524338 CTN524296:CTN524338 DDJ524296:DDJ524338 DNF524296:DNF524338 DXB524296:DXB524338 EGX524296:EGX524338 EQT524296:EQT524338 FAP524296:FAP524338 FKL524296:FKL524338 FUH524296:FUH524338 GED524296:GED524338 GNZ524296:GNZ524338 GXV524296:GXV524338 HHR524296:HHR524338 HRN524296:HRN524338 IBJ524296:IBJ524338 ILF524296:ILF524338 IVB524296:IVB524338 JEX524296:JEX524338 JOT524296:JOT524338 JYP524296:JYP524338 KIL524296:KIL524338 KSH524296:KSH524338 LCD524296:LCD524338 LLZ524296:LLZ524338 LVV524296:LVV524338 MFR524296:MFR524338 MPN524296:MPN524338 MZJ524296:MZJ524338 NJF524296:NJF524338 NTB524296:NTB524338 OCX524296:OCX524338 OMT524296:OMT524338 OWP524296:OWP524338 PGL524296:PGL524338 PQH524296:PQH524338 QAD524296:QAD524338 QJZ524296:QJZ524338 QTV524296:QTV524338 RDR524296:RDR524338 RNN524296:RNN524338 RXJ524296:RXJ524338 SHF524296:SHF524338 SRB524296:SRB524338 TAX524296:TAX524338 TKT524296:TKT524338 TUP524296:TUP524338 UEL524296:UEL524338 UOH524296:UOH524338 UYD524296:UYD524338 VHZ524296:VHZ524338 VRV524296:VRV524338 WBR524296:WBR524338 WLN524296:WLN524338 WVJ524296:WVJ524338 B589832:B589874 IX589832:IX589874 ST589832:ST589874 ACP589832:ACP589874 AML589832:AML589874 AWH589832:AWH589874 BGD589832:BGD589874 BPZ589832:BPZ589874 BZV589832:BZV589874 CJR589832:CJR589874 CTN589832:CTN589874 DDJ589832:DDJ589874 DNF589832:DNF589874 DXB589832:DXB589874 EGX589832:EGX589874 EQT589832:EQT589874 FAP589832:FAP589874 FKL589832:FKL589874 FUH589832:FUH589874 GED589832:GED589874 GNZ589832:GNZ589874 GXV589832:GXV589874 HHR589832:HHR589874 HRN589832:HRN589874 IBJ589832:IBJ589874 ILF589832:ILF589874 IVB589832:IVB589874 JEX589832:JEX589874 JOT589832:JOT589874 JYP589832:JYP589874 KIL589832:KIL589874 KSH589832:KSH589874 LCD589832:LCD589874 LLZ589832:LLZ589874 LVV589832:LVV589874 MFR589832:MFR589874 MPN589832:MPN589874 MZJ589832:MZJ589874 NJF589832:NJF589874 NTB589832:NTB589874 OCX589832:OCX589874 OMT589832:OMT589874 OWP589832:OWP589874 PGL589832:PGL589874 PQH589832:PQH589874 QAD589832:QAD589874 QJZ589832:QJZ589874 QTV589832:QTV589874 RDR589832:RDR589874 RNN589832:RNN589874 RXJ589832:RXJ589874 SHF589832:SHF589874 SRB589832:SRB589874 TAX589832:TAX589874 TKT589832:TKT589874 TUP589832:TUP589874 UEL589832:UEL589874 UOH589832:UOH589874 UYD589832:UYD589874 VHZ589832:VHZ589874 VRV589832:VRV589874 WBR589832:WBR589874 WLN589832:WLN589874 WVJ589832:WVJ589874 B655368:B655410 IX655368:IX655410 ST655368:ST655410 ACP655368:ACP655410 AML655368:AML655410 AWH655368:AWH655410 BGD655368:BGD655410 BPZ655368:BPZ655410 BZV655368:BZV655410 CJR655368:CJR655410 CTN655368:CTN655410 DDJ655368:DDJ655410 DNF655368:DNF655410 DXB655368:DXB655410 EGX655368:EGX655410 EQT655368:EQT655410 FAP655368:FAP655410 FKL655368:FKL655410 FUH655368:FUH655410 GED655368:GED655410 GNZ655368:GNZ655410 GXV655368:GXV655410 HHR655368:HHR655410 HRN655368:HRN655410 IBJ655368:IBJ655410 ILF655368:ILF655410 IVB655368:IVB655410 JEX655368:JEX655410 JOT655368:JOT655410 JYP655368:JYP655410 KIL655368:KIL655410 KSH655368:KSH655410 LCD655368:LCD655410 LLZ655368:LLZ655410 LVV655368:LVV655410 MFR655368:MFR655410 MPN655368:MPN655410 MZJ655368:MZJ655410 NJF655368:NJF655410 NTB655368:NTB655410 OCX655368:OCX655410 OMT655368:OMT655410 OWP655368:OWP655410 PGL655368:PGL655410 PQH655368:PQH655410 QAD655368:QAD655410 QJZ655368:QJZ655410 QTV655368:QTV655410 RDR655368:RDR655410 RNN655368:RNN655410 RXJ655368:RXJ655410 SHF655368:SHF655410 SRB655368:SRB655410 TAX655368:TAX655410 TKT655368:TKT655410 TUP655368:TUP655410 UEL655368:UEL655410 UOH655368:UOH655410 UYD655368:UYD655410 VHZ655368:VHZ655410 VRV655368:VRV655410 WBR655368:WBR655410 WLN655368:WLN655410 WVJ655368:WVJ655410 B720904:B720946 IX720904:IX720946 ST720904:ST720946 ACP720904:ACP720946 AML720904:AML720946 AWH720904:AWH720946 BGD720904:BGD720946 BPZ720904:BPZ720946 BZV720904:BZV720946 CJR720904:CJR720946 CTN720904:CTN720946 DDJ720904:DDJ720946 DNF720904:DNF720946 DXB720904:DXB720946 EGX720904:EGX720946 EQT720904:EQT720946 FAP720904:FAP720946 FKL720904:FKL720946 FUH720904:FUH720946 GED720904:GED720946 GNZ720904:GNZ720946 GXV720904:GXV720946 HHR720904:HHR720946 HRN720904:HRN720946 IBJ720904:IBJ720946 ILF720904:ILF720946 IVB720904:IVB720946 JEX720904:JEX720946 JOT720904:JOT720946 JYP720904:JYP720946 KIL720904:KIL720946 KSH720904:KSH720946 LCD720904:LCD720946 LLZ720904:LLZ720946 LVV720904:LVV720946 MFR720904:MFR720946 MPN720904:MPN720946 MZJ720904:MZJ720946 NJF720904:NJF720946 NTB720904:NTB720946 OCX720904:OCX720946 OMT720904:OMT720946 OWP720904:OWP720946 PGL720904:PGL720946 PQH720904:PQH720946 QAD720904:QAD720946 QJZ720904:QJZ720946 QTV720904:QTV720946 RDR720904:RDR720946 RNN720904:RNN720946 RXJ720904:RXJ720946 SHF720904:SHF720946 SRB720904:SRB720946 TAX720904:TAX720946 TKT720904:TKT720946 TUP720904:TUP720946 UEL720904:UEL720946 UOH720904:UOH720946 UYD720904:UYD720946 VHZ720904:VHZ720946 VRV720904:VRV720946 WBR720904:WBR720946 WLN720904:WLN720946 WVJ720904:WVJ720946 B786440:B786482 IX786440:IX786482 ST786440:ST786482 ACP786440:ACP786482 AML786440:AML786482 AWH786440:AWH786482 BGD786440:BGD786482 BPZ786440:BPZ786482 BZV786440:BZV786482 CJR786440:CJR786482 CTN786440:CTN786482 DDJ786440:DDJ786482 DNF786440:DNF786482 DXB786440:DXB786482 EGX786440:EGX786482 EQT786440:EQT786482 FAP786440:FAP786482 FKL786440:FKL786482 FUH786440:FUH786482 GED786440:GED786482 GNZ786440:GNZ786482 GXV786440:GXV786482 HHR786440:HHR786482 HRN786440:HRN786482 IBJ786440:IBJ786482 ILF786440:ILF786482 IVB786440:IVB786482 JEX786440:JEX786482 JOT786440:JOT786482 JYP786440:JYP786482 KIL786440:KIL786482 KSH786440:KSH786482 LCD786440:LCD786482 LLZ786440:LLZ786482 LVV786440:LVV786482 MFR786440:MFR786482 MPN786440:MPN786482 MZJ786440:MZJ786482 NJF786440:NJF786482 NTB786440:NTB786482 OCX786440:OCX786482 OMT786440:OMT786482 OWP786440:OWP786482 PGL786440:PGL786482 PQH786440:PQH786482 QAD786440:QAD786482 QJZ786440:QJZ786482 QTV786440:QTV786482 RDR786440:RDR786482 RNN786440:RNN786482 RXJ786440:RXJ786482 SHF786440:SHF786482 SRB786440:SRB786482 TAX786440:TAX786482 TKT786440:TKT786482 TUP786440:TUP786482 UEL786440:UEL786482 UOH786440:UOH786482 UYD786440:UYD786482 VHZ786440:VHZ786482 VRV786440:VRV786482 WBR786440:WBR786482 WLN786440:WLN786482 WVJ786440:WVJ786482 B851976:B852018 IX851976:IX852018 ST851976:ST852018 ACP851976:ACP852018 AML851976:AML852018 AWH851976:AWH852018 BGD851976:BGD852018 BPZ851976:BPZ852018 BZV851976:BZV852018 CJR851976:CJR852018 CTN851976:CTN852018 DDJ851976:DDJ852018 DNF851976:DNF852018 DXB851976:DXB852018 EGX851976:EGX852018 EQT851976:EQT852018 FAP851976:FAP852018 FKL851976:FKL852018 FUH851976:FUH852018 GED851976:GED852018 GNZ851976:GNZ852018 GXV851976:GXV852018 HHR851976:HHR852018 HRN851976:HRN852018 IBJ851976:IBJ852018 ILF851976:ILF852018 IVB851976:IVB852018 JEX851976:JEX852018 JOT851976:JOT852018 JYP851976:JYP852018 KIL851976:KIL852018 KSH851976:KSH852018 LCD851976:LCD852018 LLZ851976:LLZ852018 LVV851976:LVV852018 MFR851976:MFR852018 MPN851976:MPN852018 MZJ851976:MZJ852018 NJF851976:NJF852018 NTB851976:NTB852018 OCX851976:OCX852018 OMT851976:OMT852018 OWP851976:OWP852018 PGL851976:PGL852018 PQH851976:PQH852018 QAD851976:QAD852018 QJZ851976:QJZ852018 QTV851976:QTV852018 RDR851976:RDR852018 RNN851976:RNN852018 RXJ851976:RXJ852018 SHF851976:SHF852018 SRB851976:SRB852018 TAX851976:TAX852018 TKT851976:TKT852018 TUP851976:TUP852018 UEL851976:UEL852018 UOH851976:UOH852018 UYD851976:UYD852018 VHZ851976:VHZ852018 VRV851976:VRV852018 WBR851976:WBR852018 WLN851976:WLN852018 WVJ851976:WVJ852018 B917512:B917554 IX917512:IX917554 ST917512:ST917554 ACP917512:ACP917554 AML917512:AML917554 AWH917512:AWH917554 BGD917512:BGD917554 BPZ917512:BPZ917554 BZV917512:BZV917554 CJR917512:CJR917554 CTN917512:CTN917554 DDJ917512:DDJ917554 DNF917512:DNF917554 DXB917512:DXB917554 EGX917512:EGX917554 EQT917512:EQT917554 FAP917512:FAP917554 FKL917512:FKL917554 FUH917512:FUH917554 GED917512:GED917554 GNZ917512:GNZ917554 GXV917512:GXV917554 HHR917512:HHR917554 HRN917512:HRN917554 IBJ917512:IBJ917554 ILF917512:ILF917554 IVB917512:IVB917554 JEX917512:JEX917554 JOT917512:JOT917554 JYP917512:JYP917554 KIL917512:KIL917554 KSH917512:KSH917554 LCD917512:LCD917554 LLZ917512:LLZ917554 LVV917512:LVV917554 MFR917512:MFR917554 MPN917512:MPN917554 MZJ917512:MZJ917554 NJF917512:NJF917554 NTB917512:NTB917554 OCX917512:OCX917554 OMT917512:OMT917554 OWP917512:OWP917554 PGL917512:PGL917554 PQH917512:PQH917554 QAD917512:QAD917554 QJZ917512:QJZ917554 QTV917512:QTV917554 RDR917512:RDR917554 RNN917512:RNN917554 RXJ917512:RXJ917554 SHF917512:SHF917554 SRB917512:SRB917554 TAX917512:TAX917554 TKT917512:TKT917554 TUP917512:TUP917554 UEL917512:UEL917554 UOH917512:UOH917554 UYD917512:UYD917554 VHZ917512:VHZ917554 VRV917512:VRV917554 WBR917512:WBR917554 WLN917512:WLN917554 WVJ917512:WVJ917554 B983048:B983090 IX983048:IX983090 ST983048:ST983090 ACP983048:ACP983090 AML983048:AML983090 AWH983048:AWH983090 BGD983048:BGD983090 BPZ983048:BPZ983090 BZV983048:BZV983090 CJR983048:CJR983090 CTN983048:CTN983090 DDJ983048:DDJ983090 DNF983048:DNF983090 DXB983048:DXB983090 EGX983048:EGX983090 EQT983048:EQT983090 FAP983048:FAP983090 FKL983048:FKL983090 FUH983048:FUH983090 GED983048:GED983090 GNZ983048:GNZ983090 GXV983048:GXV983090 HHR983048:HHR983090 HRN983048:HRN983090 IBJ983048:IBJ983090 ILF983048:ILF983090 IVB983048:IVB983090 JEX983048:JEX983090 JOT983048:JOT983090 JYP983048:JYP983090 KIL983048:KIL983090 KSH983048:KSH983090 LCD983048:LCD983090 LLZ983048:LLZ983090 LVV983048:LVV983090 MFR983048:MFR983090 MPN983048:MPN983090 MZJ983048:MZJ983090 NJF983048:NJF983090 NTB983048:NTB983090 OCX983048:OCX983090 OMT983048:OMT983090 OWP983048:OWP983090 PGL983048:PGL983090 PQH983048:PQH983090 QAD983048:QAD983090 QJZ983048:QJZ983090 QTV983048:QTV983090 RDR983048:RDR983090 RNN983048:RNN983090 RXJ983048:RXJ983090 SHF983048:SHF983090 SRB983048:SRB983090 TAX983048:TAX983090 TKT983048:TKT983090 TUP983048:TUP983090 UEL983048:UEL983090 UOH983048:UOH983090 UYD983048:UYD983090 VHZ983048:VHZ983090 VRV983048:VRV983090 WBR983048:WBR983090 WLN983048:WLN983090 WVJ983048:WVJ983090" xr:uid="{A2926E5D-23AC-49E6-871D-24C174CBC328}">
       <formula1>8</formula1>
       <formula2>8</formula2>
     </dataValidation>
@@ -8962,530 +9009,530 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB299"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370F73DA-448C-4452-A197-9E365B49E20F}">
+  <dimension ref="A1:AB300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="21" width="2.7109375" style="8" customWidth="1"/>
-    <col min="22" max="22" width="4.42578125" style="8" customWidth="1"/>
-    <col min="23" max="23" width="7.42578125" style="8" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="256" width="11.42578125" style="1"/>
-    <col min="257" max="257" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="21" width="2.7265625" style="8" customWidth="1"/>
+    <col min="22" max="22" width="4.453125" style="8" customWidth="1"/>
+    <col min="23" max="23" width="7.453125" style="8" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="256" width="11.453125" style="1"/>
+    <col min="257" max="257" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="260" max="277" width="2.7109375" style="1" customWidth="1"/>
-    <col min="278" max="278" width="4.42578125" style="1" customWidth="1"/>
+    <col min="260" max="277" width="2.7265625" style="1" customWidth="1"/>
+    <col min="278" max="278" width="4.453125" style="1" customWidth="1"/>
     <col min="279" max="279" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="280" max="280" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="281" max="512" width="11.42578125" style="1"/>
-    <col min="513" max="513" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="281" max="512" width="11.453125" style="1"/>
+    <col min="513" max="513" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="515" max="515" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="516" max="533" width="2.7109375" style="1" customWidth="1"/>
-    <col min="534" max="534" width="4.42578125" style="1" customWidth="1"/>
+    <col min="516" max="533" width="2.7265625" style="1" customWidth="1"/>
+    <col min="534" max="534" width="4.453125" style="1" customWidth="1"/>
     <col min="535" max="535" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="536" max="536" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="537" max="768" width="11.42578125" style="1"/>
-    <col min="769" max="769" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="536" max="536" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="537" max="768" width="11.453125" style="1"/>
+    <col min="769" max="769" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="771" max="771" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="772" max="789" width="2.7109375" style="1" customWidth="1"/>
-    <col min="790" max="790" width="4.42578125" style="1" customWidth="1"/>
+    <col min="772" max="789" width="2.7265625" style="1" customWidth="1"/>
+    <col min="790" max="790" width="4.453125" style="1" customWidth="1"/>
     <col min="791" max="791" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="792" max="792" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="793" max="1024" width="11.42578125" style="1"/>
-    <col min="1025" max="1025" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="792" max="792" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="793" max="1024" width="11.453125" style="1"/>
+    <col min="1025" max="1025" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1027" max="1027" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1045" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1046" max="1046" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1028" max="1045" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1046" max="1046" width="4.453125" style="1" customWidth="1"/>
     <col min="1047" max="1047" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1048" max="1048" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1049" max="1280" width="11.42578125" style="1"/>
-    <col min="1281" max="1281" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1048" max="1048" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1049" max="1280" width="11.453125" style="1"/>
+    <col min="1281" max="1281" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1283" max="1283" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1301" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1302" max="1302" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1284" max="1301" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1302" max="1302" width="4.453125" style="1" customWidth="1"/>
     <col min="1303" max="1303" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1304" max="1304" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1305" max="1536" width="11.42578125" style="1"/>
-    <col min="1537" max="1537" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1304" max="1304" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1305" max="1536" width="11.453125" style="1"/>
+    <col min="1537" max="1537" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1539" max="1539" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1557" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1558" max="1558" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1540" max="1557" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1558" max="1558" width="4.453125" style="1" customWidth="1"/>
     <col min="1559" max="1559" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1560" max="1560" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1561" max="1792" width="11.42578125" style="1"/>
-    <col min="1793" max="1793" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1560" max="1560" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1561" max="1792" width="11.453125" style="1"/>
+    <col min="1793" max="1793" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1795" max="1795" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1813" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1814" max="1814" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1796" max="1813" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1814" max="1814" width="4.453125" style="1" customWidth="1"/>
     <col min="1815" max="1815" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1816" max="1816" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1817" max="2048" width="11.42578125" style="1"/>
-    <col min="2049" max="2049" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1816" max="1816" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1817" max="2048" width="11.453125" style="1"/>
+    <col min="2049" max="2049" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2051" max="2051" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2069" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2070" max="2070" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2052" max="2069" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2070" max="2070" width="4.453125" style="1" customWidth="1"/>
     <col min="2071" max="2071" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2072" max="2072" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2073" max="2304" width="11.42578125" style="1"/>
-    <col min="2305" max="2305" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2072" max="2072" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2073" max="2304" width="11.453125" style="1"/>
+    <col min="2305" max="2305" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2307" max="2307" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2325" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2326" max="2326" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2308" max="2325" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2326" max="2326" width="4.453125" style="1" customWidth="1"/>
     <col min="2327" max="2327" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2328" max="2328" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2329" max="2560" width="11.42578125" style="1"/>
-    <col min="2561" max="2561" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2328" max="2328" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2329" max="2560" width="11.453125" style="1"/>
+    <col min="2561" max="2561" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2563" max="2563" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2581" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2582" max="2582" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2564" max="2581" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2582" max="2582" width="4.453125" style="1" customWidth="1"/>
     <col min="2583" max="2583" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2584" max="2584" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2585" max="2816" width="11.42578125" style="1"/>
-    <col min="2817" max="2817" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2584" max="2584" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2585" max="2816" width="11.453125" style="1"/>
+    <col min="2817" max="2817" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2819" max="2819" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2837" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2838" max="2838" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2820" max="2837" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2838" max="2838" width="4.453125" style="1" customWidth="1"/>
     <col min="2839" max="2839" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2840" max="2840" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2841" max="3072" width="11.42578125" style="1"/>
-    <col min="3073" max="3073" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2840" max="2840" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2841" max="3072" width="11.453125" style="1"/>
+    <col min="3073" max="3073" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3075" max="3075" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3093" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3094" max="3094" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3076" max="3093" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3094" max="3094" width="4.453125" style="1" customWidth="1"/>
     <col min="3095" max="3095" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3096" max="3096" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3097" max="3328" width="11.42578125" style="1"/>
-    <col min="3329" max="3329" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3096" max="3096" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3097" max="3328" width="11.453125" style="1"/>
+    <col min="3329" max="3329" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3331" max="3331" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3349" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3350" max="3350" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3332" max="3349" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3350" max="3350" width="4.453125" style="1" customWidth="1"/>
     <col min="3351" max="3351" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3352" max="3352" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3353" max="3584" width="11.42578125" style="1"/>
-    <col min="3585" max="3585" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3352" max="3352" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3353" max="3584" width="11.453125" style="1"/>
+    <col min="3585" max="3585" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3587" max="3587" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3605" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3606" max="3606" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3588" max="3605" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3606" max="3606" width="4.453125" style="1" customWidth="1"/>
     <col min="3607" max="3607" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3608" max="3608" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3609" max="3840" width="11.42578125" style="1"/>
-    <col min="3841" max="3841" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3608" max="3608" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3609" max="3840" width="11.453125" style="1"/>
+    <col min="3841" max="3841" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3843" max="3843" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3861" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3862" max="3862" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3844" max="3861" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3862" max="3862" width="4.453125" style="1" customWidth="1"/>
     <col min="3863" max="3863" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3864" max="3864" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3865" max="4096" width="11.42578125" style="1"/>
-    <col min="4097" max="4097" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3864" max="3864" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3865" max="4096" width="11.453125" style="1"/>
+    <col min="4097" max="4097" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4099" max="4099" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4117" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4118" max="4118" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4100" max="4117" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4118" max="4118" width="4.453125" style="1" customWidth="1"/>
     <col min="4119" max="4119" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4120" max="4120" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4121" max="4352" width="11.42578125" style="1"/>
-    <col min="4353" max="4353" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4120" max="4120" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4121" max="4352" width="11.453125" style="1"/>
+    <col min="4353" max="4353" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4355" max="4355" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4373" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4374" max="4374" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4356" max="4373" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4374" max="4374" width="4.453125" style="1" customWidth="1"/>
     <col min="4375" max="4375" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4376" max="4376" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4377" max="4608" width="11.42578125" style="1"/>
-    <col min="4609" max="4609" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4376" max="4376" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4377" max="4608" width="11.453125" style="1"/>
+    <col min="4609" max="4609" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4611" max="4611" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4629" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4630" max="4630" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4612" max="4629" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4630" max="4630" width="4.453125" style="1" customWidth="1"/>
     <col min="4631" max="4631" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4632" max="4632" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4633" max="4864" width="11.42578125" style="1"/>
-    <col min="4865" max="4865" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4632" max="4632" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4633" max="4864" width="11.453125" style="1"/>
+    <col min="4865" max="4865" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4867" max="4867" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4885" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4886" max="4886" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4868" max="4885" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4886" max="4886" width="4.453125" style="1" customWidth="1"/>
     <col min="4887" max="4887" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4888" max="4888" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4889" max="5120" width="11.42578125" style="1"/>
-    <col min="5121" max="5121" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4888" max="4888" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4889" max="5120" width="11.453125" style="1"/>
+    <col min="5121" max="5121" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5123" max="5123" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5141" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5142" max="5142" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5124" max="5141" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5142" max="5142" width="4.453125" style="1" customWidth="1"/>
     <col min="5143" max="5143" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5144" max="5144" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5145" max="5376" width="11.42578125" style="1"/>
-    <col min="5377" max="5377" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5144" max="5144" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5145" max="5376" width="11.453125" style="1"/>
+    <col min="5377" max="5377" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5379" max="5379" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5397" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5398" max="5398" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5380" max="5397" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5398" max="5398" width="4.453125" style="1" customWidth="1"/>
     <col min="5399" max="5399" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5400" max="5400" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5401" max="5632" width="11.42578125" style="1"/>
-    <col min="5633" max="5633" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5400" max="5400" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5401" max="5632" width="11.453125" style="1"/>
+    <col min="5633" max="5633" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5635" max="5635" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5653" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5654" max="5654" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5636" max="5653" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5654" max="5654" width="4.453125" style="1" customWidth="1"/>
     <col min="5655" max="5655" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5656" max="5656" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5657" max="5888" width="11.42578125" style="1"/>
-    <col min="5889" max="5889" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5656" max="5656" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5657" max="5888" width="11.453125" style="1"/>
+    <col min="5889" max="5889" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5891" max="5891" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5909" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5910" max="5910" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5892" max="5909" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5910" max="5910" width="4.453125" style="1" customWidth="1"/>
     <col min="5911" max="5911" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5912" max="5912" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5913" max="6144" width="11.42578125" style="1"/>
-    <col min="6145" max="6145" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5912" max="5912" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5913" max="6144" width="11.453125" style="1"/>
+    <col min="6145" max="6145" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6147" max="6147" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6165" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6166" max="6166" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6148" max="6165" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6166" max="6166" width="4.453125" style="1" customWidth="1"/>
     <col min="6167" max="6167" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6168" max="6168" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6169" max="6400" width="11.42578125" style="1"/>
-    <col min="6401" max="6401" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6168" max="6168" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6169" max="6400" width="11.453125" style="1"/>
+    <col min="6401" max="6401" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6403" max="6403" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6421" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6422" max="6422" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6404" max="6421" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6422" max="6422" width="4.453125" style="1" customWidth="1"/>
     <col min="6423" max="6423" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6424" max="6424" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6425" max="6656" width="11.42578125" style="1"/>
-    <col min="6657" max="6657" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6424" max="6424" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6425" max="6656" width="11.453125" style="1"/>
+    <col min="6657" max="6657" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6659" max="6659" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6677" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6678" max="6678" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6660" max="6677" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6678" max="6678" width="4.453125" style="1" customWidth="1"/>
     <col min="6679" max="6679" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6680" max="6680" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6681" max="6912" width="11.42578125" style="1"/>
-    <col min="6913" max="6913" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6680" max="6680" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6681" max="6912" width="11.453125" style="1"/>
+    <col min="6913" max="6913" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6915" max="6915" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6933" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6934" max="6934" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6916" max="6933" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6934" max="6934" width="4.453125" style="1" customWidth="1"/>
     <col min="6935" max="6935" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6936" max="6936" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6937" max="7168" width="11.42578125" style="1"/>
-    <col min="7169" max="7169" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6936" max="6936" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6937" max="7168" width="11.453125" style="1"/>
+    <col min="7169" max="7169" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7171" max="7171" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7189" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7190" max="7190" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7172" max="7189" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7190" max="7190" width="4.453125" style="1" customWidth="1"/>
     <col min="7191" max="7191" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7192" max="7192" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7193" max="7424" width="11.42578125" style="1"/>
-    <col min="7425" max="7425" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7192" max="7192" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7193" max="7424" width="11.453125" style="1"/>
+    <col min="7425" max="7425" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7427" max="7427" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7445" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7446" max="7446" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7428" max="7445" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7446" max="7446" width="4.453125" style="1" customWidth="1"/>
     <col min="7447" max="7447" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7448" max="7448" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7449" max="7680" width="11.42578125" style="1"/>
-    <col min="7681" max="7681" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7448" max="7448" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7449" max="7680" width="11.453125" style="1"/>
+    <col min="7681" max="7681" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7683" max="7683" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7701" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7702" max="7702" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7684" max="7701" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7702" max="7702" width="4.453125" style="1" customWidth="1"/>
     <col min="7703" max="7703" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7704" max="7704" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7705" max="7936" width="11.42578125" style="1"/>
-    <col min="7937" max="7937" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7704" max="7704" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7705" max="7936" width="11.453125" style="1"/>
+    <col min="7937" max="7937" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7939" max="7939" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7957" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7958" max="7958" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7940" max="7957" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7958" max="7958" width="4.453125" style="1" customWidth="1"/>
     <col min="7959" max="7959" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7960" max="7960" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7961" max="8192" width="11.42578125" style="1"/>
-    <col min="8193" max="8193" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7960" max="7960" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7961" max="8192" width="11.453125" style="1"/>
+    <col min="8193" max="8193" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8195" max="8195" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8213" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8214" max="8214" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8196" max="8213" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8214" max="8214" width="4.453125" style="1" customWidth="1"/>
     <col min="8215" max="8215" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8216" max="8216" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8217" max="8448" width="11.42578125" style="1"/>
-    <col min="8449" max="8449" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8216" max="8216" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8217" max="8448" width="11.453125" style="1"/>
+    <col min="8449" max="8449" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8451" max="8451" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8469" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8470" max="8470" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8452" max="8469" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8470" max="8470" width="4.453125" style="1" customWidth="1"/>
     <col min="8471" max="8471" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8472" max="8472" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8473" max="8704" width="11.42578125" style="1"/>
-    <col min="8705" max="8705" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8472" max="8472" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8473" max="8704" width="11.453125" style="1"/>
+    <col min="8705" max="8705" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8707" max="8707" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8725" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8726" max="8726" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8708" max="8725" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8726" max="8726" width="4.453125" style="1" customWidth="1"/>
     <col min="8727" max="8727" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8728" max="8728" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8729" max="8960" width="11.42578125" style="1"/>
-    <col min="8961" max="8961" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8728" max="8728" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8729" max="8960" width="11.453125" style="1"/>
+    <col min="8961" max="8961" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8963" max="8963" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8981" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8982" max="8982" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8964" max="8981" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8982" max="8982" width="4.453125" style="1" customWidth="1"/>
     <col min="8983" max="8983" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8984" max="8984" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8985" max="9216" width="11.42578125" style="1"/>
-    <col min="9217" max="9217" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8984" max="8984" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8985" max="9216" width="11.453125" style="1"/>
+    <col min="9217" max="9217" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9219" max="9219" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9237" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9238" max="9238" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9220" max="9237" width="2.7265625" style="1" customWidth="1"/>
+    <col min="9238" max="9238" width="4.453125" style="1" customWidth="1"/>
     <col min="9239" max="9239" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9240" max="9240" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9241" max="9472" width="11.42578125" style="1"/>
-    <col min="9473" max="9473" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9240" max="9240" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9241" max="9472" width="11.453125" style="1"/>
+    <col min="9473" max="9473" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9475" max="9475" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9493" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9494" max="9494" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9476" max="9493" width="2.7265625" style="1" customWidth="1"/>
+    <col min="9494" max="9494" width="4.453125" style="1" customWidth="1"/>
     <col min="9495" max="9495" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9496" max="9496" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9497" max="9728" width="11.42578125" style="1"/>
-    <col min="9729" max="9729" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9496" max="9496" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9497" max="9728" width="11.453125" style="1"/>
+    <col min="9729" max="9729" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9731" max="9731" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9749" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9750" max="9750" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9732" max="9749" width="2.7265625" style="1" customWidth="1"/>
+    <col min="9750" max="9750" width="4.453125" style="1" customWidth="1"/>
     <col min="9751" max="9751" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9752" max="9752" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9753" max="9984" width="11.42578125" style="1"/>
-    <col min="9985" max="9985" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9752" max="9752" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9753" max="9984" width="11.453125" style="1"/>
+    <col min="9985" max="9985" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9987" max="9987" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9988" max="10005" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10006" max="10006" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9988" max="10005" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10006" max="10006" width="4.453125" style="1" customWidth="1"/>
     <col min="10007" max="10007" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10008" max="10008" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10009" max="10240" width="11.42578125" style="1"/>
-    <col min="10241" max="10241" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10008" max="10008" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10009" max="10240" width="11.453125" style="1"/>
+    <col min="10241" max="10241" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10243" max="10243" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10261" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10262" max="10262" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10244" max="10261" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10262" max="10262" width="4.453125" style="1" customWidth="1"/>
     <col min="10263" max="10263" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10264" max="10264" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10265" max="10496" width="11.42578125" style="1"/>
-    <col min="10497" max="10497" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10264" max="10264" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10265" max="10496" width="11.453125" style="1"/>
+    <col min="10497" max="10497" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10499" max="10499" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10517" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10518" max="10518" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10500" max="10517" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10518" max="10518" width="4.453125" style="1" customWidth="1"/>
     <col min="10519" max="10519" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10520" max="10520" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10521" max="10752" width="11.42578125" style="1"/>
-    <col min="10753" max="10753" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10520" max="10520" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10521" max="10752" width="11.453125" style="1"/>
+    <col min="10753" max="10753" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10755" max="10755" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10773" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10774" max="10774" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10756" max="10773" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10774" max="10774" width="4.453125" style="1" customWidth="1"/>
     <col min="10775" max="10775" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10776" max="10776" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10777" max="11008" width="11.42578125" style="1"/>
-    <col min="11009" max="11009" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10776" max="10776" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10777" max="11008" width="11.453125" style="1"/>
+    <col min="11009" max="11009" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11011" max="11011" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11029" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11030" max="11030" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11012" max="11029" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11030" max="11030" width="4.453125" style="1" customWidth="1"/>
     <col min="11031" max="11031" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11032" max="11032" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11033" max="11264" width="11.42578125" style="1"/>
-    <col min="11265" max="11265" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11032" max="11032" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11033" max="11264" width="11.453125" style="1"/>
+    <col min="11265" max="11265" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11267" max="11267" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11285" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11286" max="11286" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11268" max="11285" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11286" max="11286" width="4.453125" style="1" customWidth="1"/>
     <col min="11287" max="11287" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11288" max="11288" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11289" max="11520" width="11.42578125" style="1"/>
-    <col min="11521" max="11521" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11288" max="11288" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11289" max="11520" width="11.453125" style="1"/>
+    <col min="11521" max="11521" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11523" max="11523" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11541" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11542" max="11542" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11524" max="11541" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11542" max="11542" width="4.453125" style="1" customWidth="1"/>
     <col min="11543" max="11543" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11544" max="11544" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11545" max="11776" width="11.42578125" style="1"/>
-    <col min="11777" max="11777" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11544" max="11544" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11545" max="11776" width="11.453125" style="1"/>
+    <col min="11777" max="11777" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11779" max="11779" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11797" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11798" max="11798" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11780" max="11797" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11798" max="11798" width="4.453125" style="1" customWidth="1"/>
     <col min="11799" max="11799" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11800" max="11800" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11801" max="12032" width="11.42578125" style="1"/>
-    <col min="12033" max="12033" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11800" max="11800" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11801" max="12032" width="11.453125" style="1"/>
+    <col min="12033" max="12033" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12035" max="12035" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12053" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12054" max="12054" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12036" max="12053" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12054" max="12054" width="4.453125" style="1" customWidth="1"/>
     <col min="12055" max="12055" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12056" max="12056" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12057" max="12288" width="11.42578125" style="1"/>
-    <col min="12289" max="12289" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12056" max="12056" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12057" max="12288" width="11.453125" style="1"/>
+    <col min="12289" max="12289" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12291" max="12291" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12309" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12310" max="12310" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12292" max="12309" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12310" max="12310" width="4.453125" style="1" customWidth="1"/>
     <col min="12311" max="12311" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12312" max="12312" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12313" max="12544" width="11.42578125" style="1"/>
-    <col min="12545" max="12545" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12312" max="12312" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12313" max="12544" width="11.453125" style="1"/>
+    <col min="12545" max="12545" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12547" max="12547" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12565" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12566" max="12566" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12548" max="12565" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12566" max="12566" width="4.453125" style="1" customWidth="1"/>
     <col min="12567" max="12567" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12568" max="12568" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12569" max="12800" width="11.42578125" style="1"/>
-    <col min="12801" max="12801" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12568" max="12568" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12569" max="12800" width="11.453125" style="1"/>
+    <col min="12801" max="12801" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12803" max="12803" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12821" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12822" max="12822" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12804" max="12821" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12822" max="12822" width="4.453125" style="1" customWidth="1"/>
     <col min="12823" max="12823" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12824" max="12824" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12825" max="13056" width="11.42578125" style="1"/>
-    <col min="13057" max="13057" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12824" max="12824" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12825" max="13056" width="11.453125" style="1"/>
+    <col min="13057" max="13057" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13059" max="13059" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13077" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13078" max="13078" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13060" max="13077" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13078" max="13078" width="4.453125" style="1" customWidth="1"/>
     <col min="13079" max="13079" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13080" max="13080" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13081" max="13312" width="11.42578125" style="1"/>
-    <col min="13313" max="13313" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13080" max="13080" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13081" max="13312" width="11.453125" style="1"/>
+    <col min="13313" max="13313" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13315" max="13315" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13333" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13334" max="13334" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13316" max="13333" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13334" max="13334" width="4.453125" style="1" customWidth="1"/>
     <col min="13335" max="13335" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13336" max="13336" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13337" max="13568" width="11.42578125" style="1"/>
-    <col min="13569" max="13569" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13336" max="13336" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13337" max="13568" width="11.453125" style="1"/>
+    <col min="13569" max="13569" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13571" max="13571" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13589" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13590" max="13590" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13572" max="13589" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13590" max="13590" width="4.453125" style="1" customWidth="1"/>
     <col min="13591" max="13591" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13592" max="13592" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13593" max="13824" width="11.42578125" style="1"/>
-    <col min="13825" max="13825" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13592" max="13592" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13593" max="13824" width="11.453125" style="1"/>
+    <col min="13825" max="13825" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13827" max="13827" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13845" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13846" max="13846" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13828" max="13845" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13846" max="13846" width="4.453125" style="1" customWidth="1"/>
     <col min="13847" max="13847" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13848" max="13848" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13849" max="14080" width="11.42578125" style="1"/>
-    <col min="14081" max="14081" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13848" max="13848" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13849" max="14080" width="11.453125" style="1"/>
+    <col min="14081" max="14081" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14083" max="14083" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14101" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14102" max="14102" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14084" max="14101" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14102" max="14102" width="4.453125" style="1" customWidth="1"/>
     <col min="14103" max="14103" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14104" max="14104" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14105" max="14336" width="11.42578125" style="1"/>
-    <col min="14337" max="14337" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14104" max="14104" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14105" max="14336" width="11.453125" style="1"/>
+    <col min="14337" max="14337" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14339" max="14339" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14357" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14358" max="14358" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14340" max="14357" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14358" max="14358" width="4.453125" style="1" customWidth="1"/>
     <col min="14359" max="14359" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14360" max="14360" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14361" max="14592" width="11.42578125" style="1"/>
-    <col min="14593" max="14593" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14360" max="14360" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14361" max="14592" width="11.453125" style="1"/>
+    <col min="14593" max="14593" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14595" max="14595" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14613" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14614" max="14614" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14596" max="14613" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14614" max="14614" width="4.453125" style="1" customWidth="1"/>
     <col min="14615" max="14615" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14616" max="14616" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14617" max="14848" width="11.42578125" style="1"/>
-    <col min="14849" max="14849" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14616" max="14616" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14617" max="14848" width="11.453125" style="1"/>
+    <col min="14849" max="14849" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14851" max="14851" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14869" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14870" max="14870" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14852" max="14869" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14870" max="14870" width="4.453125" style="1" customWidth="1"/>
     <col min="14871" max="14871" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14872" max="14872" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14873" max="15104" width="11.42578125" style="1"/>
-    <col min="15105" max="15105" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14872" max="14872" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14873" max="15104" width="11.453125" style="1"/>
+    <col min="15105" max="15105" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15107" max="15107" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15125" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15126" max="15126" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15108" max="15125" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15126" max="15126" width="4.453125" style="1" customWidth="1"/>
     <col min="15127" max="15127" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15128" max="15128" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15129" max="15360" width="11.42578125" style="1"/>
-    <col min="15361" max="15361" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15128" max="15128" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15129" max="15360" width="11.453125" style="1"/>
+    <col min="15361" max="15361" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15363" max="15363" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15381" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15382" max="15382" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15364" max="15381" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15382" max="15382" width="4.453125" style="1" customWidth="1"/>
     <col min="15383" max="15383" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15384" max="15384" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15385" max="15616" width="11.42578125" style="1"/>
-    <col min="15617" max="15617" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15384" max="15384" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15385" max="15616" width="11.453125" style="1"/>
+    <col min="15617" max="15617" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15619" max="15619" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15637" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15638" max="15638" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15620" max="15637" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15638" max="15638" width="4.453125" style="1" customWidth="1"/>
     <col min="15639" max="15639" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15640" max="15640" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15641" max="15872" width="11.42578125" style="1"/>
-    <col min="15873" max="15873" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15640" max="15640" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15641" max="15872" width="11.453125" style="1"/>
+    <col min="15873" max="15873" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15875" max="15875" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15893" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15894" max="15894" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15876" max="15893" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15894" max="15894" width="4.453125" style="1" customWidth="1"/>
     <col min="15895" max="15895" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15896" max="15896" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15897" max="16128" width="11.42578125" style="1"/>
-    <col min="16129" max="16129" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15896" max="15896" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15897" max="16128" width="11.453125" style="1"/>
+    <col min="16129" max="16129" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="16131" max="16131" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16149" width="2.7109375" style="1" customWidth="1"/>
-    <col min="16150" max="16150" width="4.42578125" style="1" customWidth="1"/>
+    <col min="16132" max="16149" width="2.7265625" style="1" customWidth="1"/>
+    <col min="16150" max="16150" width="4.453125" style="1" customWidth="1"/>
     <col min="16151" max="16151" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="16152" max="16152" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16153" max="16384" width="11.42578125" style="1"/>
+    <col min="16152" max="16152" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16153" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9519,7 +9566,7 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
     </row>
-    <row r="2" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -9549,7 +9596,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
     </row>
-    <row r="3" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -9579,7 +9626,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
     </row>
-    <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -9609,7 +9656,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -9617,7 +9664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -9700,7 +9747,7 @@
       </c>
       <c r="AB7" s="12"/>
     </row>
-    <row r="8" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -9850,7 +9897,7 @@
       </c>
       <c r="Y9" s="8"/>
     </row>
-    <row r="10" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -9925,7 +9972,7 @@
       </c>
       <c r="Y10" s="8"/>
     </row>
-    <row r="11" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -10000,7 +10047,7 @@
       </c>
       <c r="Y11" s="8"/>
     </row>
-    <row r="12" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -10075,7 +10122,7 @@
       </c>
       <c r="Y12" s="8"/>
     </row>
-    <row r="13" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -10150,7 +10197,7 @@
       </c>
       <c r="Y13" s="8"/>
     </row>
-    <row r="14" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>113</v>
       </c>
@@ -10225,7 +10272,7 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="15" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -10300,7 +10347,7 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="16" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -10375,7 +10422,7 @@
       </c>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -10450,7 +10497,7 @@
       </c>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>115</v>
       </c>
@@ -10600,7 +10647,7 @@
       </c>
       <c r="Y19" s="8"/>
     </row>
-    <row r="20" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>117</v>
       </c>
@@ -10750,7 +10797,7 @@
       </c>
       <c r="Y21" s="8"/>
     </row>
-    <row r="22" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -10825,7 +10872,7 @@
       </c>
       <c r="Y22" s="8"/>
     </row>
-    <row r="23" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -10900,7 +10947,7 @@
       </c>
       <c r="Y23" s="8"/>
     </row>
-    <row r="24" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -10975,7 +11022,7 @@
       </c>
       <c r="Y24" s="8"/>
     </row>
-    <row r="25" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>123</v>
       </c>
@@ -11050,7 +11097,7 @@
       </c>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
@@ -11427,10 +11474,10 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>203</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>71</v>
+        <v>202</v>
       </c>
       <c r="C31" s="8">
         <v>5.8</v>
@@ -11652,61 +11699,61 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>131</v>
+        <v>205</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>132</v>
+        <v>204</v>
       </c>
       <c r="C34" s="8">
-        <v>5.5</v>
+        <v>2.4</v>
       </c>
       <c r="D34" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E34" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F34" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G34" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H34" s="8">
+        <v>6</v>
+      </c>
+      <c r="I34" s="8">
+        <v>4</v>
+      </c>
+      <c r="J34" s="8">
+        <v>6</v>
+      </c>
+      <c r="K34" s="8">
+        <v>4</v>
+      </c>
+      <c r="L34" s="8">
         <v>7</v>
       </c>
-      <c r="I34" s="8">
-        <v>5</v>
-      </c>
-      <c r="J34" s="8">
-        <v>4</v>
-      </c>
-      <c r="K34" s="8">
-        <v>3</v>
-      </c>
-      <c r="L34" s="8">
-        <v>6</v>
-      </c>
       <c r="M34" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N34" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O34" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P34" s="8">
         <v>6</v>
       </c>
       <c r="Q34" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R34" s="8">
         <v>5</v>
       </c>
       <c r="S34" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T34" s="8">
         <v>4</v>
@@ -11718,7 +11765,7 @@
         <v>85</v>
       </c>
       <c r="W34" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="X34" s="8">
         <v>80</v>
@@ -11727,34 +11774,34 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C35" s="8">
-        <v>19.2</v>
+        <v>5.5</v>
       </c>
       <c r="D35" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E35" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" s="8">
         <v>5</v>
       </c>
       <c r="G35" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H35" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I35" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J35" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K35" s="8">
         <v>3</v>
@@ -11763,25 +11810,25 @@
         <v>6</v>
       </c>
       <c r="M35" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N35" s="8">
         <v>4</v>
       </c>
       <c r="O35" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P35" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q35" s="8">
         <v>4</v>
       </c>
       <c r="R35" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S35" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T35" s="8">
         <v>4</v>
@@ -11790,37 +11837,37 @@
         <v>5</v>
       </c>
       <c r="V35" s="8">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W35" s="1">
-        <v>-5</v>
+        <v>8</v>
       </c>
       <c r="X35" s="8">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Y35" s="8"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="C36" s="8">
-        <v>6.4</v>
+        <v>19.2</v>
       </c>
       <c r="D36" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E36" s="8">
         <v>5</v>
       </c>
       <c r="F36" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G36" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H36" s="8">
         <v>6</v>
@@ -11832,13 +11879,13 @@
         <v>5</v>
       </c>
       <c r="K36" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L36" s="8">
         <v>6</v>
       </c>
       <c r="M36" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N36" s="8">
         <v>4</v>
@@ -11850,52 +11897,52 @@
         <v>7</v>
       </c>
       <c r="Q36" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R36" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S36" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T36" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U36" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V36" s="8">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="W36" s="1">
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="X36" s="8">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Y36" s="8"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C37" s="8">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="D37" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E37" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F37" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G37" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H37" s="8">
         <v>6</v>
@@ -11907,7 +11954,7 @@
         <v>5</v>
       </c>
       <c r="K37" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L37" s="8">
         <v>6</v>
@@ -11919,7 +11966,7 @@
         <v>4</v>
       </c>
       <c r="O37" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P37" s="8">
         <v>7</v>
@@ -11928,45 +11975,46 @@
         <v>5</v>
       </c>
       <c r="R37" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S37" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T37" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U37" s="8">
         <v>6</v>
       </c>
       <c r="V37" s="8">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W37" s="1">
         <v>10</v>
       </c>
       <c r="X37" s="8">
-        <v>84</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="Y37" s="8"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>135</v>
+        <v>72</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>136</v>
+        <v>73</v>
       </c>
       <c r="C38" s="8">
-        <v>9.3000000000000007</v>
+        <v>6.9</v>
       </c>
       <c r="D38" s="8">
         <v>4</v>
       </c>
       <c r="E38" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F38" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G38" s="8">
         <v>5</v>
@@ -11975,28 +12023,28 @@
         <v>6</v>
       </c>
       <c r="I38" s="8">
+        <v>4</v>
+      </c>
+      <c r="J38" s="8">
+        <v>5</v>
+      </c>
+      <c r="K38" s="8">
+        <v>5</v>
+      </c>
+      <c r="L38" s="8">
+        <v>6</v>
+      </c>
+      <c r="M38" s="8">
+        <v>5</v>
+      </c>
+      <c r="N38" s="8">
+        <v>4</v>
+      </c>
+      <c r="O38" s="8">
+        <v>4</v>
+      </c>
+      <c r="P38" s="8">
         <v>7</v>
-      </c>
-      <c r="J38" s="8">
-        <v>6</v>
-      </c>
-      <c r="K38" s="8">
-        <v>4</v>
-      </c>
-      <c r="L38" s="8">
-        <v>5</v>
-      </c>
-      <c r="M38" s="8">
-        <v>5</v>
-      </c>
-      <c r="N38" s="8">
-        <v>4</v>
-      </c>
-      <c r="O38" s="8">
-        <v>5</v>
-      </c>
-      <c r="P38" s="8">
-        <v>6</v>
       </c>
       <c r="Q38" s="8">
         <v>5</v>
@@ -12008,30 +12056,30 @@
         <v>4</v>
       </c>
       <c r="T38" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U38" s="8">
         <v>6</v>
       </c>
       <c r="V38" s="8">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="W38" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="X38" s="8">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="C39" s="8">
-        <v>26.8</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D39" s="8">
         <v>4</v>
@@ -12040,58 +12088,58 @@
         <v>5</v>
       </c>
       <c r="F39" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G39" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H39" s="8">
         <v>6</v>
       </c>
       <c r="I39" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J39" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K39" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L39" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M39" s="8">
         <v>5</v>
       </c>
       <c r="N39" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O39" s="8">
         <v>5</v>
       </c>
       <c r="P39" s="8">
+        <v>6</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>5</v>
+      </c>
+      <c r="R39" s="8">
         <v>7</v>
       </c>
-      <c r="Q39" s="8">
-        <v>4</v>
-      </c>
-      <c r="R39" s="8">
-        <v>8</v>
-      </c>
       <c r="S39" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T39" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="U39" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V39" s="8">
         <v>93</v>
       </c>
       <c r="W39" s="1">
-        <v>-6</v>
+        <v>12</v>
       </c>
       <c r="X39" s="8">
         <v>88</v>
@@ -12099,13 +12147,13 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C40" s="8">
-        <v>7.4</v>
+        <v>26.8</v>
       </c>
       <c r="D40" s="8">
         <v>4</v>
@@ -12117,69 +12165,69 @@
         <v>5</v>
       </c>
       <c r="G40" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H40" s="8">
         <v>6</v>
       </c>
       <c r="I40" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J40" s="8">
         <v>4</v>
       </c>
       <c r="K40" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L40" s="8">
+        <v>6</v>
+      </c>
+      <c r="M40" s="8">
+        <v>5</v>
+      </c>
+      <c r="N40" s="8">
+        <v>3</v>
+      </c>
+      <c r="O40" s="8">
+        <v>5</v>
+      </c>
+      <c r="P40" s="8">
         <v>7</v>
       </c>
-      <c r="M40" s="8">
-        <v>5</v>
-      </c>
-      <c r="N40" s="8">
-        <v>4</v>
-      </c>
-      <c r="O40" s="8">
-        <v>6</v>
-      </c>
-      <c r="P40" s="8">
+      <c r="Q40" s="8">
+        <v>4</v>
+      </c>
+      <c r="R40" s="8">
         <v>8</v>
       </c>
-      <c r="Q40" s="8">
-        <v>6</v>
-      </c>
-      <c r="R40" s="8">
-        <v>6</v>
-      </c>
       <c r="S40" s="8">
         <v>6</v>
       </c>
       <c r="T40" s="8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="U40" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V40" s="8">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W40" s="1">
-        <v>15</v>
+        <v>-6</v>
       </c>
       <c r="X40" s="8">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C41" s="8">
-        <v>16.7</v>
+        <v>7.4</v>
       </c>
       <c r="D41" s="8">
         <v>4</v>
@@ -12191,75 +12239,132 @@
         <v>5</v>
       </c>
       <c r="G41" s="8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H41" s="8">
         <v>6</v>
       </c>
       <c r="I41" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J41" s="8">
         <v>4</v>
       </c>
       <c r="K41" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L41" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M41" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N41" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O41" s="8">
         <v>6</v>
       </c>
       <c r="P41" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q41" s="8">
         <v>6</v>
       </c>
       <c r="R41" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S41" s="8">
         <v>6</v>
       </c>
       <c r="T41" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="U41" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V41" s="8">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="W41" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="X41" s="8">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="V42" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="W42" s="1" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="X42" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="8">
+        <v>16.7</v>
+      </c>
+      <c r="D42" s="8">
+        <v>4</v>
+      </c>
+      <c r="E42" s="8">
+        <v>5</v>
+      </c>
+      <c r="F42" s="8">
+        <v>5</v>
+      </c>
+      <c r="G42" s="8">
+        <v>6</v>
+      </c>
+      <c r="H42" s="8">
+        <v>6</v>
+      </c>
+      <c r="I42" s="8">
+        <v>3</v>
+      </c>
+      <c r="J42" s="8">
+        <v>4</v>
+      </c>
+      <c r="K42" s="8">
+        <v>5</v>
+      </c>
+      <c r="L42" s="8">
+        <v>6</v>
+      </c>
+      <c r="M42" s="8">
+        <v>6</v>
+      </c>
+      <c r="N42" s="8">
+        <v>6</v>
+      </c>
+      <c r="O42" s="8">
+        <v>6</v>
+      </c>
+      <c r="P42" s="8">
+        <v>9</v>
+      </c>
+      <c r="Q42" s="8">
+        <v>6</v>
+      </c>
+      <c r="R42" s="8">
+        <v>7</v>
+      </c>
+      <c r="S42" s="8">
+        <v>6</v>
+      </c>
+      <c r="T42" s="8">
+        <v>5</v>
+      </c>
+      <c r="U42" s="8">
+        <v>7</v>
+      </c>
+      <c r="V42" s="8">
+        <v>102</v>
+      </c>
+      <c r="W42" s="1">
+        <v>13</v>
+      </c>
+      <c r="X42" s="8">
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
@@ -14935,6 +15040,9 @@
       <c r="A200" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="C200" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="V200" s="8" t="s">
         <v>107</v>
       </c>
@@ -15106,7 +15214,7 @@
       <c r="V212" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="W212" s="8" t="e">
+      <c r="W212" s="1" t="e">
         <v>#VALUE!</v>
       </c>
       <c r="X212" s="8" t="s">
@@ -15145,6 +15253,15 @@
       <c r="A215" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="V215" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="W215" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X215" s="8" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="216" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
@@ -15566,9 +15683,14 @@
         <v>106</v>
       </c>
     </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B65543:B65585 IX65543:IX65585 ST65543:ST65585 ACP65543:ACP65585 AML65543:AML65585 AWH65543:AWH65585 BGD65543:BGD65585 BPZ65543:BPZ65585 BZV65543:BZV65585 CJR65543:CJR65585 CTN65543:CTN65585 DDJ65543:DDJ65585 DNF65543:DNF65585 DXB65543:DXB65585 EGX65543:EGX65585 EQT65543:EQT65585 FAP65543:FAP65585 FKL65543:FKL65585 FUH65543:FUH65585 GED65543:GED65585 GNZ65543:GNZ65585 GXV65543:GXV65585 HHR65543:HHR65585 HRN65543:HRN65585 IBJ65543:IBJ65585 ILF65543:ILF65585 IVB65543:IVB65585 JEX65543:JEX65585 JOT65543:JOT65585 JYP65543:JYP65585 KIL65543:KIL65585 KSH65543:KSH65585 LCD65543:LCD65585 LLZ65543:LLZ65585 LVV65543:LVV65585 MFR65543:MFR65585 MPN65543:MPN65585 MZJ65543:MZJ65585 NJF65543:NJF65585 NTB65543:NTB65585 OCX65543:OCX65585 OMT65543:OMT65585 OWP65543:OWP65585 PGL65543:PGL65585 PQH65543:PQH65585 QAD65543:QAD65585 QJZ65543:QJZ65585 QTV65543:QTV65585 RDR65543:RDR65585 RNN65543:RNN65585 RXJ65543:RXJ65585 SHF65543:SHF65585 SRB65543:SRB65585 TAX65543:TAX65585 TKT65543:TKT65585 TUP65543:TUP65585 UEL65543:UEL65585 UOH65543:UOH65585 UYD65543:UYD65585 VHZ65543:VHZ65585 VRV65543:VRV65585 WBR65543:WBR65585 WLN65543:WLN65585 WVJ65543:WVJ65585 B131079:B131121 IX131079:IX131121 ST131079:ST131121 ACP131079:ACP131121 AML131079:AML131121 AWH131079:AWH131121 BGD131079:BGD131121 BPZ131079:BPZ131121 BZV131079:BZV131121 CJR131079:CJR131121 CTN131079:CTN131121 DDJ131079:DDJ131121 DNF131079:DNF131121 DXB131079:DXB131121 EGX131079:EGX131121 EQT131079:EQT131121 FAP131079:FAP131121 FKL131079:FKL131121 FUH131079:FUH131121 GED131079:GED131121 GNZ131079:GNZ131121 GXV131079:GXV131121 HHR131079:HHR131121 HRN131079:HRN131121 IBJ131079:IBJ131121 ILF131079:ILF131121 IVB131079:IVB131121 JEX131079:JEX131121 JOT131079:JOT131121 JYP131079:JYP131121 KIL131079:KIL131121 KSH131079:KSH131121 LCD131079:LCD131121 LLZ131079:LLZ131121 LVV131079:LVV131121 MFR131079:MFR131121 MPN131079:MPN131121 MZJ131079:MZJ131121 NJF131079:NJF131121 NTB131079:NTB131121 OCX131079:OCX131121 OMT131079:OMT131121 OWP131079:OWP131121 PGL131079:PGL131121 PQH131079:PQH131121 QAD131079:QAD131121 QJZ131079:QJZ131121 QTV131079:QTV131121 RDR131079:RDR131121 RNN131079:RNN131121 RXJ131079:RXJ131121 SHF131079:SHF131121 SRB131079:SRB131121 TAX131079:TAX131121 TKT131079:TKT131121 TUP131079:TUP131121 UEL131079:UEL131121 UOH131079:UOH131121 UYD131079:UYD131121 VHZ131079:VHZ131121 VRV131079:VRV131121 WBR131079:WBR131121 WLN131079:WLN131121 WVJ131079:WVJ131121 B196615:B196657 IX196615:IX196657 ST196615:ST196657 ACP196615:ACP196657 AML196615:AML196657 AWH196615:AWH196657 BGD196615:BGD196657 BPZ196615:BPZ196657 BZV196615:BZV196657 CJR196615:CJR196657 CTN196615:CTN196657 DDJ196615:DDJ196657 DNF196615:DNF196657 DXB196615:DXB196657 EGX196615:EGX196657 EQT196615:EQT196657 FAP196615:FAP196657 FKL196615:FKL196657 FUH196615:FUH196657 GED196615:GED196657 GNZ196615:GNZ196657 GXV196615:GXV196657 HHR196615:HHR196657 HRN196615:HRN196657 IBJ196615:IBJ196657 ILF196615:ILF196657 IVB196615:IVB196657 JEX196615:JEX196657 JOT196615:JOT196657 JYP196615:JYP196657 KIL196615:KIL196657 KSH196615:KSH196657 LCD196615:LCD196657 LLZ196615:LLZ196657 LVV196615:LVV196657 MFR196615:MFR196657 MPN196615:MPN196657 MZJ196615:MZJ196657 NJF196615:NJF196657 NTB196615:NTB196657 OCX196615:OCX196657 OMT196615:OMT196657 OWP196615:OWP196657 PGL196615:PGL196657 PQH196615:PQH196657 QAD196615:QAD196657 QJZ196615:QJZ196657 QTV196615:QTV196657 RDR196615:RDR196657 RNN196615:RNN196657 RXJ196615:RXJ196657 SHF196615:SHF196657 SRB196615:SRB196657 TAX196615:TAX196657 TKT196615:TKT196657 TUP196615:TUP196657 UEL196615:UEL196657 UOH196615:UOH196657 UYD196615:UYD196657 VHZ196615:VHZ196657 VRV196615:VRV196657 WBR196615:WBR196657 WLN196615:WLN196657 WVJ196615:WVJ196657 B262151:B262193 IX262151:IX262193 ST262151:ST262193 ACP262151:ACP262193 AML262151:AML262193 AWH262151:AWH262193 BGD262151:BGD262193 BPZ262151:BPZ262193 BZV262151:BZV262193 CJR262151:CJR262193 CTN262151:CTN262193 DDJ262151:DDJ262193 DNF262151:DNF262193 DXB262151:DXB262193 EGX262151:EGX262193 EQT262151:EQT262193 FAP262151:FAP262193 FKL262151:FKL262193 FUH262151:FUH262193 GED262151:GED262193 GNZ262151:GNZ262193 GXV262151:GXV262193 HHR262151:HHR262193 HRN262151:HRN262193 IBJ262151:IBJ262193 ILF262151:ILF262193 IVB262151:IVB262193 JEX262151:JEX262193 JOT262151:JOT262193 JYP262151:JYP262193 KIL262151:KIL262193 KSH262151:KSH262193 LCD262151:LCD262193 LLZ262151:LLZ262193 LVV262151:LVV262193 MFR262151:MFR262193 MPN262151:MPN262193 MZJ262151:MZJ262193 NJF262151:NJF262193 NTB262151:NTB262193 OCX262151:OCX262193 OMT262151:OMT262193 OWP262151:OWP262193 PGL262151:PGL262193 PQH262151:PQH262193 QAD262151:QAD262193 QJZ262151:QJZ262193 QTV262151:QTV262193 RDR262151:RDR262193 RNN262151:RNN262193 RXJ262151:RXJ262193 SHF262151:SHF262193 SRB262151:SRB262193 TAX262151:TAX262193 TKT262151:TKT262193 TUP262151:TUP262193 UEL262151:UEL262193 UOH262151:UOH262193 UYD262151:UYD262193 VHZ262151:VHZ262193 VRV262151:VRV262193 WBR262151:WBR262193 WLN262151:WLN262193 WVJ262151:WVJ262193 B327687:B327729 IX327687:IX327729 ST327687:ST327729 ACP327687:ACP327729 AML327687:AML327729 AWH327687:AWH327729 BGD327687:BGD327729 BPZ327687:BPZ327729 BZV327687:BZV327729 CJR327687:CJR327729 CTN327687:CTN327729 DDJ327687:DDJ327729 DNF327687:DNF327729 DXB327687:DXB327729 EGX327687:EGX327729 EQT327687:EQT327729 FAP327687:FAP327729 FKL327687:FKL327729 FUH327687:FUH327729 GED327687:GED327729 GNZ327687:GNZ327729 GXV327687:GXV327729 HHR327687:HHR327729 HRN327687:HRN327729 IBJ327687:IBJ327729 ILF327687:ILF327729 IVB327687:IVB327729 JEX327687:JEX327729 JOT327687:JOT327729 JYP327687:JYP327729 KIL327687:KIL327729 KSH327687:KSH327729 LCD327687:LCD327729 LLZ327687:LLZ327729 LVV327687:LVV327729 MFR327687:MFR327729 MPN327687:MPN327729 MZJ327687:MZJ327729 NJF327687:NJF327729 NTB327687:NTB327729 OCX327687:OCX327729 OMT327687:OMT327729 OWP327687:OWP327729 PGL327687:PGL327729 PQH327687:PQH327729 QAD327687:QAD327729 QJZ327687:QJZ327729 QTV327687:QTV327729 RDR327687:RDR327729 RNN327687:RNN327729 RXJ327687:RXJ327729 SHF327687:SHF327729 SRB327687:SRB327729 TAX327687:TAX327729 TKT327687:TKT327729 TUP327687:TUP327729 UEL327687:UEL327729 UOH327687:UOH327729 UYD327687:UYD327729 VHZ327687:VHZ327729 VRV327687:VRV327729 WBR327687:WBR327729 WLN327687:WLN327729 WVJ327687:WVJ327729 B393223:B393265 IX393223:IX393265 ST393223:ST393265 ACP393223:ACP393265 AML393223:AML393265 AWH393223:AWH393265 BGD393223:BGD393265 BPZ393223:BPZ393265 BZV393223:BZV393265 CJR393223:CJR393265 CTN393223:CTN393265 DDJ393223:DDJ393265 DNF393223:DNF393265 DXB393223:DXB393265 EGX393223:EGX393265 EQT393223:EQT393265 FAP393223:FAP393265 FKL393223:FKL393265 FUH393223:FUH393265 GED393223:GED393265 GNZ393223:GNZ393265 GXV393223:GXV393265 HHR393223:HHR393265 HRN393223:HRN393265 IBJ393223:IBJ393265 ILF393223:ILF393265 IVB393223:IVB393265 JEX393223:JEX393265 JOT393223:JOT393265 JYP393223:JYP393265 KIL393223:KIL393265 KSH393223:KSH393265 LCD393223:LCD393265 LLZ393223:LLZ393265 LVV393223:LVV393265 MFR393223:MFR393265 MPN393223:MPN393265 MZJ393223:MZJ393265 NJF393223:NJF393265 NTB393223:NTB393265 OCX393223:OCX393265 OMT393223:OMT393265 OWP393223:OWP393265 PGL393223:PGL393265 PQH393223:PQH393265 QAD393223:QAD393265 QJZ393223:QJZ393265 QTV393223:QTV393265 RDR393223:RDR393265 RNN393223:RNN393265 RXJ393223:RXJ393265 SHF393223:SHF393265 SRB393223:SRB393265 TAX393223:TAX393265 TKT393223:TKT393265 TUP393223:TUP393265 UEL393223:UEL393265 UOH393223:UOH393265 UYD393223:UYD393265 VHZ393223:VHZ393265 VRV393223:VRV393265 WBR393223:WBR393265 WLN393223:WLN393265 WVJ393223:WVJ393265 B458759:B458801 IX458759:IX458801 ST458759:ST458801 ACP458759:ACP458801 AML458759:AML458801 AWH458759:AWH458801 BGD458759:BGD458801 BPZ458759:BPZ458801 BZV458759:BZV458801 CJR458759:CJR458801 CTN458759:CTN458801 DDJ458759:DDJ458801 DNF458759:DNF458801 DXB458759:DXB458801 EGX458759:EGX458801 EQT458759:EQT458801 FAP458759:FAP458801 FKL458759:FKL458801 FUH458759:FUH458801 GED458759:GED458801 GNZ458759:GNZ458801 GXV458759:GXV458801 HHR458759:HHR458801 HRN458759:HRN458801 IBJ458759:IBJ458801 ILF458759:ILF458801 IVB458759:IVB458801 JEX458759:JEX458801 JOT458759:JOT458801 JYP458759:JYP458801 KIL458759:KIL458801 KSH458759:KSH458801 LCD458759:LCD458801 LLZ458759:LLZ458801 LVV458759:LVV458801 MFR458759:MFR458801 MPN458759:MPN458801 MZJ458759:MZJ458801 NJF458759:NJF458801 NTB458759:NTB458801 OCX458759:OCX458801 OMT458759:OMT458801 OWP458759:OWP458801 PGL458759:PGL458801 PQH458759:PQH458801 QAD458759:QAD458801 QJZ458759:QJZ458801 QTV458759:QTV458801 RDR458759:RDR458801 RNN458759:RNN458801 RXJ458759:RXJ458801 SHF458759:SHF458801 SRB458759:SRB458801 TAX458759:TAX458801 TKT458759:TKT458801 TUP458759:TUP458801 UEL458759:UEL458801 UOH458759:UOH458801 UYD458759:UYD458801 VHZ458759:VHZ458801 VRV458759:VRV458801 WBR458759:WBR458801 WLN458759:WLN458801 WVJ458759:WVJ458801 B524295:B524337 IX524295:IX524337 ST524295:ST524337 ACP524295:ACP524337 AML524295:AML524337 AWH524295:AWH524337 BGD524295:BGD524337 BPZ524295:BPZ524337 BZV524295:BZV524337 CJR524295:CJR524337 CTN524295:CTN524337 DDJ524295:DDJ524337 DNF524295:DNF524337 DXB524295:DXB524337 EGX524295:EGX524337 EQT524295:EQT524337 FAP524295:FAP524337 FKL524295:FKL524337 FUH524295:FUH524337 GED524295:GED524337 GNZ524295:GNZ524337 GXV524295:GXV524337 HHR524295:HHR524337 HRN524295:HRN524337 IBJ524295:IBJ524337 ILF524295:ILF524337 IVB524295:IVB524337 JEX524295:JEX524337 JOT524295:JOT524337 JYP524295:JYP524337 KIL524295:KIL524337 KSH524295:KSH524337 LCD524295:LCD524337 LLZ524295:LLZ524337 LVV524295:LVV524337 MFR524295:MFR524337 MPN524295:MPN524337 MZJ524295:MZJ524337 NJF524295:NJF524337 NTB524295:NTB524337 OCX524295:OCX524337 OMT524295:OMT524337 OWP524295:OWP524337 PGL524295:PGL524337 PQH524295:PQH524337 QAD524295:QAD524337 QJZ524295:QJZ524337 QTV524295:QTV524337 RDR524295:RDR524337 RNN524295:RNN524337 RXJ524295:RXJ524337 SHF524295:SHF524337 SRB524295:SRB524337 TAX524295:TAX524337 TKT524295:TKT524337 TUP524295:TUP524337 UEL524295:UEL524337 UOH524295:UOH524337 UYD524295:UYD524337 VHZ524295:VHZ524337 VRV524295:VRV524337 WBR524295:WBR524337 WLN524295:WLN524337 WVJ524295:WVJ524337 B589831:B589873 IX589831:IX589873 ST589831:ST589873 ACP589831:ACP589873 AML589831:AML589873 AWH589831:AWH589873 BGD589831:BGD589873 BPZ589831:BPZ589873 BZV589831:BZV589873 CJR589831:CJR589873 CTN589831:CTN589873 DDJ589831:DDJ589873 DNF589831:DNF589873 DXB589831:DXB589873 EGX589831:EGX589873 EQT589831:EQT589873 FAP589831:FAP589873 FKL589831:FKL589873 FUH589831:FUH589873 GED589831:GED589873 GNZ589831:GNZ589873 GXV589831:GXV589873 HHR589831:HHR589873 HRN589831:HRN589873 IBJ589831:IBJ589873 ILF589831:ILF589873 IVB589831:IVB589873 JEX589831:JEX589873 JOT589831:JOT589873 JYP589831:JYP589873 KIL589831:KIL589873 KSH589831:KSH589873 LCD589831:LCD589873 LLZ589831:LLZ589873 LVV589831:LVV589873 MFR589831:MFR589873 MPN589831:MPN589873 MZJ589831:MZJ589873 NJF589831:NJF589873 NTB589831:NTB589873 OCX589831:OCX589873 OMT589831:OMT589873 OWP589831:OWP589873 PGL589831:PGL589873 PQH589831:PQH589873 QAD589831:QAD589873 QJZ589831:QJZ589873 QTV589831:QTV589873 RDR589831:RDR589873 RNN589831:RNN589873 RXJ589831:RXJ589873 SHF589831:SHF589873 SRB589831:SRB589873 TAX589831:TAX589873 TKT589831:TKT589873 TUP589831:TUP589873 UEL589831:UEL589873 UOH589831:UOH589873 UYD589831:UYD589873 VHZ589831:VHZ589873 VRV589831:VRV589873 WBR589831:WBR589873 WLN589831:WLN589873 WVJ589831:WVJ589873 B655367:B655409 IX655367:IX655409 ST655367:ST655409 ACP655367:ACP655409 AML655367:AML655409 AWH655367:AWH655409 BGD655367:BGD655409 BPZ655367:BPZ655409 BZV655367:BZV655409 CJR655367:CJR655409 CTN655367:CTN655409 DDJ655367:DDJ655409 DNF655367:DNF655409 DXB655367:DXB655409 EGX655367:EGX655409 EQT655367:EQT655409 FAP655367:FAP655409 FKL655367:FKL655409 FUH655367:FUH655409 GED655367:GED655409 GNZ655367:GNZ655409 GXV655367:GXV655409 HHR655367:HHR655409 HRN655367:HRN655409 IBJ655367:IBJ655409 ILF655367:ILF655409 IVB655367:IVB655409 JEX655367:JEX655409 JOT655367:JOT655409 JYP655367:JYP655409 KIL655367:KIL655409 KSH655367:KSH655409 LCD655367:LCD655409 LLZ655367:LLZ655409 LVV655367:LVV655409 MFR655367:MFR655409 MPN655367:MPN655409 MZJ655367:MZJ655409 NJF655367:NJF655409 NTB655367:NTB655409 OCX655367:OCX655409 OMT655367:OMT655409 OWP655367:OWP655409 PGL655367:PGL655409 PQH655367:PQH655409 QAD655367:QAD655409 QJZ655367:QJZ655409 QTV655367:QTV655409 RDR655367:RDR655409 RNN655367:RNN655409 RXJ655367:RXJ655409 SHF655367:SHF655409 SRB655367:SRB655409 TAX655367:TAX655409 TKT655367:TKT655409 TUP655367:TUP655409 UEL655367:UEL655409 UOH655367:UOH655409 UYD655367:UYD655409 VHZ655367:VHZ655409 VRV655367:VRV655409 WBR655367:WBR655409 WLN655367:WLN655409 WVJ655367:WVJ655409 B720903:B720945 IX720903:IX720945 ST720903:ST720945 ACP720903:ACP720945 AML720903:AML720945 AWH720903:AWH720945 BGD720903:BGD720945 BPZ720903:BPZ720945 BZV720903:BZV720945 CJR720903:CJR720945 CTN720903:CTN720945 DDJ720903:DDJ720945 DNF720903:DNF720945 DXB720903:DXB720945 EGX720903:EGX720945 EQT720903:EQT720945 FAP720903:FAP720945 FKL720903:FKL720945 FUH720903:FUH720945 GED720903:GED720945 GNZ720903:GNZ720945 GXV720903:GXV720945 HHR720903:HHR720945 HRN720903:HRN720945 IBJ720903:IBJ720945 ILF720903:ILF720945 IVB720903:IVB720945 JEX720903:JEX720945 JOT720903:JOT720945 JYP720903:JYP720945 KIL720903:KIL720945 KSH720903:KSH720945 LCD720903:LCD720945 LLZ720903:LLZ720945 LVV720903:LVV720945 MFR720903:MFR720945 MPN720903:MPN720945 MZJ720903:MZJ720945 NJF720903:NJF720945 NTB720903:NTB720945 OCX720903:OCX720945 OMT720903:OMT720945 OWP720903:OWP720945 PGL720903:PGL720945 PQH720903:PQH720945 QAD720903:QAD720945 QJZ720903:QJZ720945 QTV720903:QTV720945 RDR720903:RDR720945 RNN720903:RNN720945 RXJ720903:RXJ720945 SHF720903:SHF720945 SRB720903:SRB720945 TAX720903:TAX720945 TKT720903:TKT720945 TUP720903:TUP720945 UEL720903:UEL720945 UOH720903:UOH720945 UYD720903:UYD720945 VHZ720903:VHZ720945 VRV720903:VRV720945 WBR720903:WBR720945 WLN720903:WLN720945 WVJ720903:WVJ720945 B786439:B786481 IX786439:IX786481 ST786439:ST786481 ACP786439:ACP786481 AML786439:AML786481 AWH786439:AWH786481 BGD786439:BGD786481 BPZ786439:BPZ786481 BZV786439:BZV786481 CJR786439:CJR786481 CTN786439:CTN786481 DDJ786439:DDJ786481 DNF786439:DNF786481 DXB786439:DXB786481 EGX786439:EGX786481 EQT786439:EQT786481 FAP786439:FAP786481 FKL786439:FKL786481 FUH786439:FUH786481 GED786439:GED786481 GNZ786439:GNZ786481 GXV786439:GXV786481 HHR786439:HHR786481 HRN786439:HRN786481 IBJ786439:IBJ786481 ILF786439:ILF786481 IVB786439:IVB786481 JEX786439:JEX786481 JOT786439:JOT786481 JYP786439:JYP786481 KIL786439:KIL786481 KSH786439:KSH786481 LCD786439:LCD786481 LLZ786439:LLZ786481 LVV786439:LVV786481 MFR786439:MFR786481 MPN786439:MPN786481 MZJ786439:MZJ786481 NJF786439:NJF786481 NTB786439:NTB786481 OCX786439:OCX786481 OMT786439:OMT786481 OWP786439:OWP786481 PGL786439:PGL786481 PQH786439:PQH786481 QAD786439:QAD786481 QJZ786439:QJZ786481 QTV786439:QTV786481 RDR786439:RDR786481 RNN786439:RNN786481 RXJ786439:RXJ786481 SHF786439:SHF786481 SRB786439:SRB786481 TAX786439:TAX786481 TKT786439:TKT786481 TUP786439:TUP786481 UEL786439:UEL786481 UOH786439:UOH786481 UYD786439:UYD786481 VHZ786439:VHZ786481 VRV786439:VRV786481 WBR786439:WBR786481 WLN786439:WLN786481 WVJ786439:WVJ786481 B851975:B852017 IX851975:IX852017 ST851975:ST852017 ACP851975:ACP852017 AML851975:AML852017 AWH851975:AWH852017 BGD851975:BGD852017 BPZ851975:BPZ852017 BZV851975:BZV852017 CJR851975:CJR852017 CTN851975:CTN852017 DDJ851975:DDJ852017 DNF851975:DNF852017 DXB851975:DXB852017 EGX851975:EGX852017 EQT851975:EQT852017 FAP851975:FAP852017 FKL851975:FKL852017 FUH851975:FUH852017 GED851975:GED852017 GNZ851975:GNZ852017 GXV851975:GXV852017 HHR851975:HHR852017 HRN851975:HRN852017 IBJ851975:IBJ852017 ILF851975:ILF852017 IVB851975:IVB852017 JEX851975:JEX852017 JOT851975:JOT852017 JYP851975:JYP852017 KIL851975:KIL852017 KSH851975:KSH852017 LCD851975:LCD852017 LLZ851975:LLZ852017 LVV851975:LVV852017 MFR851975:MFR852017 MPN851975:MPN852017 MZJ851975:MZJ852017 NJF851975:NJF852017 NTB851975:NTB852017 OCX851975:OCX852017 OMT851975:OMT852017 OWP851975:OWP852017 PGL851975:PGL852017 PQH851975:PQH852017 QAD851975:QAD852017 QJZ851975:QJZ852017 QTV851975:QTV852017 RDR851975:RDR852017 RNN851975:RNN852017 RXJ851975:RXJ852017 SHF851975:SHF852017 SRB851975:SRB852017 TAX851975:TAX852017 TKT851975:TKT852017 TUP851975:TUP852017 UEL851975:UEL852017 UOH851975:UOH852017 UYD851975:UYD852017 VHZ851975:VHZ852017 VRV851975:VRV852017 WBR851975:WBR852017 WLN851975:WLN852017 WVJ851975:WVJ852017 B917511:B917553 IX917511:IX917553 ST917511:ST917553 ACP917511:ACP917553 AML917511:AML917553 AWH917511:AWH917553 BGD917511:BGD917553 BPZ917511:BPZ917553 BZV917511:BZV917553 CJR917511:CJR917553 CTN917511:CTN917553 DDJ917511:DDJ917553 DNF917511:DNF917553 DXB917511:DXB917553 EGX917511:EGX917553 EQT917511:EQT917553 FAP917511:FAP917553 FKL917511:FKL917553 FUH917511:FUH917553 GED917511:GED917553 GNZ917511:GNZ917553 GXV917511:GXV917553 HHR917511:HHR917553 HRN917511:HRN917553 IBJ917511:IBJ917553 ILF917511:ILF917553 IVB917511:IVB917553 JEX917511:JEX917553 JOT917511:JOT917553 JYP917511:JYP917553 KIL917511:KIL917553 KSH917511:KSH917553 LCD917511:LCD917553 LLZ917511:LLZ917553 LVV917511:LVV917553 MFR917511:MFR917553 MPN917511:MPN917553 MZJ917511:MZJ917553 NJF917511:NJF917553 NTB917511:NTB917553 OCX917511:OCX917553 OMT917511:OMT917553 OWP917511:OWP917553 PGL917511:PGL917553 PQH917511:PQH917553 QAD917511:QAD917553 QJZ917511:QJZ917553 QTV917511:QTV917553 RDR917511:RDR917553 RNN917511:RNN917553 RXJ917511:RXJ917553 SHF917511:SHF917553 SRB917511:SRB917553 TAX917511:TAX917553 TKT917511:TKT917553 TUP917511:TUP917553 UEL917511:UEL917553 UOH917511:UOH917553 UYD917511:UYD917553 VHZ917511:VHZ917553 VRV917511:VRV917553 WBR917511:WBR917553 WLN917511:WLN917553 WVJ917511:WVJ917553 B983047:B983089 IX983047:IX983089 ST983047:ST983089 ACP983047:ACP983089 AML983047:AML983089 AWH983047:AWH983089 BGD983047:BGD983089 BPZ983047:BPZ983089 BZV983047:BZV983089 CJR983047:CJR983089 CTN983047:CTN983089 DDJ983047:DDJ983089 DNF983047:DNF983089 DXB983047:DXB983089 EGX983047:EGX983089 EQT983047:EQT983089 FAP983047:FAP983089 FKL983047:FKL983089 FUH983047:FUH983089 GED983047:GED983089 GNZ983047:GNZ983089 GXV983047:GXV983089 HHR983047:HHR983089 HRN983047:HRN983089 IBJ983047:IBJ983089 ILF983047:ILF983089 IVB983047:IVB983089 JEX983047:JEX983089 JOT983047:JOT983089 JYP983047:JYP983089 KIL983047:KIL983089 KSH983047:KSH983089 LCD983047:LCD983089 LLZ983047:LLZ983089 LVV983047:LVV983089 MFR983047:MFR983089 MPN983047:MPN983089 MZJ983047:MZJ983089 NJF983047:NJF983089 NTB983047:NTB983089 OCX983047:OCX983089 OMT983047:OMT983089 OWP983047:OWP983089 PGL983047:PGL983089 PQH983047:PQH983089 QAD983047:QAD983089 QJZ983047:QJZ983089 QTV983047:QTV983089 RDR983047:RDR983089 RNN983047:RNN983089 RXJ983047:RXJ983089 SHF983047:SHF983089 SRB983047:SRB983089 TAX983047:TAX983089 TKT983047:TKT983089 TUP983047:TUP983089 UEL983047:UEL983089 UOH983047:UOH983089 UYD983047:UYD983089 VHZ983047:VHZ983089 VRV983047:VRV983089 WBR983047:WBR983089 WLN983047:WLN983089 WVJ983047:WVJ983089 WVJ8:WVJ49 WLN8:WLN49 WBR8:WBR49 VRV8:VRV49 VHZ8:VHZ49 UYD8:UYD49 UOH8:UOH49 UEL8:UEL49 TUP8:TUP49 TKT8:TKT49 TAX8:TAX49 SRB8:SRB49 SHF8:SHF49 RXJ8:RXJ49 RNN8:RNN49 RDR8:RDR49 QTV8:QTV49 QJZ8:QJZ49 QAD8:QAD49 PQH8:PQH49 PGL8:PGL49 OWP8:OWP49 OMT8:OMT49 OCX8:OCX49 NTB8:NTB49 NJF8:NJF49 MZJ8:MZJ49 MPN8:MPN49 MFR8:MFR49 LVV8:LVV49 LLZ8:LLZ49 LCD8:LCD49 KSH8:KSH49 KIL8:KIL49 JYP8:JYP49 JOT8:JOT49 JEX8:JEX49 IVB8:IVB49 ILF8:ILF49 IBJ8:IBJ49 HRN8:HRN49 HHR8:HHR49 GXV8:GXV49 GNZ8:GNZ49 GED8:GED49 FUH8:FUH49 FKL8:FKL49 FAP8:FAP49 EQT8:EQT49 EGX8:EGX49 DXB8:DXB49 DNF8:DNF49 DDJ8:DDJ49 CTN8:CTN49 CJR8:CJR49 BZV8:BZV49 BPZ8:BPZ49 BGD8:BGD49 AWH8:AWH49 AML8:AML49 ACP8:ACP49 ST8:ST49 IX8:IX49 B8:B49">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B50 IX8:IX50 ST8:ST50 ACP8:ACP50 AML8:AML50 AWH8:AWH50 BGD8:BGD50 BPZ8:BPZ50 BZV8:BZV50 CJR8:CJR50 CTN8:CTN50 DDJ8:DDJ50 DNF8:DNF50 DXB8:DXB50 EGX8:EGX50 EQT8:EQT50 FAP8:FAP50 FKL8:FKL50 FUH8:FUH50 GED8:GED50 GNZ8:GNZ50 GXV8:GXV50 HHR8:HHR50 HRN8:HRN50 IBJ8:IBJ50 ILF8:ILF50 IVB8:IVB50 JEX8:JEX50 JOT8:JOT50 JYP8:JYP50 KIL8:KIL50 KSH8:KSH50 LCD8:LCD50 LLZ8:LLZ50 LVV8:LVV50 MFR8:MFR50 MPN8:MPN50 MZJ8:MZJ50 NJF8:NJF50 NTB8:NTB50 OCX8:OCX50 OMT8:OMT50 OWP8:OWP50 PGL8:PGL50 PQH8:PQH50 QAD8:QAD50 QJZ8:QJZ50 QTV8:QTV50 RDR8:RDR50 RNN8:RNN50 RXJ8:RXJ50 SHF8:SHF50 SRB8:SRB50 TAX8:TAX50 TKT8:TKT50 TUP8:TUP50 UEL8:UEL50 UOH8:UOH50 UYD8:UYD50 VHZ8:VHZ50 VRV8:VRV50 WBR8:WBR50 WLN8:WLN50 WVJ8:WVJ50 B65544:B65586 IX65544:IX65586 ST65544:ST65586 ACP65544:ACP65586 AML65544:AML65586 AWH65544:AWH65586 BGD65544:BGD65586 BPZ65544:BPZ65586 BZV65544:BZV65586 CJR65544:CJR65586 CTN65544:CTN65586 DDJ65544:DDJ65586 DNF65544:DNF65586 DXB65544:DXB65586 EGX65544:EGX65586 EQT65544:EQT65586 FAP65544:FAP65586 FKL65544:FKL65586 FUH65544:FUH65586 GED65544:GED65586 GNZ65544:GNZ65586 GXV65544:GXV65586 HHR65544:HHR65586 HRN65544:HRN65586 IBJ65544:IBJ65586 ILF65544:ILF65586 IVB65544:IVB65586 JEX65544:JEX65586 JOT65544:JOT65586 JYP65544:JYP65586 KIL65544:KIL65586 KSH65544:KSH65586 LCD65544:LCD65586 LLZ65544:LLZ65586 LVV65544:LVV65586 MFR65544:MFR65586 MPN65544:MPN65586 MZJ65544:MZJ65586 NJF65544:NJF65586 NTB65544:NTB65586 OCX65544:OCX65586 OMT65544:OMT65586 OWP65544:OWP65586 PGL65544:PGL65586 PQH65544:PQH65586 QAD65544:QAD65586 QJZ65544:QJZ65586 QTV65544:QTV65586 RDR65544:RDR65586 RNN65544:RNN65586 RXJ65544:RXJ65586 SHF65544:SHF65586 SRB65544:SRB65586 TAX65544:TAX65586 TKT65544:TKT65586 TUP65544:TUP65586 UEL65544:UEL65586 UOH65544:UOH65586 UYD65544:UYD65586 VHZ65544:VHZ65586 VRV65544:VRV65586 WBR65544:WBR65586 WLN65544:WLN65586 WVJ65544:WVJ65586 B131080:B131122 IX131080:IX131122 ST131080:ST131122 ACP131080:ACP131122 AML131080:AML131122 AWH131080:AWH131122 BGD131080:BGD131122 BPZ131080:BPZ131122 BZV131080:BZV131122 CJR131080:CJR131122 CTN131080:CTN131122 DDJ131080:DDJ131122 DNF131080:DNF131122 DXB131080:DXB131122 EGX131080:EGX131122 EQT131080:EQT131122 FAP131080:FAP131122 FKL131080:FKL131122 FUH131080:FUH131122 GED131080:GED131122 GNZ131080:GNZ131122 GXV131080:GXV131122 HHR131080:HHR131122 HRN131080:HRN131122 IBJ131080:IBJ131122 ILF131080:ILF131122 IVB131080:IVB131122 JEX131080:JEX131122 JOT131080:JOT131122 JYP131080:JYP131122 KIL131080:KIL131122 KSH131080:KSH131122 LCD131080:LCD131122 LLZ131080:LLZ131122 LVV131080:LVV131122 MFR131080:MFR131122 MPN131080:MPN131122 MZJ131080:MZJ131122 NJF131080:NJF131122 NTB131080:NTB131122 OCX131080:OCX131122 OMT131080:OMT131122 OWP131080:OWP131122 PGL131080:PGL131122 PQH131080:PQH131122 QAD131080:QAD131122 QJZ131080:QJZ131122 QTV131080:QTV131122 RDR131080:RDR131122 RNN131080:RNN131122 RXJ131080:RXJ131122 SHF131080:SHF131122 SRB131080:SRB131122 TAX131080:TAX131122 TKT131080:TKT131122 TUP131080:TUP131122 UEL131080:UEL131122 UOH131080:UOH131122 UYD131080:UYD131122 VHZ131080:VHZ131122 VRV131080:VRV131122 WBR131080:WBR131122 WLN131080:WLN131122 WVJ131080:WVJ131122 B196616:B196658 IX196616:IX196658 ST196616:ST196658 ACP196616:ACP196658 AML196616:AML196658 AWH196616:AWH196658 BGD196616:BGD196658 BPZ196616:BPZ196658 BZV196616:BZV196658 CJR196616:CJR196658 CTN196616:CTN196658 DDJ196616:DDJ196658 DNF196616:DNF196658 DXB196616:DXB196658 EGX196616:EGX196658 EQT196616:EQT196658 FAP196616:FAP196658 FKL196616:FKL196658 FUH196616:FUH196658 GED196616:GED196658 GNZ196616:GNZ196658 GXV196616:GXV196658 HHR196616:HHR196658 HRN196616:HRN196658 IBJ196616:IBJ196658 ILF196616:ILF196658 IVB196616:IVB196658 JEX196616:JEX196658 JOT196616:JOT196658 JYP196616:JYP196658 KIL196616:KIL196658 KSH196616:KSH196658 LCD196616:LCD196658 LLZ196616:LLZ196658 LVV196616:LVV196658 MFR196616:MFR196658 MPN196616:MPN196658 MZJ196616:MZJ196658 NJF196616:NJF196658 NTB196616:NTB196658 OCX196616:OCX196658 OMT196616:OMT196658 OWP196616:OWP196658 PGL196616:PGL196658 PQH196616:PQH196658 QAD196616:QAD196658 QJZ196616:QJZ196658 QTV196616:QTV196658 RDR196616:RDR196658 RNN196616:RNN196658 RXJ196616:RXJ196658 SHF196616:SHF196658 SRB196616:SRB196658 TAX196616:TAX196658 TKT196616:TKT196658 TUP196616:TUP196658 UEL196616:UEL196658 UOH196616:UOH196658 UYD196616:UYD196658 VHZ196616:VHZ196658 VRV196616:VRV196658 WBR196616:WBR196658 WLN196616:WLN196658 WVJ196616:WVJ196658 B262152:B262194 IX262152:IX262194 ST262152:ST262194 ACP262152:ACP262194 AML262152:AML262194 AWH262152:AWH262194 BGD262152:BGD262194 BPZ262152:BPZ262194 BZV262152:BZV262194 CJR262152:CJR262194 CTN262152:CTN262194 DDJ262152:DDJ262194 DNF262152:DNF262194 DXB262152:DXB262194 EGX262152:EGX262194 EQT262152:EQT262194 FAP262152:FAP262194 FKL262152:FKL262194 FUH262152:FUH262194 GED262152:GED262194 GNZ262152:GNZ262194 GXV262152:GXV262194 HHR262152:HHR262194 HRN262152:HRN262194 IBJ262152:IBJ262194 ILF262152:ILF262194 IVB262152:IVB262194 JEX262152:JEX262194 JOT262152:JOT262194 JYP262152:JYP262194 KIL262152:KIL262194 KSH262152:KSH262194 LCD262152:LCD262194 LLZ262152:LLZ262194 LVV262152:LVV262194 MFR262152:MFR262194 MPN262152:MPN262194 MZJ262152:MZJ262194 NJF262152:NJF262194 NTB262152:NTB262194 OCX262152:OCX262194 OMT262152:OMT262194 OWP262152:OWP262194 PGL262152:PGL262194 PQH262152:PQH262194 QAD262152:QAD262194 QJZ262152:QJZ262194 QTV262152:QTV262194 RDR262152:RDR262194 RNN262152:RNN262194 RXJ262152:RXJ262194 SHF262152:SHF262194 SRB262152:SRB262194 TAX262152:TAX262194 TKT262152:TKT262194 TUP262152:TUP262194 UEL262152:UEL262194 UOH262152:UOH262194 UYD262152:UYD262194 VHZ262152:VHZ262194 VRV262152:VRV262194 WBR262152:WBR262194 WLN262152:WLN262194 WVJ262152:WVJ262194 B327688:B327730 IX327688:IX327730 ST327688:ST327730 ACP327688:ACP327730 AML327688:AML327730 AWH327688:AWH327730 BGD327688:BGD327730 BPZ327688:BPZ327730 BZV327688:BZV327730 CJR327688:CJR327730 CTN327688:CTN327730 DDJ327688:DDJ327730 DNF327688:DNF327730 DXB327688:DXB327730 EGX327688:EGX327730 EQT327688:EQT327730 FAP327688:FAP327730 FKL327688:FKL327730 FUH327688:FUH327730 GED327688:GED327730 GNZ327688:GNZ327730 GXV327688:GXV327730 HHR327688:HHR327730 HRN327688:HRN327730 IBJ327688:IBJ327730 ILF327688:ILF327730 IVB327688:IVB327730 JEX327688:JEX327730 JOT327688:JOT327730 JYP327688:JYP327730 KIL327688:KIL327730 KSH327688:KSH327730 LCD327688:LCD327730 LLZ327688:LLZ327730 LVV327688:LVV327730 MFR327688:MFR327730 MPN327688:MPN327730 MZJ327688:MZJ327730 NJF327688:NJF327730 NTB327688:NTB327730 OCX327688:OCX327730 OMT327688:OMT327730 OWP327688:OWP327730 PGL327688:PGL327730 PQH327688:PQH327730 QAD327688:QAD327730 QJZ327688:QJZ327730 QTV327688:QTV327730 RDR327688:RDR327730 RNN327688:RNN327730 RXJ327688:RXJ327730 SHF327688:SHF327730 SRB327688:SRB327730 TAX327688:TAX327730 TKT327688:TKT327730 TUP327688:TUP327730 UEL327688:UEL327730 UOH327688:UOH327730 UYD327688:UYD327730 VHZ327688:VHZ327730 VRV327688:VRV327730 WBR327688:WBR327730 WLN327688:WLN327730 WVJ327688:WVJ327730 B393224:B393266 IX393224:IX393266 ST393224:ST393266 ACP393224:ACP393266 AML393224:AML393266 AWH393224:AWH393266 BGD393224:BGD393266 BPZ393224:BPZ393266 BZV393224:BZV393266 CJR393224:CJR393266 CTN393224:CTN393266 DDJ393224:DDJ393266 DNF393224:DNF393266 DXB393224:DXB393266 EGX393224:EGX393266 EQT393224:EQT393266 FAP393224:FAP393266 FKL393224:FKL393266 FUH393224:FUH393266 GED393224:GED393266 GNZ393224:GNZ393266 GXV393224:GXV393266 HHR393224:HHR393266 HRN393224:HRN393266 IBJ393224:IBJ393266 ILF393224:ILF393266 IVB393224:IVB393266 JEX393224:JEX393266 JOT393224:JOT393266 JYP393224:JYP393266 KIL393224:KIL393266 KSH393224:KSH393266 LCD393224:LCD393266 LLZ393224:LLZ393266 LVV393224:LVV393266 MFR393224:MFR393266 MPN393224:MPN393266 MZJ393224:MZJ393266 NJF393224:NJF393266 NTB393224:NTB393266 OCX393224:OCX393266 OMT393224:OMT393266 OWP393224:OWP393266 PGL393224:PGL393266 PQH393224:PQH393266 QAD393224:QAD393266 QJZ393224:QJZ393266 QTV393224:QTV393266 RDR393224:RDR393266 RNN393224:RNN393266 RXJ393224:RXJ393266 SHF393224:SHF393266 SRB393224:SRB393266 TAX393224:TAX393266 TKT393224:TKT393266 TUP393224:TUP393266 UEL393224:UEL393266 UOH393224:UOH393266 UYD393224:UYD393266 VHZ393224:VHZ393266 VRV393224:VRV393266 WBR393224:WBR393266 WLN393224:WLN393266 WVJ393224:WVJ393266 B458760:B458802 IX458760:IX458802 ST458760:ST458802 ACP458760:ACP458802 AML458760:AML458802 AWH458760:AWH458802 BGD458760:BGD458802 BPZ458760:BPZ458802 BZV458760:BZV458802 CJR458760:CJR458802 CTN458760:CTN458802 DDJ458760:DDJ458802 DNF458760:DNF458802 DXB458760:DXB458802 EGX458760:EGX458802 EQT458760:EQT458802 FAP458760:FAP458802 FKL458760:FKL458802 FUH458760:FUH458802 GED458760:GED458802 GNZ458760:GNZ458802 GXV458760:GXV458802 HHR458760:HHR458802 HRN458760:HRN458802 IBJ458760:IBJ458802 ILF458760:ILF458802 IVB458760:IVB458802 JEX458760:JEX458802 JOT458760:JOT458802 JYP458760:JYP458802 KIL458760:KIL458802 KSH458760:KSH458802 LCD458760:LCD458802 LLZ458760:LLZ458802 LVV458760:LVV458802 MFR458760:MFR458802 MPN458760:MPN458802 MZJ458760:MZJ458802 NJF458760:NJF458802 NTB458760:NTB458802 OCX458760:OCX458802 OMT458760:OMT458802 OWP458760:OWP458802 PGL458760:PGL458802 PQH458760:PQH458802 QAD458760:QAD458802 QJZ458760:QJZ458802 QTV458760:QTV458802 RDR458760:RDR458802 RNN458760:RNN458802 RXJ458760:RXJ458802 SHF458760:SHF458802 SRB458760:SRB458802 TAX458760:TAX458802 TKT458760:TKT458802 TUP458760:TUP458802 UEL458760:UEL458802 UOH458760:UOH458802 UYD458760:UYD458802 VHZ458760:VHZ458802 VRV458760:VRV458802 WBR458760:WBR458802 WLN458760:WLN458802 WVJ458760:WVJ458802 B524296:B524338 IX524296:IX524338 ST524296:ST524338 ACP524296:ACP524338 AML524296:AML524338 AWH524296:AWH524338 BGD524296:BGD524338 BPZ524296:BPZ524338 BZV524296:BZV524338 CJR524296:CJR524338 CTN524296:CTN524338 DDJ524296:DDJ524338 DNF524296:DNF524338 DXB524296:DXB524338 EGX524296:EGX524338 EQT524296:EQT524338 FAP524296:FAP524338 FKL524296:FKL524338 FUH524296:FUH524338 GED524296:GED524338 GNZ524296:GNZ524338 GXV524296:GXV524338 HHR524296:HHR524338 HRN524296:HRN524338 IBJ524296:IBJ524338 ILF524296:ILF524338 IVB524296:IVB524338 JEX524296:JEX524338 JOT524296:JOT524338 JYP524296:JYP524338 KIL524296:KIL524338 KSH524296:KSH524338 LCD524296:LCD524338 LLZ524296:LLZ524338 LVV524296:LVV524338 MFR524296:MFR524338 MPN524296:MPN524338 MZJ524296:MZJ524338 NJF524296:NJF524338 NTB524296:NTB524338 OCX524296:OCX524338 OMT524296:OMT524338 OWP524296:OWP524338 PGL524296:PGL524338 PQH524296:PQH524338 QAD524296:QAD524338 QJZ524296:QJZ524338 QTV524296:QTV524338 RDR524296:RDR524338 RNN524296:RNN524338 RXJ524296:RXJ524338 SHF524296:SHF524338 SRB524296:SRB524338 TAX524296:TAX524338 TKT524296:TKT524338 TUP524296:TUP524338 UEL524296:UEL524338 UOH524296:UOH524338 UYD524296:UYD524338 VHZ524296:VHZ524338 VRV524296:VRV524338 WBR524296:WBR524338 WLN524296:WLN524338 WVJ524296:WVJ524338 B589832:B589874 IX589832:IX589874 ST589832:ST589874 ACP589832:ACP589874 AML589832:AML589874 AWH589832:AWH589874 BGD589832:BGD589874 BPZ589832:BPZ589874 BZV589832:BZV589874 CJR589832:CJR589874 CTN589832:CTN589874 DDJ589832:DDJ589874 DNF589832:DNF589874 DXB589832:DXB589874 EGX589832:EGX589874 EQT589832:EQT589874 FAP589832:FAP589874 FKL589832:FKL589874 FUH589832:FUH589874 GED589832:GED589874 GNZ589832:GNZ589874 GXV589832:GXV589874 HHR589832:HHR589874 HRN589832:HRN589874 IBJ589832:IBJ589874 ILF589832:ILF589874 IVB589832:IVB589874 JEX589832:JEX589874 JOT589832:JOT589874 JYP589832:JYP589874 KIL589832:KIL589874 KSH589832:KSH589874 LCD589832:LCD589874 LLZ589832:LLZ589874 LVV589832:LVV589874 MFR589832:MFR589874 MPN589832:MPN589874 MZJ589832:MZJ589874 NJF589832:NJF589874 NTB589832:NTB589874 OCX589832:OCX589874 OMT589832:OMT589874 OWP589832:OWP589874 PGL589832:PGL589874 PQH589832:PQH589874 QAD589832:QAD589874 QJZ589832:QJZ589874 QTV589832:QTV589874 RDR589832:RDR589874 RNN589832:RNN589874 RXJ589832:RXJ589874 SHF589832:SHF589874 SRB589832:SRB589874 TAX589832:TAX589874 TKT589832:TKT589874 TUP589832:TUP589874 UEL589832:UEL589874 UOH589832:UOH589874 UYD589832:UYD589874 VHZ589832:VHZ589874 VRV589832:VRV589874 WBR589832:WBR589874 WLN589832:WLN589874 WVJ589832:WVJ589874 B655368:B655410 IX655368:IX655410 ST655368:ST655410 ACP655368:ACP655410 AML655368:AML655410 AWH655368:AWH655410 BGD655368:BGD655410 BPZ655368:BPZ655410 BZV655368:BZV655410 CJR655368:CJR655410 CTN655368:CTN655410 DDJ655368:DDJ655410 DNF655368:DNF655410 DXB655368:DXB655410 EGX655368:EGX655410 EQT655368:EQT655410 FAP655368:FAP655410 FKL655368:FKL655410 FUH655368:FUH655410 GED655368:GED655410 GNZ655368:GNZ655410 GXV655368:GXV655410 HHR655368:HHR655410 HRN655368:HRN655410 IBJ655368:IBJ655410 ILF655368:ILF655410 IVB655368:IVB655410 JEX655368:JEX655410 JOT655368:JOT655410 JYP655368:JYP655410 KIL655368:KIL655410 KSH655368:KSH655410 LCD655368:LCD655410 LLZ655368:LLZ655410 LVV655368:LVV655410 MFR655368:MFR655410 MPN655368:MPN655410 MZJ655368:MZJ655410 NJF655368:NJF655410 NTB655368:NTB655410 OCX655368:OCX655410 OMT655368:OMT655410 OWP655368:OWP655410 PGL655368:PGL655410 PQH655368:PQH655410 QAD655368:QAD655410 QJZ655368:QJZ655410 QTV655368:QTV655410 RDR655368:RDR655410 RNN655368:RNN655410 RXJ655368:RXJ655410 SHF655368:SHF655410 SRB655368:SRB655410 TAX655368:TAX655410 TKT655368:TKT655410 TUP655368:TUP655410 UEL655368:UEL655410 UOH655368:UOH655410 UYD655368:UYD655410 VHZ655368:VHZ655410 VRV655368:VRV655410 WBR655368:WBR655410 WLN655368:WLN655410 WVJ655368:WVJ655410 B720904:B720946 IX720904:IX720946 ST720904:ST720946 ACP720904:ACP720946 AML720904:AML720946 AWH720904:AWH720946 BGD720904:BGD720946 BPZ720904:BPZ720946 BZV720904:BZV720946 CJR720904:CJR720946 CTN720904:CTN720946 DDJ720904:DDJ720946 DNF720904:DNF720946 DXB720904:DXB720946 EGX720904:EGX720946 EQT720904:EQT720946 FAP720904:FAP720946 FKL720904:FKL720946 FUH720904:FUH720946 GED720904:GED720946 GNZ720904:GNZ720946 GXV720904:GXV720946 HHR720904:HHR720946 HRN720904:HRN720946 IBJ720904:IBJ720946 ILF720904:ILF720946 IVB720904:IVB720946 JEX720904:JEX720946 JOT720904:JOT720946 JYP720904:JYP720946 KIL720904:KIL720946 KSH720904:KSH720946 LCD720904:LCD720946 LLZ720904:LLZ720946 LVV720904:LVV720946 MFR720904:MFR720946 MPN720904:MPN720946 MZJ720904:MZJ720946 NJF720904:NJF720946 NTB720904:NTB720946 OCX720904:OCX720946 OMT720904:OMT720946 OWP720904:OWP720946 PGL720904:PGL720946 PQH720904:PQH720946 QAD720904:QAD720946 QJZ720904:QJZ720946 QTV720904:QTV720946 RDR720904:RDR720946 RNN720904:RNN720946 RXJ720904:RXJ720946 SHF720904:SHF720946 SRB720904:SRB720946 TAX720904:TAX720946 TKT720904:TKT720946 TUP720904:TUP720946 UEL720904:UEL720946 UOH720904:UOH720946 UYD720904:UYD720946 VHZ720904:VHZ720946 VRV720904:VRV720946 WBR720904:WBR720946 WLN720904:WLN720946 WVJ720904:WVJ720946 B786440:B786482 IX786440:IX786482 ST786440:ST786482 ACP786440:ACP786482 AML786440:AML786482 AWH786440:AWH786482 BGD786440:BGD786482 BPZ786440:BPZ786482 BZV786440:BZV786482 CJR786440:CJR786482 CTN786440:CTN786482 DDJ786440:DDJ786482 DNF786440:DNF786482 DXB786440:DXB786482 EGX786440:EGX786482 EQT786440:EQT786482 FAP786440:FAP786482 FKL786440:FKL786482 FUH786440:FUH786482 GED786440:GED786482 GNZ786440:GNZ786482 GXV786440:GXV786482 HHR786440:HHR786482 HRN786440:HRN786482 IBJ786440:IBJ786482 ILF786440:ILF786482 IVB786440:IVB786482 JEX786440:JEX786482 JOT786440:JOT786482 JYP786440:JYP786482 KIL786440:KIL786482 KSH786440:KSH786482 LCD786440:LCD786482 LLZ786440:LLZ786482 LVV786440:LVV786482 MFR786440:MFR786482 MPN786440:MPN786482 MZJ786440:MZJ786482 NJF786440:NJF786482 NTB786440:NTB786482 OCX786440:OCX786482 OMT786440:OMT786482 OWP786440:OWP786482 PGL786440:PGL786482 PQH786440:PQH786482 QAD786440:QAD786482 QJZ786440:QJZ786482 QTV786440:QTV786482 RDR786440:RDR786482 RNN786440:RNN786482 RXJ786440:RXJ786482 SHF786440:SHF786482 SRB786440:SRB786482 TAX786440:TAX786482 TKT786440:TKT786482 TUP786440:TUP786482 UEL786440:UEL786482 UOH786440:UOH786482 UYD786440:UYD786482 VHZ786440:VHZ786482 VRV786440:VRV786482 WBR786440:WBR786482 WLN786440:WLN786482 WVJ786440:WVJ786482 B851976:B852018 IX851976:IX852018 ST851976:ST852018 ACP851976:ACP852018 AML851976:AML852018 AWH851976:AWH852018 BGD851976:BGD852018 BPZ851976:BPZ852018 BZV851976:BZV852018 CJR851976:CJR852018 CTN851976:CTN852018 DDJ851976:DDJ852018 DNF851976:DNF852018 DXB851976:DXB852018 EGX851976:EGX852018 EQT851976:EQT852018 FAP851976:FAP852018 FKL851976:FKL852018 FUH851976:FUH852018 GED851976:GED852018 GNZ851976:GNZ852018 GXV851976:GXV852018 HHR851976:HHR852018 HRN851976:HRN852018 IBJ851976:IBJ852018 ILF851976:ILF852018 IVB851976:IVB852018 JEX851976:JEX852018 JOT851976:JOT852018 JYP851976:JYP852018 KIL851976:KIL852018 KSH851976:KSH852018 LCD851976:LCD852018 LLZ851976:LLZ852018 LVV851976:LVV852018 MFR851976:MFR852018 MPN851976:MPN852018 MZJ851976:MZJ852018 NJF851976:NJF852018 NTB851976:NTB852018 OCX851976:OCX852018 OMT851976:OMT852018 OWP851976:OWP852018 PGL851976:PGL852018 PQH851976:PQH852018 QAD851976:QAD852018 QJZ851976:QJZ852018 QTV851976:QTV852018 RDR851976:RDR852018 RNN851976:RNN852018 RXJ851976:RXJ852018 SHF851976:SHF852018 SRB851976:SRB852018 TAX851976:TAX852018 TKT851976:TKT852018 TUP851976:TUP852018 UEL851976:UEL852018 UOH851976:UOH852018 UYD851976:UYD852018 VHZ851976:VHZ852018 VRV851976:VRV852018 WBR851976:WBR852018 WLN851976:WLN852018 WVJ851976:WVJ852018 B917512:B917554 IX917512:IX917554 ST917512:ST917554 ACP917512:ACP917554 AML917512:AML917554 AWH917512:AWH917554 BGD917512:BGD917554 BPZ917512:BPZ917554 BZV917512:BZV917554 CJR917512:CJR917554 CTN917512:CTN917554 DDJ917512:DDJ917554 DNF917512:DNF917554 DXB917512:DXB917554 EGX917512:EGX917554 EQT917512:EQT917554 FAP917512:FAP917554 FKL917512:FKL917554 FUH917512:FUH917554 GED917512:GED917554 GNZ917512:GNZ917554 GXV917512:GXV917554 HHR917512:HHR917554 HRN917512:HRN917554 IBJ917512:IBJ917554 ILF917512:ILF917554 IVB917512:IVB917554 JEX917512:JEX917554 JOT917512:JOT917554 JYP917512:JYP917554 KIL917512:KIL917554 KSH917512:KSH917554 LCD917512:LCD917554 LLZ917512:LLZ917554 LVV917512:LVV917554 MFR917512:MFR917554 MPN917512:MPN917554 MZJ917512:MZJ917554 NJF917512:NJF917554 NTB917512:NTB917554 OCX917512:OCX917554 OMT917512:OMT917554 OWP917512:OWP917554 PGL917512:PGL917554 PQH917512:PQH917554 QAD917512:QAD917554 QJZ917512:QJZ917554 QTV917512:QTV917554 RDR917512:RDR917554 RNN917512:RNN917554 RXJ917512:RXJ917554 SHF917512:SHF917554 SRB917512:SRB917554 TAX917512:TAX917554 TKT917512:TKT917554 TUP917512:TUP917554 UEL917512:UEL917554 UOH917512:UOH917554 UYD917512:UYD917554 VHZ917512:VHZ917554 VRV917512:VRV917554 WBR917512:WBR917554 WLN917512:WLN917554 WVJ917512:WVJ917554 B983048:B983090 IX983048:IX983090 ST983048:ST983090 ACP983048:ACP983090 AML983048:AML983090 AWH983048:AWH983090 BGD983048:BGD983090 BPZ983048:BPZ983090 BZV983048:BZV983090 CJR983048:CJR983090 CTN983048:CTN983090 DDJ983048:DDJ983090 DNF983048:DNF983090 DXB983048:DXB983090 EGX983048:EGX983090 EQT983048:EQT983090 FAP983048:FAP983090 FKL983048:FKL983090 FUH983048:FUH983090 GED983048:GED983090 GNZ983048:GNZ983090 GXV983048:GXV983090 HHR983048:HHR983090 HRN983048:HRN983090 IBJ983048:IBJ983090 ILF983048:ILF983090 IVB983048:IVB983090 JEX983048:JEX983090 JOT983048:JOT983090 JYP983048:JYP983090 KIL983048:KIL983090 KSH983048:KSH983090 LCD983048:LCD983090 LLZ983048:LLZ983090 LVV983048:LVV983090 MFR983048:MFR983090 MPN983048:MPN983090 MZJ983048:MZJ983090 NJF983048:NJF983090 NTB983048:NTB983090 OCX983048:OCX983090 OMT983048:OMT983090 OWP983048:OWP983090 PGL983048:PGL983090 PQH983048:PQH983090 QAD983048:QAD983090 QJZ983048:QJZ983090 QTV983048:QTV983090 RDR983048:RDR983090 RNN983048:RNN983090 RXJ983048:RXJ983090 SHF983048:SHF983090 SRB983048:SRB983090 TAX983048:TAX983090 TKT983048:TKT983090 TUP983048:TUP983090 UEL983048:UEL983090 UOH983048:UOH983090 UYD983048:UYD983090 VHZ983048:VHZ983090 VRV983048:VRV983090 WBR983048:WBR983090 WLN983048:WLN983090 WVJ983048:WVJ983090" xr:uid="{8CEDB7BC-78C4-41C7-9E12-0C9372650A52}">
       <formula1>8</formula1>
       <formula2>8</formula2>
     </dataValidation>
@@ -15579,530 +15701,530 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A948D5B-AEC9-4E1F-B546-98666C12B045}">
   <dimension ref="A1:AB300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="21" width="2.7109375" style="8" customWidth="1"/>
-    <col min="22" max="22" width="4.42578125" style="8" customWidth="1"/>
-    <col min="23" max="23" width="7.42578125" style="8" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="256" width="11.42578125" style="1"/>
-    <col min="257" max="257" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="21" width="2.7265625" style="8" customWidth="1"/>
+    <col min="22" max="22" width="4.453125" style="8" customWidth="1"/>
+    <col min="23" max="23" width="7.453125" style="8" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="5.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="256" width="11.453125" style="1"/>
+    <col min="257" max="257" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="260" max="277" width="2.7109375" style="1" customWidth="1"/>
-    <col min="278" max="278" width="4.42578125" style="1" customWidth="1"/>
+    <col min="260" max="277" width="2.7265625" style="1" customWidth="1"/>
+    <col min="278" max="278" width="4.453125" style="1" customWidth="1"/>
     <col min="279" max="279" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="280" max="280" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="281" max="512" width="11.42578125" style="1"/>
-    <col min="513" max="513" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="281" max="512" width="11.453125" style="1"/>
+    <col min="513" max="513" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="515" max="515" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="516" max="533" width="2.7109375" style="1" customWidth="1"/>
-    <col min="534" max="534" width="4.42578125" style="1" customWidth="1"/>
+    <col min="516" max="533" width="2.7265625" style="1" customWidth="1"/>
+    <col min="534" max="534" width="4.453125" style="1" customWidth="1"/>
     <col min="535" max="535" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="536" max="536" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="537" max="768" width="11.42578125" style="1"/>
-    <col min="769" max="769" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="536" max="536" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="537" max="768" width="11.453125" style="1"/>
+    <col min="769" max="769" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="771" max="771" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="772" max="789" width="2.7109375" style="1" customWidth="1"/>
-    <col min="790" max="790" width="4.42578125" style="1" customWidth="1"/>
+    <col min="772" max="789" width="2.7265625" style="1" customWidth="1"/>
+    <col min="790" max="790" width="4.453125" style="1" customWidth="1"/>
     <col min="791" max="791" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="792" max="792" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="793" max="1024" width="11.42578125" style="1"/>
-    <col min="1025" max="1025" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="792" max="792" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="793" max="1024" width="11.453125" style="1"/>
+    <col min="1025" max="1025" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1027" max="1027" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1045" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1046" max="1046" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1028" max="1045" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1046" max="1046" width="4.453125" style="1" customWidth="1"/>
     <col min="1047" max="1047" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1048" max="1048" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1049" max="1280" width="11.42578125" style="1"/>
-    <col min="1281" max="1281" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1048" max="1048" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1049" max="1280" width="11.453125" style="1"/>
+    <col min="1281" max="1281" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1283" max="1283" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1301" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1302" max="1302" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1284" max="1301" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1302" max="1302" width="4.453125" style="1" customWidth="1"/>
     <col min="1303" max="1303" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1304" max="1304" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1305" max="1536" width="11.42578125" style="1"/>
-    <col min="1537" max="1537" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1304" max="1304" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1305" max="1536" width="11.453125" style="1"/>
+    <col min="1537" max="1537" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1539" max="1539" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1557" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1558" max="1558" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1540" max="1557" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1558" max="1558" width="4.453125" style="1" customWidth="1"/>
     <col min="1559" max="1559" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1560" max="1560" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1561" max="1792" width="11.42578125" style="1"/>
-    <col min="1793" max="1793" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1560" max="1560" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1561" max="1792" width="11.453125" style="1"/>
+    <col min="1793" max="1793" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="1795" max="1795" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1813" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1814" max="1814" width="4.42578125" style="1" customWidth="1"/>
+    <col min="1796" max="1813" width="2.7265625" style="1" customWidth="1"/>
+    <col min="1814" max="1814" width="4.453125" style="1" customWidth="1"/>
     <col min="1815" max="1815" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="1816" max="1816" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1817" max="2048" width="11.42578125" style="1"/>
-    <col min="2049" max="2049" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1816" max="1816" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1817" max="2048" width="11.453125" style="1"/>
+    <col min="2049" max="2049" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2051" max="2051" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2069" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2070" max="2070" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2052" max="2069" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2070" max="2070" width="4.453125" style="1" customWidth="1"/>
     <col min="2071" max="2071" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2072" max="2072" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2073" max="2304" width="11.42578125" style="1"/>
-    <col min="2305" max="2305" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2072" max="2072" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2073" max="2304" width="11.453125" style="1"/>
+    <col min="2305" max="2305" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2307" max="2307" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2325" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2326" max="2326" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2308" max="2325" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2326" max="2326" width="4.453125" style="1" customWidth="1"/>
     <col min="2327" max="2327" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2328" max="2328" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2329" max="2560" width="11.42578125" style="1"/>
-    <col min="2561" max="2561" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2328" max="2328" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2329" max="2560" width="11.453125" style="1"/>
+    <col min="2561" max="2561" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2563" max="2563" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2581" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2582" max="2582" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2564" max="2581" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2582" max="2582" width="4.453125" style="1" customWidth="1"/>
     <col min="2583" max="2583" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2584" max="2584" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2585" max="2816" width="11.42578125" style="1"/>
-    <col min="2817" max="2817" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2584" max="2584" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2585" max="2816" width="11.453125" style="1"/>
+    <col min="2817" max="2817" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2819" max="2819" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2837" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2838" max="2838" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2820" max="2837" width="2.7265625" style="1" customWidth="1"/>
+    <col min="2838" max="2838" width="4.453125" style="1" customWidth="1"/>
     <col min="2839" max="2839" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2840" max="2840" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2841" max="3072" width="11.42578125" style="1"/>
-    <col min="3073" max="3073" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2840" max="2840" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2841" max="3072" width="11.453125" style="1"/>
+    <col min="3073" max="3073" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3075" max="3075" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3093" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3094" max="3094" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3076" max="3093" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3094" max="3094" width="4.453125" style="1" customWidth="1"/>
     <col min="3095" max="3095" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3096" max="3096" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3097" max="3328" width="11.42578125" style="1"/>
-    <col min="3329" max="3329" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3096" max="3096" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3097" max="3328" width="11.453125" style="1"/>
+    <col min="3329" max="3329" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3331" max="3331" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3349" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3350" max="3350" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3332" max="3349" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3350" max="3350" width="4.453125" style="1" customWidth="1"/>
     <col min="3351" max="3351" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3352" max="3352" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3353" max="3584" width="11.42578125" style="1"/>
-    <col min="3585" max="3585" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3352" max="3352" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3353" max="3584" width="11.453125" style="1"/>
+    <col min="3585" max="3585" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3587" max="3587" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3605" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3606" max="3606" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3588" max="3605" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3606" max="3606" width="4.453125" style="1" customWidth="1"/>
     <col min="3607" max="3607" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3608" max="3608" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3609" max="3840" width="11.42578125" style="1"/>
-    <col min="3841" max="3841" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3608" max="3608" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3609" max="3840" width="11.453125" style="1"/>
+    <col min="3841" max="3841" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3843" max="3843" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3861" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3862" max="3862" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3844" max="3861" width="2.7265625" style="1" customWidth="1"/>
+    <col min="3862" max="3862" width="4.453125" style="1" customWidth="1"/>
     <col min="3863" max="3863" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="3864" max="3864" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3865" max="4096" width="11.42578125" style="1"/>
-    <col min="4097" max="4097" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3864" max="3864" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3865" max="4096" width="11.453125" style="1"/>
+    <col min="4097" max="4097" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4099" max="4099" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4117" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4118" max="4118" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4100" max="4117" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4118" max="4118" width="4.453125" style="1" customWidth="1"/>
     <col min="4119" max="4119" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4120" max="4120" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4121" max="4352" width="11.42578125" style="1"/>
-    <col min="4353" max="4353" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4120" max="4120" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4121" max="4352" width="11.453125" style="1"/>
+    <col min="4353" max="4353" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4355" max="4355" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4373" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4374" max="4374" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4356" max="4373" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4374" max="4374" width="4.453125" style="1" customWidth="1"/>
     <col min="4375" max="4375" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4376" max="4376" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4377" max="4608" width="11.42578125" style="1"/>
-    <col min="4609" max="4609" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4376" max="4376" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4377" max="4608" width="11.453125" style="1"/>
+    <col min="4609" max="4609" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4611" max="4611" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4629" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4630" max="4630" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4612" max="4629" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4630" max="4630" width="4.453125" style="1" customWidth="1"/>
     <col min="4631" max="4631" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4632" max="4632" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4633" max="4864" width="11.42578125" style="1"/>
-    <col min="4865" max="4865" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4632" max="4632" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4633" max="4864" width="11.453125" style="1"/>
+    <col min="4865" max="4865" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4867" max="4867" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4885" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4886" max="4886" width="4.42578125" style="1" customWidth="1"/>
+    <col min="4868" max="4885" width="2.7265625" style="1" customWidth="1"/>
+    <col min="4886" max="4886" width="4.453125" style="1" customWidth="1"/>
     <col min="4887" max="4887" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4888" max="4888" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4889" max="5120" width="11.42578125" style="1"/>
-    <col min="5121" max="5121" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4888" max="4888" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4889" max="5120" width="11.453125" style="1"/>
+    <col min="5121" max="5121" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5123" max="5123" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5141" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5142" max="5142" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5124" max="5141" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5142" max="5142" width="4.453125" style="1" customWidth="1"/>
     <col min="5143" max="5143" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5144" max="5144" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5145" max="5376" width="11.42578125" style="1"/>
-    <col min="5377" max="5377" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5144" max="5144" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5145" max="5376" width="11.453125" style="1"/>
+    <col min="5377" max="5377" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5379" max="5379" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5397" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5398" max="5398" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5380" max="5397" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5398" max="5398" width="4.453125" style="1" customWidth="1"/>
     <col min="5399" max="5399" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5400" max="5400" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5401" max="5632" width="11.42578125" style="1"/>
-    <col min="5633" max="5633" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5400" max="5400" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5401" max="5632" width="11.453125" style="1"/>
+    <col min="5633" max="5633" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5635" max="5635" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5653" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5654" max="5654" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5636" max="5653" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5654" max="5654" width="4.453125" style="1" customWidth="1"/>
     <col min="5655" max="5655" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5656" max="5656" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5657" max="5888" width="11.42578125" style="1"/>
-    <col min="5889" max="5889" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5656" max="5656" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5657" max="5888" width="11.453125" style="1"/>
+    <col min="5889" max="5889" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5891" max="5891" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5909" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5910" max="5910" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5892" max="5909" width="2.7265625" style="1" customWidth="1"/>
+    <col min="5910" max="5910" width="4.453125" style="1" customWidth="1"/>
     <col min="5911" max="5911" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5912" max="5912" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5913" max="6144" width="11.42578125" style="1"/>
-    <col min="6145" max="6145" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5912" max="5912" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5913" max="6144" width="11.453125" style="1"/>
+    <col min="6145" max="6145" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6147" max="6147" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6165" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6166" max="6166" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6148" max="6165" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6166" max="6166" width="4.453125" style="1" customWidth="1"/>
     <col min="6167" max="6167" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6168" max="6168" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6169" max="6400" width="11.42578125" style="1"/>
-    <col min="6401" max="6401" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6168" max="6168" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6169" max="6400" width="11.453125" style="1"/>
+    <col min="6401" max="6401" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6403" max="6403" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6421" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6422" max="6422" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6404" max="6421" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6422" max="6422" width="4.453125" style="1" customWidth="1"/>
     <col min="6423" max="6423" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6424" max="6424" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6425" max="6656" width="11.42578125" style="1"/>
-    <col min="6657" max="6657" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6424" max="6424" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6425" max="6656" width="11.453125" style="1"/>
+    <col min="6657" max="6657" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6659" max="6659" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6677" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6678" max="6678" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6660" max="6677" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6678" max="6678" width="4.453125" style="1" customWidth="1"/>
     <col min="6679" max="6679" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6680" max="6680" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6681" max="6912" width="11.42578125" style="1"/>
-    <col min="6913" max="6913" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6680" max="6680" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6681" max="6912" width="11.453125" style="1"/>
+    <col min="6913" max="6913" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6915" max="6915" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6933" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6934" max="6934" width="4.42578125" style="1" customWidth="1"/>
+    <col min="6916" max="6933" width="2.7265625" style="1" customWidth="1"/>
+    <col min="6934" max="6934" width="4.453125" style="1" customWidth="1"/>
     <col min="6935" max="6935" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6936" max="6936" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6937" max="7168" width="11.42578125" style="1"/>
-    <col min="7169" max="7169" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6936" max="6936" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6937" max="7168" width="11.453125" style="1"/>
+    <col min="7169" max="7169" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7171" max="7171" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7189" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7190" max="7190" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7172" max="7189" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7190" max="7190" width="4.453125" style="1" customWidth="1"/>
     <col min="7191" max="7191" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7192" max="7192" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7193" max="7424" width="11.42578125" style="1"/>
-    <col min="7425" max="7425" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7192" max="7192" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7193" max="7424" width="11.453125" style="1"/>
+    <col min="7425" max="7425" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7427" max="7427" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7445" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7446" max="7446" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7428" max="7445" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7446" max="7446" width="4.453125" style="1" customWidth="1"/>
     <col min="7447" max="7447" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7448" max="7448" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7449" max="7680" width="11.42578125" style="1"/>
-    <col min="7681" max="7681" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7448" max="7448" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7449" max="7680" width="11.453125" style="1"/>
+    <col min="7681" max="7681" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7683" max="7683" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7701" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7702" max="7702" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7684" max="7701" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7702" max="7702" width="4.453125" style="1" customWidth="1"/>
     <col min="7703" max="7703" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7704" max="7704" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7705" max="7936" width="11.42578125" style="1"/>
-    <col min="7937" max="7937" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7704" max="7704" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7705" max="7936" width="11.453125" style="1"/>
+    <col min="7937" max="7937" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7939" max="7939" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7957" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7958" max="7958" width="4.42578125" style="1" customWidth="1"/>
+    <col min="7940" max="7957" width="2.7265625" style="1" customWidth="1"/>
+    <col min="7958" max="7958" width="4.453125" style="1" customWidth="1"/>
     <col min="7959" max="7959" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7960" max="7960" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7961" max="8192" width="11.42578125" style="1"/>
-    <col min="8193" max="8193" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7960" max="7960" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7961" max="8192" width="11.453125" style="1"/>
+    <col min="8193" max="8193" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8195" max="8195" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8213" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8214" max="8214" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8196" max="8213" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8214" max="8214" width="4.453125" style="1" customWidth="1"/>
     <col min="8215" max="8215" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8216" max="8216" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8217" max="8448" width="11.42578125" style="1"/>
-    <col min="8449" max="8449" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8216" max="8216" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8217" max="8448" width="11.453125" style="1"/>
+    <col min="8449" max="8449" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8451" max="8451" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8469" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8470" max="8470" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8452" max="8469" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8470" max="8470" width="4.453125" style="1" customWidth="1"/>
     <col min="8471" max="8471" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8472" max="8472" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8473" max="8704" width="11.42578125" style="1"/>
-    <col min="8705" max="8705" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8472" max="8472" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8473" max="8704" width="11.453125" style="1"/>
+    <col min="8705" max="8705" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8707" max="8707" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8725" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8726" max="8726" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8708" max="8725" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8726" max="8726" width="4.453125" style="1" customWidth="1"/>
     <col min="8727" max="8727" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8728" max="8728" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8729" max="8960" width="11.42578125" style="1"/>
-    <col min="8961" max="8961" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8728" max="8728" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8729" max="8960" width="11.453125" style="1"/>
+    <col min="8961" max="8961" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8963" max="8963" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8981" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8982" max="8982" width="4.42578125" style="1" customWidth="1"/>
+    <col min="8964" max="8981" width="2.7265625" style="1" customWidth="1"/>
+    <col min="8982" max="8982" width="4.453125" style="1" customWidth="1"/>
     <col min="8983" max="8983" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8984" max="8984" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8985" max="9216" width="11.42578125" style="1"/>
-    <col min="9217" max="9217" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8984" max="8984" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8985" max="9216" width="11.453125" style="1"/>
+    <col min="9217" max="9217" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9219" max="9219" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9237" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9238" max="9238" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9220" max="9237" width="2.7265625" style="1" customWidth="1"/>
+    <col min="9238" max="9238" width="4.453125" style="1" customWidth="1"/>
     <col min="9239" max="9239" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9240" max="9240" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9241" max="9472" width="11.42578125" style="1"/>
-    <col min="9473" max="9473" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9240" max="9240" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9241" max="9472" width="11.453125" style="1"/>
+    <col min="9473" max="9473" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9475" max="9475" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9493" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9494" max="9494" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9476" max="9493" width="2.7265625" style="1" customWidth="1"/>
+    <col min="9494" max="9494" width="4.453125" style="1" customWidth="1"/>
     <col min="9495" max="9495" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9496" max="9496" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9497" max="9728" width="11.42578125" style="1"/>
-    <col min="9729" max="9729" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9496" max="9496" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9497" max="9728" width="11.453125" style="1"/>
+    <col min="9729" max="9729" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9731" max="9731" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9749" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9750" max="9750" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9732" max="9749" width="2.7265625" style="1" customWidth="1"/>
+    <col min="9750" max="9750" width="4.453125" style="1" customWidth="1"/>
     <col min="9751" max="9751" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9752" max="9752" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9753" max="9984" width="11.42578125" style="1"/>
-    <col min="9985" max="9985" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9752" max="9752" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9753" max="9984" width="11.453125" style="1"/>
+    <col min="9985" max="9985" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9987" max="9987" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9988" max="10005" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10006" max="10006" width="4.42578125" style="1" customWidth="1"/>
+    <col min="9988" max="10005" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10006" max="10006" width="4.453125" style="1" customWidth="1"/>
     <col min="10007" max="10007" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10008" max="10008" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10009" max="10240" width="11.42578125" style="1"/>
-    <col min="10241" max="10241" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10008" max="10008" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10009" max="10240" width="11.453125" style="1"/>
+    <col min="10241" max="10241" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10243" max="10243" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10261" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10262" max="10262" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10244" max="10261" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10262" max="10262" width="4.453125" style="1" customWidth="1"/>
     <col min="10263" max="10263" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10264" max="10264" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10265" max="10496" width="11.42578125" style="1"/>
-    <col min="10497" max="10497" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10264" max="10264" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10265" max="10496" width="11.453125" style="1"/>
+    <col min="10497" max="10497" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10499" max="10499" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10517" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10518" max="10518" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10500" max="10517" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10518" max="10518" width="4.453125" style="1" customWidth="1"/>
     <col min="10519" max="10519" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10520" max="10520" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10521" max="10752" width="11.42578125" style="1"/>
-    <col min="10753" max="10753" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10520" max="10520" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10521" max="10752" width="11.453125" style="1"/>
+    <col min="10753" max="10753" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10755" max="10755" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10773" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10774" max="10774" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10756" max="10773" width="2.7265625" style="1" customWidth="1"/>
+    <col min="10774" max="10774" width="4.453125" style="1" customWidth="1"/>
     <col min="10775" max="10775" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="10776" max="10776" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10777" max="11008" width="11.42578125" style="1"/>
-    <col min="11009" max="11009" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10776" max="10776" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10777" max="11008" width="11.453125" style="1"/>
+    <col min="11009" max="11009" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11011" max="11011" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11029" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11030" max="11030" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11012" max="11029" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11030" max="11030" width="4.453125" style="1" customWidth="1"/>
     <col min="11031" max="11031" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11032" max="11032" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11033" max="11264" width="11.42578125" style="1"/>
-    <col min="11265" max="11265" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11032" max="11032" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11033" max="11264" width="11.453125" style="1"/>
+    <col min="11265" max="11265" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11267" max="11267" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11285" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11286" max="11286" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11268" max="11285" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11286" max="11286" width="4.453125" style="1" customWidth="1"/>
     <col min="11287" max="11287" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11288" max="11288" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11289" max="11520" width="11.42578125" style="1"/>
-    <col min="11521" max="11521" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11288" max="11288" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11289" max="11520" width="11.453125" style="1"/>
+    <col min="11521" max="11521" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11523" max="11523" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11541" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11542" max="11542" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11524" max="11541" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11542" max="11542" width="4.453125" style="1" customWidth="1"/>
     <col min="11543" max="11543" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11544" max="11544" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11545" max="11776" width="11.42578125" style="1"/>
-    <col min="11777" max="11777" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11544" max="11544" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11545" max="11776" width="11.453125" style="1"/>
+    <col min="11777" max="11777" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11779" max="11779" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11797" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11798" max="11798" width="4.42578125" style="1" customWidth="1"/>
+    <col min="11780" max="11797" width="2.7265625" style="1" customWidth="1"/>
+    <col min="11798" max="11798" width="4.453125" style="1" customWidth="1"/>
     <col min="11799" max="11799" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11800" max="11800" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11801" max="12032" width="11.42578125" style="1"/>
-    <col min="12033" max="12033" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11800" max="11800" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11801" max="12032" width="11.453125" style="1"/>
+    <col min="12033" max="12033" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12035" max="12035" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12053" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12054" max="12054" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12036" max="12053" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12054" max="12054" width="4.453125" style="1" customWidth="1"/>
     <col min="12055" max="12055" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12056" max="12056" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12057" max="12288" width="11.42578125" style="1"/>
-    <col min="12289" max="12289" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12056" max="12056" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12057" max="12288" width="11.453125" style="1"/>
+    <col min="12289" max="12289" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12291" max="12291" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12309" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12310" max="12310" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12292" max="12309" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12310" max="12310" width="4.453125" style="1" customWidth="1"/>
     <col min="12311" max="12311" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12312" max="12312" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12313" max="12544" width="11.42578125" style="1"/>
-    <col min="12545" max="12545" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12312" max="12312" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12313" max="12544" width="11.453125" style="1"/>
+    <col min="12545" max="12545" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12547" max="12547" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12565" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12566" max="12566" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12548" max="12565" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12566" max="12566" width="4.453125" style="1" customWidth="1"/>
     <col min="12567" max="12567" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12568" max="12568" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12569" max="12800" width="11.42578125" style="1"/>
-    <col min="12801" max="12801" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12568" max="12568" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12569" max="12800" width="11.453125" style="1"/>
+    <col min="12801" max="12801" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12803" max="12803" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12821" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12822" max="12822" width="4.42578125" style="1" customWidth="1"/>
+    <col min="12804" max="12821" width="2.7265625" style="1" customWidth="1"/>
+    <col min="12822" max="12822" width="4.453125" style="1" customWidth="1"/>
     <col min="12823" max="12823" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12824" max="12824" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12825" max="13056" width="11.42578125" style="1"/>
-    <col min="13057" max="13057" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12824" max="12824" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12825" max="13056" width="11.453125" style="1"/>
+    <col min="13057" max="13057" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13059" max="13059" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13077" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13078" max="13078" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13060" max="13077" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13078" max="13078" width="4.453125" style="1" customWidth="1"/>
     <col min="13079" max="13079" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13080" max="13080" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13081" max="13312" width="11.42578125" style="1"/>
-    <col min="13313" max="13313" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13080" max="13080" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13081" max="13312" width="11.453125" style="1"/>
+    <col min="13313" max="13313" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13315" max="13315" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13333" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13334" max="13334" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13316" max="13333" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13334" max="13334" width="4.453125" style="1" customWidth="1"/>
     <col min="13335" max="13335" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13336" max="13336" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13337" max="13568" width="11.42578125" style="1"/>
-    <col min="13569" max="13569" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13336" max="13336" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13337" max="13568" width="11.453125" style="1"/>
+    <col min="13569" max="13569" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13571" max="13571" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13589" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13590" max="13590" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13572" max="13589" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13590" max="13590" width="4.453125" style="1" customWidth="1"/>
     <col min="13591" max="13591" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13592" max="13592" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13593" max="13824" width="11.42578125" style="1"/>
-    <col min="13825" max="13825" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13592" max="13592" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13593" max="13824" width="11.453125" style="1"/>
+    <col min="13825" max="13825" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13827" max="13827" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13845" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13846" max="13846" width="4.42578125" style="1" customWidth="1"/>
+    <col min="13828" max="13845" width="2.7265625" style="1" customWidth="1"/>
+    <col min="13846" max="13846" width="4.453125" style="1" customWidth="1"/>
     <col min="13847" max="13847" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13848" max="13848" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13849" max="14080" width="11.42578125" style="1"/>
-    <col min="14081" max="14081" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13848" max="13848" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13849" max="14080" width="11.453125" style="1"/>
+    <col min="14081" max="14081" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14083" max="14083" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14101" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14102" max="14102" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14084" max="14101" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14102" max="14102" width="4.453125" style="1" customWidth="1"/>
     <col min="14103" max="14103" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14104" max="14104" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14105" max="14336" width="11.42578125" style="1"/>
-    <col min="14337" max="14337" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14104" max="14104" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14105" max="14336" width="11.453125" style="1"/>
+    <col min="14337" max="14337" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14339" max="14339" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14357" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14358" max="14358" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14340" max="14357" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14358" max="14358" width="4.453125" style="1" customWidth="1"/>
     <col min="14359" max="14359" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14360" max="14360" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14361" max="14592" width="11.42578125" style="1"/>
-    <col min="14593" max="14593" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14360" max="14360" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14361" max="14592" width="11.453125" style="1"/>
+    <col min="14593" max="14593" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14595" max="14595" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14613" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14614" max="14614" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14596" max="14613" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14614" max="14614" width="4.453125" style="1" customWidth="1"/>
     <col min="14615" max="14615" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14616" max="14616" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14617" max="14848" width="11.42578125" style="1"/>
-    <col min="14849" max="14849" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14616" max="14616" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14617" max="14848" width="11.453125" style="1"/>
+    <col min="14849" max="14849" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="14851" max="14851" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14869" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14870" max="14870" width="4.42578125" style="1" customWidth="1"/>
+    <col min="14852" max="14869" width="2.7265625" style="1" customWidth="1"/>
+    <col min="14870" max="14870" width="4.453125" style="1" customWidth="1"/>
     <col min="14871" max="14871" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14872" max="14872" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14873" max="15104" width="11.42578125" style="1"/>
-    <col min="15105" max="15105" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14872" max="14872" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14873" max="15104" width="11.453125" style="1"/>
+    <col min="15105" max="15105" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15107" max="15107" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15125" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15126" max="15126" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15108" max="15125" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15126" max="15126" width="4.453125" style="1" customWidth="1"/>
     <col min="15127" max="15127" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15128" max="15128" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15129" max="15360" width="11.42578125" style="1"/>
-    <col min="15361" max="15361" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15128" max="15128" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15129" max="15360" width="11.453125" style="1"/>
+    <col min="15361" max="15361" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15363" max="15363" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15381" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15382" max="15382" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15364" max="15381" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15382" max="15382" width="4.453125" style="1" customWidth="1"/>
     <col min="15383" max="15383" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15384" max="15384" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15385" max="15616" width="11.42578125" style="1"/>
-    <col min="15617" max="15617" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15384" max="15384" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15385" max="15616" width="11.453125" style="1"/>
+    <col min="15617" max="15617" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15619" max="15619" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15637" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15638" max="15638" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15620" max="15637" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15638" max="15638" width="4.453125" style="1" customWidth="1"/>
     <col min="15639" max="15639" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15640" max="15640" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15641" max="15872" width="11.42578125" style="1"/>
-    <col min="15873" max="15873" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15640" max="15640" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15641" max="15872" width="11.453125" style="1"/>
+    <col min="15873" max="15873" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="15875" max="15875" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15893" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15894" max="15894" width="4.42578125" style="1" customWidth="1"/>
+    <col min="15876" max="15893" width="2.7265625" style="1" customWidth="1"/>
+    <col min="15894" max="15894" width="4.453125" style="1" customWidth="1"/>
     <col min="15895" max="15895" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15896" max="15896" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15897" max="16128" width="11.42578125" style="1"/>
-    <col min="16129" max="16129" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15896" max="15896" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15897" max="16128" width="11.453125" style="1"/>
+    <col min="16129" max="16129" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="16131" max="16131" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16149" width="2.7109375" style="1" customWidth="1"/>
-    <col min="16150" max="16150" width="4.42578125" style="1" customWidth="1"/>
+    <col min="16132" max="16149" width="2.7265625" style="1" customWidth="1"/>
+    <col min="16150" max="16150" width="4.453125" style="1" customWidth="1"/>
     <col min="16151" max="16151" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="16152" max="16152" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16153" max="16384" width="11.42578125" style="1"/>
+    <col min="16152" max="16152" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16153" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16136,7 +16258,7 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
     </row>
-    <row r="2" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -16166,7 +16288,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
     </row>
-    <row r="3" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -16196,7 +16318,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
     </row>
-    <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -16226,7 +16348,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -16234,7 +16356,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -16317,7 +16439,7 @@
       </c>
       <c r="AB7" s="12"/>
     </row>
-    <row r="8" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>140</v>
       </c>
@@ -16467,7 +16589,7 @@
       </c>
       <c r="Y9" s="8"/>
     </row>
-    <row r="10" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>144</v>
       </c>
@@ -16542,7 +16664,7 @@
       </c>
       <c r="Y10" s="8"/>
     </row>
-    <row r="11" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>
@@ -16617,7 +16739,7 @@
       </c>
       <c r="Y11" s="8"/>
     </row>
-    <row r="12" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>148</v>
       </c>
@@ -16692,7 +16814,7 @@
       </c>
       <c r="Y12" s="8"/>
     </row>
-    <row r="13" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>150</v>
       </c>
@@ -16767,7 +16889,7 @@
       </c>
       <c r="Y13" s="8"/>
     </row>
-    <row r="14" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>152</v>
       </c>
@@ -16842,7 +16964,7 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="15" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>154</v>
       </c>
@@ -16917,7 +17039,7 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="16" spans="1:28" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>156</v>
       </c>
@@ -16992,7 +17114,7 @@
       </c>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>158</v>
       </c>
@@ -17067,7 +17189,7 @@
       </c>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>160</v>
       </c>
@@ -17142,7 +17264,7 @@
       </c>
       <c r="Y18" s="8"/>
     </row>
-    <row r="19" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>162</v>
       </c>
@@ -17217,7 +17339,7 @@
       </c>
       <c r="Y19" s="8"/>
     </row>
-    <row r="20" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>164</v>
       </c>
@@ -17292,7 +17414,7 @@
       </c>
       <c r="Y20" s="8"/>
     </row>
-    <row r="21" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>166</v>
       </c>
@@ -17442,7 +17564,7 @@
       </c>
       <c r="Y22" s="8"/>
     </row>
-    <row r="23" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>170</v>
       </c>
@@ -17517,7 +17639,7 @@
       </c>
       <c r="Y23" s="8"/>
     </row>
-    <row r="24" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -17592,7 +17714,7 @@
       </c>
       <c r="Y24" s="8"/>
     </row>
-    <row r="25" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>174</v>
       </c>
@@ -17667,7 +17789,7 @@
       </c>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>176</v>
       </c>
@@ -22032,7 +22154,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B50 IX8:IX50 ST8:ST50 ACP8:ACP50 AML8:AML50 AWH8:AWH50 BGD8:BGD50 BPZ8:BPZ50 BZV8:BZV50 CJR8:CJR50 CTN8:CTN50 DDJ8:DDJ50 DNF8:DNF50 DXB8:DXB50 EGX8:EGX50 EQT8:EQT50 FAP8:FAP50 FKL8:FKL50 FUH8:FUH50 GED8:GED50 GNZ8:GNZ50 GXV8:GXV50 HHR8:HHR50 HRN8:HRN50 IBJ8:IBJ50 ILF8:ILF50 IVB8:IVB50 JEX8:JEX50 JOT8:JOT50 JYP8:JYP50 KIL8:KIL50 KSH8:KSH50 LCD8:LCD50 LLZ8:LLZ50 LVV8:LVV50 MFR8:MFR50 MPN8:MPN50 MZJ8:MZJ50 NJF8:NJF50 NTB8:NTB50 OCX8:OCX50 OMT8:OMT50 OWP8:OWP50 PGL8:PGL50 PQH8:PQH50 QAD8:QAD50 QJZ8:QJZ50 QTV8:QTV50 RDR8:RDR50 RNN8:RNN50 RXJ8:RXJ50 SHF8:SHF50 SRB8:SRB50 TAX8:TAX50 TKT8:TKT50 TUP8:TUP50 UEL8:UEL50 UOH8:UOH50 UYD8:UYD50 VHZ8:VHZ50 VRV8:VRV50 WBR8:WBR50 WLN8:WLN50 WVJ8:WVJ50 B65544:B65586 IX65544:IX65586 ST65544:ST65586 ACP65544:ACP65586 AML65544:AML65586 AWH65544:AWH65586 BGD65544:BGD65586 BPZ65544:BPZ65586 BZV65544:BZV65586 CJR65544:CJR65586 CTN65544:CTN65586 DDJ65544:DDJ65586 DNF65544:DNF65586 DXB65544:DXB65586 EGX65544:EGX65586 EQT65544:EQT65586 FAP65544:FAP65586 FKL65544:FKL65586 FUH65544:FUH65586 GED65544:GED65586 GNZ65544:GNZ65586 GXV65544:GXV65586 HHR65544:HHR65586 HRN65544:HRN65586 IBJ65544:IBJ65586 ILF65544:ILF65586 IVB65544:IVB65586 JEX65544:JEX65586 JOT65544:JOT65586 JYP65544:JYP65586 KIL65544:KIL65586 KSH65544:KSH65586 LCD65544:LCD65586 LLZ65544:LLZ65586 LVV65544:LVV65586 MFR65544:MFR65586 MPN65544:MPN65586 MZJ65544:MZJ65586 NJF65544:NJF65586 NTB65544:NTB65586 OCX65544:OCX65586 OMT65544:OMT65586 OWP65544:OWP65586 PGL65544:PGL65586 PQH65544:PQH65586 QAD65544:QAD65586 QJZ65544:QJZ65586 QTV65544:QTV65586 RDR65544:RDR65586 RNN65544:RNN65586 RXJ65544:RXJ65586 SHF65544:SHF65586 SRB65544:SRB65586 TAX65544:TAX65586 TKT65544:TKT65586 TUP65544:TUP65586 UEL65544:UEL65586 UOH65544:UOH65586 UYD65544:UYD65586 VHZ65544:VHZ65586 VRV65544:VRV65586 WBR65544:WBR65586 WLN65544:WLN65586 WVJ65544:WVJ65586 B131080:B131122 IX131080:IX131122 ST131080:ST131122 ACP131080:ACP131122 AML131080:AML131122 AWH131080:AWH131122 BGD131080:BGD131122 BPZ131080:BPZ131122 BZV131080:BZV131122 CJR131080:CJR131122 CTN131080:CTN131122 DDJ131080:DDJ131122 DNF131080:DNF131122 DXB131080:DXB131122 EGX131080:EGX131122 EQT131080:EQT131122 FAP131080:FAP131122 FKL131080:FKL131122 FUH131080:FUH131122 GED131080:GED131122 GNZ131080:GNZ131122 GXV131080:GXV131122 HHR131080:HHR131122 HRN131080:HRN131122 IBJ131080:IBJ131122 ILF131080:ILF131122 IVB131080:IVB131122 JEX131080:JEX131122 JOT131080:JOT131122 JYP131080:JYP131122 KIL131080:KIL131122 KSH131080:KSH131122 LCD131080:LCD131122 LLZ131080:LLZ131122 LVV131080:LVV131122 MFR131080:MFR131122 MPN131080:MPN131122 MZJ131080:MZJ131122 NJF131080:NJF131122 NTB131080:NTB131122 OCX131080:OCX131122 OMT131080:OMT131122 OWP131080:OWP131122 PGL131080:PGL131122 PQH131080:PQH131122 QAD131080:QAD131122 QJZ131080:QJZ131122 QTV131080:QTV131122 RDR131080:RDR131122 RNN131080:RNN131122 RXJ131080:RXJ131122 SHF131080:SHF131122 SRB131080:SRB131122 TAX131080:TAX131122 TKT131080:TKT131122 TUP131080:TUP131122 UEL131080:UEL131122 UOH131080:UOH131122 UYD131080:UYD131122 VHZ131080:VHZ131122 VRV131080:VRV131122 WBR131080:WBR131122 WLN131080:WLN131122 WVJ131080:WVJ131122 B196616:B196658 IX196616:IX196658 ST196616:ST196658 ACP196616:ACP196658 AML196616:AML196658 AWH196616:AWH196658 BGD196616:BGD196658 BPZ196616:BPZ196658 BZV196616:BZV196658 CJR196616:CJR196658 CTN196616:CTN196658 DDJ196616:DDJ196658 DNF196616:DNF196658 DXB196616:DXB196658 EGX196616:EGX196658 EQT196616:EQT196658 FAP196616:FAP196658 FKL196616:FKL196658 FUH196616:FUH196658 GED196616:GED196658 GNZ196616:GNZ196658 GXV196616:GXV196658 HHR196616:HHR196658 HRN196616:HRN196658 IBJ196616:IBJ196658 ILF196616:ILF196658 IVB196616:IVB196658 JEX196616:JEX196658 JOT196616:JOT196658 JYP196616:JYP196658 KIL196616:KIL196658 KSH196616:KSH196658 LCD196616:LCD196658 LLZ196616:LLZ196658 LVV196616:LVV196658 MFR196616:MFR196658 MPN196616:MPN196658 MZJ196616:MZJ196658 NJF196616:NJF196658 NTB196616:NTB196658 OCX196616:OCX196658 OMT196616:OMT196658 OWP196616:OWP196658 PGL196616:PGL196658 PQH196616:PQH196658 QAD196616:QAD196658 QJZ196616:QJZ196658 QTV196616:QTV196658 RDR196616:RDR196658 RNN196616:RNN196658 RXJ196616:RXJ196658 SHF196616:SHF196658 SRB196616:SRB196658 TAX196616:TAX196658 TKT196616:TKT196658 TUP196616:TUP196658 UEL196616:UEL196658 UOH196616:UOH196658 UYD196616:UYD196658 VHZ196616:VHZ196658 VRV196616:VRV196658 WBR196616:WBR196658 WLN196616:WLN196658 WVJ196616:WVJ196658 B262152:B262194 IX262152:IX262194 ST262152:ST262194 ACP262152:ACP262194 AML262152:AML262194 AWH262152:AWH262194 BGD262152:BGD262194 BPZ262152:BPZ262194 BZV262152:BZV262194 CJR262152:CJR262194 CTN262152:CTN262194 DDJ262152:DDJ262194 DNF262152:DNF262194 DXB262152:DXB262194 EGX262152:EGX262194 EQT262152:EQT262194 FAP262152:FAP262194 FKL262152:FKL262194 FUH262152:FUH262194 GED262152:GED262194 GNZ262152:GNZ262194 GXV262152:GXV262194 HHR262152:HHR262194 HRN262152:HRN262194 IBJ262152:IBJ262194 ILF262152:ILF262194 IVB262152:IVB262194 JEX262152:JEX262194 JOT262152:JOT262194 JYP262152:JYP262194 KIL262152:KIL262194 KSH262152:KSH262194 LCD262152:LCD262194 LLZ262152:LLZ262194 LVV262152:LVV262194 MFR262152:MFR262194 MPN262152:MPN262194 MZJ262152:MZJ262194 NJF262152:NJF262194 NTB262152:NTB262194 OCX262152:OCX262194 OMT262152:OMT262194 OWP262152:OWP262194 PGL262152:PGL262194 PQH262152:PQH262194 QAD262152:QAD262194 QJZ262152:QJZ262194 QTV262152:QTV262194 RDR262152:RDR262194 RNN262152:RNN262194 RXJ262152:RXJ262194 SHF262152:SHF262194 SRB262152:SRB262194 TAX262152:TAX262194 TKT262152:TKT262194 TUP262152:TUP262194 UEL262152:UEL262194 UOH262152:UOH262194 UYD262152:UYD262194 VHZ262152:VHZ262194 VRV262152:VRV262194 WBR262152:WBR262194 WLN262152:WLN262194 WVJ262152:WVJ262194 B327688:B327730 IX327688:IX327730 ST327688:ST327730 ACP327688:ACP327730 AML327688:AML327730 AWH327688:AWH327730 BGD327688:BGD327730 BPZ327688:BPZ327730 BZV327688:BZV327730 CJR327688:CJR327730 CTN327688:CTN327730 DDJ327688:DDJ327730 DNF327688:DNF327730 DXB327688:DXB327730 EGX327688:EGX327730 EQT327688:EQT327730 FAP327688:FAP327730 FKL327688:FKL327730 FUH327688:FUH327730 GED327688:GED327730 GNZ327688:GNZ327730 GXV327688:GXV327730 HHR327688:HHR327730 HRN327688:HRN327730 IBJ327688:IBJ327730 ILF327688:ILF327730 IVB327688:IVB327730 JEX327688:JEX327730 JOT327688:JOT327730 JYP327688:JYP327730 KIL327688:KIL327730 KSH327688:KSH327730 LCD327688:LCD327730 LLZ327688:LLZ327730 LVV327688:LVV327730 MFR327688:MFR327730 MPN327688:MPN327730 MZJ327688:MZJ327730 NJF327688:NJF327730 NTB327688:NTB327730 OCX327688:OCX327730 OMT327688:OMT327730 OWP327688:OWP327730 PGL327688:PGL327730 PQH327688:PQH327730 QAD327688:QAD327730 QJZ327688:QJZ327730 QTV327688:QTV327730 RDR327688:RDR327730 RNN327688:RNN327730 RXJ327688:RXJ327730 SHF327688:SHF327730 SRB327688:SRB327730 TAX327688:TAX327730 TKT327688:TKT327730 TUP327688:TUP327730 UEL327688:UEL327730 UOH327688:UOH327730 UYD327688:UYD327730 VHZ327688:VHZ327730 VRV327688:VRV327730 WBR327688:WBR327730 WLN327688:WLN327730 WVJ327688:WVJ327730 B393224:B393266 IX393224:IX393266 ST393224:ST393266 ACP393224:ACP393266 AML393224:AML393266 AWH393224:AWH393266 BGD393224:BGD393266 BPZ393224:BPZ393266 BZV393224:BZV393266 CJR393224:CJR393266 CTN393224:CTN393266 DDJ393224:DDJ393266 DNF393224:DNF393266 DXB393224:DXB393266 EGX393224:EGX393266 EQT393224:EQT393266 FAP393224:FAP393266 FKL393224:FKL393266 FUH393224:FUH393266 GED393224:GED393266 GNZ393224:GNZ393266 GXV393224:GXV393266 HHR393224:HHR393266 HRN393224:HRN393266 IBJ393224:IBJ393266 ILF393224:ILF393266 IVB393224:IVB393266 JEX393224:JEX393266 JOT393224:JOT393266 JYP393224:JYP393266 KIL393224:KIL393266 KSH393224:KSH393266 LCD393224:LCD393266 LLZ393224:LLZ393266 LVV393224:LVV393266 MFR393224:MFR393266 MPN393224:MPN393266 MZJ393224:MZJ393266 NJF393224:NJF393266 NTB393224:NTB393266 OCX393224:OCX393266 OMT393224:OMT393266 OWP393224:OWP393266 PGL393224:PGL393266 PQH393224:PQH393266 QAD393224:QAD393266 QJZ393224:QJZ393266 QTV393224:QTV393266 RDR393224:RDR393266 RNN393224:RNN393266 RXJ393224:RXJ393266 SHF393224:SHF393266 SRB393224:SRB393266 TAX393224:TAX393266 TKT393224:TKT393266 TUP393224:TUP393266 UEL393224:UEL393266 UOH393224:UOH393266 UYD393224:UYD393266 VHZ393224:VHZ393266 VRV393224:VRV393266 WBR393224:WBR393266 WLN393224:WLN393266 WVJ393224:WVJ393266 B458760:B458802 IX458760:IX458802 ST458760:ST458802 ACP458760:ACP458802 AML458760:AML458802 AWH458760:AWH458802 BGD458760:BGD458802 BPZ458760:BPZ458802 BZV458760:BZV458802 CJR458760:CJR458802 CTN458760:CTN458802 DDJ458760:DDJ458802 DNF458760:DNF458802 DXB458760:DXB458802 EGX458760:EGX458802 EQT458760:EQT458802 FAP458760:FAP458802 FKL458760:FKL458802 FUH458760:FUH458802 GED458760:GED458802 GNZ458760:GNZ458802 GXV458760:GXV458802 HHR458760:HHR458802 HRN458760:HRN458802 IBJ458760:IBJ458802 ILF458760:ILF458802 IVB458760:IVB458802 JEX458760:JEX458802 JOT458760:JOT458802 JYP458760:JYP458802 KIL458760:KIL458802 KSH458760:KSH458802 LCD458760:LCD458802 LLZ458760:LLZ458802 LVV458760:LVV458802 MFR458760:MFR458802 MPN458760:MPN458802 MZJ458760:MZJ458802 NJF458760:NJF458802 NTB458760:NTB458802 OCX458760:OCX458802 OMT458760:OMT458802 OWP458760:OWP458802 PGL458760:PGL458802 PQH458760:PQH458802 QAD458760:QAD458802 QJZ458760:QJZ458802 QTV458760:QTV458802 RDR458760:RDR458802 RNN458760:RNN458802 RXJ458760:RXJ458802 SHF458760:SHF458802 SRB458760:SRB458802 TAX458760:TAX458802 TKT458760:TKT458802 TUP458760:TUP458802 UEL458760:UEL458802 UOH458760:UOH458802 UYD458760:UYD458802 VHZ458760:VHZ458802 VRV458760:VRV458802 WBR458760:WBR458802 WLN458760:WLN458802 WVJ458760:WVJ458802 B524296:B524338 IX524296:IX524338 ST524296:ST524338 ACP524296:ACP524338 AML524296:AML524338 AWH524296:AWH524338 BGD524296:BGD524338 BPZ524296:BPZ524338 BZV524296:BZV524338 CJR524296:CJR524338 CTN524296:CTN524338 DDJ524296:DDJ524338 DNF524296:DNF524338 DXB524296:DXB524338 EGX524296:EGX524338 EQT524296:EQT524338 FAP524296:FAP524338 FKL524296:FKL524338 FUH524296:FUH524338 GED524296:GED524338 GNZ524296:GNZ524338 GXV524296:GXV524338 HHR524296:HHR524338 HRN524296:HRN524338 IBJ524296:IBJ524338 ILF524296:ILF524338 IVB524296:IVB524338 JEX524296:JEX524338 JOT524296:JOT524338 JYP524296:JYP524338 KIL524296:KIL524338 KSH524296:KSH524338 LCD524296:LCD524338 LLZ524296:LLZ524338 LVV524296:LVV524338 MFR524296:MFR524338 MPN524296:MPN524338 MZJ524296:MZJ524338 NJF524296:NJF524338 NTB524296:NTB524338 OCX524296:OCX524338 OMT524296:OMT524338 OWP524296:OWP524338 PGL524296:PGL524338 PQH524296:PQH524338 QAD524296:QAD524338 QJZ524296:QJZ524338 QTV524296:QTV524338 RDR524296:RDR524338 RNN524296:RNN524338 RXJ524296:RXJ524338 SHF524296:SHF524338 SRB524296:SRB524338 TAX524296:TAX524338 TKT524296:TKT524338 TUP524296:TUP524338 UEL524296:UEL524338 UOH524296:UOH524338 UYD524296:UYD524338 VHZ524296:VHZ524338 VRV524296:VRV524338 WBR524296:WBR524338 WLN524296:WLN524338 WVJ524296:WVJ524338 B589832:B589874 IX589832:IX589874 ST589832:ST589874 ACP589832:ACP589874 AML589832:AML589874 AWH589832:AWH589874 BGD589832:BGD589874 BPZ589832:BPZ589874 BZV589832:BZV589874 CJR589832:CJR589874 CTN589832:CTN589874 DDJ589832:DDJ589874 DNF589832:DNF589874 DXB589832:DXB589874 EGX589832:EGX589874 EQT589832:EQT589874 FAP589832:FAP589874 FKL589832:FKL589874 FUH589832:FUH589874 GED589832:GED589874 GNZ589832:GNZ589874 GXV589832:GXV589874 HHR589832:HHR589874 HRN589832:HRN589874 IBJ589832:IBJ589874 ILF589832:ILF589874 IVB589832:IVB589874 JEX589832:JEX589874 JOT589832:JOT589874 JYP589832:JYP589874 KIL589832:KIL589874 KSH589832:KSH589874 LCD589832:LCD589874 LLZ589832:LLZ589874 LVV589832:LVV589874 MFR589832:MFR589874 MPN589832:MPN589874 MZJ589832:MZJ589874 NJF589832:NJF589874 NTB589832:NTB589874 OCX589832:OCX589874 OMT589832:OMT589874 OWP589832:OWP589874 PGL589832:PGL589874 PQH589832:PQH589874 QAD589832:QAD589874 QJZ589832:QJZ589874 QTV589832:QTV589874 RDR589832:RDR589874 RNN589832:RNN589874 RXJ589832:RXJ589874 SHF589832:SHF589874 SRB589832:SRB589874 TAX589832:TAX589874 TKT589832:TKT589874 TUP589832:TUP589874 UEL589832:UEL589874 UOH589832:UOH589874 UYD589832:UYD589874 VHZ589832:VHZ589874 VRV589832:VRV589874 WBR589832:WBR589874 WLN589832:WLN589874 WVJ589832:WVJ589874 B655368:B655410 IX655368:IX655410 ST655368:ST655410 ACP655368:ACP655410 AML655368:AML655410 AWH655368:AWH655410 BGD655368:BGD655410 BPZ655368:BPZ655410 BZV655368:BZV655410 CJR655368:CJR655410 CTN655368:CTN655410 DDJ655368:DDJ655410 DNF655368:DNF655410 DXB655368:DXB655410 EGX655368:EGX655410 EQT655368:EQT655410 FAP655368:FAP655410 FKL655368:FKL655410 FUH655368:FUH655410 GED655368:GED655410 GNZ655368:GNZ655410 GXV655368:GXV655410 HHR655368:HHR655410 HRN655368:HRN655410 IBJ655368:IBJ655410 ILF655368:ILF655410 IVB655368:IVB655410 JEX655368:JEX655410 JOT655368:JOT655410 JYP655368:JYP655410 KIL655368:KIL655410 KSH655368:KSH655410 LCD655368:LCD655410 LLZ655368:LLZ655410 LVV655368:LVV655410 MFR655368:MFR655410 MPN655368:MPN655410 MZJ655368:MZJ655410 NJF655368:NJF655410 NTB655368:NTB655410 OCX655368:OCX655410 OMT655368:OMT655410 OWP655368:OWP655410 PGL655368:PGL655410 PQH655368:PQH655410 QAD655368:QAD655410 QJZ655368:QJZ655410 QTV655368:QTV655410 RDR655368:RDR655410 RNN655368:RNN655410 RXJ655368:RXJ655410 SHF655368:SHF655410 SRB655368:SRB655410 TAX655368:TAX655410 TKT655368:TKT655410 TUP655368:TUP655410 UEL655368:UEL655410 UOH655368:UOH655410 UYD655368:UYD655410 VHZ655368:VHZ655410 VRV655368:VRV655410 WBR655368:WBR655410 WLN655368:WLN655410 WVJ655368:WVJ655410 B720904:B720946 IX720904:IX720946 ST720904:ST720946 ACP720904:ACP720946 AML720904:AML720946 AWH720904:AWH720946 BGD720904:BGD720946 BPZ720904:BPZ720946 BZV720904:BZV720946 CJR720904:CJR720946 CTN720904:CTN720946 DDJ720904:DDJ720946 DNF720904:DNF720946 DXB720904:DXB720946 EGX720904:EGX720946 EQT720904:EQT720946 FAP720904:FAP720946 FKL720904:FKL720946 FUH720904:FUH720946 GED720904:GED720946 GNZ720904:GNZ720946 GXV720904:GXV720946 HHR720904:HHR720946 HRN720904:HRN720946 IBJ720904:IBJ720946 ILF720904:ILF720946 IVB720904:IVB720946 JEX720904:JEX720946 JOT720904:JOT720946 JYP720904:JYP720946 KIL720904:KIL720946 KSH720904:KSH720946 LCD720904:LCD720946 LLZ720904:LLZ720946 LVV720904:LVV720946 MFR720904:MFR720946 MPN720904:MPN720946 MZJ720904:MZJ720946 NJF720904:NJF720946 NTB720904:NTB720946 OCX720904:OCX720946 OMT720904:OMT720946 OWP720904:OWP720946 PGL720904:PGL720946 PQH720904:PQH720946 QAD720904:QAD720946 QJZ720904:QJZ720946 QTV720904:QTV720946 RDR720904:RDR720946 RNN720904:RNN720946 RXJ720904:RXJ720946 SHF720904:SHF720946 SRB720904:SRB720946 TAX720904:TAX720946 TKT720904:TKT720946 TUP720904:TUP720946 UEL720904:UEL720946 UOH720904:UOH720946 UYD720904:UYD720946 VHZ720904:VHZ720946 VRV720904:VRV720946 WBR720904:WBR720946 WLN720904:WLN720946 WVJ720904:WVJ720946 B786440:B786482 IX786440:IX786482 ST786440:ST786482 ACP786440:ACP786482 AML786440:AML786482 AWH786440:AWH786482 BGD786440:BGD786482 BPZ786440:BPZ786482 BZV786440:BZV786482 CJR786440:CJR786482 CTN786440:CTN786482 DDJ786440:DDJ786482 DNF786440:DNF786482 DXB786440:DXB786482 EGX786440:EGX786482 EQT786440:EQT786482 FAP786440:FAP786482 FKL786440:FKL786482 FUH786440:FUH786482 GED786440:GED786482 GNZ786440:GNZ786482 GXV786440:GXV786482 HHR786440:HHR786482 HRN786440:HRN786482 IBJ786440:IBJ786482 ILF786440:ILF786482 IVB786440:IVB786482 JEX786440:JEX786482 JOT786440:JOT786482 JYP786440:JYP786482 KIL786440:KIL786482 KSH786440:KSH786482 LCD786440:LCD786482 LLZ786440:LLZ786482 LVV786440:LVV786482 MFR786440:MFR786482 MPN786440:MPN786482 MZJ786440:MZJ786482 NJF786440:NJF786482 NTB786440:NTB786482 OCX786440:OCX786482 OMT786440:OMT786482 OWP786440:OWP786482 PGL786440:PGL786482 PQH786440:PQH786482 QAD786440:QAD786482 QJZ786440:QJZ786482 QTV786440:QTV786482 RDR786440:RDR786482 RNN786440:RNN786482 RXJ786440:RXJ786482 SHF786440:SHF786482 SRB786440:SRB786482 TAX786440:TAX786482 TKT786440:TKT786482 TUP786440:TUP786482 UEL786440:UEL786482 UOH786440:UOH786482 UYD786440:UYD786482 VHZ786440:VHZ786482 VRV786440:VRV786482 WBR786440:WBR786482 WLN786440:WLN786482 WVJ786440:WVJ786482 B851976:B852018 IX851976:IX852018 ST851976:ST852018 ACP851976:ACP852018 AML851976:AML852018 AWH851976:AWH852018 BGD851976:BGD852018 BPZ851976:BPZ852018 BZV851976:BZV852018 CJR851976:CJR852018 CTN851976:CTN852018 DDJ851976:DDJ852018 DNF851976:DNF852018 DXB851976:DXB852018 EGX851976:EGX852018 EQT851976:EQT852018 FAP851976:FAP852018 FKL851976:FKL852018 FUH851976:FUH852018 GED851976:GED852018 GNZ851976:GNZ852018 GXV851976:GXV852018 HHR851976:HHR852018 HRN851976:HRN852018 IBJ851976:IBJ852018 ILF851976:ILF852018 IVB851976:IVB852018 JEX851976:JEX852018 JOT851976:JOT852018 JYP851976:JYP852018 KIL851976:KIL852018 KSH851976:KSH852018 LCD851976:LCD852018 LLZ851976:LLZ852018 LVV851976:LVV852018 MFR851976:MFR852018 MPN851976:MPN852018 MZJ851976:MZJ852018 NJF851976:NJF852018 NTB851976:NTB852018 OCX851976:OCX852018 OMT851976:OMT852018 OWP851976:OWP852018 PGL851976:PGL852018 PQH851976:PQH852018 QAD851976:QAD852018 QJZ851976:QJZ852018 QTV851976:QTV852018 RDR851976:RDR852018 RNN851976:RNN852018 RXJ851976:RXJ852018 SHF851976:SHF852018 SRB851976:SRB852018 TAX851976:TAX852018 TKT851976:TKT852018 TUP851976:TUP852018 UEL851976:UEL852018 UOH851976:UOH852018 UYD851976:UYD852018 VHZ851976:VHZ852018 VRV851976:VRV852018 WBR851976:WBR852018 WLN851976:WLN852018 WVJ851976:WVJ852018 B917512:B917554 IX917512:IX917554 ST917512:ST917554 ACP917512:ACP917554 AML917512:AML917554 AWH917512:AWH917554 BGD917512:BGD917554 BPZ917512:BPZ917554 BZV917512:BZV917554 CJR917512:CJR917554 CTN917512:CTN917554 DDJ917512:DDJ917554 DNF917512:DNF917554 DXB917512:DXB917554 EGX917512:EGX917554 EQT917512:EQT917554 FAP917512:FAP917554 FKL917512:FKL917554 FUH917512:FUH917554 GED917512:GED917554 GNZ917512:GNZ917554 GXV917512:GXV917554 HHR917512:HHR917554 HRN917512:HRN917554 IBJ917512:IBJ917554 ILF917512:ILF917554 IVB917512:IVB917554 JEX917512:JEX917554 JOT917512:JOT917554 JYP917512:JYP917554 KIL917512:KIL917554 KSH917512:KSH917554 LCD917512:LCD917554 LLZ917512:LLZ917554 LVV917512:LVV917554 MFR917512:MFR917554 MPN917512:MPN917554 MZJ917512:MZJ917554 NJF917512:NJF917554 NTB917512:NTB917554 OCX917512:OCX917554 OMT917512:OMT917554 OWP917512:OWP917554 PGL917512:PGL917554 PQH917512:PQH917554 QAD917512:QAD917554 QJZ917512:QJZ917554 QTV917512:QTV917554 RDR917512:RDR917554 RNN917512:RNN917554 RXJ917512:RXJ917554 SHF917512:SHF917554 SRB917512:SRB917554 TAX917512:TAX917554 TKT917512:TKT917554 TUP917512:TUP917554 UEL917512:UEL917554 UOH917512:UOH917554 UYD917512:UYD917554 VHZ917512:VHZ917554 VRV917512:VRV917554 WBR917512:WBR917554 WLN917512:WLN917554 WVJ917512:WVJ917554 B983048:B983090 IX983048:IX983090 ST983048:ST983090 ACP983048:ACP983090 AML983048:AML983090 AWH983048:AWH983090 BGD983048:BGD983090 BPZ983048:BPZ983090 BZV983048:BZV983090 CJR983048:CJR983090 CTN983048:CTN983090 DDJ983048:DDJ983090 DNF983048:DNF983090 DXB983048:DXB983090 EGX983048:EGX983090 EQT983048:EQT983090 FAP983048:FAP983090 FKL983048:FKL983090 FUH983048:FUH983090 GED983048:GED983090 GNZ983048:GNZ983090 GXV983048:GXV983090 HHR983048:HHR983090 HRN983048:HRN983090 IBJ983048:IBJ983090 ILF983048:ILF983090 IVB983048:IVB983090 JEX983048:JEX983090 JOT983048:JOT983090 JYP983048:JYP983090 KIL983048:KIL983090 KSH983048:KSH983090 LCD983048:LCD983090 LLZ983048:LLZ983090 LVV983048:LVV983090 MFR983048:MFR983090 MPN983048:MPN983090 MZJ983048:MZJ983090 NJF983048:NJF983090 NTB983048:NTB983090 OCX983048:OCX983090 OMT983048:OMT983090 OWP983048:OWP983090 PGL983048:PGL983090 PQH983048:PQH983090 QAD983048:QAD983090 QJZ983048:QJZ983090 QTV983048:QTV983090 RDR983048:RDR983090 RNN983048:RNN983090 RXJ983048:RXJ983090 SHF983048:SHF983090 SRB983048:SRB983090 TAX983048:TAX983090 TKT983048:TKT983090 TUP983048:TUP983090 UEL983048:UEL983090 UOH983048:UOH983090 UYD983048:UYD983090 VHZ983048:VHZ983090 VRV983048:VRV983090 WBR983048:WBR983090 WLN983048:WLN983090 WVJ983048:WVJ983090">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B50 IX8:IX50 ST8:ST50 ACP8:ACP50 AML8:AML50 AWH8:AWH50 BGD8:BGD50 BPZ8:BPZ50 BZV8:BZV50 CJR8:CJR50 CTN8:CTN50 DDJ8:DDJ50 DNF8:DNF50 DXB8:DXB50 EGX8:EGX50 EQT8:EQT50 FAP8:FAP50 FKL8:FKL50 FUH8:FUH50 GED8:GED50 GNZ8:GNZ50 GXV8:GXV50 HHR8:HHR50 HRN8:HRN50 IBJ8:IBJ50 ILF8:ILF50 IVB8:IVB50 JEX8:JEX50 JOT8:JOT50 JYP8:JYP50 KIL8:KIL50 KSH8:KSH50 LCD8:LCD50 LLZ8:LLZ50 LVV8:LVV50 MFR8:MFR50 MPN8:MPN50 MZJ8:MZJ50 NJF8:NJF50 NTB8:NTB50 OCX8:OCX50 OMT8:OMT50 OWP8:OWP50 PGL8:PGL50 PQH8:PQH50 QAD8:QAD50 QJZ8:QJZ50 QTV8:QTV50 RDR8:RDR50 RNN8:RNN50 RXJ8:RXJ50 SHF8:SHF50 SRB8:SRB50 TAX8:TAX50 TKT8:TKT50 TUP8:TUP50 UEL8:UEL50 UOH8:UOH50 UYD8:UYD50 VHZ8:VHZ50 VRV8:VRV50 WBR8:WBR50 WLN8:WLN50 WVJ8:WVJ50 B65544:B65586 IX65544:IX65586 ST65544:ST65586 ACP65544:ACP65586 AML65544:AML65586 AWH65544:AWH65586 BGD65544:BGD65586 BPZ65544:BPZ65586 BZV65544:BZV65586 CJR65544:CJR65586 CTN65544:CTN65586 DDJ65544:DDJ65586 DNF65544:DNF65586 DXB65544:DXB65586 EGX65544:EGX65586 EQT65544:EQT65586 FAP65544:FAP65586 FKL65544:FKL65586 FUH65544:FUH65586 GED65544:GED65586 GNZ65544:GNZ65586 GXV65544:GXV65586 HHR65544:HHR65586 HRN65544:HRN65586 IBJ65544:IBJ65586 ILF65544:ILF65586 IVB65544:IVB65586 JEX65544:JEX65586 JOT65544:JOT65586 JYP65544:JYP65586 KIL65544:KIL65586 KSH65544:KSH65586 LCD65544:LCD65586 LLZ65544:LLZ65586 LVV65544:LVV65586 MFR65544:MFR65586 MPN65544:MPN65586 MZJ65544:MZJ65586 NJF65544:NJF65586 NTB65544:NTB65586 OCX65544:OCX65586 OMT65544:OMT65586 OWP65544:OWP65586 PGL65544:PGL65586 PQH65544:PQH65586 QAD65544:QAD65586 QJZ65544:QJZ65586 QTV65544:QTV65586 RDR65544:RDR65586 RNN65544:RNN65586 RXJ65544:RXJ65586 SHF65544:SHF65586 SRB65544:SRB65586 TAX65544:TAX65586 TKT65544:TKT65586 TUP65544:TUP65586 UEL65544:UEL65586 UOH65544:UOH65586 UYD65544:UYD65586 VHZ65544:VHZ65586 VRV65544:VRV65586 WBR65544:WBR65586 WLN65544:WLN65586 WVJ65544:WVJ65586 B131080:B131122 IX131080:IX131122 ST131080:ST131122 ACP131080:ACP131122 AML131080:AML131122 AWH131080:AWH131122 BGD131080:BGD131122 BPZ131080:BPZ131122 BZV131080:BZV131122 CJR131080:CJR131122 CTN131080:CTN131122 DDJ131080:DDJ131122 DNF131080:DNF131122 DXB131080:DXB131122 EGX131080:EGX131122 EQT131080:EQT131122 FAP131080:FAP131122 FKL131080:FKL131122 FUH131080:FUH131122 GED131080:GED131122 GNZ131080:GNZ131122 GXV131080:GXV131122 HHR131080:HHR131122 HRN131080:HRN131122 IBJ131080:IBJ131122 ILF131080:ILF131122 IVB131080:IVB131122 JEX131080:JEX131122 JOT131080:JOT131122 JYP131080:JYP131122 KIL131080:KIL131122 KSH131080:KSH131122 LCD131080:LCD131122 LLZ131080:LLZ131122 LVV131080:LVV131122 MFR131080:MFR131122 MPN131080:MPN131122 MZJ131080:MZJ131122 NJF131080:NJF131122 NTB131080:NTB131122 OCX131080:OCX131122 OMT131080:OMT131122 OWP131080:OWP131122 PGL131080:PGL131122 PQH131080:PQH131122 QAD131080:QAD131122 QJZ131080:QJZ131122 QTV131080:QTV131122 RDR131080:RDR131122 RNN131080:RNN131122 RXJ131080:RXJ131122 SHF131080:SHF131122 SRB131080:SRB131122 TAX131080:TAX131122 TKT131080:TKT131122 TUP131080:TUP131122 UEL131080:UEL131122 UOH131080:UOH131122 UYD131080:UYD131122 VHZ131080:VHZ131122 VRV131080:VRV131122 WBR131080:WBR131122 WLN131080:WLN131122 WVJ131080:WVJ131122 B196616:B196658 IX196616:IX196658 ST196616:ST196658 ACP196616:ACP196658 AML196616:AML196658 AWH196616:AWH196658 BGD196616:BGD196658 BPZ196616:BPZ196658 BZV196616:BZV196658 CJR196616:CJR196658 CTN196616:CTN196658 DDJ196616:DDJ196658 DNF196616:DNF196658 DXB196616:DXB196658 EGX196616:EGX196658 EQT196616:EQT196658 FAP196616:FAP196658 FKL196616:FKL196658 FUH196616:FUH196658 GED196616:GED196658 GNZ196616:GNZ196658 GXV196616:GXV196658 HHR196616:HHR196658 HRN196616:HRN196658 IBJ196616:IBJ196658 ILF196616:ILF196658 IVB196616:IVB196658 JEX196616:JEX196658 JOT196616:JOT196658 JYP196616:JYP196658 KIL196616:KIL196658 KSH196616:KSH196658 LCD196616:LCD196658 LLZ196616:LLZ196658 LVV196616:LVV196658 MFR196616:MFR196658 MPN196616:MPN196658 MZJ196616:MZJ196658 NJF196616:NJF196658 NTB196616:NTB196658 OCX196616:OCX196658 OMT196616:OMT196658 OWP196616:OWP196658 PGL196616:PGL196658 PQH196616:PQH196658 QAD196616:QAD196658 QJZ196616:QJZ196658 QTV196616:QTV196658 RDR196616:RDR196658 RNN196616:RNN196658 RXJ196616:RXJ196658 SHF196616:SHF196658 SRB196616:SRB196658 TAX196616:TAX196658 TKT196616:TKT196658 TUP196616:TUP196658 UEL196616:UEL196658 UOH196616:UOH196658 UYD196616:UYD196658 VHZ196616:VHZ196658 VRV196616:VRV196658 WBR196616:WBR196658 WLN196616:WLN196658 WVJ196616:WVJ196658 B262152:B262194 IX262152:IX262194 ST262152:ST262194 ACP262152:ACP262194 AML262152:AML262194 AWH262152:AWH262194 BGD262152:BGD262194 BPZ262152:BPZ262194 BZV262152:BZV262194 CJR262152:CJR262194 CTN262152:CTN262194 DDJ262152:DDJ262194 DNF262152:DNF262194 DXB262152:DXB262194 EGX262152:EGX262194 EQT262152:EQT262194 FAP262152:FAP262194 FKL262152:FKL262194 FUH262152:FUH262194 GED262152:GED262194 GNZ262152:GNZ262194 GXV262152:GXV262194 HHR262152:HHR262194 HRN262152:HRN262194 IBJ262152:IBJ262194 ILF262152:ILF262194 IVB262152:IVB262194 JEX262152:JEX262194 JOT262152:JOT262194 JYP262152:JYP262194 KIL262152:KIL262194 KSH262152:KSH262194 LCD262152:LCD262194 LLZ262152:LLZ262194 LVV262152:LVV262194 MFR262152:MFR262194 MPN262152:MPN262194 MZJ262152:MZJ262194 NJF262152:NJF262194 NTB262152:NTB262194 OCX262152:OCX262194 OMT262152:OMT262194 OWP262152:OWP262194 PGL262152:PGL262194 PQH262152:PQH262194 QAD262152:QAD262194 QJZ262152:QJZ262194 QTV262152:QTV262194 RDR262152:RDR262194 RNN262152:RNN262194 RXJ262152:RXJ262194 SHF262152:SHF262194 SRB262152:SRB262194 TAX262152:TAX262194 TKT262152:TKT262194 TUP262152:TUP262194 UEL262152:UEL262194 UOH262152:UOH262194 UYD262152:UYD262194 VHZ262152:VHZ262194 VRV262152:VRV262194 WBR262152:WBR262194 WLN262152:WLN262194 WVJ262152:WVJ262194 B327688:B327730 IX327688:IX327730 ST327688:ST327730 ACP327688:ACP327730 AML327688:AML327730 AWH327688:AWH327730 BGD327688:BGD327730 BPZ327688:BPZ327730 BZV327688:BZV327730 CJR327688:CJR327730 CTN327688:CTN327730 DDJ327688:DDJ327730 DNF327688:DNF327730 DXB327688:DXB327730 EGX327688:EGX327730 EQT327688:EQT327730 FAP327688:FAP327730 FKL327688:FKL327730 FUH327688:FUH327730 GED327688:GED327730 GNZ327688:GNZ327730 GXV327688:GXV327730 HHR327688:HHR327730 HRN327688:HRN327730 IBJ327688:IBJ327730 ILF327688:ILF327730 IVB327688:IVB327730 JEX327688:JEX327730 JOT327688:JOT327730 JYP327688:JYP327730 KIL327688:KIL327730 KSH327688:KSH327730 LCD327688:LCD327730 LLZ327688:LLZ327730 LVV327688:LVV327730 MFR327688:MFR327730 MPN327688:MPN327730 MZJ327688:MZJ327730 NJF327688:NJF327730 NTB327688:NTB327730 OCX327688:OCX327730 OMT327688:OMT327730 OWP327688:OWP327730 PGL327688:PGL327730 PQH327688:PQH327730 QAD327688:QAD327730 QJZ327688:QJZ327730 QTV327688:QTV327730 RDR327688:RDR327730 RNN327688:RNN327730 RXJ327688:RXJ327730 SHF327688:SHF327730 SRB327688:SRB327730 TAX327688:TAX327730 TKT327688:TKT327730 TUP327688:TUP327730 UEL327688:UEL327730 UOH327688:UOH327730 UYD327688:UYD327730 VHZ327688:VHZ327730 VRV327688:VRV327730 WBR327688:WBR327730 WLN327688:WLN327730 WVJ327688:WVJ327730 B393224:B393266 IX393224:IX393266 ST393224:ST393266 ACP393224:ACP393266 AML393224:AML393266 AWH393224:AWH393266 BGD393224:BGD393266 BPZ393224:BPZ393266 BZV393224:BZV393266 CJR393224:CJR393266 CTN393224:CTN393266 DDJ393224:DDJ393266 DNF393224:DNF393266 DXB393224:DXB393266 EGX393224:EGX393266 EQT393224:EQT393266 FAP393224:FAP393266 FKL393224:FKL393266 FUH393224:FUH393266 GED393224:GED393266 GNZ393224:GNZ393266 GXV393224:GXV393266 HHR393224:HHR393266 HRN393224:HRN393266 IBJ393224:IBJ393266 ILF393224:ILF393266 IVB393224:IVB393266 JEX393224:JEX393266 JOT393224:JOT393266 JYP393224:JYP393266 KIL393224:KIL393266 KSH393224:KSH393266 LCD393224:LCD393266 LLZ393224:LLZ393266 LVV393224:LVV393266 MFR393224:MFR393266 MPN393224:MPN393266 MZJ393224:MZJ393266 NJF393224:NJF393266 NTB393224:NTB393266 OCX393224:OCX393266 OMT393224:OMT393266 OWP393224:OWP393266 PGL393224:PGL393266 PQH393224:PQH393266 QAD393224:QAD393266 QJZ393224:QJZ393266 QTV393224:QTV393266 RDR393224:RDR393266 RNN393224:RNN393266 RXJ393224:RXJ393266 SHF393224:SHF393266 SRB393224:SRB393266 TAX393224:TAX393266 TKT393224:TKT393266 TUP393224:TUP393266 UEL393224:UEL393266 UOH393224:UOH393266 UYD393224:UYD393266 VHZ393224:VHZ393266 VRV393224:VRV393266 WBR393224:WBR393266 WLN393224:WLN393266 WVJ393224:WVJ393266 B458760:B458802 IX458760:IX458802 ST458760:ST458802 ACP458760:ACP458802 AML458760:AML458802 AWH458760:AWH458802 BGD458760:BGD458802 BPZ458760:BPZ458802 BZV458760:BZV458802 CJR458760:CJR458802 CTN458760:CTN458802 DDJ458760:DDJ458802 DNF458760:DNF458802 DXB458760:DXB458802 EGX458760:EGX458802 EQT458760:EQT458802 FAP458760:FAP458802 FKL458760:FKL458802 FUH458760:FUH458802 GED458760:GED458802 GNZ458760:GNZ458802 GXV458760:GXV458802 HHR458760:HHR458802 HRN458760:HRN458802 IBJ458760:IBJ458802 ILF458760:ILF458802 IVB458760:IVB458802 JEX458760:JEX458802 JOT458760:JOT458802 JYP458760:JYP458802 KIL458760:KIL458802 KSH458760:KSH458802 LCD458760:LCD458802 LLZ458760:LLZ458802 LVV458760:LVV458802 MFR458760:MFR458802 MPN458760:MPN458802 MZJ458760:MZJ458802 NJF458760:NJF458802 NTB458760:NTB458802 OCX458760:OCX458802 OMT458760:OMT458802 OWP458760:OWP458802 PGL458760:PGL458802 PQH458760:PQH458802 QAD458760:QAD458802 QJZ458760:QJZ458802 QTV458760:QTV458802 RDR458760:RDR458802 RNN458760:RNN458802 RXJ458760:RXJ458802 SHF458760:SHF458802 SRB458760:SRB458802 TAX458760:TAX458802 TKT458760:TKT458802 TUP458760:TUP458802 UEL458760:UEL458802 UOH458760:UOH458802 UYD458760:UYD458802 VHZ458760:VHZ458802 VRV458760:VRV458802 WBR458760:WBR458802 WLN458760:WLN458802 WVJ458760:WVJ458802 B524296:B524338 IX524296:IX524338 ST524296:ST524338 ACP524296:ACP524338 AML524296:AML524338 AWH524296:AWH524338 BGD524296:BGD524338 BPZ524296:BPZ524338 BZV524296:BZV524338 CJR524296:CJR524338 CTN524296:CTN524338 DDJ524296:DDJ524338 DNF524296:DNF524338 DXB524296:DXB524338 EGX524296:EGX524338 EQT524296:EQT524338 FAP524296:FAP524338 FKL524296:FKL524338 FUH524296:FUH524338 GED524296:GED524338 GNZ524296:GNZ524338 GXV524296:GXV524338 HHR524296:HHR524338 HRN524296:HRN524338 IBJ524296:IBJ524338 ILF524296:ILF524338 IVB524296:IVB524338 JEX524296:JEX524338 JOT524296:JOT524338 JYP524296:JYP524338 KIL524296:KIL524338 KSH524296:KSH524338 LCD524296:LCD524338 LLZ524296:LLZ524338 LVV524296:LVV524338 MFR524296:MFR524338 MPN524296:MPN524338 MZJ524296:MZJ524338 NJF524296:NJF524338 NTB524296:NTB524338 OCX524296:OCX524338 OMT524296:OMT524338 OWP524296:OWP524338 PGL524296:PGL524338 PQH524296:PQH524338 QAD524296:QAD524338 QJZ524296:QJZ524338 QTV524296:QTV524338 RDR524296:RDR524338 RNN524296:RNN524338 RXJ524296:RXJ524338 SHF524296:SHF524338 SRB524296:SRB524338 TAX524296:TAX524338 TKT524296:TKT524338 TUP524296:TUP524338 UEL524296:UEL524338 UOH524296:UOH524338 UYD524296:UYD524338 VHZ524296:VHZ524338 VRV524296:VRV524338 WBR524296:WBR524338 WLN524296:WLN524338 WVJ524296:WVJ524338 B589832:B589874 IX589832:IX589874 ST589832:ST589874 ACP589832:ACP589874 AML589832:AML589874 AWH589832:AWH589874 BGD589832:BGD589874 BPZ589832:BPZ589874 BZV589832:BZV589874 CJR589832:CJR589874 CTN589832:CTN589874 DDJ589832:DDJ589874 DNF589832:DNF589874 DXB589832:DXB589874 EGX589832:EGX589874 EQT589832:EQT589874 FAP589832:FAP589874 FKL589832:FKL589874 FUH589832:FUH589874 GED589832:GED589874 GNZ589832:GNZ589874 GXV589832:GXV589874 HHR589832:HHR589874 HRN589832:HRN589874 IBJ589832:IBJ589874 ILF589832:ILF589874 IVB589832:IVB589874 JEX589832:JEX589874 JOT589832:JOT589874 JYP589832:JYP589874 KIL589832:KIL589874 KSH589832:KSH589874 LCD589832:LCD589874 LLZ589832:LLZ589874 LVV589832:LVV589874 MFR589832:MFR589874 MPN589832:MPN589874 MZJ589832:MZJ589874 NJF589832:NJF589874 NTB589832:NTB589874 OCX589832:OCX589874 OMT589832:OMT589874 OWP589832:OWP589874 PGL589832:PGL589874 PQH589832:PQH589874 QAD589832:QAD589874 QJZ589832:QJZ589874 QTV589832:QTV589874 RDR589832:RDR589874 RNN589832:RNN589874 RXJ589832:RXJ589874 SHF589832:SHF589874 SRB589832:SRB589874 TAX589832:TAX589874 TKT589832:TKT589874 TUP589832:TUP589874 UEL589832:UEL589874 UOH589832:UOH589874 UYD589832:UYD589874 VHZ589832:VHZ589874 VRV589832:VRV589874 WBR589832:WBR589874 WLN589832:WLN589874 WVJ589832:WVJ589874 B655368:B655410 IX655368:IX655410 ST655368:ST655410 ACP655368:ACP655410 AML655368:AML655410 AWH655368:AWH655410 BGD655368:BGD655410 BPZ655368:BPZ655410 BZV655368:BZV655410 CJR655368:CJR655410 CTN655368:CTN655410 DDJ655368:DDJ655410 DNF655368:DNF655410 DXB655368:DXB655410 EGX655368:EGX655410 EQT655368:EQT655410 FAP655368:FAP655410 FKL655368:FKL655410 FUH655368:FUH655410 GED655368:GED655410 GNZ655368:GNZ655410 GXV655368:GXV655410 HHR655368:HHR655410 HRN655368:HRN655410 IBJ655368:IBJ655410 ILF655368:ILF655410 IVB655368:IVB655410 JEX655368:JEX655410 JOT655368:JOT655410 JYP655368:JYP655410 KIL655368:KIL655410 KSH655368:KSH655410 LCD655368:LCD655410 LLZ655368:LLZ655410 LVV655368:LVV655410 MFR655368:MFR655410 MPN655368:MPN655410 MZJ655368:MZJ655410 NJF655368:NJF655410 NTB655368:NTB655410 OCX655368:OCX655410 OMT655368:OMT655410 OWP655368:OWP655410 PGL655368:PGL655410 PQH655368:PQH655410 QAD655368:QAD655410 QJZ655368:QJZ655410 QTV655368:QTV655410 RDR655368:RDR655410 RNN655368:RNN655410 RXJ655368:RXJ655410 SHF655368:SHF655410 SRB655368:SRB655410 TAX655368:TAX655410 TKT655368:TKT655410 TUP655368:TUP655410 UEL655368:UEL655410 UOH655368:UOH655410 UYD655368:UYD655410 VHZ655368:VHZ655410 VRV655368:VRV655410 WBR655368:WBR655410 WLN655368:WLN655410 WVJ655368:WVJ655410 B720904:B720946 IX720904:IX720946 ST720904:ST720946 ACP720904:ACP720946 AML720904:AML720946 AWH720904:AWH720946 BGD720904:BGD720946 BPZ720904:BPZ720946 BZV720904:BZV720946 CJR720904:CJR720946 CTN720904:CTN720946 DDJ720904:DDJ720946 DNF720904:DNF720946 DXB720904:DXB720946 EGX720904:EGX720946 EQT720904:EQT720946 FAP720904:FAP720946 FKL720904:FKL720946 FUH720904:FUH720946 GED720904:GED720946 GNZ720904:GNZ720946 GXV720904:GXV720946 HHR720904:HHR720946 HRN720904:HRN720946 IBJ720904:IBJ720946 ILF720904:ILF720946 IVB720904:IVB720946 JEX720904:JEX720946 JOT720904:JOT720946 JYP720904:JYP720946 KIL720904:KIL720946 KSH720904:KSH720946 LCD720904:LCD720946 LLZ720904:LLZ720946 LVV720904:LVV720946 MFR720904:MFR720946 MPN720904:MPN720946 MZJ720904:MZJ720946 NJF720904:NJF720946 NTB720904:NTB720946 OCX720904:OCX720946 OMT720904:OMT720946 OWP720904:OWP720946 PGL720904:PGL720946 PQH720904:PQH720946 QAD720904:QAD720946 QJZ720904:QJZ720946 QTV720904:QTV720946 RDR720904:RDR720946 RNN720904:RNN720946 RXJ720904:RXJ720946 SHF720904:SHF720946 SRB720904:SRB720946 TAX720904:TAX720946 TKT720904:TKT720946 TUP720904:TUP720946 UEL720904:UEL720946 UOH720904:UOH720946 UYD720904:UYD720946 VHZ720904:VHZ720946 VRV720904:VRV720946 WBR720904:WBR720946 WLN720904:WLN720946 WVJ720904:WVJ720946 B786440:B786482 IX786440:IX786482 ST786440:ST786482 ACP786440:ACP786482 AML786440:AML786482 AWH786440:AWH786482 BGD786440:BGD786482 BPZ786440:BPZ786482 BZV786440:BZV786482 CJR786440:CJR786482 CTN786440:CTN786482 DDJ786440:DDJ786482 DNF786440:DNF786482 DXB786440:DXB786482 EGX786440:EGX786482 EQT786440:EQT786482 FAP786440:FAP786482 FKL786440:FKL786482 FUH786440:FUH786482 GED786440:GED786482 GNZ786440:GNZ786482 GXV786440:GXV786482 HHR786440:HHR786482 HRN786440:HRN786482 IBJ786440:IBJ786482 ILF786440:ILF786482 IVB786440:IVB786482 JEX786440:JEX786482 JOT786440:JOT786482 JYP786440:JYP786482 KIL786440:KIL786482 KSH786440:KSH786482 LCD786440:LCD786482 LLZ786440:LLZ786482 LVV786440:LVV786482 MFR786440:MFR786482 MPN786440:MPN786482 MZJ786440:MZJ786482 NJF786440:NJF786482 NTB786440:NTB786482 OCX786440:OCX786482 OMT786440:OMT786482 OWP786440:OWP786482 PGL786440:PGL786482 PQH786440:PQH786482 QAD786440:QAD786482 QJZ786440:QJZ786482 QTV786440:QTV786482 RDR786440:RDR786482 RNN786440:RNN786482 RXJ786440:RXJ786482 SHF786440:SHF786482 SRB786440:SRB786482 TAX786440:TAX786482 TKT786440:TKT786482 TUP786440:TUP786482 UEL786440:UEL786482 UOH786440:UOH786482 UYD786440:UYD786482 VHZ786440:VHZ786482 VRV786440:VRV786482 WBR786440:WBR786482 WLN786440:WLN786482 WVJ786440:WVJ786482 B851976:B852018 IX851976:IX852018 ST851976:ST852018 ACP851976:ACP852018 AML851976:AML852018 AWH851976:AWH852018 BGD851976:BGD852018 BPZ851976:BPZ852018 BZV851976:BZV852018 CJR851976:CJR852018 CTN851976:CTN852018 DDJ851976:DDJ852018 DNF851976:DNF852018 DXB851976:DXB852018 EGX851976:EGX852018 EQT851976:EQT852018 FAP851976:FAP852018 FKL851976:FKL852018 FUH851976:FUH852018 GED851976:GED852018 GNZ851976:GNZ852018 GXV851976:GXV852018 HHR851976:HHR852018 HRN851976:HRN852018 IBJ851976:IBJ852018 ILF851976:ILF852018 IVB851976:IVB852018 JEX851976:JEX852018 JOT851976:JOT852018 JYP851976:JYP852018 KIL851976:KIL852018 KSH851976:KSH852018 LCD851976:LCD852018 LLZ851976:LLZ852018 LVV851976:LVV852018 MFR851976:MFR852018 MPN851976:MPN852018 MZJ851976:MZJ852018 NJF851976:NJF852018 NTB851976:NTB852018 OCX851976:OCX852018 OMT851976:OMT852018 OWP851976:OWP852018 PGL851976:PGL852018 PQH851976:PQH852018 QAD851976:QAD852018 QJZ851976:QJZ852018 QTV851976:QTV852018 RDR851976:RDR852018 RNN851976:RNN852018 RXJ851976:RXJ852018 SHF851976:SHF852018 SRB851976:SRB852018 TAX851976:TAX852018 TKT851976:TKT852018 TUP851976:TUP852018 UEL851976:UEL852018 UOH851976:UOH852018 UYD851976:UYD852018 VHZ851976:VHZ852018 VRV851976:VRV852018 WBR851976:WBR852018 WLN851976:WLN852018 WVJ851976:WVJ852018 B917512:B917554 IX917512:IX917554 ST917512:ST917554 ACP917512:ACP917554 AML917512:AML917554 AWH917512:AWH917554 BGD917512:BGD917554 BPZ917512:BPZ917554 BZV917512:BZV917554 CJR917512:CJR917554 CTN917512:CTN917554 DDJ917512:DDJ917554 DNF917512:DNF917554 DXB917512:DXB917554 EGX917512:EGX917554 EQT917512:EQT917554 FAP917512:FAP917554 FKL917512:FKL917554 FUH917512:FUH917554 GED917512:GED917554 GNZ917512:GNZ917554 GXV917512:GXV917554 HHR917512:HHR917554 HRN917512:HRN917554 IBJ917512:IBJ917554 ILF917512:ILF917554 IVB917512:IVB917554 JEX917512:JEX917554 JOT917512:JOT917554 JYP917512:JYP917554 KIL917512:KIL917554 KSH917512:KSH917554 LCD917512:LCD917554 LLZ917512:LLZ917554 LVV917512:LVV917554 MFR917512:MFR917554 MPN917512:MPN917554 MZJ917512:MZJ917554 NJF917512:NJF917554 NTB917512:NTB917554 OCX917512:OCX917554 OMT917512:OMT917554 OWP917512:OWP917554 PGL917512:PGL917554 PQH917512:PQH917554 QAD917512:QAD917554 QJZ917512:QJZ917554 QTV917512:QTV917554 RDR917512:RDR917554 RNN917512:RNN917554 RXJ917512:RXJ917554 SHF917512:SHF917554 SRB917512:SRB917554 TAX917512:TAX917554 TKT917512:TKT917554 TUP917512:TUP917554 UEL917512:UEL917554 UOH917512:UOH917554 UYD917512:UYD917554 VHZ917512:VHZ917554 VRV917512:VRV917554 WBR917512:WBR917554 WLN917512:WLN917554 WVJ917512:WVJ917554 B983048:B983090 IX983048:IX983090 ST983048:ST983090 ACP983048:ACP983090 AML983048:AML983090 AWH983048:AWH983090 BGD983048:BGD983090 BPZ983048:BPZ983090 BZV983048:BZV983090 CJR983048:CJR983090 CTN983048:CTN983090 DDJ983048:DDJ983090 DNF983048:DNF983090 DXB983048:DXB983090 EGX983048:EGX983090 EQT983048:EQT983090 FAP983048:FAP983090 FKL983048:FKL983090 FUH983048:FUH983090 GED983048:GED983090 GNZ983048:GNZ983090 GXV983048:GXV983090 HHR983048:HHR983090 HRN983048:HRN983090 IBJ983048:IBJ983090 ILF983048:ILF983090 IVB983048:IVB983090 JEX983048:JEX983090 JOT983048:JOT983090 JYP983048:JYP983090 KIL983048:KIL983090 KSH983048:KSH983090 LCD983048:LCD983090 LLZ983048:LLZ983090 LVV983048:LVV983090 MFR983048:MFR983090 MPN983048:MPN983090 MZJ983048:MZJ983090 NJF983048:NJF983090 NTB983048:NTB983090 OCX983048:OCX983090 OMT983048:OMT983090 OWP983048:OWP983090 PGL983048:PGL983090 PQH983048:PQH983090 QAD983048:QAD983090 QJZ983048:QJZ983090 QTV983048:QTV983090 RDR983048:RDR983090 RNN983048:RNN983090 RXJ983048:RXJ983090 SHF983048:SHF983090 SRB983048:SRB983090 TAX983048:TAX983090 TKT983048:TKT983090 TUP983048:TUP983090 UEL983048:UEL983090 UOH983048:UOH983090 UYD983048:UYD983090 VHZ983048:VHZ983090 VRV983048:VRV983090 WBR983048:WBR983090 WLN983048:WLN983090 WVJ983048:WVJ983090" xr:uid="{3BCDAFA9-70FD-42ED-B088-113DD368B30F}">
       <formula1>8</formula1>
       <formula2>8</formula2>
     </dataValidation>

</xml_diff>